<commit_message>
place order page and data xlx
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/Test_Data.xlsx
+++ b/src/main/resources/test_data/Test_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verkh\IdeaProjects\pom6\src\main\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13FCD2E-08CD-44C9-A780-2AA02D357616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0508121D-B3D8-413C-A51B-122EAD547857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1500" windowWidth="23040" windowHeight="12180" xr2:uid="{56D596F5-221D-421D-9FC5-55182B639D44}"/>
+    <workbookView xWindow="0" yWindow="1500" windowWidth="23040" windowHeight="12180" activeTab="1" xr2:uid="{56D596F5-221D-421D-9FC5-55182B639D44}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="2" r:id="rId1"/>
@@ -1280,8 +1280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{955D89E2-A883-499B-AA82-70224D6F8F96}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2042,7 +2042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0775DEA-3893-49AA-8C48-45DC29C761B9}">
   <dimension ref="A1:AE16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
data updated and place order page
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/Test_Data.xlsx
+++ b/src/main/resources/test_data/Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verkh\IdeaProjects\pom6\src\main\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A1E8A6-1E4C-40E2-B273-2A8DCAF4382B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622F14EF-7B4D-43E0-AA2E-273DFEAD8CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1500" windowWidth="23040" windowHeight="12180" activeTab="1" xr2:uid="{56D596F5-221D-421D-9FC5-55182B639D44}"/>
   </bookViews>
@@ -714,28 +714,28 @@
     <t>Error: An account is already registered with that username. Please choose another.</t>
   </si>
   <si>
-    <t>AutomationTestPalatine8</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine9</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine8@gmail.com</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine9@gmail.com</t>
-  </si>
-  <si>
-    <t>TestChicagoCity7</t>
-  </si>
-  <si>
-    <t>TestChicagoCity7@gmail.com</t>
-  </si>
-  <si>
-    <t>TestChicagoCity8</t>
-  </si>
-  <si>
-    <t>TestChicagoCity8@gmail.com</t>
+    <t>AutomationTestPalatine10</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine10@gmail.com</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine11</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine11@gmail.com</t>
+  </si>
+  <si>
+    <t>TestChicagoCity9</t>
+  </si>
+  <si>
+    <t>TestChicagoCity9@gmail.com</t>
+  </si>
+  <si>
+    <t>TestChicagoCity10</t>
+  </si>
+  <si>
+    <t>TestChicagoCity10@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1284,8 +1284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{955D89E2-A883-499B-AA82-70224D6F8F96}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1368,7 +1368,7 @@
         <v>222</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>43</v>
@@ -1403,7 +1403,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>222</v>
@@ -2047,7 +2047,7 @@
   <dimension ref="A1:AD16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated data driver and store page
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/Test_Data.xlsx
+++ b/src/main/resources/test_data/Test_Data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verkh\IdeaProjects\pom6\src\main\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909CA855-F02F-4052-985F-73C9F39211CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52733BE-9755-4EFB-BEBB-8CAB78EE701E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="594" xr2:uid="{56D596F5-221D-421D-9FC5-55182B639D44}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="594" activeTab="1" xr2:uid="{56D596F5-221D-421D-9FC5-55182B639D44}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="2" r:id="rId1"/>
     <sheet name="order" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="267">
   <si>
     <t>run</t>
   </si>
@@ -381,9 +382,6 @@
     <t>58604</t>
   </si>
   <si>
-    <t>@mail.com</t>
-  </si>
-  <si>
     <t>TestChicagoCity</t>
   </si>
   <si>
@@ -633,214 +631,214 @@
     <t>home139</t>
   </si>
   <si>
-    <t>TestChicagoCity185</t>
-  </si>
-  <si>
-    <t>TestChicagoCity185@mail.com</t>
-  </si>
-  <si>
-    <t>TestChicagoCity186</t>
-  </si>
-  <si>
-    <t>TestChicagoCity186@mail.com</t>
-  </si>
-  <si>
-    <t>TestChicagoCity187</t>
-  </si>
-  <si>
-    <t>TestChicagoCity187@mail.com</t>
-  </si>
-  <si>
-    <t>TestChicagoCity188</t>
-  </si>
-  <si>
-    <t>TestChicagoCity188@mail.com</t>
-  </si>
-  <si>
-    <t>TestChicagoCity189</t>
-  </si>
-  <si>
-    <t>TestChicagoCity189@mail.com</t>
-  </si>
-  <si>
-    <t>TestChicagoCity190</t>
-  </si>
-  <si>
-    <t>TestChicagoCity190@mail.com</t>
-  </si>
-  <si>
-    <t>TestChicagoCity191</t>
-  </si>
-  <si>
-    <t>TestChicagoCity191@mail.com</t>
-  </si>
-  <si>
-    <t>TestChicagoCity192</t>
-  </si>
-  <si>
-    <t>TestChicagoCity192@mail.com</t>
-  </si>
-  <si>
-    <t>TestChicagoCity193</t>
-  </si>
-  <si>
-    <t>TestChicagoCity193@mail.com</t>
-  </si>
-  <si>
-    <t>TestChicagoCity194</t>
-  </si>
-  <si>
-    <t>TestChicagoCity194@mail.com</t>
-  </si>
-  <si>
-    <t>TestChicagoCity195</t>
-  </si>
-  <si>
-    <t>TestChicagoCity195@mail.com</t>
-  </si>
-  <si>
-    <t>TestChicagoCity196</t>
-  </si>
-  <si>
-    <t>TestChicagoCity196@mail.com</t>
-  </si>
-  <si>
-    <t>TestChicagoCity197</t>
-  </si>
-  <si>
-    <t>TestChicagoCity197@mail.com</t>
-  </si>
-  <si>
-    <t>TestChicagoCity198</t>
-  </si>
-  <si>
-    <t>TestChicagoCity198@mail.com</t>
-  </si>
-  <si>
-    <t>TestChicagoCity199</t>
-  </si>
-  <si>
-    <t>TestChicagoCity199@mail.com</t>
-  </si>
-  <si>
-    <t>TestChicagoCity200</t>
-  </si>
-  <si>
-    <t>TestChicagoCity200@mail.com</t>
-  </si>
-  <si>
-    <t>TestChicagoCity201</t>
-  </si>
-  <si>
-    <t>TestChicagoCity201@mail.com</t>
-  </si>
-  <si>
-    <t>TestChicagoCity202</t>
-  </si>
-  <si>
-    <t>TestChicagoCity202@mail.com</t>
-  </si>
-  <si>
-    <t>TestChicagoCity203</t>
-  </si>
-  <si>
-    <t>TestChicagoCity203@mail.com</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine155</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine155@gmail.com</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine156</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine156@gmail.com</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine157</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine157@gmail.com</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine158</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine158@gmail.com</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine159</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine159@gmail.com</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine160</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine160@gmail.com</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine161</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine161@gmail.com</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine162</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine162@gmail.com</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine163</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine163@gmail.com</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine164</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine164@gmail.com</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine165</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine165@gmail.com</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine166</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine166@gmail.com</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine167</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine167@gmail.com</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine168</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine168@gmail.com</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine169</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine169@gmail.com</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine170</t>
-  </si>
-  <si>
-    <t>AutomationTestPalatine170@gmail.com</t>
+    <t>TestChicagoCity204</t>
+  </si>
+  <si>
+    <t>TestChicagoCity204@gmail.com</t>
+  </si>
+  <si>
+    <t>TestChicagoCity205</t>
+  </si>
+  <si>
+    <t>TestChicagoCity205@gmail.com</t>
+  </si>
+  <si>
+    <t>TestChicagoCity206</t>
+  </si>
+  <si>
+    <t>TestChicagoCity206@gmail.com</t>
+  </si>
+  <si>
+    <t>TestChicagoCity207</t>
+  </si>
+  <si>
+    <t>TestChicagoCity207@gmail.com</t>
+  </si>
+  <si>
+    <t>TestChicagoCity208</t>
+  </si>
+  <si>
+    <t>TestChicagoCity208@gmail.com</t>
+  </si>
+  <si>
+    <t>TestChicagoCity209</t>
+  </si>
+  <si>
+    <t>TestChicagoCity209@gmail.com</t>
+  </si>
+  <si>
+    <t>TestChicagoCity210</t>
+  </si>
+  <si>
+    <t>TestChicagoCity210@gmail.com</t>
+  </si>
+  <si>
+    <t>TestChicagoCity211</t>
+  </si>
+  <si>
+    <t>TestChicagoCity211@gmail.com</t>
+  </si>
+  <si>
+    <t>TestChicagoCity212</t>
+  </si>
+  <si>
+    <t>TestChicagoCity212@gmail.com</t>
+  </si>
+  <si>
+    <t>TestChicagoCity213</t>
+  </si>
+  <si>
+    <t>TestChicagoCity213@gmail.com</t>
+  </si>
+  <si>
+    <t>TestChicagoCity214</t>
+  </si>
+  <si>
+    <t>TestChicagoCity214@gmail.com</t>
+  </si>
+  <si>
+    <t>TestChicagoCity215</t>
+  </si>
+  <si>
+    <t>TestChicagoCity215@gmail.com</t>
+  </si>
+  <si>
+    <t>TestChicagoCity216</t>
+  </si>
+  <si>
+    <t>TestChicagoCity216@gmail.com</t>
+  </si>
+  <si>
+    <t>TestChicagoCity217</t>
+  </si>
+  <si>
+    <t>TestChicagoCity217@gmail.com</t>
+  </si>
+  <si>
+    <t>TestChicagoCity218</t>
+  </si>
+  <si>
+    <t>TestChicagoCity218@gmail.com</t>
+  </si>
+  <si>
+    <t>TestChicagoCity219</t>
+  </si>
+  <si>
+    <t>TestChicagoCity219@gmail.com</t>
+  </si>
+  <si>
+    <t>TestChicagoCity220</t>
+  </si>
+  <si>
+    <t>TestChicagoCity220@gmail.com</t>
+  </si>
+  <si>
+    <t>TestChicagoCity221</t>
+  </si>
+  <si>
+    <t>TestChicagoCity221@gmail.com</t>
+  </si>
+  <si>
+    <t>TestChicagoCity222</t>
+  </si>
+  <si>
+    <t>TestChicagoCity222@gmail.com</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine171</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine171@gmail.com</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine172</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine172@gmail.com</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine173</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine173@gmail.com</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine174</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine174@gmail.com</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine175</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine175@gmail.com</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine176</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine176@gmail.com</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine177</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine177@gmail.com</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine178</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine178@gmail.com</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine179</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine179@gmail.com</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine180</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine180@gmail.com</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine181</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine181@gmail.com</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine182</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine182@gmail.com</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine183</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine183@gmail.com</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine184</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine184@gmail.com</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine185</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine185@gmail.com</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine186</t>
+  </si>
+  <si>
+    <t>AutomationTestPalatine186@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1367,8 +1365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{955D89E2-A883-499B-AA82-70224D6F8F96}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1451,13 +1449,13 @@
         <v>82</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="I2" s="11" t="s">
         <v>236</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>237</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>30</v>
@@ -1474,12 +1472,7 @@
       <c r="N2" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="O2">
-        <v>155</v>
-      </c>
-      <c r="P2" s="19" t="s">
-        <v>116</v>
-      </c>
+      <c r="P2" s="19"/>
     </row>
     <row r="3" spans="1:16" ht="22.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -1499,13 +1492,13 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="I3" s="11" t="s">
         <v>238</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>239</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>61</v>
@@ -1521,9 +1514,6 @@
       </c>
       <c r="N3" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="O3">
-        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="22.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1544,13 +1534,13 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="I4" s="11" t="s">
         <v>240</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>241</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>30</v>
@@ -1566,9 +1556,6 @@
       </c>
       <c r="N4" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="O4">
-        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="22.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1589,13 +1576,13 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="I5" s="11" t="s">
         <v>242</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>243</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>61</v>
@@ -1611,9 +1598,6 @@
       </c>
       <c r="N5" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="O5">
-        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="22.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1634,13 +1618,13 @@
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="I6" s="11" t="s">
         <v>244</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>245</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>30</v>
@@ -1656,9 +1640,6 @@
       </c>
       <c r="N6" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="O6">
-        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="22.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1679,13 +1660,13 @@
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="I7" s="11" t="s">
         <v>246</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>247</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>61</v>
@@ -1701,9 +1682,6 @@
       </c>
       <c r="N7" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="O7">
-        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="22.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1724,13 +1702,13 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="I8" s="11" t="s">
         <v>248</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>249</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>30</v>
@@ -1746,9 +1724,6 @@
       </c>
       <c r="N8" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="O8">
-        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="22.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1769,13 +1744,13 @@
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="I9" s="11" t="s">
         <v>250</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>251</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>61</v>
@@ -1791,9 +1766,6 @@
       </c>
       <c r="N9" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="O9">
-        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="22.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1814,13 +1786,13 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="I10" s="11" t="s">
         <v>252</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>253</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>30</v>
@@ -1836,9 +1808,6 @@
       </c>
       <c r="N10" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="O10">
-        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="22.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1859,13 +1828,13 @@
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="I11" s="11" t="s">
         <v>254</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>255</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>61</v>
@@ -1881,9 +1850,6 @@
       </c>
       <c r="N11" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="O11">
-        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="22.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1904,13 +1870,13 @@
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="I12" s="11" t="s">
         <v>256</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>257</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>30</v>
@@ -1926,9 +1892,6 @@
       </c>
       <c r="N12" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="O12">
-        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="22.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1949,13 +1912,13 @@
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="I13" s="11" t="s">
         <v>258</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>259</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>61</v>
@@ -1971,9 +1934,6 @@
       </c>
       <c r="N13" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="O13">
-        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="22.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1994,13 +1954,13 @@
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="I14" s="11" t="s">
         <v>260</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>261</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>30</v>
@@ -2016,9 +1976,6 @@
       </c>
       <c r="N14" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="O14">
-        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="22.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2039,13 +1996,13 @@
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="I15" s="11" t="s">
         <v>262</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>263</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>61</v>
@@ -2061,9 +2018,6 @@
       </c>
       <c r="N15" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="O15">
-        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="22.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2084,13 +2038,13 @@
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="I16" s="11" t="s">
         <v>264</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>265</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>30</v>
@@ -2107,11 +2061,8 @@
       <c r="N16" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="O16">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="22.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:14" ht="22.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
@@ -2129,13 +2080,13 @@
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="I17" s="11" t="s">
         <v>266</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>267</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>61</v>
@@ -2151,9 +2102,6 @@
       </c>
       <c r="N17" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="O17">
-        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2194,8 +2142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0775DEA-3893-49AA-8C48-45DC29C761B9}">
   <dimension ref="A1:AG20"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AF2" sqref="AF2:AH25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2336,10 +2284,10 @@
         <v>80</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F2" s="4">
         <v>1</v>
@@ -2351,22 +2299,22 @@
         <v>44</v>
       </c>
       <c r="I2" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>67</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>27</v>
@@ -2378,19 +2326,19 @@
         <v>81</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="S2" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="U2" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="T2" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="U2" s="11" t="s">
-        <v>199</v>
-      </c>
       <c r="V2" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="W2" s="5" t="s">
         <v>31</v>
@@ -2399,16 +2347,16 @@
         <v>44</v>
       </c>
       <c r="Y2" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z2" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="Z2" s="5" t="s">
-        <v>123</v>
-      </c>
       <c r="AA2" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB2" s="6" t="s">
         <v>128</v>
-      </c>
-      <c r="AB2" s="6" t="s">
-        <v>129</v>
       </c>
       <c r="AC2" s="6" t="s">
         <v>23</v>
@@ -2419,12 +2367,7 @@
       <c r="AE2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="AF2">
-        <v>185</v>
-      </c>
-      <c r="AG2" s="18" t="s">
-        <v>114</v>
-      </c>
+      <c r="AG2" s="18"/>
     </row>
     <row r="3" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
@@ -2437,10 +2380,10 @@
         <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F3" s="4">
         <v>2</v>
@@ -2452,16 +2395,16 @@
         <v>45</v>
       </c>
       <c r="I3" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="6" t="s">
         <v>132</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>133</v>
       </c>
       <c r="M3" s="6" t="s">
         <v>23</v>
@@ -2480,16 +2423,16 @@
       </c>
       <c r="R3" s="7"/>
       <c r="S3" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="U3" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="T3" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="U3" s="11" t="s">
-        <v>201</v>
-      </c>
       <c r="V3" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="W3" s="5" t="s">
         <v>32</v>
@@ -2498,16 +2441,16 @@
         <v>45</v>
       </c>
       <c r="Y3" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Z3" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AA3" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="AB3" s="6" t="s">
         <v>134</v>
-      </c>
-      <c r="AB3" s="6" t="s">
-        <v>135</v>
       </c>
       <c r="AC3" s="6" t="s">
         <v>23</v>
@@ -2517,9 +2460,6 @@
       </c>
       <c r="AE3" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="AF3">
-        <v>186</v>
       </c>
       <c r="AG3" s="18"/>
     </row>
@@ -2534,10 +2474,10 @@
         <v>80</v>
       </c>
       <c r="D4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F4" s="4">
         <v>1</v>
@@ -2549,22 +2489,22 @@
         <v>46</v>
       </c>
       <c r="I4" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="K4" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J4" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="K4" s="6" t="s">
+      <c r="L4" s="6" t="s">
         <v>138</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>139</v>
       </c>
       <c r="M4" s="6" t="s">
         <v>67</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O4" s="4" t="s">
         <v>27</v>
@@ -2577,16 +2517,16 @@
       </c>
       <c r="R4" s="7"/>
       <c r="S4" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="U4" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="T4" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="U4" s="11" t="s">
-        <v>203</v>
-      </c>
       <c r="V4" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="W4" s="5" t="s">
         <v>33</v>
@@ -2595,16 +2535,16 @@
         <v>46</v>
       </c>
       <c r="Y4" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Z4" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AA4" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB4" s="6" t="s">
         <v>140</v>
-      </c>
-      <c r="AB4" s="6" t="s">
-        <v>141</v>
       </c>
       <c r="AC4" s="6" t="s">
         <v>23</v>
@@ -2614,9 +2554,6 @@
       </c>
       <c r="AE4" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="AF4">
-        <v>187</v>
       </c>
       <c r="AG4" s="18"/>
     </row>
@@ -2631,10 +2568,10 @@
         <v>80</v>
       </c>
       <c r="D5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F5" s="4">
         <v>2</v>
@@ -2646,16 +2583,16 @@
         <v>47</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K5" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>128</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>129</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>23</v>
@@ -2674,16 +2611,16 @@
       </c>
       <c r="R5" s="7"/>
       <c r="S5" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="U5" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="T5" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="U5" s="11" t="s">
-        <v>205</v>
-      </c>
       <c r="V5" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="W5" s="5" t="s">
         <v>34</v>
@@ -2692,16 +2629,16 @@
         <v>47</v>
       </c>
       <c r="Y5" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z5" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA5" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="Z5" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA5" s="6" t="s">
+      <c r="AB5" s="6" t="s">
         <v>144</v>
-      </c>
-      <c r="AB5" s="6" t="s">
-        <v>145</v>
       </c>
       <c r="AC5" s="6" t="s">
         <v>23</v>
@@ -2711,9 +2648,6 @@
       </c>
       <c r="AE5" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="AF5">
-        <v>188</v>
       </c>
       <c r="AG5" s="18"/>
     </row>
@@ -2728,10 +2662,10 @@
         <v>80</v>
       </c>
       <c r="D6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F6" s="4">
         <v>1</v>
@@ -2743,22 +2677,22 @@
         <v>48</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K6" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>134</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>135</v>
       </c>
       <c r="M6" s="6" t="s">
         <v>67</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O6" s="4" t="s">
         <v>27</v>
@@ -2771,16 +2705,16 @@
       </c>
       <c r="R6" s="7"/>
       <c r="S6" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="U6" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="T6" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="U6" s="11" t="s">
-        <v>207</v>
-      </c>
       <c r="V6" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="W6" s="5" t="s">
         <v>35</v>
@@ -2789,16 +2723,16 @@
         <v>48</v>
       </c>
       <c r="Y6" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="Z6" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA6" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="Z6" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA6" s="6" t="s">
+      <c r="AB6" s="6" t="s">
         <v>148</v>
-      </c>
-      <c r="AB6" s="6" t="s">
-        <v>149</v>
       </c>
       <c r="AC6" s="6" t="s">
         <v>23</v>
@@ -2808,9 +2742,6 @@
       </c>
       <c r="AE6" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="AF6">
-        <v>189</v>
       </c>
       <c r="AG6" s="18"/>
     </row>
@@ -2825,10 +2756,10 @@
         <v>80</v>
       </c>
       <c r="D7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F7" s="4">
         <v>2</v>
@@ -2840,16 +2771,16 @@
         <v>49</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K7" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="L7" s="6" t="s">
         <v>140</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>141</v>
       </c>
       <c r="M7" s="6" t="s">
         <v>23</v>
@@ -2868,16 +2799,16 @@
       </c>
       <c r="R7" s="7"/>
       <c r="S7" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="U7" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="T7" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="U7" s="11" t="s">
-        <v>209</v>
-      </c>
       <c r="V7" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="W7" s="5" t="s">
         <v>36</v>
@@ -2886,16 +2817,16 @@
         <v>49</v>
       </c>
       <c r="Y7" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z7" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA7" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="Z7" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA7" s="6" t="s">
+      <c r="AB7" s="6" t="s">
         <v>152</v>
-      </c>
-      <c r="AB7" s="6" t="s">
-        <v>153</v>
       </c>
       <c r="AC7" s="6" t="s">
         <v>23</v>
@@ -2905,9 +2836,6 @@
       </c>
       <c r="AE7" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="AF7">
-        <v>190</v>
       </c>
       <c r="AG7" s="18"/>
     </row>
@@ -2922,10 +2850,10 @@
         <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F8" s="4">
         <v>1</v>
@@ -2937,22 +2865,22 @@
         <v>50</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K8" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="L8" s="6" t="s">
         <v>144</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>145</v>
       </c>
       <c r="M8" s="6" t="s">
         <v>67</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O8" s="4" t="s">
         <v>27</v>
@@ -2965,16 +2893,16 @@
       </c>
       <c r="R8" s="7"/>
       <c r="S8" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="U8" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="T8" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="U8" s="11" t="s">
-        <v>211</v>
-      </c>
       <c r="V8" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="W8" s="5" t="s">
         <v>37</v>
@@ -2983,16 +2911,16 @@
         <v>50</v>
       </c>
       <c r="Y8" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z8" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA8" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="Z8" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA8" s="6" t="s">
+      <c r="AB8" s="6" t="s">
         <v>156</v>
-      </c>
-      <c r="AB8" s="6" t="s">
-        <v>157</v>
       </c>
       <c r="AC8" s="6" t="s">
         <v>23</v>
@@ -3002,9 +2930,6 @@
       </c>
       <c r="AE8" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="AF8">
-        <v>191</v>
       </c>
       <c r="AG8" s="18"/>
     </row>
@@ -3019,10 +2944,10 @@
         <v>80</v>
       </c>
       <c r="D9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F9" s="4">
         <v>2</v>
@@ -3034,16 +2959,16 @@
         <v>51</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K9" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="L9" s="6" t="s">
         <v>148</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>149</v>
       </c>
       <c r="M9" s="6" t="s">
         <v>23</v>
@@ -3062,16 +2987,16 @@
       </c>
       <c r="R9" s="7"/>
       <c r="S9" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="U9" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="T9" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="U9" s="11" t="s">
-        <v>213</v>
-      </c>
       <c r="V9" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="W9" s="5" t="s">
         <v>38</v>
@@ -3080,16 +3005,16 @@
         <v>51</v>
       </c>
       <c r="Y9" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z9" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA9" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="Z9" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA9" s="6" t="s">
+      <c r="AB9" s="6" t="s">
         <v>160</v>
-      </c>
-      <c r="AB9" s="6" t="s">
-        <v>161</v>
       </c>
       <c r="AC9" s="6" t="s">
         <v>23</v>
@@ -3099,9 +3024,6 @@
       </c>
       <c r="AE9" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="AF9">
-        <v>192</v>
       </c>
       <c r="AG9" s="18"/>
     </row>
@@ -3116,10 +3038,10 @@
         <v>80</v>
       </c>
       <c r="D10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F10" s="4">
         <v>1</v>
@@ -3131,22 +3053,22 @@
         <v>52</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K10" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="L10" s="6" t="s">
         <v>152</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>153</v>
       </c>
       <c r="M10" s="6" t="s">
         <v>67</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O10" s="4" t="s">
         <v>27</v>
@@ -3159,16 +3081,16 @@
       </c>
       <c r="R10" s="7"/>
       <c r="S10" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="U10" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="T10" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="U10" s="11" t="s">
-        <v>215</v>
-      </c>
       <c r="V10" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="W10" s="5" t="s">
         <v>39</v>
@@ -3177,16 +3099,16 @@
         <v>52</v>
       </c>
       <c r="Y10" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="Z10" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA10" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="Z10" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA10" s="6" t="s">
+      <c r="AB10" s="6" t="s">
         <v>164</v>
-      </c>
-      <c r="AB10" s="6" t="s">
-        <v>165</v>
       </c>
       <c r="AC10" s="6" t="s">
         <v>23</v>
@@ -3196,9 +3118,6 @@
       </c>
       <c r="AE10" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="AF10">
-        <v>193</v>
       </c>
       <c r="AG10" s="18"/>
     </row>
@@ -3213,10 +3132,10 @@
         <v>80</v>
       </c>
       <c r="D11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F11" s="4">
         <v>2</v>
@@ -3228,16 +3147,16 @@
         <v>53</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K11" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="L11" s="6" t="s">
         <v>156</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>157</v>
       </c>
       <c r="M11" s="6" t="s">
         <v>23</v>
@@ -3256,16 +3175,16 @@
       </c>
       <c r="R11" s="7"/>
       <c r="S11" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="U11" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="T11" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="U11" s="11" t="s">
-        <v>217</v>
-      </c>
       <c r="V11" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="W11" s="5" t="s">
         <v>40</v>
@@ -3274,16 +3193,16 @@
         <v>53</v>
       </c>
       <c r="Y11" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z11" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA11" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="Z11" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA11" s="6" t="s">
+      <c r="AB11" s="6" t="s">
         <v>168</v>
-      </c>
-      <c r="AB11" s="6" t="s">
-        <v>169</v>
       </c>
       <c r="AC11" s="6" t="s">
         <v>23</v>
@@ -3293,9 +3212,6 @@
       </c>
       <c r="AE11" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="AF11">
-        <v>194</v>
       </c>
       <c r="AG11" s="18"/>
     </row>
@@ -3310,10 +3226,10 @@
         <v>80</v>
       </c>
       <c r="D12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F12" s="4">
         <v>1</v>
@@ -3325,22 +3241,22 @@
         <v>54</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K12" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="L12" s="6" t="s">
         <v>160</v>
-      </c>
-      <c r="L12" s="6" t="s">
-        <v>161</v>
       </c>
       <c r="M12" s="6" t="s">
         <v>67</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O12" s="4" t="s">
         <v>27</v>
@@ -3353,16 +3269,16 @@
       </c>
       <c r="R12" s="7"/>
       <c r="S12" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="U12" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="T12" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="U12" s="11" t="s">
-        <v>219</v>
-      </c>
       <c r="V12" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="W12" s="5" t="s">
         <v>41</v>
@@ -3371,16 +3287,16 @@
         <v>54</v>
       </c>
       <c r="Y12" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z12" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA12" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="Z12" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA12" s="6" t="s">
+      <c r="AB12" s="6" t="s">
         <v>172</v>
-      </c>
-      <c r="AB12" s="6" t="s">
-        <v>173</v>
       </c>
       <c r="AC12" s="6" t="s">
         <v>23</v>
@@ -3390,9 +3306,6 @@
       </c>
       <c r="AE12" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="AF12">
-        <v>195</v>
       </c>
       <c r="AG12" s="18"/>
     </row>
@@ -3407,10 +3320,10 @@
         <v>80</v>
       </c>
       <c r="D13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F13" s="4">
         <v>2</v>
@@ -3422,16 +3335,16 @@
         <v>55</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K13" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="L13" s="6" t="s">
         <v>164</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>165</v>
       </c>
       <c r="M13" s="6" t="s">
         <v>23</v>
@@ -3450,16 +3363,16 @@
       </c>
       <c r="R13" s="7"/>
       <c r="S13" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="U13" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="T13" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="U13" s="11" t="s">
-        <v>221</v>
-      </c>
       <c r="V13" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="W13" s="5" t="s">
         <v>42</v>
@@ -3468,16 +3381,16 @@
         <v>55</v>
       </c>
       <c r="Y13" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="Z13" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA13" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="Z13" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA13" s="6" t="s">
+      <c r="AB13" s="6" t="s">
         <v>175</v>
-      </c>
-      <c r="AB13" s="6" t="s">
-        <v>176</v>
       </c>
       <c r="AC13" s="6" t="s">
         <v>23</v>
@@ -3487,9 +3400,6 @@
       </c>
       <c r="AE13" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="AF13">
-        <v>196</v>
       </c>
       <c r="AG13" s="18"/>
     </row>
@@ -3504,10 +3414,10 @@
         <v>80</v>
       </c>
       <c r="D14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F14" s="4">
         <v>1</v>
@@ -3519,22 +3429,22 @@
         <v>56</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K14" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="L14" s="6" t="s">
         <v>168</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>169</v>
       </c>
       <c r="M14" s="6" t="s">
         <v>67</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O14" s="4" t="s">
         <v>27</v>
@@ -3547,16 +3457,16 @@
       </c>
       <c r="R14" s="7"/>
       <c r="S14" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="U14" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="T14" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="U14" s="11" t="s">
-        <v>223</v>
-      </c>
       <c r="V14" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="W14" s="5" t="s">
         <v>43</v>
@@ -3565,16 +3475,16 @@
         <v>56</v>
       </c>
       <c r="Y14" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="Z14" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA14" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="Z14" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA14" s="6" t="s">
+      <c r="AB14" s="6" t="s">
         <v>178</v>
-      </c>
-      <c r="AB14" s="6" t="s">
-        <v>179</v>
       </c>
       <c r="AC14" s="6" t="s">
         <v>23</v>
@@ -3584,9 +3494,6 @@
       </c>
       <c r="AE14" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="AF14">
-        <v>197</v>
       </c>
       <c r="AG14" s="18"/>
     </row>
@@ -3601,10 +3508,10 @@
         <v>80</v>
       </c>
       <c r="D15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F15" s="4">
         <v>2</v>
@@ -3616,16 +3523,16 @@
         <v>97</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K15" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="L15" s="6" t="s">
         <v>172</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>173</v>
       </c>
       <c r="M15" s="6" t="s">
         <v>23</v>
@@ -3644,16 +3551,16 @@
       </c>
       <c r="R15" s="7"/>
       <c r="S15" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="U15" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="T15" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="U15" s="11" t="s">
-        <v>225</v>
-      </c>
       <c r="V15" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="W15" s="5" t="s">
         <v>96</v>
@@ -3662,16 +3569,16 @@
         <v>97</v>
       </c>
       <c r="Y15" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z15" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA15" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="Z15" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA15" s="6" t="s">
+      <c r="AB15" s="6" t="s">
         <v>181</v>
-      </c>
-      <c r="AB15" s="6" t="s">
-        <v>182</v>
       </c>
       <c r="AC15" s="6" t="s">
         <v>23</v>
@@ -3681,9 +3588,6 @@
       </c>
       <c r="AE15" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="AF15">
-        <v>198</v>
       </c>
       <c r="AG15" s="18"/>
     </row>
@@ -3698,10 +3602,10 @@
         <v>80</v>
       </c>
       <c r="D16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F16" s="4">
         <v>1</v>
@@ -3713,22 +3617,22 @@
         <v>100</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K16" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="L16" s="6" t="s">
         <v>175</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>176</v>
       </c>
       <c r="M16" s="6" t="s">
         <v>67</v>
       </c>
       <c r="N16" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O16" s="4" t="s">
         <v>27</v>
@@ -3741,16 +3645,16 @@
       </c>
       <c r="R16" s="7"/>
       <c r="S16" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="U16" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="T16" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="U16" s="11" t="s">
-        <v>227</v>
-      </c>
       <c r="V16" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="W16" s="5" t="s">
         <v>99</v>
@@ -3759,16 +3663,16 @@
         <v>100</v>
       </c>
       <c r="Y16" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="Z16" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA16" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="Z16" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA16" s="6" t="s">
+      <c r="AB16" s="6" t="s">
         <v>184</v>
-      </c>
-      <c r="AB16" s="6" t="s">
-        <v>185</v>
       </c>
       <c r="AC16" s="6" t="s">
         <v>23</v>
@@ -3779,12 +3683,9 @@
       <c r="AE16" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="AF16">
-        <v>199</v>
-      </c>
       <c r="AG16" s="18"/>
     </row>
-    <row r="17" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>1</v>
       </c>
@@ -3795,10 +3696,10 @@
         <v>80</v>
       </c>
       <c r="D17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F17" s="4">
         <v>2</v>
@@ -3810,16 +3711,16 @@
         <v>103</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K17" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="L17" s="6" t="s">
         <v>178</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>179</v>
       </c>
       <c r="M17" s="6" t="s">
         <v>23</v>
@@ -3838,16 +3739,16 @@
       </c>
       <c r="R17" s="7"/>
       <c r="S17" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="U17" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="T17" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="U17" s="11" t="s">
-        <v>229</v>
-      </c>
       <c r="V17" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="W17" s="5" t="s">
         <v>102</v>
@@ -3856,16 +3757,16 @@
         <v>103</v>
       </c>
       <c r="Y17" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z17" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA17" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="Z17" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA17" s="6" t="s">
+      <c r="AB17" s="6" t="s">
         <v>187</v>
-      </c>
-      <c r="AB17" s="6" t="s">
-        <v>188</v>
       </c>
       <c r="AC17" s="6" t="s">
         <v>23</v>
@@ -3876,11 +3777,8 @@
       <c r="AE17" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="AF17">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="18" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>1</v>
       </c>
@@ -3891,10 +3789,10 @@
         <v>80</v>
       </c>
       <c r="D18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F18" s="4">
         <v>1</v>
@@ -3906,22 +3804,22 @@
         <v>106</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K18" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="L18" s="6" t="s">
         <v>181</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>182</v>
       </c>
       <c r="M18" s="6" t="s">
         <v>67</v>
       </c>
       <c r="N18" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O18" s="4" t="s">
         <v>27</v>
@@ -3934,16 +3832,16 @@
       </c>
       <c r="R18" s="7"/>
       <c r="S18" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="U18" s="11" t="s">
         <v>230</v>
       </c>
-      <c r="T18" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="U18" s="11" t="s">
-        <v>231</v>
-      </c>
       <c r="V18" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="W18" s="5" t="s">
         <v>105</v>
@@ -3952,16 +3850,16 @@
         <v>106</v>
       </c>
       <c r="Y18" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="Z18" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA18" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="Z18" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA18" s="6" t="s">
+      <c r="AB18" s="6" t="s">
         <v>190</v>
-      </c>
-      <c r="AB18" s="6" t="s">
-        <v>191</v>
       </c>
       <c r="AC18" s="6" t="s">
         <v>23</v>
@@ -3972,11 +3870,8 @@
       <c r="AE18" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="AF18">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="19" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>1</v>
       </c>
@@ -3987,10 +3882,10 @@
         <v>80</v>
       </c>
       <c r="D19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F19" s="4">
         <v>2</v>
@@ -4002,16 +3897,16 @@
         <v>109</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K19" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="L19" s="6" t="s">
         <v>184</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>185</v>
       </c>
       <c r="M19" s="6" t="s">
         <v>23</v>
@@ -4030,16 +3925,16 @@
       </c>
       <c r="R19" s="7"/>
       <c r="S19" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="U19" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="T19" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="U19" s="11" t="s">
-        <v>233</v>
-      </c>
       <c r="V19" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="W19" s="5" t="s">
         <v>108</v>
@@ -4048,16 +3943,16 @@
         <v>109</v>
       </c>
       <c r="Y19" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="Z19" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA19" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="Z19" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA19" s="6" t="s">
+      <c r="AB19" s="6" t="s">
         <v>193</v>
-      </c>
-      <c r="AB19" s="6" t="s">
-        <v>194</v>
       </c>
       <c r="AC19" s="6" t="s">
         <v>23</v>
@@ -4068,11 +3963,8 @@
       <c r="AE19" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="AF19">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="20" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>1</v>
       </c>
@@ -4083,10 +3975,10 @@
         <v>80</v>
       </c>
       <c r="D20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F20" s="4">
         <v>1</v>
@@ -4098,22 +3990,22 @@
         <v>112</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K20" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="L20" s="6" t="s">
         <v>187</v>
-      </c>
-      <c r="L20" s="6" t="s">
-        <v>188</v>
       </c>
       <c r="M20" s="6" t="s">
         <v>67</v>
       </c>
       <c r="N20" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O20" s="4" t="s">
         <v>27</v>
@@ -4126,16 +4018,16 @@
       </c>
       <c r="R20" s="7"/>
       <c r="S20" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="U20" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="T20" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="U20" s="11" t="s">
-        <v>235</v>
-      </c>
       <c r="V20" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="W20" s="5" t="s">
         <v>111</v>
@@ -4144,16 +4036,16 @@
         <v>112</v>
       </c>
       <c r="Y20" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="Z20" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA20" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="Z20" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA20" s="6" t="s">
+      <c r="AB20" s="6" t="s">
         <v>196</v>
-      </c>
-      <c r="AB20" s="6" t="s">
-        <v>197</v>
       </c>
       <c r="AC20" s="6" t="s">
         <v>23</v>
@@ -4163,9 +4055,6 @@
       </c>
       <c r="AE20" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="AF20">
-        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -4195,4 +4084,670 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FABAB06A-EAA7-4BA7-8A4C-8C5EF7E0517A}">
+  <dimension ref="A1:I37"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>CONCATENATE($G$1,$I1)</f>
+        <v>TestChicagoCity204</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <f>CONCATENATE($G$1,$I1)</f>
+        <v>TestChicagoCity204</v>
+      </c>
+      <c r="C1" s="11" t="str">
+        <f>CONCATENATE($G$1,$I1,$H$1)</f>
+        <v>TestChicagoCity204@gmail.com</v>
+      </c>
+      <c r="G1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="str">
+        <f t="shared" ref="A2:B19" si="0">CONCATENATE($G$1,$I2)</f>
+        <v>TestChicagoCity205</v>
+      </c>
+      <c r="B2" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity205</v>
+      </c>
+      <c r="C2" s="11" t="str">
+        <f t="shared" ref="C2:C19" si="1">CONCATENATE($G$1,$I2,$H$1)</f>
+        <v>TestChicagoCity205@gmail.com</v>
+      </c>
+      <c r="I2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity206</v>
+      </c>
+      <c r="B3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity206</v>
+      </c>
+      <c r="C3" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>TestChicagoCity206@gmail.com</v>
+      </c>
+      <c r="I3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity207</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity207</v>
+      </c>
+      <c r="C4" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>TestChicagoCity207@gmail.com</v>
+      </c>
+      <c r="I4">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity208</v>
+      </c>
+      <c r="B5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity208</v>
+      </c>
+      <c r="C5" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>TestChicagoCity208@gmail.com</v>
+      </c>
+      <c r="I5">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity209</v>
+      </c>
+      <c r="B6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity209</v>
+      </c>
+      <c r="C6" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>TestChicagoCity209@gmail.com</v>
+      </c>
+      <c r="I6">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity210</v>
+      </c>
+      <c r="B7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity210</v>
+      </c>
+      <c r="C7" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>TestChicagoCity210@gmail.com</v>
+      </c>
+      <c r="I7">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity211</v>
+      </c>
+      <c r="B8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity211</v>
+      </c>
+      <c r="C8" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>TestChicagoCity211@gmail.com</v>
+      </c>
+      <c r="I8">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity212</v>
+      </c>
+      <c r="B9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity212</v>
+      </c>
+      <c r="C9" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>TestChicagoCity212@gmail.com</v>
+      </c>
+      <c r="I9">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity213</v>
+      </c>
+      <c r="B10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity213</v>
+      </c>
+      <c r="C10" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>TestChicagoCity213@gmail.com</v>
+      </c>
+      <c r="I10">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity214</v>
+      </c>
+      <c r="B11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity214</v>
+      </c>
+      <c r="C11" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>TestChicagoCity214@gmail.com</v>
+      </c>
+      <c r="I11">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity215</v>
+      </c>
+      <c r="B12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity215</v>
+      </c>
+      <c r="C12" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>TestChicagoCity215@gmail.com</v>
+      </c>
+      <c r="I12">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity216</v>
+      </c>
+      <c r="B13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity216</v>
+      </c>
+      <c r="C13" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>TestChicagoCity216@gmail.com</v>
+      </c>
+      <c r="I13">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity217</v>
+      </c>
+      <c r="B14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity217</v>
+      </c>
+      <c r="C14" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>TestChicagoCity217@gmail.com</v>
+      </c>
+      <c r="I14">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity218</v>
+      </c>
+      <c r="B15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity218</v>
+      </c>
+      <c r="C15" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>TestChicagoCity218@gmail.com</v>
+      </c>
+      <c r="I15">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity219</v>
+      </c>
+      <c r="B16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity219</v>
+      </c>
+      <c r="C16" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>TestChicagoCity219@gmail.com</v>
+      </c>
+      <c r="I16">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity220</v>
+      </c>
+      <c r="B17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity220</v>
+      </c>
+      <c r="C17" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>TestChicagoCity220@gmail.com</v>
+      </c>
+      <c r="I17">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity221</v>
+      </c>
+      <c r="B18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity221</v>
+      </c>
+      <c r="C18" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>TestChicagoCity221@gmail.com</v>
+      </c>
+      <c r="I18">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity222</v>
+      </c>
+      <c r="B19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>TestChicagoCity222</v>
+      </c>
+      <c r="C19" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>TestChicagoCity222@gmail.com</v>
+      </c>
+      <c r="I19">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="str">
+        <f>CONCATENATE($G$22,$I22)</f>
+        <v>AutomationTestPalatine171</v>
+      </c>
+      <c r="B22" s="1" t="str">
+        <f>CONCATENATE($G$22,$I22)</f>
+        <v>AutomationTestPalatine171</v>
+      </c>
+      <c r="C22" s="11" t="str">
+        <f>CONCATENATE($G$22,$I22,$H$22)</f>
+        <v>AutomationTestPalatine171@gmail.com</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I22">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="str">
+        <f t="shared" ref="A23:B37" si="2">CONCATENATE($G$22,$I23)</f>
+        <v>AutomationTestPalatine172</v>
+      </c>
+      <c r="B23" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine172</v>
+      </c>
+      <c r="C23" s="11" t="str">
+        <f t="shared" ref="C23:C37" si="3">CONCATENATE($G$22,$I23,$H$22)</f>
+        <v>AutomationTestPalatine172@gmail.com</v>
+      </c>
+      <c r="I23">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine173</v>
+      </c>
+      <c r="B24" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine173</v>
+      </c>
+      <c r="C24" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>AutomationTestPalatine173@gmail.com</v>
+      </c>
+      <c r="I24">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine174</v>
+      </c>
+      <c r="B25" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine174</v>
+      </c>
+      <c r="C25" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>AutomationTestPalatine174@gmail.com</v>
+      </c>
+      <c r="I25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine175</v>
+      </c>
+      <c r="B26" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine175</v>
+      </c>
+      <c r="C26" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>AutomationTestPalatine175@gmail.com</v>
+      </c>
+      <c r="I26">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine176</v>
+      </c>
+      <c r="B27" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine176</v>
+      </c>
+      <c r="C27" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>AutomationTestPalatine176@gmail.com</v>
+      </c>
+      <c r="I27">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine177</v>
+      </c>
+      <c r="B28" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine177</v>
+      </c>
+      <c r="C28" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>AutomationTestPalatine177@gmail.com</v>
+      </c>
+      <c r="I28">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine178</v>
+      </c>
+      <c r="B29" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine178</v>
+      </c>
+      <c r="C29" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>AutomationTestPalatine178@gmail.com</v>
+      </c>
+      <c r="I29">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine179</v>
+      </c>
+      <c r="B30" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine179</v>
+      </c>
+      <c r="C30" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>AutomationTestPalatine179@gmail.com</v>
+      </c>
+      <c r="I30">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine180</v>
+      </c>
+      <c r="B31" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine180</v>
+      </c>
+      <c r="C31" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>AutomationTestPalatine180@gmail.com</v>
+      </c>
+      <c r="I31">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine181</v>
+      </c>
+      <c r="B32" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine181</v>
+      </c>
+      <c r="C32" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>AutomationTestPalatine181@gmail.com</v>
+      </c>
+      <c r="I32">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine182</v>
+      </c>
+      <c r="B33" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine182</v>
+      </c>
+      <c r="C33" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>AutomationTestPalatine182@gmail.com</v>
+      </c>
+      <c r="I33">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine183</v>
+      </c>
+      <c r="B34" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine183</v>
+      </c>
+      <c r="C34" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>AutomationTestPalatine183@gmail.com</v>
+      </c>
+      <c r="I34">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine184</v>
+      </c>
+      <c r="B35" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine184</v>
+      </c>
+      <c r="C35" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>AutomationTestPalatine184@gmail.com</v>
+      </c>
+      <c r="I35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine185</v>
+      </c>
+      <c r="B36" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine185</v>
+      </c>
+      <c r="C36" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>AutomationTestPalatine185@gmail.com</v>
+      </c>
+      <c r="I36">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine186</v>
+      </c>
+      <c r="B37" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AutomationTestPalatine186</v>
+      </c>
+      <c r="C37" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>AutomationTestPalatine186@gmail.com</v>
+      </c>
+      <c r="I37">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1" display="TestChicagoCity32@gmail.com" xr:uid="{FC4C4380-D018-44C6-8680-86CBCE1CE3FD}"/>
+    <hyperlink ref="C2" r:id="rId2" display="TestChicagoCity32@gmail.com" xr:uid="{45A4E974-3337-4131-BE48-37FA2E2AE43A}"/>
+    <hyperlink ref="C3" r:id="rId3" display="TestChicagoCity32@gmail.com" xr:uid="{901959C7-6E03-43EA-A626-C7E9E11EAB62}"/>
+    <hyperlink ref="C4" r:id="rId4" display="TestChicagoCity32@gmail.com" xr:uid="{7C44DB3F-C396-4489-9BEA-E852FFBE54FA}"/>
+    <hyperlink ref="C5" r:id="rId5" display="TestChicagoCity32@gmail.com" xr:uid="{B0FAE8B7-278B-47F0-9924-9F2FF04A897B}"/>
+    <hyperlink ref="C6" r:id="rId6" display="TestChicagoCity32@gmail.com" xr:uid="{EEB58044-D0B3-4E3D-883D-DF692941E0E6}"/>
+    <hyperlink ref="C7" r:id="rId7" display="TestChicagoCity32@gmail.com" xr:uid="{70A9BAB6-F1A2-483E-8294-CA7D9DD5B28A}"/>
+    <hyperlink ref="C8" r:id="rId8" display="TestChicagoCity32@gmail.com" xr:uid="{C445C991-F19B-4624-8362-D72F36956C8A}"/>
+    <hyperlink ref="C9" r:id="rId9" display="TestChicagoCity32@gmail.com" xr:uid="{82F568CD-AD24-42AB-BA03-C5DFBC60E539}"/>
+    <hyperlink ref="C10" r:id="rId10" display="TestChicagoCity32@gmail.com" xr:uid="{E1A67F48-2876-4DB4-AA9A-5E93B23595E3}"/>
+    <hyperlink ref="C11" r:id="rId11" display="TestChicagoCity32@gmail.com" xr:uid="{749725A6-D080-4968-B2B2-79995275FD7F}"/>
+    <hyperlink ref="C12" r:id="rId12" display="TestChicagoCity32@gmail.com" xr:uid="{4FAB9072-528A-4C7D-9DBA-88541E333D85}"/>
+    <hyperlink ref="C13" r:id="rId13" display="TestChicagoCity32@gmail.com" xr:uid="{32B05F64-527B-46B7-ABF1-E3D6CB6D5545}"/>
+    <hyperlink ref="C14" r:id="rId14" display="TestChicagoCity32@gmail.com" xr:uid="{79A009C9-E1FB-46F8-B867-83503D832A5F}"/>
+    <hyperlink ref="C15" r:id="rId15" display="TestChicagoCity32@gmail.com" xr:uid="{41A9CC07-BF2E-49F5-9AE6-8583E341FA90}"/>
+    <hyperlink ref="C16" r:id="rId16" display="TestChicagoCity32@gmail.com" xr:uid="{B81DD619-166B-43BD-BF7E-16BCC748CDB4}"/>
+    <hyperlink ref="C17" r:id="rId17" display="TestChicagoCity32@gmail.com" xr:uid="{065BAE80-2ECF-4DE6-ADC8-0A3E52C91867}"/>
+    <hyperlink ref="C18" r:id="rId18" display="TestChicagoCity32@gmail.com" xr:uid="{2DEC13AE-B830-4BAD-9267-E51138A9A9ED}"/>
+    <hyperlink ref="C19" r:id="rId19" display="TestChicagoCity32@gmail.com" xr:uid="{F50C95AB-3A94-4CFC-9DE4-AAA1EC80A480}"/>
+    <hyperlink ref="C22" r:id="rId20" display="TestChicagoCity32@gmail.com" xr:uid="{1485756C-D9B4-4A31-B49B-B6CC03417D24}"/>
+    <hyperlink ref="C23" r:id="rId21" display="TestChicagoCity32@gmail.com" xr:uid="{26D9370E-2322-48F5-9A65-E129B922074B}"/>
+    <hyperlink ref="C24" r:id="rId22" display="TestChicagoCity32@gmail.com" xr:uid="{AB727918-B49E-4C6F-845F-4AFE15A9959D}"/>
+    <hyperlink ref="C25" r:id="rId23" display="TestChicagoCity32@gmail.com" xr:uid="{D843A248-DA64-406D-B8EE-BDD59E176D46}"/>
+    <hyperlink ref="C26" r:id="rId24" display="TestChicagoCity32@gmail.com" xr:uid="{2680ACB2-54A0-4BC6-9CDE-C7B5E7C78A07}"/>
+    <hyperlink ref="C27" r:id="rId25" display="TestChicagoCity32@gmail.com" xr:uid="{079EABA6-05A1-438E-A247-6FA819F88B13}"/>
+    <hyperlink ref="C28" r:id="rId26" display="TestChicagoCity32@gmail.com" xr:uid="{1B119723-3B5C-445F-9E39-18831759EF5F}"/>
+    <hyperlink ref="C29" r:id="rId27" display="TestChicagoCity32@gmail.com" xr:uid="{9A082C71-8274-47C1-B111-E683E89A6C79}"/>
+    <hyperlink ref="C30" r:id="rId28" display="TestChicagoCity32@gmail.com" xr:uid="{25CE969B-2FDB-41E8-BBCB-3D079CE6B040}"/>
+    <hyperlink ref="C31" r:id="rId29" display="TestChicagoCity32@gmail.com" xr:uid="{810134B7-2EE9-428C-92B4-17A9BE608F31}"/>
+    <hyperlink ref="C32" r:id="rId30" display="TestChicagoCity32@gmail.com" xr:uid="{4454DFC2-2A11-4DFF-9E1D-DA0F2B116130}"/>
+    <hyperlink ref="C33" r:id="rId31" display="TestChicagoCity32@gmail.com" xr:uid="{66E2E80E-F87C-4564-B943-FC32D8493F2C}"/>
+    <hyperlink ref="C34" r:id="rId32" display="TestChicagoCity32@gmail.com" xr:uid="{2D26ADFB-749D-41D6-BC4C-53F63C6C959F}"/>
+    <hyperlink ref="C35" r:id="rId33" display="TestChicagoCity32@gmail.com" xr:uid="{AB781A60-FAF3-4BDC-80BF-61F84F0FA8A3}"/>
+    <hyperlink ref="C36" r:id="rId34" display="TestChicagoCity32@gmail.com" xr:uid="{F6137712-9F9A-491B-8AFE-3708A26E793E}"/>
+    <hyperlink ref="C37" r:id="rId35" display="TestChicagoCity32@gmail.com" xr:uid="{40D3AB2D-1824-495D-8503-9DE16777AB4F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated data and place order
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/Test_Data.xlsx
+++ b/src/main/resources/test_data/Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verkh\IdeaProjects\pom6\src\main\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8E61B6-83BE-446A-8D52-E7C409B2CAB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8620BB-958A-48F0-8A0C-1040CD0E26F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="594" activeTab="1" xr2:uid="{56D596F5-221D-421D-9FC5-55182B639D44}"/>
   </bookViews>
@@ -1171,124 +1171,124 @@
     <t>LucilleGriffiths4@gmail.com</t>
   </si>
   <si>
-    <t>DonnellJernigan5</t>
-  </si>
-  <si>
-    <t>DonnellJernigan5@gmail.com</t>
-  </si>
-  <si>
-    <t>MalikOtoole5</t>
-  </si>
-  <si>
-    <t>MalikOtoole5@gmail.com</t>
-  </si>
-  <si>
-    <t>AlanCaudill5</t>
-  </si>
-  <si>
-    <t>AlanCaudill5@gmail.com</t>
-  </si>
-  <si>
-    <t>AdanApplegate5</t>
-  </si>
-  <si>
-    <t>AdanApplegate5@gmail.com</t>
-  </si>
-  <si>
-    <t>AiyanaWhitworth5</t>
-  </si>
-  <si>
-    <t>AiyanaWhitworth5@gmail.com</t>
-  </si>
-  <si>
-    <t>MercedezBrien5</t>
-  </si>
-  <si>
-    <t>MercedezBrien5@gmail.com</t>
-  </si>
-  <si>
-    <t>DuaneHager5</t>
-  </si>
-  <si>
-    <t>DuaneHager5@gmail.com</t>
-  </si>
-  <si>
-    <t>LorenBell5</t>
-  </si>
-  <si>
-    <t>LorenBell5@gmail.com</t>
-  </si>
-  <si>
-    <t>GeraldHiller5</t>
-  </si>
-  <si>
-    <t>GeraldHiller5@gmail.com</t>
-  </si>
-  <si>
-    <t>DeionBranch5</t>
-  </si>
-  <si>
-    <t>DeionBranch5@gmail.com</t>
-  </si>
-  <si>
-    <t>DakotaHalstead5</t>
-  </si>
-  <si>
-    <t>DakotaHalstead5@gmail.com</t>
-  </si>
-  <si>
-    <t>ElliottFurman5</t>
-  </si>
-  <si>
-    <t>ElliottFurman5@gmail.com</t>
-  </si>
-  <si>
-    <t>MiltonCamp5</t>
-  </si>
-  <si>
-    <t>MiltonCamp5@gmail.com</t>
-  </si>
-  <si>
-    <t>DawnChester5</t>
-  </si>
-  <si>
-    <t>DawnChester5@gmail.com</t>
-  </si>
-  <si>
-    <t>ZacheryPetrie5</t>
-  </si>
-  <si>
-    <t>ZacheryPetrie5@gmail.com</t>
-  </si>
-  <si>
-    <t>EstebanAngel5</t>
-  </si>
-  <si>
-    <t>EstebanAngel5@gmail.com</t>
-  </si>
-  <si>
-    <t>JimmyBlankenship5</t>
-  </si>
-  <si>
-    <t>JimmyBlankenship5@gmail.com</t>
-  </si>
-  <si>
-    <t>AllysaGrice5</t>
-  </si>
-  <si>
-    <t>AllysaGrice5@gmail.com</t>
-  </si>
-  <si>
-    <t>AugustineYoo5</t>
-  </si>
-  <si>
-    <t>AugustineYoo5@gmail.com</t>
-  </si>
-  <si>
-    <t>BrandiSouthard5</t>
-  </si>
-  <si>
-    <t>BrandiSouthard5@gmail.com</t>
+    <t>DonnellJernigan6</t>
+  </si>
+  <si>
+    <t>DonnellJernigan6@gmail.com</t>
+  </si>
+  <si>
+    <t>MalikOtoole6</t>
+  </si>
+  <si>
+    <t>MalikOtoole6@gmail.com</t>
+  </si>
+  <si>
+    <t>AlanCaudill6</t>
+  </si>
+  <si>
+    <t>AlanCaudill6@gmail.com</t>
+  </si>
+  <si>
+    <t>AdanApplegate6</t>
+  </si>
+  <si>
+    <t>AdanApplegate6@gmail.com</t>
+  </si>
+  <si>
+    <t>AiyanaWhitworth6</t>
+  </si>
+  <si>
+    <t>AiyanaWhitworth6@gmail.com</t>
+  </si>
+  <si>
+    <t>MercedezBrien6</t>
+  </si>
+  <si>
+    <t>MercedezBrien6@gmail.com</t>
+  </si>
+  <si>
+    <t>DuaneHager6</t>
+  </si>
+  <si>
+    <t>DuaneHager6@gmail.com</t>
+  </si>
+  <si>
+    <t>LorenBell6</t>
+  </si>
+  <si>
+    <t>LorenBell6@gmail.com</t>
+  </si>
+  <si>
+    <t>GeraldHiller6</t>
+  </si>
+  <si>
+    <t>GeraldHiller6@gmail.com</t>
+  </si>
+  <si>
+    <t>DeionBranch6</t>
+  </si>
+  <si>
+    <t>DeionBranch6@gmail.com</t>
+  </si>
+  <si>
+    <t>DakotaHalstead6</t>
+  </si>
+  <si>
+    <t>DakotaHalstead6@gmail.com</t>
+  </si>
+  <si>
+    <t>ElliottFurman6</t>
+  </si>
+  <si>
+    <t>ElliottFurman6@gmail.com</t>
+  </si>
+  <si>
+    <t>MiltonCamp6</t>
+  </si>
+  <si>
+    <t>MiltonCamp6@gmail.com</t>
+  </si>
+  <si>
+    <t>DawnChester6</t>
+  </si>
+  <si>
+    <t>DawnChester6@gmail.com</t>
+  </si>
+  <si>
+    <t>ZacheryPetrie6</t>
+  </si>
+  <si>
+    <t>ZacheryPetrie6@gmail.com</t>
+  </si>
+  <si>
+    <t>EstebanAngel6</t>
+  </si>
+  <si>
+    <t>EstebanAngel6@gmail.com</t>
+  </si>
+  <si>
+    <t>JimmyBlankenship6</t>
+  </si>
+  <si>
+    <t>JimmyBlankenship6@gmail.com</t>
+  </si>
+  <si>
+    <t>AllysaGrice6</t>
+  </si>
+  <si>
+    <t>AllysaGrice6@gmail.com</t>
+  </si>
+  <si>
+    <t>AugustineYoo6</t>
+  </si>
+  <si>
+    <t>AugustineYoo6@gmail.com</t>
+  </si>
+  <si>
+    <t>BrandiSouthard6</t>
+  </si>
+  <si>
+    <t>BrandiSouthard6@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2909,7 +2909,7 @@
   <dimension ref="A1:AF21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+      <selection activeCell="R2" sqref="R2:T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5315,15 +5315,15 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="str">
         <f>CONCATENATE($G23,$I$23)</f>
-        <v>DonnellJernigan5</v>
+        <v>DonnellJernigan6</v>
       </c>
       <c r="B23" s="1" t="str">
         <f>CONCATENATE($G23,$I$23)</f>
-        <v>DonnellJernigan5</v>
+        <v>DonnellJernigan6</v>
       </c>
       <c r="C23" s="2" t="str">
         <f>CONCATENATE($G23,$I$23,$H$23)</f>
-        <v>DonnellJernigan5@gmail.com</v>
+        <v>DonnellJernigan6@gmail.com</v>
       </c>
       <c r="G23" s="24" t="s">
         <v>212</v>
@@ -5332,21 +5332,21 @@
         <v>94</v>
       </c>
       <c r="I23">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="str">
         <f t="shared" ref="A24:B42" si="2">CONCATENATE($G24,$I$23)</f>
-        <v>MalikOtoole5</v>
+        <v>MalikOtoole6</v>
       </c>
       <c r="B24" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MalikOtoole5</v>
+        <v>MalikOtoole6</v>
       </c>
       <c r="C24" s="2" t="str">
         <f t="shared" ref="C24:C42" si="3">CONCATENATE($G24,$I$23,$H$23)</f>
-        <v>MalikOtoole5@gmail.com</v>
+        <v>MalikOtoole6@gmail.com</v>
       </c>
       <c r="G24" t="s">
         <v>213</v>
@@ -5355,15 +5355,15 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AlanCaudill5</v>
+        <v>AlanCaudill6</v>
       </c>
       <c r="B25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AlanCaudill5</v>
+        <v>AlanCaudill6</v>
       </c>
       <c r="C25" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AlanCaudill5@gmail.com</v>
+        <v>AlanCaudill6@gmail.com</v>
       </c>
       <c r="G25" t="s">
         <v>214</v>
@@ -5372,15 +5372,15 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AdanApplegate5</v>
+        <v>AdanApplegate6</v>
       </c>
       <c r="B26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AdanApplegate5</v>
+        <v>AdanApplegate6</v>
       </c>
       <c r="C26" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AdanApplegate5@gmail.com</v>
+        <v>AdanApplegate6@gmail.com</v>
       </c>
       <c r="G26" t="s">
         <v>215</v>
@@ -5389,15 +5389,15 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AiyanaWhitworth5</v>
+        <v>AiyanaWhitworth6</v>
       </c>
       <c r="B27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AiyanaWhitworth5</v>
+        <v>AiyanaWhitworth6</v>
       </c>
       <c r="C27" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AiyanaWhitworth5@gmail.com</v>
+        <v>AiyanaWhitworth6@gmail.com</v>
       </c>
       <c r="G27" t="s">
         <v>216</v>
@@ -5406,15 +5406,15 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MercedezBrien5</v>
+        <v>MercedezBrien6</v>
       </c>
       <c r="B28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MercedezBrien5</v>
+        <v>MercedezBrien6</v>
       </c>
       <c r="C28" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>MercedezBrien5@gmail.com</v>
+        <v>MercedezBrien6@gmail.com</v>
       </c>
       <c r="G28" t="s">
         <v>217</v>
@@ -5423,15 +5423,15 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DuaneHager5</v>
+        <v>DuaneHager6</v>
       </c>
       <c r="B29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DuaneHager5</v>
+        <v>DuaneHager6</v>
       </c>
       <c r="C29" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DuaneHager5@gmail.com</v>
+        <v>DuaneHager6@gmail.com</v>
       </c>
       <c r="G29" t="s">
         <v>218</v>
@@ -5440,15 +5440,15 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>LorenBell5</v>
+        <v>LorenBell6</v>
       </c>
       <c r="B30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>LorenBell5</v>
+        <v>LorenBell6</v>
       </c>
       <c r="C30" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>LorenBell5@gmail.com</v>
+        <v>LorenBell6@gmail.com</v>
       </c>
       <c r="G30" t="s">
         <v>219</v>
@@ -5457,15 +5457,15 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>GeraldHiller5</v>
+        <v>GeraldHiller6</v>
       </c>
       <c r="B31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>GeraldHiller5</v>
+        <v>GeraldHiller6</v>
       </c>
       <c r="C31" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>GeraldHiller5@gmail.com</v>
+        <v>GeraldHiller6@gmail.com</v>
       </c>
       <c r="G31" t="s">
         <v>220</v>
@@ -5474,15 +5474,15 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DeionBranch5</v>
+        <v>DeionBranch6</v>
       </c>
       <c r="B32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DeionBranch5</v>
+        <v>DeionBranch6</v>
       </c>
       <c r="C32" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DeionBranch5@gmail.com</v>
+        <v>DeionBranch6@gmail.com</v>
       </c>
       <c r="G32" t="s">
         <v>221</v>
@@ -5491,15 +5491,15 @@
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DakotaHalstead5</v>
+        <v>DakotaHalstead6</v>
       </c>
       <c r="B33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DakotaHalstead5</v>
+        <v>DakotaHalstead6</v>
       </c>
       <c r="C33" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DakotaHalstead5@gmail.com</v>
+        <v>DakotaHalstead6@gmail.com</v>
       </c>
       <c r="G33" t="s">
         <v>222</v>
@@ -5508,15 +5508,15 @@
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ElliottFurman5</v>
+        <v>ElliottFurman6</v>
       </c>
       <c r="B34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ElliottFurman5</v>
+        <v>ElliottFurman6</v>
       </c>
       <c r="C34" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>ElliottFurman5@gmail.com</v>
+        <v>ElliottFurman6@gmail.com</v>
       </c>
       <c r="G34" t="s">
         <v>223</v>
@@ -5525,15 +5525,15 @@
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MiltonCamp5</v>
+        <v>MiltonCamp6</v>
       </c>
       <c r="B35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MiltonCamp5</v>
+        <v>MiltonCamp6</v>
       </c>
       <c r="C35" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>MiltonCamp5@gmail.com</v>
+        <v>MiltonCamp6@gmail.com</v>
       </c>
       <c r="G35" t="s">
         <v>224</v>
@@ -5542,15 +5542,15 @@
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DawnChester5</v>
+        <v>DawnChester6</v>
       </c>
       <c r="B36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DawnChester5</v>
+        <v>DawnChester6</v>
       </c>
       <c r="C36" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DawnChester5@gmail.com</v>
+        <v>DawnChester6@gmail.com</v>
       </c>
       <c r="G36" t="s">
         <v>225</v>
@@ -5559,15 +5559,15 @@
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ZacheryPetrie5</v>
+        <v>ZacheryPetrie6</v>
       </c>
       <c r="B37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ZacheryPetrie5</v>
+        <v>ZacheryPetrie6</v>
       </c>
       <c r="C37" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>ZacheryPetrie5@gmail.com</v>
+        <v>ZacheryPetrie6@gmail.com</v>
       </c>
       <c r="G37" t="s">
         <v>226</v>
@@ -5576,15 +5576,15 @@
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>EstebanAngel5</v>
+        <v>EstebanAngel6</v>
       </c>
       <c r="B38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>EstebanAngel5</v>
+        <v>EstebanAngel6</v>
       </c>
       <c r="C38" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>EstebanAngel5@gmail.com</v>
+        <v>EstebanAngel6@gmail.com</v>
       </c>
       <c r="G38" t="s">
         <v>227</v>
@@ -5593,15 +5593,15 @@
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>JimmyBlankenship5</v>
+        <v>JimmyBlankenship6</v>
       </c>
       <c r="B39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>JimmyBlankenship5</v>
+        <v>JimmyBlankenship6</v>
       </c>
       <c r="C39" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>JimmyBlankenship5@gmail.com</v>
+        <v>JimmyBlankenship6@gmail.com</v>
       </c>
       <c r="G39" t="s">
         <v>228</v>
@@ -5610,15 +5610,15 @@
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AllysaGrice5</v>
+        <v>AllysaGrice6</v>
       </c>
       <c r="B40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AllysaGrice5</v>
+        <v>AllysaGrice6</v>
       </c>
       <c r="C40" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AllysaGrice5@gmail.com</v>
+        <v>AllysaGrice6@gmail.com</v>
       </c>
       <c r="G40" t="s">
         <v>229</v>
@@ -5627,15 +5627,15 @@
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AugustineYoo5</v>
+        <v>AugustineYoo6</v>
       </c>
       <c r="B41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AugustineYoo5</v>
+        <v>AugustineYoo6</v>
       </c>
       <c r="C41" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AugustineYoo5@gmail.com</v>
+        <v>AugustineYoo6@gmail.com</v>
       </c>
       <c r="G41" t="s">
         <v>230</v>
@@ -5644,15 +5644,15 @@
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BrandiSouthard5</v>
+        <v>BrandiSouthard6</v>
       </c>
       <c r="B42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BrandiSouthard5</v>
+        <v>BrandiSouthard6</v>
       </c>
       <c r="C42" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>BrandiSouthard5@gmail.com</v>
+        <v>BrandiSouthard6@gmail.com</v>
       </c>
       <c r="G42" t="s">
         <v>231</v>

</xml_diff>

<commit_message>
updated data and cart page
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/Test_Data.xlsx
+++ b/src/main/resources/test_data/Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verkh\IdeaProjects\pom6\src\main\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA650496-19F7-4795-97B3-5A9850CED6FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB4504B-164E-4482-A7BF-B059D363A83D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="594" activeTab="1" xr2:uid="{56D596F5-221D-421D-9FC5-55182B639D44}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="419">
   <si>
     <t>run</t>
   </si>
@@ -133,45 +133,6 @@
     <t>AutoTestChicago2@gmail.com</t>
   </si>
   <si>
-    <t>David6</t>
-  </si>
-  <si>
-    <t>David7</t>
-  </si>
-  <si>
-    <t>David8</t>
-  </si>
-  <si>
-    <t>David9</t>
-  </si>
-  <si>
-    <t>David10</t>
-  </si>
-  <si>
-    <t>David11</t>
-  </si>
-  <si>
-    <t>David12</t>
-  </si>
-  <si>
-    <t>David13</t>
-  </si>
-  <si>
-    <t>David14</t>
-  </si>
-  <si>
-    <t>David15</t>
-  </si>
-  <si>
-    <t>David16</t>
-  </si>
-  <si>
-    <t>David17</t>
-  </si>
-  <si>
-    <t>David18</t>
-  </si>
-  <si>
     <t>team_members</t>
   </si>
   <si>
@@ -286,39 +247,21 @@
     <t>58598</t>
   </si>
   <si>
-    <t>David19</t>
-  </si>
-  <si>
     <t>58599</t>
   </si>
   <si>
-    <t>David20</t>
-  </si>
-  <si>
     <t>58600</t>
   </si>
   <si>
-    <t>David21</t>
-  </si>
-  <si>
     <t>58601</t>
   </si>
   <si>
-    <t>David22</t>
-  </si>
-  <si>
     <t>58602</t>
   </si>
   <si>
-    <t>David23</t>
-  </si>
-  <si>
     <t>58603</t>
   </si>
   <si>
-    <t>David24</t>
-  </si>
-  <si>
     <t>58604</t>
   </si>
   <si>
@@ -502,120 +445,6 @@
     <t>Thank you. Your order has been received.</t>
   </si>
   <si>
-    <t>David Inc 6</t>
-  </si>
-  <si>
-    <t>David Inc 7</t>
-  </si>
-  <si>
-    <t>David Inc 8</t>
-  </si>
-  <si>
-    <t>David Inc 9</t>
-  </si>
-  <si>
-    <t>David Inc 10</t>
-  </si>
-  <si>
-    <t>David Inc 11</t>
-  </si>
-  <si>
-    <t>David Inc 12</t>
-  </si>
-  <si>
-    <t>David Inc 13</t>
-  </si>
-  <si>
-    <t>David Inc 14</t>
-  </si>
-  <si>
-    <t>David Inc 15</t>
-  </si>
-  <si>
-    <t>David Inc 16</t>
-  </si>
-  <si>
-    <t>David Inc 17</t>
-  </si>
-  <si>
-    <t>David Inc 18</t>
-  </si>
-  <si>
-    <t>David Inc 19</t>
-  </si>
-  <si>
-    <t>David Inc 20</t>
-  </si>
-  <si>
-    <t>David Inc 21</t>
-  </si>
-  <si>
-    <t>David Inc 22</t>
-  </si>
-  <si>
-    <t>David Inc 23</t>
-  </si>
-  <si>
-    <t>David Inc 24</t>
-  </si>
-  <si>
-    <t>Jackson 6</t>
-  </si>
-  <si>
-    <t>Jackson 7</t>
-  </si>
-  <si>
-    <t>Jackson 8</t>
-  </si>
-  <si>
-    <t>Jackson 9</t>
-  </si>
-  <si>
-    <t>Jackson 10</t>
-  </si>
-  <si>
-    <t>Jackson 11</t>
-  </si>
-  <si>
-    <t>Jackson 12</t>
-  </si>
-  <si>
-    <t>Jackson 13</t>
-  </si>
-  <si>
-    <t>Jackson 14</t>
-  </si>
-  <si>
-    <t>Jackson 15</t>
-  </si>
-  <si>
-    <t>Jackson 16</t>
-  </si>
-  <si>
-    <t>Jackson 17</t>
-  </si>
-  <si>
-    <t>Jackson 18</t>
-  </si>
-  <si>
-    <t>Jackson 19</t>
-  </si>
-  <si>
-    <t>Jackson 20</t>
-  </si>
-  <si>
-    <t>Jackson 21</t>
-  </si>
-  <si>
-    <t>Jackson 22</t>
-  </si>
-  <si>
-    <t>Jackson 23</t>
-  </si>
-  <si>
-    <t>Jackson 24</t>
-  </si>
-  <si>
     <t>EthanBaker</t>
   </si>
   <si>
@@ -1027,15 +856,6 @@
     <t>Angel Row</t>
   </si>
   <si>
-    <t>David25</t>
-  </si>
-  <si>
-    <t>Jackson 25</t>
-  </si>
-  <si>
-    <t>David Inc 25</t>
-  </si>
-  <si>
     <t>152 Kevin Dr</t>
   </si>
   <si>
@@ -1171,124 +991,310 @@
     <t>LucilleGriffiths4@gmail.com</t>
   </si>
   <si>
-    <t>DonnellJernigan7</t>
-  </si>
-  <si>
-    <t>DonnellJernigan7@gmail.com</t>
-  </si>
-  <si>
-    <t>MalikOtoole7</t>
-  </si>
-  <si>
-    <t>MalikOtoole7@gmail.com</t>
-  </si>
-  <si>
-    <t>AlanCaudill7</t>
-  </si>
-  <si>
-    <t>AlanCaudill7@gmail.com</t>
-  </si>
-  <si>
-    <t>AdanApplegate7</t>
-  </si>
-  <si>
-    <t>AdanApplegate7@gmail.com</t>
-  </si>
-  <si>
-    <t>AiyanaWhitworth7</t>
-  </si>
-  <si>
-    <t>AiyanaWhitworth7@gmail.com</t>
-  </si>
-  <si>
-    <t>MercedezBrien7</t>
-  </si>
-  <si>
-    <t>MercedezBrien7@gmail.com</t>
-  </si>
-  <si>
-    <t>DuaneHager7</t>
-  </si>
-  <si>
-    <t>DuaneHager7@gmail.com</t>
-  </si>
-  <si>
-    <t>LorenBell7</t>
-  </si>
-  <si>
-    <t>LorenBell7@gmail.com</t>
-  </si>
-  <si>
-    <t>GeraldHiller7</t>
-  </si>
-  <si>
-    <t>GeraldHiller7@gmail.com</t>
-  </si>
-  <si>
-    <t>DeionBranch7</t>
-  </si>
-  <si>
-    <t>DeionBranch7@gmail.com</t>
-  </si>
-  <si>
-    <t>DakotaHalstead7</t>
-  </si>
-  <si>
-    <t>DakotaHalstead7@gmail.com</t>
-  </si>
-  <si>
-    <t>ElliottFurman7</t>
-  </si>
-  <si>
-    <t>ElliottFurman7@gmail.com</t>
-  </si>
-  <si>
-    <t>MiltonCamp7</t>
-  </si>
-  <si>
-    <t>MiltonCamp7@gmail.com</t>
-  </si>
-  <si>
-    <t>DawnChester7</t>
-  </si>
-  <si>
-    <t>DawnChester7@gmail.com</t>
-  </si>
-  <si>
-    <t>ZacheryPetrie7</t>
-  </si>
-  <si>
-    <t>ZacheryPetrie7@gmail.com</t>
-  </si>
-  <si>
-    <t>EstebanAngel7</t>
-  </si>
-  <si>
-    <t>EstebanAngel7@gmail.com</t>
-  </si>
-  <si>
-    <t>JimmyBlankenship7</t>
-  </si>
-  <si>
-    <t>JimmyBlankenship7@gmail.com</t>
-  </si>
-  <si>
-    <t>AllysaGrice7</t>
-  </si>
-  <si>
-    <t>AllysaGrice7@gmail.com</t>
-  </si>
-  <si>
-    <t>AugustineYoo7</t>
-  </si>
-  <si>
-    <t>AugustineYoo7@gmail.com</t>
-  </si>
-  <si>
-    <t>BrandiSouthard7</t>
-  </si>
-  <si>
-    <t>BrandiSouthard7@gmail.com</t>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Marcelo</t>
+  </si>
+  <si>
+    <t>Trenton</t>
+  </si>
+  <si>
+    <t>Kane</t>
+  </si>
+  <si>
+    <t>Blaine</t>
+  </si>
+  <si>
+    <t>Dawson</t>
+  </si>
+  <si>
+    <t>Yvonne</t>
+  </si>
+  <si>
+    <t>Madalynn</t>
+  </si>
+  <si>
+    <t>Joana</t>
+  </si>
+  <si>
+    <t>Jeff</t>
+  </si>
+  <si>
+    <t>Darcy</t>
+  </si>
+  <si>
+    <t>Lindsay</t>
+  </si>
+  <si>
+    <t>Ty</t>
+  </si>
+  <si>
+    <t>Trista</t>
+  </si>
+  <si>
+    <t>Vicente</t>
+  </si>
+  <si>
+    <t>Turner</t>
+  </si>
+  <si>
+    <t>Robin</t>
+  </si>
+  <si>
+    <t>Antonio</t>
+  </si>
+  <si>
+    <t>Jena</t>
+  </si>
+  <si>
+    <t>Kimberlee</t>
+  </si>
+  <si>
+    <t>Hollie</t>
+  </si>
+  <si>
+    <t>Sanders</t>
+  </si>
+  <si>
+    <t>Allison</t>
+  </si>
+  <si>
+    <t>Bartley</t>
+  </si>
+  <si>
+    <t>Beck</t>
+  </si>
+  <si>
+    <t>Lanning</t>
+  </si>
+  <si>
+    <t>Goode</t>
+  </si>
+  <si>
+    <t>Nielson</t>
+  </si>
+  <si>
+    <t>Poore</t>
+  </si>
+  <si>
+    <t>Vernon</t>
+  </si>
+  <si>
+    <t>Reinhart</t>
+  </si>
+  <si>
+    <t>Montez</t>
+  </si>
+  <si>
+    <t>Palermo</t>
+  </si>
+  <si>
+    <t>Gardiner</t>
+  </si>
+  <si>
+    <t>Paulson</t>
+  </si>
+  <si>
+    <t>Brock</t>
+  </si>
+  <si>
+    <t>Webb</t>
+  </si>
+  <si>
+    <t>Cunningham</t>
+  </si>
+  <si>
+    <t>Ledesma</t>
+  </si>
+  <si>
+    <t>Ralston</t>
+  </si>
+  <si>
+    <t>Abrams</t>
+  </si>
+  <si>
+    <t>Mr. Venegas</t>
+  </si>
+  <si>
+    <t>Duckworth</t>
+  </si>
+  <si>
+    <t>Bone</t>
+  </si>
+  <si>
+    <t>Ms. Fitzgerald</t>
+  </si>
+  <si>
+    <t>Stroud</t>
+  </si>
+  <si>
+    <t>Conroy</t>
+  </si>
+  <si>
+    <t>Ms. Schulte</t>
+  </si>
+  <si>
+    <t>Ms. Chatman</t>
+  </si>
+  <si>
+    <t>Mr. Bray</t>
+  </si>
+  <si>
+    <t>Ngo</t>
+  </si>
+  <si>
+    <t>Hoff</t>
+  </si>
+  <si>
+    <t>Mr. Zeller</t>
+  </si>
+  <si>
+    <t>Mr. Hood</t>
+  </si>
+  <si>
+    <t>Ms. Vail</t>
+  </si>
+  <si>
+    <t>Mr. Hurt</t>
+  </si>
+  <si>
+    <t>Mr. Healey</t>
+  </si>
+  <si>
+    <t>Ms. Gaffney</t>
+  </si>
+  <si>
+    <t>Montero</t>
+  </si>
+  <si>
+    <t>Mr. Pool</t>
+  </si>
+  <si>
+    <t>Ms. Jacobsen</t>
+  </si>
+  <si>
+    <t>DonnellJernigan8</t>
+  </si>
+  <si>
+    <t>DonnellJernigan8@gmail.com</t>
+  </si>
+  <si>
+    <t>MalikOtoole8</t>
+  </si>
+  <si>
+    <t>MalikOtoole8@gmail.com</t>
+  </si>
+  <si>
+    <t>AlanCaudill8</t>
+  </si>
+  <si>
+    <t>AlanCaudill8@gmail.com</t>
+  </si>
+  <si>
+    <t>AdanApplegate8</t>
+  </si>
+  <si>
+    <t>AdanApplegate8@gmail.com</t>
+  </si>
+  <si>
+    <t>AiyanaWhitworth8</t>
+  </si>
+  <si>
+    <t>AiyanaWhitworth8@gmail.com</t>
+  </si>
+  <si>
+    <t>MercedezBrien8</t>
+  </si>
+  <si>
+    <t>MercedezBrien8@gmail.com</t>
+  </si>
+  <si>
+    <t>DuaneHager8</t>
+  </si>
+  <si>
+    <t>DuaneHager8@gmail.com</t>
+  </si>
+  <si>
+    <t>LorenBell8</t>
+  </si>
+  <si>
+    <t>LorenBell8@gmail.com</t>
+  </si>
+  <si>
+    <t>GeraldHiller8</t>
+  </si>
+  <si>
+    <t>GeraldHiller8@gmail.com</t>
+  </si>
+  <si>
+    <t>DeionBranch8</t>
+  </si>
+  <si>
+    <t>DeionBranch8@gmail.com</t>
+  </si>
+  <si>
+    <t>DakotaHalstead8</t>
+  </si>
+  <si>
+    <t>DakotaHalstead8@gmail.com</t>
+  </si>
+  <si>
+    <t>ElliottFurman8</t>
+  </si>
+  <si>
+    <t>ElliottFurman8@gmail.com</t>
+  </si>
+  <si>
+    <t>MiltonCamp8</t>
+  </si>
+  <si>
+    <t>MiltonCamp8@gmail.com</t>
+  </si>
+  <si>
+    <t>DawnChester8</t>
+  </si>
+  <si>
+    <t>DawnChester8@gmail.com</t>
+  </si>
+  <si>
+    <t>ZacheryPetrie8</t>
+  </si>
+  <si>
+    <t>ZacheryPetrie8@gmail.com</t>
+  </si>
+  <si>
+    <t>EstebanAngel8</t>
+  </si>
+  <si>
+    <t>EstebanAngel8@gmail.com</t>
+  </si>
+  <si>
+    <t>JimmyBlankenship8</t>
+  </si>
+  <si>
+    <t>JimmyBlankenship8@gmail.com</t>
+  </si>
+  <si>
+    <t>AllysaGrice8</t>
+  </si>
+  <si>
+    <t>AllysaGrice8@gmail.com</t>
+  </si>
+  <si>
+    <t>AugustineYoo8</t>
+  </si>
+  <si>
+    <t>AugustineYoo8@gmail.com</t>
+  </si>
+  <si>
+    <t>BrandiSouthard8</t>
+  </si>
+  <si>
+    <t>BrandiSouthard8@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2010,16 +2016,16 @@
         <v>29</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2027,10 +2033,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>12</v>
@@ -2039,31 +2045,31 @@
         <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>337</v>
+        <v>277</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>337</v>
+        <v>277</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>338</v>
+        <v>278</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="P2" s="7"/>
     </row>
@@ -2072,10 +2078,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
@@ -2085,28 +2091,28 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>339</v>
+        <v>279</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>339</v>
+        <v>279</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>340</v>
+        <v>280</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2114,10 +2120,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>12</v>
@@ -2127,28 +2133,28 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>341</v>
+        <v>281</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>341</v>
+        <v>281</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>342</v>
+        <v>282</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N4" s="10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2156,10 +2162,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
@@ -2169,28 +2175,28 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>343</v>
+        <v>283</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>343</v>
+        <v>283</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>344</v>
+        <v>284</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2198,10 +2204,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>12</v>
@@ -2211,28 +2217,28 @@
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>345</v>
+        <v>285</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>345</v>
+        <v>285</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>346</v>
+        <v>286</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2240,10 +2246,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>8</v>
@@ -2253,28 +2259,28 @@
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>347</v>
+        <v>287</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>347</v>
+        <v>287</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>348</v>
+        <v>288</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2282,10 +2288,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>12</v>
@@ -2295,28 +2301,28 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>349</v>
+        <v>289</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>349</v>
+        <v>289</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>350</v>
+        <v>290</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N8" s="10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2324,10 +2330,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
@@ -2337,28 +2343,28 @@
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>351</v>
+        <v>291</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>351</v>
+        <v>291</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>352</v>
+        <v>292</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N9" s="10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2366,10 +2372,10 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>12</v>
@@ -2379,28 +2385,28 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>353</v>
+        <v>293</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>353</v>
+        <v>293</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>354</v>
+        <v>294</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N10" s="10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2408,10 +2414,10 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>8</v>
@@ -2421,28 +2427,28 @@
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>355</v>
+        <v>295</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>355</v>
+        <v>295</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>356</v>
+        <v>296</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="M11" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N11" s="10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2450,10 +2456,10 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>12</v>
@@ -2463,28 +2469,28 @@
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>357</v>
+        <v>297</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>357</v>
+        <v>297</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>358</v>
+        <v>298</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="M12" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N12" s="10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2492,10 +2498,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>8</v>
@@ -2505,28 +2511,28 @@
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>359</v>
+        <v>299</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>359</v>
+        <v>299</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>360</v>
+        <v>300</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="M13" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N13" s="10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2534,10 +2540,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>12</v>
@@ -2547,28 +2553,28 @@
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>361</v>
+        <v>301</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>361</v>
+        <v>301</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>362</v>
+        <v>302</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="M14" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N14" s="10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2576,10 +2582,10 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>8</v>
@@ -2589,28 +2595,28 @@
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>363</v>
+        <v>303</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>363</v>
+        <v>303</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>364</v>
+        <v>304</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="L15" s="11" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="M15" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N15" s="10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2618,10 +2624,10 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>12</v>
@@ -2631,28 +2637,28 @@
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>365</v>
+        <v>305</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>365</v>
+        <v>305</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>366</v>
+        <v>306</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>30</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="L16" s="11" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="M16" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N16" s="10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2660,10 +2666,10 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>8</v>
@@ -2673,28 +2679,28 @@
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>367</v>
+        <v>307</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>367</v>
+        <v>307</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>368</v>
+        <v>308</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="M17" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N17" s="10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2702,10 +2708,10 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>8</v>
@@ -2715,28 +2721,28 @@
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="12" t="s">
-        <v>369</v>
+        <v>309</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>369</v>
+        <v>309</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>370</v>
+        <v>310</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N18" s="10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2744,10 +2750,10 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>8</v>
@@ -2757,28 +2763,28 @@
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="12" t="s">
-        <v>371</v>
+        <v>311</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>371</v>
+        <v>311</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>372</v>
+        <v>312</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="L19" s="11" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="M19" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N19" s="10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2786,10 +2792,10 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>8</v>
@@ -2799,28 +2805,28 @@
       </c>
       <c r="F20" s="12"/>
       <c r="G20" s="12" t="s">
-        <v>373</v>
+        <v>313</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>373</v>
+        <v>313</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>374</v>
+        <v>314</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="L20" s="11" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="M20" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N20" s="10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2828,10 +2834,10 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>8</v>
@@ -2841,28 +2847,28 @@
       </c>
       <c r="F21" s="12"/>
       <c r="G21" s="12" t="s">
-        <v>375</v>
+        <v>315</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>375</v>
+        <v>315</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>376</v>
+        <v>316</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="L21" s="11" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="M21" s="10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N21" s="10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2908,8 +2914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0775DEA-3893-49AA-8C48-45DC29C761B9}">
   <dimension ref="A1:AF21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2:T21"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3007,34 +3013,34 @@
         <v>11</v>
       </c>
       <c r="U1" s="17" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="Z1" s="4" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="AA1" s="4" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="AB1" s="4" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="AC1" s="4" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="AD1" s="4" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3042,43 +3048,43 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="F2" s="20">
-        <v>1</v>
+        <v>80</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>318</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>252</v>
+        <v>195</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>253</v>
+        <v>196</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>232</v>
+        <v>175</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>292</v>
+        <v>235</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>300</v>
+        <v>243</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="O2" s="20" t="s">
         <v>27</v>
@@ -3087,37 +3093,37 @@
         <v>26</v>
       </c>
       <c r="Q2" s="21" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="R2" s="14" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="S2" s="14" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="T2" s="22" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="U2" s="15" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="V2" s="14" t="s">
-        <v>31</v>
+        <v>319</v>
       </c>
       <c r="W2" s="14" t="s">
-        <v>173</v>
+        <v>339</v>
       </c>
       <c r="X2" s="14" t="s">
-        <v>154</v>
+        <v>359</v>
       </c>
       <c r="Y2" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="Z2" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA2" s="14" t="s">
         <v>112</v>
-      </c>
-      <c r="AA2" s="14" t="s">
-        <v>131</v>
       </c>
       <c r="AB2" s="14" t="s">
         <v>23</v>
@@ -3126,7 +3132,7 @@
         <v>24</v>
       </c>
       <c r="AD2" s="20" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="AF2" s="16"/>
     </row>
@@ -3135,43 +3141,43 @@
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="F3" s="20">
-        <v>2</v>
+        <v>81</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>317</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>254</v>
+        <v>197</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>255</v>
+        <v>198</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>233</v>
+        <v>176</v>
       </c>
       <c r="J3" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="L3" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="K3" s="14" t="s">
-        <v>293</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>129</v>
-      </c>
       <c r="M3" s="14" t="s">
-        <v>301</v>
+        <v>244</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="O3" s="20" t="s">
         <v>27</v>
@@ -3180,37 +3186,37 @@
         <v>26</v>
       </c>
       <c r="Q3" s="21" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="R3" s="14" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="S3" s="14" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="T3" s="22" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="U3" s="15" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="V3" s="14" t="s">
-        <v>32</v>
+        <v>320</v>
       </c>
       <c r="W3" s="14" t="s">
-        <v>174</v>
+        <v>340</v>
       </c>
       <c r="X3" s="14" t="s">
-        <v>155</v>
+        <v>360</v>
       </c>
       <c r="Y3" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="Z3" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA3" s="14" t="s">
         <v>113</v>
-      </c>
-      <c r="AA3" s="14" t="s">
-        <v>132</v>
       </c>
       <c r="AB3" s="14" t="s">
         <v>23</v>
@@ -3219,7 +3225,7 @@
         <v>24</v>
       </c>
       <c r="AD3" s="20" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="AF3" s="16"/>
     </row>
@@ -3228,43 +3234,43 @@
         <v>1</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="F4" s="20">
-        <v>1</v>
+        <v>82</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>318</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>256</v>
+        <v>199</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>257</v>
+        <v>200</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>234</v>
+        <v>177</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>292</v>
+        <v>235</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>302</v>
+        <v>245</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="O4" s="20" t="s">
         <v>27</v>
@@ -3273,37 +3279,37 @@
         <v>26</v>
       </c>
       <c r="Q4" s="21" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="R4" s="14" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="S4" s="14" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="T4" s="22" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="U4" s="15" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="V4" s="14" t="s">
-        <v>33</v>
+        <v>321</v>
       </c>
       <c r="W4" s="14" t="s">
-        <v>175</v>
+        <v>341</v>
       </c>
       <c r="X4" s="14" t="s">
-        <v>156</v>
+        <v>361</v>
       </c>
       <c r="Y4" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="Z4" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA4" s="14" t="s">
         <v>114</v>
-      </c>
-      <c r="AA4" s="14" t="s">
-        <v>133</v>
       </c>
       <c r="AB4" s="14" t="s">
         <v>23</v>
@@ -3312,7 +3318,7 @@
         <v>24</v>
       </c>
       <c r="AD4" s="20" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="AF4" s="16"/>
     </row>
@@ -3321,43 +3327,43 @@
         <v>1</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="F5" s="20">
-        <v>2</v>
+        <v>83</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>317</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>258</v>
+        <v>201</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>259</v>
+        <v>202</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>235</v>
+        <v>178</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>294</v>
+        <v>237</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>303</v>
+        <v>246</v>
       </c>
       <c r="N5" s="14" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="O5" s="20" t="s">
         <v>27</v>
@@ -3366,37 +3372,37 @@
         <v>26</v>
       </c>
       <c r="Q5" s="21" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="R5" s="14" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="S5" s="14" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="T5" s="22" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="U5" s="15" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="V5" s="14" t="s">
-        <v>34</v>
+        <v>322</v>
       </c>
       <c r="W5" s="14" t="s">
-        <v>176</v>
+        <v>342</v>
       </c>
       <c r="X5" s="14" t="s">
-        <v>157</v>
+        <v>362</v>
       </c>
       <c r="Y5" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="Z5" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA5" s="14" t="s">
         <v>115</v>
-      </c>
-      <c r="AA5" s="14" t="s">
-        <v>134</v>
       </c>
       <c r="AB5" s="14" t="s">
         <v>23</v>
@@ -3405,7 +3411,7 @@
         <v>24</v>
       </c>
       <c r="AD5" s="20" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="AF5" s="16"/>
     </row>
@@ -3414,43 +3420,43 @@
         <v>1</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="F6" s="20">
-        <v>1</v>
+        <v>84</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>318</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>260</v>
+        <v>203</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>261</v>
+        <v>204</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>236</v>
+        <v>179</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>295</v>
+        <v>238</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>304</v>
+        <v>247</v>
       </c>
       <c r="N6" s="14" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="O6" s="20" t="s">
         <v>27</v>
@@ -3459,37 +3465,37 @@
         <v>26</v>
       </c>
       <c r="Q6" s="21" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="R6" s="14" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="S6" s="14" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="T6" s="22" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="U6" s="15" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="V6" s="14" t="s">
-        <v>35</v>
+        <v>323</v>
       </c>
       <c r="W6" s="14" t="s">
-        <v>177</v>
+        <v>343</v>
       </c>
       <c r="X6" s="14" t="s">
-        <v>158</v>
+        <v>363</v>
       </c>
       <c r="Y6" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="Z6" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA6" s="14" t="s">
         <v>116</v>
-      </c>
-      <c r="AA6" s="14" t="s">
-        <v>135</v>
       </c>
       <c r="AB6" s="14" t="s">
         <v>23</v>
@@ -3498,7 +3504,7 @@
         <v>24</v>
       </c>
       <c r="AD6" s="20" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="AF6" s="16"/>
     </row>
@@ -3507,43 +3513,43 @@
         <v>1</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="F7" s="20">
-        <v>2</v>
+        <v>85</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>317</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>262</v>
+        <v>205</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>263</v>
+        <v>206</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>237</v>
+        <v>180</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>292</v>
+        <v>235</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="M7" s="14" t="s">
-        <v>305</v>
+        <v>248</v>
       </c>
       <c r="N7" s="14" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="O7" s="20" t="s">
         <v>27</v>
@@ -3552,37 +3558,37 @@
         <v>26</v>
       </c>
       <c r="Q7" s="21" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="R7" s="14" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="S7" s="14" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="T7" s="22" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="U7" s="15" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="V7" s="14" t="s">
-        <v>36</v>
+        <v>324</v>
       </c>
       <c r="W7" s="14" t="s">
-        <v>178</v>
+        <v>344</v>
       </c>
       <c r="X7" s="14" t="s">
-        <v>159</v>
+        <v>364</v>
       </c>
       <c r="Y7" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="Z7" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA7" s="14" t="s">
         <v>117</v>
-      </c>
-      <c r="AA7" s="14" t="s">
-        <v>136</v>
       </c>
       <c r="AB7" s="14" t="s">
         <v>23</v>
@@ -3591,7 +3597,7 @@
         <v>24</v>
       </c>
       <c r="AD7" s="20" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="AF7" s="16"/>
     </row>
@@ -3600,43 +3606,43 @@
         <v>1</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="F8" s="20">
-        <v>1</v>
+        <v>86</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>318</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>264</v>
+        <v>207</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>265</v>
+        <v>208</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>238</v>
+        <v>181</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>296</v>
+        <v>239</v>
       </c>
       <c r="L8" s="14" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>306</v>
+        <v>249</v>
       </c>
       <c r="N8" s="14" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="O8" s="20" t="s">
         <v>27</v>
@@ -3645,37 +3651,37 @@
         <v>26</v>
       </c>
       <c r="Q8" s="21" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="R8" s="14" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="S8" s="14" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="T8" s="22" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="U8" s="15" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="V8" s="14" t="s">
-        <v>37</v>
+        <v>325</v>
       </c>
       <c r="W8" s="14" t="s">
-        <v>179</v>
+        <v>345</v>
       </c>
       <c r="X8" s="14" t="s">
-        <v>160</v>
+        <v>365</v>
       </c>
       <c r="Y8" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="Z8" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA8" s="14" t="s">
         <v>118</v>
-      </c>
-      <c r="AA8" s="14" t="s">
-        <v>137</v>
       </c>
       <c r="AB8" s="14" t="s">
         <v>23</v>
@@ -3684,7 +3690,7 @@
         <v>24</v>
       </c>
       <c r="AD8" s="20" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="AF8" s="16"/>
     </row>
@@ -3693,43 +3699,43 @@
         <v>1</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="F9" s="20">
-        <v>2</v>
+        <v>87</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>317</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>266</v>
+        <v>209</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>267</v>
+        <v>210</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>239</v>
+        <v>182</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>297</v>
+        <v>240</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="M9" s="14" t="s">
-        <v>307</v>
+        <v>250</v>
       </c>
       <c r="N9" s="14" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="O9" s="20" t="s">
         <v>27</v>
@@ -3738,37 +3744,37 @@
         <v>26</v>
       </c>
       <c r="Q9" s="21" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="R9" s="14" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="S9" s="14" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="T9" s="22" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="U9" s="15" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="V9" s="14" t="s">
-        <v>38</v>
+        <v>326</v>
       </c>
       <c r="W9" s="14" t="s">
-        <v>180</v>
+        <v>346</v>
       </c>
       <c r="X9" s="14" t="s">
-        <v>161</v>
+        <v>366</v>
       </c>
       <c r="Y9" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="Z9" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA9" s="14" t="s">
         <v>119</v>
-      </c>
-      <c r="AA9" s="14" t="s">
-        <v>138</v>
       </c>
       <c r="AB9" s="14" t="s">
         <v>23</v>
@@ -3777,7 +3783,7 @@
         <v>24</v>
       </c>
       <c r="AD9" s="20" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="AF9" s="16"/>
     </row>
@@ -3786,43 +3792,43 @@
         <v>1</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="F10" s="20">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>318</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>268</v>
+        <v>211</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>269</v>
+        <v>212</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>240</v>
+        <v>183</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>298</v>
+        <v>241</v>
       </c>
       <c r="L10" s="14" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="M10" s="14" t="s">
-        <v>308</v>
+        <v>251</v>
       </c>
       <c r="N10" s="14" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="O10" s="20" t="s">
         <v>27</v>
@@ -3831,37 +3837,37 @@
         <v>26</v>
       </c>
       <c r="Q10" s="21" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="R10" s="14" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="S10" s="14" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="T10" s="22" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="U10" s="15" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="V10" s="14" t="s">
-        <v>39</v>
+        <v>327</v>
       </c>
       <c r="W10" s="14" t="s">
-        <v>181</v>
+        <v>347</v>
       </c>
       <c r="X10" s="14" t="s">
-        <v>162</v>
+        <v>367</v>
       </c>
       <c r="Y10" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="Z10" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA10" s="14" t="s">
         <v>120</v>
-      </c>
-      <c r="AA10" s="14" t="s">
-        <v>139</v>
       </c>
       <c r="AB10" s="14" t="s">
         <v>23</v>
@@ -3870,7 +3876,7 @@
         <v>24</v>
       </c>
       <c r="AD10" s="20" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="AF10" s="16"/>
     </row>
@@ -3879,43 +3885,43 @@
         <v>1</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="F11" s="20">
-        <v>2</v>
+        <v>89</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>317</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>270</v>
+        <v>213</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>271</v>
+        <v>214</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>241</v>
+        <v>184</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>299</v>
+        <v>242</v>
       </c>
       <c r="L11" s="14" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="M11" s="14" t="s">
-        <v>309</v>
+        <v>252</v>
       </c>
       <c r="N11" s="14" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="O11" s="20" t="s">
         <v>27</v>
@@ -3924,37 +3930,37 @@
         <v>26</v>
       </c>
       <c r="Q11" s="21" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="R11" s="14" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="S11" s="14" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="T11" s="22" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="U11" s="15" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="V11" s="14" t="s">
-        <v>40</v>
+        <v>328</v>
       </c>
       <c r="W11" s="14" t="s">
-        <v>182</v>
+        <v>348</v>
       </c>
       <c r="X11" s="14" t="s">
-        <v>163</v>
+        <v>368</v>
       </c>
       <c r="Y11" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="Z11" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA11" s="14" t="s">
         <v>121</v>
-      </c>
-      <c r="AA11" s="14" t="s">
-        <v>140</v>
       </c>
       <c r="AB11" s="14" t="s">
         <v>23</v>
@@ -3963,7 +3969,7 @@
         <v>24</v>
       </c>
       <c r="AD11" s="20" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="AF11" s="16"/>
     </row>
@@ -3972,43 +3978,43 @@
         <v>1</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="F12" s="20">
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>318</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>272</v>
+        <v>215</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>273</v>
+        <v>216</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>242</v>
+        <v>185</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>320</v>
+        <v>263</v>
       </c>
       <c r="L12" s="14" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="M12" s="14" t="s">
-        <v>310</v>
+        <v>253</v>
       </c>
       <c r="N12" s="14" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="O12" s="20" t="s">
         <v>27</v>
@@ -4017,37 +4023,37 @@
         <v>26</v>
       </c>
       <c r="Q12" s="21" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="R12" s="14" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="S12" s="14" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="T12" s="22" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="U12" s="15" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="V12" s="14" t="s">
-        <v>41</v>
+        <v>329</v>
       </c>
       <c r="W12" s="14" t="s">
-        <v>183</v>
+        <v>349</v>
       </c>
       <c r="X12" s="14" t="s">
-        <v>164</v>
+        <v>369</v>
       </c>
       <c r="Y12" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="Z12" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA12" s="14" t="s">
         <v>122</v>
-      </c>
-      <c r="AA12" s="14" t="s">
-        <v>141</v>
       </c>
       <c r="AB12" s="14" t="s">
         <v>23</v>
@@ -4056,7 +4062,7 @@
         <v>24</v>
       </c>
       <c r="AD12" s="20" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="AF12" s="16"/>
     </row>
@@ -4065,43 +4071,43 @@
         <v>1</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="F13" s="20">
-        <v>2</v>
+        <v>80</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>317</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>274</v>
+        <v>217</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>275</v>
+        <v>218</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>243</v>
+        <v>186</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="K13" s="14" t="s">
-        <v>321</v>
+        <v>264</v>
       </c>
       <c r="L13" s="14" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="M13" s="14" t="s">
-        <v>311</v>
+        <v>254</v>
       </c>
       <c r="N13" s="14" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="O13" s="20" t="s">
         <v>27</v>
@@ -4110,37 +4116,37 @@
         <v>26</v>
       </c>
       <c r="Q13" s="21" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="R13" s="14" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="S13" s="14" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="T13" s="22" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="U13" s="15" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="V13" s="14" t="s">
-        <v>42</v>
+        <v>330</v>
       </c>
       <c r="W13" s="14" t="s">
-        <v>184</v>
+        <v>350</v>
       </c>
       <c r="X13" s="14" t="s">
-        <v>165</v>
+        <v>370</v>
       </c>
       <c r="Y13" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="Z13" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA13" s="14" t="s">
         <v>123</v>
-      </c>
-      <c r="AA13" s="14" t="s">
-        <v>142</v>
       </c>
       <c r="AB13" s="14" t="s">
         <v>23</v>
@@ -4149,7 +4155,7 @@
         <v>24</v>
       </c>
       <c r="AD13" s="20" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="AF13" s="16"/>
     </row>
@@ -4158,43 +4164,43 @@
         <v>1</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="F14" s="20">
-        <v>1</v>
+        <v>81</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>318</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>276</v>
+        <v>219</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>277</v>
+        <v>220</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>244</v>
+        <v>187</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="K14" s="14" t="s">
-        <v>299</v>
+        <v>242</v>
       </c>
       <c r="L14" s="14" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="M14" s="14" t="s">
-        <v>312</v>
+        <v>255</v>
       </c>
       <c r="N14" s="14" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="O14" s="20" t="s">
         <v>27</v>
@@ -4203,37 +4209,37 @@
         <v>26</v>
       </c>
       <c r="Q14" s="21" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="R14" s="14" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="S14" s="14" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="T14" s="22" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="U14" s="15" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="V14" s="14" t="s">
-        <v>43</v>
+        <v>331</v>
       </c>
       <c r="W14" s="14" t="s">
-        <v>185</v>
+        <v>351</v>
       </c>
       <c r="X14" s="14" t="s">
-        <v>166</v>
+        <v>371</v>
       </c>
       <c r="Y14" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="Z14" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA14" s="14" t="s">
         <v>124</v>
-      </c>
-      <c r="AA14" s="14" t="s">
-        <v>143</v>
       </c>
       <c r="AB14" s="14" t="s">
         <v>23</v>
@@ -4242,7 +4248,7 @@
         <v>24</v>
       </c>
       <c r="AD14" s="20" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="AF14" s="16"/>
     </row>
@@ -4251,43 +4257,43 @@
         <v>1</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="F15" s="20">
-        <v>2</v>
+        <v>82</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>317</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>278</v>
+        <v>221</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>279</v>
+        <v>222</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>245</v>
+        <v>188</v>
       </c>
       <c r="J15" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="K15" s="14" t="s">
-        <v>322</v>
+        <v>265</v>
       </c>
       <c r="L15" s="14" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="M15" s="14" t="s">
-        <v>313</v>
+        <v>256</v>
       </c>
       <c r="N15" s="14" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="O15" s="20" t="s">
         <v>27</v>
@@ -4296,37 +4302,37 @@
         <v>26</v>
       </c>
       <c r="Q15" s="21" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="R15" s="14" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="S15" s="14" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="T15" s="22" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="U15" s="15" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="V15" s="14" t="s">
-        <v>82</v>
+        <v>332</v>
       </c>
       <c r="W15" s="14" t="s">
-        <v>186</v>
+        <v>352</v>
       </c>
       <c r="X15" s="14" t="s">
-        <v>167</v>
+        <v>372</v>
       </c>
       <c r="Y15" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="Z15" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA15" s="14" t="s">
         <v>125</v>
-      </c>
-      <c r="AA15" s="14" t="s">
-        <v>144</v>
       </c>
       <c r="AB15" s="14" t="s">
         <v>23</v>
@@ -4335,7 +4341,7 @@
         <v>24</v>
       </c>
       <c r="AD15" s="20" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="AF15" s="16"/>
     </row>
@@ -4344,43 +4350,43 @@
         <v>1</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="F16" s="20">
-        <v>1</v>
+        <v>83</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>318</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>280</v>
+        <v>223</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>281</v>
+        <v>224</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>246</v>
+        <v>189</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="K16" s="14" t="s">
-        <v>323</v>
+        <v>266</v>
       </c>
       <c r="L16" s="14" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="M16" s="14" t="s">
-        <v>314</v>
+        <v>257</v>
       </c>
       <c r="N16" s="14" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="O16" s="20" t="s">
         <v>27</v>
@@ -4389,37 +4395,37 @@
         <v>26</v>
       </c>
       <c r="Q16" s="21" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="R16" s="14" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="S16" s="14" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="T16" s="22" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="U16" s="15" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="V16" s="14" t="s">
-        <v>84</v>
+        <v>333</v>
       </c>
       <c r="W16" s="14" t="s">
-        <v>187</v>
+        <v>353</v>
       </c>
       <c r="X16" s="14" t="s">
-        <v>168</v>
+        <v>373</v>
       </c>
       <c r="Y16" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="Z16" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA16" s="14" t="s">
         <v>126</v>
-      </c>
-      <c r="AA16" s="14" t="s">
-        <v>145</v>
       </c>
       <c r="AB16" s="14" t="s">
         <v>23</v>
@@ -4428,7 +4434,7 @@
         <v>24</v>
       </c>
       <c r="AD16" s="20" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="AF16" s="16"/>
     </row>
@@ -4437,43 +4443,43 @@
         <v>1</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="F17" s="20">
-        <v>2</v>
+        <v>84</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>317</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>282</v>
+        <v>225</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>283</v>
+        <v>226</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>247</v>
+        <v>190</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>324</v>
+        <v>267</v>
       </c>
       <c r="L17" s="14" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="M17" s="14" t="s">
-        <v>315</v>
+        <v>258</v>
       </c>
       <c r="N17" s="14" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="O17" s="20" t="s">
         <v>27</v>
@@ -4482,37 +4488,37 @@
         <v>26</v>
       </c>
       <c r="Q17" s="21" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="R17" s="14" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="S17" s="14" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="T17" s="22" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="U17" s="15" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="V17" s="14" t="s">
-        <v>86</v>
+        <v>334</v>
       </c>
       <c r="W17" s="14" t="s">
-        <v>188</v>
+        <v>354</v>
       </c>
       <c r="X17" s="14" t="s">
-        <v>169</v>
+        <v>374</v>
       </c>
       <c r="Y17" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="Z17" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA17" s="14" t="s">
         <v>127</v>
-      </c>
-      <c r="AA17" s="14" t="s">
-        <v>146</v>
       </c>
       <c r="AB17" s="14" t="s">
         <v>23</v>
@@ -4521,7 +4527,7 @@
         <v>24</v>
       </c>
       <c r="AD17" s="20" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
@@ -4529,43 +4535,43 @@
         <v>1</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="F18" s="20">
-        <v>1</v>
+        <v>85</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>318</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>284</v>
+        <v>227</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>285</v>
+        <v>228</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>248</v>
+        <v>191</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="K18" s="14" t="s">
-        <v>325</v>
+        <v>268</v>
       </c>
       <c r="L18" s="14" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="M18" s="14" t="s">
-        <v>316</v>
+        <v>259</v>
       </c>
       <c r="N18" s="14" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="O18" s="20" t="s">
         <v>27</v>
@@ -4574,37 +4580,37 @@
         <v>26</v>
       </c>
       <c r="Q18" s="21" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="R18" s="14" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="S18" s="14" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="T18" s="22" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="U18" s="15" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="V18" s="14" t="s">
-        <v>88</v>
+        <v>335</v>
       </c>
       <c r="W18" s="14" t="s">
-        <v>189</v>
+        <v>355</v>
       </c>
       <c r="X18" s="14" t="s">
-        <v>170</v>
+        <v>375</v>
       </c>
       <c r="Y18" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="Z18" s="14" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="AA18" s="14" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="AB18" s="14" t="s">
         <v>23</v>
@@ -4613,7 +4619,7 @@
         <v>24</v>
       </c>
       <c r="AD18" s="20" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
@@ -4621,43 +4627,43 @@
         <v>1</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="F19" s="20">
-        <v>2</v>
+        <v>86</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>317</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>286</v>
+        <v>229</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>287</v>
+        <v>230</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>249</v>
+        <v>192</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>326</v>
+        <v>269</v>
       </c>
       <c r="L19" s="14" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="M19" s="14" t="s">
-        <v>317</v>
+        <v>260</v>
       </c>
       <c r="N19" s="14" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="O19" s="20" t="s">
         <v>27</v>
@@ -4666,37 +4672,37 @@
         <v>26</v>
       </c>
       <c r="Q19" s="21" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="R19" s="14" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="S19" s="14" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="T19" s="22" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="U19" s="15" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="V19" s="14" t="s">
-        <v>90</v>
+        <v>336</v>
       </c>
       <c r="W19" s="14" t="s">
-        <v>190</v>
+        <v>356</v>
       </c>
       <c r="X19" s="14" t="s">
-        <v>171</v>
+        <v>376</v>
       </c>
       <c r="Y19" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="Z19" s="14" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="AA19" s="14" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="AB19" s="14" t="s">
         <v>23</v>
@@ -4705,7 +4711,7 @@
         <v>24</v>
       </c>
       <c r="AD19" s="20" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
@@ -4713,43 +4719,43 @@
         <v>1</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="F20" s="20">
-        <v>1</v>
+        <v>87</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>318</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>288</v>
+        <v>231</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>289</v>
+        <v>232</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>250</v>
+        <v>193</v>
       </c>
       <c r="J20" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="K20" s="14" t="s">
-        <v>327</v>
+        <v>270</v>
       </c>
       <c r="L20" s="14" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="M20" s="14" t="s">
-        <v>318</v>
+        <v>261</v>
       </c>
       <c r="N20" s="14" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="O20" s="20" t="s">
         <v>27</v>
@@ -4758,37 +4764,37 @@
         <v>26</v>
       </c>
       <c r="Q20" s="21" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="R20" s="14" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="S20" s="14" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="T20" s="22" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="U20" s="15" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="V20" s="14" t="s">
-        <v>92</v>
+        <v>337</v>
       </c>
       <c r="W20" s="14" t="s">
-        <v>191</v>
+        <v>357</v>
       </c>
       <c r="X20" s="14" t="s">
-        <v>172</v>
+        <v>377</v>
       </c>
       <c r="Y20" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="Z20" s="14" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="AA20" s="14" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="AB20" s="14" t="s">
         <v>23</v>
@@ -4797,7 +4803,7 @@
         <v>24</v>
       </c>
       <c r="AD20" s="20" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:30" ht="28.8" x14ac:dyDescent="0.3">
@@ -4805,43 +4811,43 @@
         <v>1</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="F21" s="20">
-        <v>2</v>
+        <v>84</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>317</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>290</v>
+        <v>233</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>291</v>
+        <v>234</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>251</v>
+        <v>194</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="K21" s="14" t="s">
-        <v>328</v>
+        <v>271</v>
       </c>
       <c r="L21" s="14" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="M21" s="14" t="s">
-        <v>319</v>
+        <v>262</v>
       </c>
       <c r="N21" s="14" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="O21" s="20" t="s">
         <v>27</v>
@@ -4850,37 +4856,37 @@
         <v>26</v>
       </c>
       <c r="Q21" s="21" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="R21" s="19" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="S21" s="19" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="T21" s="25" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="U21" s="15" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="V21" s="14" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="W21" s="14" t="s">
-        <v>330</v>
+        <v>358</v>
       </c>
       <c r="X21" s="14" t="s">
-        <v>331</v>
+        <v>378</v>
       </c>
       <c r="Y21" s="14" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="Z21" s="14" t="s">
-        <v>332</v>
+        <v>272</v>
       </c>
       <c r="AA21" s="14" t="s">
-        <v>333</v>
+        <v>273</v>
       </c>
       <c r="AB21" s="14" t="s">
         <v>23</v>
@@ -4889,7 +4895,7 @@
         <v>24</v>
       </c>
       <c r="AD21" s="20" t="s">
-        <v>334</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -4942,7 +4948,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="26" t="s">
-        <v>335</v>
+        <v>275</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -4967,10 +4973,10 @@
         <v>EthanBaker4@gmail.com</v>
       </c>
       <c r="G2" t="s">
-        <v>192</v>
+        <v>135</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="I2">
         <v>4</v>
@@ -4990,7 +4996,7 @@
         <v>DelanieCarman4@gmail.com</v>
       </c>
       <c r="G3" t="s">
-        <v>193</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -5007,7 +5013,7 @@
         <v>BretAgnew4@gmail.com</v>
       </c>
       <c r="G4" t="s">
-        <v>194</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -5024,7 +5030,7 @@
         <v>EdgardoTaylor4@gmail.com</v>
       </c>
       <c r="G5" t="s">
-        <v>195</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -5041,7 +5047,7 @@
         <v>TyrekReis4@gmail.com</v>
       </c>
       <c r="G6" t="s">
-        <v>196</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -5058,7 +5064,7 @@
         <v>LeannaChow4@gmail.com</v>
       </c>
       <c r="G7" t="s">
-        <v>197</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -5075,7 +5081,7 @@
         <v>TuckerCarlson4@gmail.com</v>
       </c>
       <c r="G8" t="s">
-        <v>198</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -5092,7 +5098,7 @@
         <v>AnnmarieConnor4@gmail.com</v>
       </c>
       <c r="G9" t="s">
-        <v>199</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -5109,7 +5115,7 @@
         <v>MoniqueWitte4@gmail.com</v>
       </c>
       <c r="G10" t="s">
-        <v>200</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -5126,7 +5132,7 @@
         <v>MikelWhitlock4@gmail.com</v>
       </c>
       <c r="G11" t="s">
-        <v>201</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -5143,7 +5149,7 @@
         <v>VincentAmaya4@gmail.com</v>
       </c>
       <c r="G12" t="s">
-        <v>202</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -5160,7 +5166,7 @@
         <v>KeiraQuiroz4@gmail.com</v>
       </c>
       <c r="G13" t="s">
-        <v>203</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -5177,7 +5183,7 @@
         <v>EllisCreech4@gmail.com</v>
       </c>
       <c r="G14" t="s">
-        <v>204</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -5194,7 +5200,7 @@
         <v>DionteCreel4@gmail.com</v>
       </c>
       <c r="G15" t="s">
-        <v>205</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -5211,7 +5217,7 @@
         <v>NicholeFoust4@gmail.com</v>
       </c>
       <c r="G16" t="s">
-        <v>206</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -5228,7 +5234,7 @@
         <v>ManuelConnell4@gmail.com</v>
       </c>
       <c r="G17" t="s">
-        <v>207</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -5245,7 +5251,7 @@
         <v>LourdesElam4@gmail.com</v>
       </c>
       <c r="G18" t="s">
-        <v>208</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -5262,7 +5268,7 @@
         <v>LincolnFrederick4@gmail.com</v>
       </c>
       <c r="G19" t="s">
-        <v>209</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -5279,7 +5285,7 @@
         <v>AlisaCash4@gmail.com</v>
       </c>
       <c r="G20" t="s">
-        <v>210</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5296,12 +5302,12 @@
         <v>LucilleGriffiths4@gmail.com</v>
       </c>
       <c r="G21" t="s">
-        <v>211</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="23" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A22" s="30" t="s">
-        <v>336</v>
+        <v>276</v>
       </c>
       <c r="B22" s="31"/>
       <c r="C22" s="31"/>
@@ -5315,347 +5321,347 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="str">
         <f>CONCATENATE($G23,$I$23)</f>
-        <v>DonnellJernigan7</v>
+        <v>DonnellJernigan8</v>
       </c>
       <c r="B23" s="1" t="str">
         <f>CONCATENATE($G23,$I$23)</f>
-        <v>DonnellJernigan7</v>
+        <v>DonnellJernigan8</v>
       </c>
       <c r="C23" s="2" t="str">
         <f>CONCATENATE($G23,$I$23,$H$23)</f>
-        <v>DonnellJernigan7@gmail.com</v>
+        <v>DonnellJernigan8@gmail.com</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>212</v>
+        <v>155</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="I23">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="str">
         <f t="shared" ref="A24:B42" si="2">CONCATENATE($G24,$I$23)</f>
-        <v>MalikOtoole7</v>
+        <v>MalikOtoole8</v>
       </c>
       <c r="B24" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MalikOtoole7</v>
+        <v>MalikOtoole8</v>
       </c>
       <c r="C24" s="2" t="str">
         <f t="shared" ref="C24:C42" si="3">CONCATENATE($G24,$I$23,$H$23)</f>
-        <v>MalikOtoole7@gmail.com</v>
+        <v>MalikOtoole8@gmail.com</v>
       </c>
       <c r="G24" t="s">
-        <v>213</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AlanCaudill7</v>
+        <v>AlanCaudill8</v>
       </c>
       <c r="B25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AlanCaudill7</v>
+        <v>AlanCaudill8</v>
       </c>
       <c r="C25" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AlanCaudill7@gmail.com</v>
+        <v>AlanCaudill8@gmail.com</v>
       </c>
       <c r="G25" t="s">
-        <v>214</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AdanApplegate7</v>
+        <v>AdanApplegate8</v>
       </c>
       <c r="B26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AdanApplegate7</v>
+        <v>AdanApplegate8</v>
       </c>
       <c r="C26" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AdanApplegate7@gmail.com</v>
+        <v>AdanApplegate8@gmail.com</v>
       </c>
       <c r="G26" t="s">
-        <v>215</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AiyanaWhitworth7</v>
+        <v>AiyanaWhitworth8</v>
       </c>
       <c r="B27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AiyanaWhitworth7</v>
+        <v>AiyanaWhitworth8</v>
       </c>
       <c r="C27" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AiyanaWhitworth7@gmail.com</v>
+        <v>AiyanaWhitworth8@gmail.com</v>
       </c>
       <c r="G27" t="s">
-        <v>216</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MercedezBrien7</v>
+        <v>MercedezBrien8</v>
       </c>
       <c r="B28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MercedezBrien7</v>
+        <v>MercedezBrien8</v>
       </c>
       <c r="C28" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>MercedezBrien7@gmail.com</v>
+        <v>MercedezBrien8@gmail.com</v>
       </c>
       <c r="G28" t="s">
-        <v>217</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DuaneHager7</v>
+        <v>DuaneHager8</v>
       </c>
       <c r="B29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DuaneHager7</v>
+        <v>DuaneHager8</v>
       </c>
       <c r="C29" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DuaneHager7@gmail.com</v>
+        <v>DuaneHager8@gmail.com</v>
       </c>
       <c r="G29" t="s">
-        <v>218</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>LorenBell7</v>
+        <v>LorenBell8</v>
       </c>
       <c r="B30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>LorenBell7</v>
+        <v>LorenBell8</v>
       </c>
       <c r="C30" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>LorenBell7@gmail.com</v>
+        <v>LorenBell8@gmail.com</v>
       </c>
       <c r="G30" t="s">
-        <v>219</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>GeraldHiller7</v>
+        <v>GeraldHiller8</v>
       </c>
       <c r="B31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>GeraldHiller7</v>
+        <v>GeraldHiller8</v>
       </c>
       <c r="C31" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>GeraldHiller7@gmail.com</v>
+        <v>GeraldHiller8@gmail.com</v>
       </c>
       <c r="G31" t="s">
-        <v>220</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DeionBranch7</v>
+        <v>DeionBranch8</v>
       </c>
       <c r="B32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DeionBranch7</v>
+        <v>DeionBranch8</v>
       </c>
       <c r="C32" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DeionBranch7@gmail.com</v>
+        <v>DeionBranch8@gmail.com</v>
       </c>
       <c r="G32" t="s">
-        <v>221</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DakotaHalstead7</v>
+        <v>DakotaHalstead8</v>
       </c>
       <c r="B33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DakotaHalstead7</v>
+        <v>DakotaHalstead8</v>
       </c>
       <c r="C33" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DakotaHalstead7@gmail.com</v>
+        <v>DakotaHalstead8@gmail.com</v>
       </c>
       <c r="G33" t="s">
-        <v>222</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ElliottFurman7</v>
+        <v>ElliottFurman8</v>
       </c>
       <c r="B34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ElliottFurman7</v>
+        <v>ElliottFurman8</v>
       </c>
       <c r="C34" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>ElliottFurman7@gmail.com</v>
+        <v>ElliottFurman8@gmail.com</v>
       </c>
       <c r="G34" t="s">
-        <v>223</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MiltonCamp7</v>
+        <v>MiltonCamp8</v>
       </c>
       <c r="B35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MiltonCamp7</v>
+        <v>MiltonCamp8</v>
       </c>
       <c r="C35" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>MiltonCamp7@gmail.com</v>
+        <v>MiltonCamp8@gmail.com</v>
       </c>
       <c r="G35" t="s">
-        <v>224</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DawnChester7</v>
+        <v>DawnChester8</v>
       </c>
       <c r="B36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DawnChester7</v>
+        <v>DawnChester8</v>
       </c>
       <c r="C36" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DawnChester7@gmail.com</v>
+        <v>DawnChester8@gmail.com</v>
       </c>
       <c r="G36" t="s">
-        <v>225</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ZacheryPetrie7</v>
+        <v>ZacheryPetrie8</v>
       </c>
       <c r="B37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ZacheryPetrie7</v>
+        <v>ZacheryPetrie8</v>
       </c>
       <c r="C37" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>ZacheryPetrie7@gmail.com</v>
+        <v>ZacheryPetrie8@gmail.com</v>
       </c>
       <c r="G37" t="s">
-        <v>226</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>EstebanAngel7</v>
+        <v>EstebanAngel8</v>
       </c>
       <c r="B38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>EstebanAngel7</v>
+        <v>EstebanAngel8</v>
       </c>
       <c r="C38" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>EstebanAngel7@gmail.com</v>
+        <v>EstebanAngel8@gmail.com</v>
       </c>
       <c r="G38" t="s">
-        <v>227</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>JimmyBlankenship7</v>
+        <v>JimmyBlankenship8</v>
       </c>
       <c r="B39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>JimmyBlankenship7</v>
+        <v>JimmyBlankenship8</v>
       </c>
       <c r="C39" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>JimmyBlankenship7@gmail.com</v>
+        <v>JimmyBlankenship8@gmail.com</v>
       </c>
       <c r="G39" t="s">
-        <v>228</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AllysaGrice7</v>
+        <v>AllysaGrice8</v>
       </c>
       <c r="B40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AllysaGrice7</v>
+        <v>AllysaGrice8</v>
       </c>
       <c r="C40" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AllysaGrice7@gmail.com</v>
+        <v>AllysaGrice8@gmail.com</v>
       </c>
       <c r="G40" t="s">
-        <v>229</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AugustineYoo7</v>
+        <v>AugustineYoo8</v>
       </c>
       <c r="B41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AugustineYoo7</v>
+        <v>AugustineYoo8</v>
       </c>
       <c r="C41" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AugustineYoo7@gmail.com</v>
+        <v>AugustineYoo8@gmail.com</v>
       </c>
       <c r="G41" t="s">
-        <v>230</v>
+        <v>173</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BrandiSouthard7</v>
+        <v>BrandiSouthard8</v>
       </c>
       <c r="B42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BrandiSouthard7</v>
+        <v>BrandiSouthard8</v>
       </c>
       <c r="C42" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>BrandiSouthard7@gmail.com</v>
+        <v>BrandiSouthard8@gmail.com</v>
       </c>
       <c r="G42" t="s">
-        <v>231</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated added sleep 3s
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/Test_Data.xlsx
+++ b/src/main/resources/test_data/Test_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verkh\IdeaProjects\pom6\src\main\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65643223-7420-48C0-A71E-6C9D05C153CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC4278F-A065-4370-8802-865FE7941070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="594" xr2:uid="{56D596F5-221D-421D-9FC5-55182B639D44}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="594" activeTab="1" xr2:uid="{56D596F5-221D-421D-9FC5-55182B639D44}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="420">
   <si>
     <t>run</t>
   </si>
@@ -1057,244 +1057,247 @@
     <t>Tyth</t>
   </si>
   <si>
-    <t>DonnellJernigan10</t>
-  </si>
-  <si>
-    <t>DonnellJernigan10@gmail.com</t>
-  </si>
-  <si>
-    <t>MalikOtoole10</t>
-  </si>
-  <si>
-    <t>MalikOtoole10@gmail.com</t>
-  </si>
-  <si>
-    <t>AlanCaudill10</t>
-  </si>
-  <si>
-    <t>AlanCaudill10@gmail.com</t>
-  </si>
-  <si>
-    <t>AdanApplegate10</t>
-  </si>
-  <si>
-    <t>AdanApplegate10@gmail.com</t>
-  </si>
-  <si>
-    <t>AiyanaWhitworth10</t>
-  </si>
-  <si>
-    <t>AiyanaWhitworth10@gmail.com</t>
-  </si>
-  <si>
-    <t>MercedezBrien10</t>
-  </si>
-  <si>
-    <t>MercedezBrien10@gmail.com</t>
-  </si>
-  <si>
-    <t>DuaneHager10</t>
-  </si>
-  <si>
-    <t>DuaneHager10@gmail.com</t>
-  </si>
-  <si>
-    <t>LorenBell10</t>
-  </si>
-  <si>
-    <t>LorenBell10@gmail.com</t>
-  </si>
-  <si>
-    <t>GeraldHiller10</t>
-  </si>
-  <si>
-    <t>GeraldHiller10@gmail.com</t>
-  </si>
-  <si>
-    <t>DeionBranch10</t>
-  </si>
-  <si>
-    <t>DeionBranch10@gmail.com</t>
-  </si>
-  <si>
-    <t>DakotaHalstead10</t>
-  </si>
-  <si>
-    <t>DakotaHalstead10@gmail.com</t>
-  </si>
-  <si>
-    <t>ElliottFurman10</t>
-  </si>
-  <si>
-    <t>ElliottFurman10@gmail.com</t>
-  </si>
-  <si>
-    <t>MiltonCamp10</t>
-  </si>
-  <si>
-    <t>MiltonCamp10@gmail.com</t>
-  </si>
-  <si>
-    <t>DawnChester10</t>
-  </si>
-  <si>
-    <t>DawnChester10@gmail.com</t>
-  </si>
-  <si>
-    <t>ZacheryPetrie10</t>
-  </si>
-  <si>
-    <t>ZacheryPetrie10@gmail.com</t>
-  </si>
-  <si>
-    <t>EstebanAngel10</t>
-  </si>
-  <si>
-    <t>EstebanAngel10@gmail.com</t>
-  </si>
-  <si>
-    <t>JimmyBlankenship10</t>
-  </si>
-  <si>
-    <t>JimmyBlankenship10@gmail.com</t>
-  </si>
-  <si>
-    <t>AllysaGrice10</t>
-  </si>
-  <si>
-    <t>AllysaGrice10@gmail.com</t>
-  </si>
-  <si>
-    <t>AugustineYoo10</t>
-  </si>
-  <si>
-    <t>AugustineYoo10@gmail.com</t>
-  </si>
-  <si>
-    <t>BrandiSouthard10</t>
-  </si>
-  <si>
-    <t>BrandiSouthard10@gmail.com</t>
-  </si>
-  <si>
-    <t>EthanBaker5</t>
-  </si>
-  <si>
-    <t>EthanBaker5@gmail.com</t>
-  </si>
-  <si>
-    <t>DelanieCarman5</t>
-  </si>
-  <si>
-    <t>DelanieCarman5@gmail.com</t>
-  </si>
-  <si>
-    <t>BretAgnew5</t>
-  </si>
-  <si>
-    <t>BretAgnew5@gmail.com</t>
-  </si>
-  <si>
-    <t>EdgardoTaylor5</t>
-  </si>
-  <si>
-    <t>EdgardoTaylor5@gmail.com</t>
-  </si>
-  <si>
-    <t>TyrekReis5</t>
-  </si>
-  <si>
-    <t>TyrekReis5@gmail.com</t>
-  </si>
-  <si>
-    <t>LeannaChow5</t>
-  </si>
-  <si>
-    <t>LeannaChow5@gmail.com</t>
-  </si>
-  <si>
-    <t>TuckerCarlson5</t>
-  </si>
-  <si>
-    <t>TuckerCarlson5@gmail.com</t>
-  </si>
-  <si>
-    <t>AnnmarieConnor5</t>
-  </si>
-  <si>
-    <t>AnnmarieConnor5@gmail.com</t>
-  </si>
-  <si>
-    <t>MoniqueWitte5</t>
-  </si>
-  <si>
-    <t>MoniqueWitte5@gmail.com</t>
-  </si>
-  <si>
-    <t>MikelWhitlock5</t>
-  </si>
-  <si>
-    <t>MikelWhitlock5@gmail.com</t>
-  </si>
-  <si>
-    <t>VincentAmaya5</t>
-  </si>
-  <si>
-    <t>VincentAmaya5@gmail.com</t>
-  </si>
-  <si>
-    <t>KeiraQuiroz5</t>
-  </si>
-  <si>
-    <t>KeiraQuiroz5@gmail.com</t>
-  </si>
-  <si>
-    <t>EllisCreech5</t>
-  </si>
-  <si>
-    <t>EllisCreech5@gmail.com</t>
-  </si>
-  <si>
-    <t>DionteCreel5</t>
-  </si>
-  <si>
-    <t>DionteCreel5@gmail.com</t>
-  </si>
-  <si>
-    <t>NicholeFoust5</t>
-  </si>
-  <si>
-    <t>NicholeFoust5@gmail.com</t>
-  </si>
-  <si>
-    <t>ManuelConnell5</t>
-  </si>
-  <si>
-    <t>ManuelConnell5@gmail.com</t>
-  </si>
-  <si>
-    <t>LourdesElam5</t>
-  </si>
-  <si>
-    <t>LourdesElam5@gmail.com</t>
-  </si>
-  <si>
-    <t>LincolnFrederick5</t>
-  </si>
-  <si>
-    <t>LincolnFrederick5@gmail.com</t>
-  </si>
-  <si>
-    <t>AlisaCash5</t>
-  </si>
-  <si>
-    <t>AlisaCash5@gmail.com</t>
-  </si>
-  <si>
-    <t>LucilleGriffiths5</t>
-  </si>
-  <si>
-    <t>LucilleGriffiths5@gmail.com</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t>EthanBaker6</t>
+  </si>
+  <si>
+    <t>EthanBaker6@gmail.com</t>
+  </si>
+  <si>
+    <t>DelanieCarman6</t>
+  </si>
+  <si>
+    <t>DelanieCarman6@gmail.com</t>
+  </si>
+  <si>
+    <t>BretAgnew6</t>
+  </si>
+  <si>
+    <t>BretAgnew6@gmail.com</t>
+  </si>
+  <si>
+    <t>EdgardoTaylor6</t>
+  </si>
+  <si>
+    <t>EdgardoTaylor6@gmail.com</t>
+  </si>
+  <si>
+    <t>TyrekReis6</t>
+  </si>
+  <si>
+    <t>TyrekReis6@gmail.com</t>
+  </si>
+  <si>
+    <t>LeannaChow6</t>
+  </si>
+  <si>
+    <t>LeannaChow6@gmail.com</t>
+  </si>
+  <si>
+    <t>TuckerCarlson6</t>
+  </si>
+  <si>
+    <t>TuckerCarlson6@gmail.com</t>
+  </si>
+  <si>
+    <t>AnnmarieConnor6</t>
+  </si>
+  <si>
+    <t>AnnmarieConnor6@gmail.com</t>
+  </si>
+  <si>
+    <t>MoniqueWitte6</t>
+  </si>
+  <si>
+    <t>MoniqueWitte6@gmail.com</t>
+  </si>
+  <si>
+    <t>MikelWhitlock6</t>
+  </si>
+  <si>
+    <t>MikelWhitlock6@gmail.com</t>
+  </si>
+  <si>
+    <t>VincentAmaya6</t>
+  </si>
+  <si>
+    <t>VincentAmaya6@gmail.com</t>
+  </si>
+  <si>
+    <t>KeiraQuiroz6</t>
+  </si>
+  <si>
+    <t>KeiraQuiroz6@gmail.com</t>
+  </si>
+  <si>
+    <t>EllisCreech6</t>
+  </si>
+  <si>
+    <t>EllisCreech6@gmail.com</t>
+  </si>
+  <si>
+    <t>DionteCreel6</t>
+  </si>
+  <si>
+    <t>DionteCreel6@gmail.com</t>
+  </si>
+  <si>
+    <t>NicholeFoust6</t>
+  </si>
+  <si>
+    <t>NicholeFoust6@gmail.com</t>
+  </si>
+  <si>
+    <t>ManuelConnell6</t>
+  </si>
+  <si>
+    <t>ManuelConnell6@gmail.com</t>
+  </si>
+  <si>
+    <t>LourdesElam6</t>
+  </si>
+  <si>
+    <t>LourdesElam6@gmail.com</t>
+  </si>
+  <si>
+    <t>LincolnFrederick6</t>
+  </si>
+  <si>
+    <t>LincolnFrederick6@gmail.com</t>
+  </si>
+  <si>
+    <t>AlisaCash6</t>
+  </si>
+  <si>
+    <t>AlisaCash6@gmail.com</t>
+  </si>
+  <si>
+    <t>LucilleGriffiths6</t>
+  </si>
+  <si>
+    <t>LucilleGriffiths6@gmail.com</t>
+  </si>
+  <si>
+    <t>DonnellJernigan11</t>
+  </si>
+  <si>
+    <t>DonnellJernigan11@gmail.com</t>
+  </si>
+  <si>
+    <t>MalikOtoole11</t>
+  </si>
+  <si>
+    <t>MalikOtoole11@gmail.com</t>
+  </si>
+  <si>
+    <t>AlanCaudill11</t>
+  </si>
+  <si>
+    <t>AlanCaudill11@gmail.com</t>
+  </si>
+  <si>
+    <t>AdanApplegate11</t>
+  </si>
+  <si>
+    <t>AdanApplegate11@gmail.com</t>
+  </si>
+  <si>
+    <t>AiyanaWhitworth11</t>
+  </si>
+  <si>
+    <t>AiyanaWhitworth11@gmail.com</t>
+  </si>
+  <si>
+    <t>MercedezBrien11</t>
+  </si>
+  <si>
+    <t>MercedezBrien11@gmail.com</t>
+  </si>
+  <si>
+    <t>DuaneHager11</t>
+  </si>
+  <si>
+    <t>DuaneHager11@gmail.com</t>
+  </si>
+  <si>
+    <t>LorenBell11</t>
+  </si>
+  <si>
+    <t>LorenBell11@gmail.com</t>
+  </si>
+  <si>
+    <t>GeraldHiller11</t>
+  </si>
+  <si>
+    <t>GeraldHiller11@gmail.com</t>
+  </si>
+  <si>
+    <t>DeionBranch11</t>
+  </si>
+  <si>
+    <t>DeionBranch11@gmail.com</t>
+  </si>
+  <si>
+    <t>DakotaHalstead11</t>
+  </si>
+  <si>
+    <t>DakotaHalstead11@gmail.com</t>
+  </si>
+  <si>
+    <t>ElliottFurman11</t>
+  </si>
+  <si>
+    <t>ElliottFurman11@gmail.com</t>
+  </si>
+  <si>
+    <t>MiltonCamp11</t>
+  </si>
+  <si>
+    <t>MiltonCamp11@gmail.com</t>
+  </si>
+  <si>
+    <t>DawnChester11</t>
+  </si>
+  <si>
+    <t>DawnChester11@gmail.com</t>
+  </si>
+  <si>
+    <t>ZacheryPetrie11</t>
+  </si>
+  <si>
+    <t>ZacheryPetrie11@gmail.com</t>
+  </si>
+  <si>
+    <t>EstebanAngel11</t>
+  </si>
+  <si>
+    <t>EstebanAngel11@gmail.com</t>
+  </si>
+  <si>
+    <t>JimmyBlankenship11</t>
+  </si>
+  <si>
+    <t>JimmyBlankenship11@gmail.com</t>
+  </si>
+  <si>
+    <t>AllysaGrice11</t>
+  </si>
+  <si>
+    <t>AllysaGrice11@gmail.com</t>
+  </si>
+  <si>
+    <t>AugustineYoo11</t>
+  </si>
+  <si>
+    <t>AugustineYoo11@gmail.com</t>
+  </si>
+  <si>
+    <t>BrandiSouthard11</t>
+  </si>
+  <si>
+    <t>BrandiSouthard11@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1369,7 +1372,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1403,6 +1406,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1537,7 +1546,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1611,6 +1620,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1635,7 +1647,7 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1976,7 +1988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{955D89E2-A883-499B-AA82-70224D6F8F96}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2:I21"/>
     </sheetView>
   </sheetViews>
@@ -2060,13 +2072,13 @@
         <v>55</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>379</v>
+        <v>340</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>379</v>
+        <v>340</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>380</v>
+        <v>341</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>30</v>
@@ -2103,13 +2115,13 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>381</v>
+        <v>342</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>381</v>
+        <v>342</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>382</v>
+        <v>343</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>35</v>
@@ -2145,13 +2157,13 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>383</v>
+        <v>344</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>383</v>
+        <v>344</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>384</v>
+        <v>345</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>30</v>
@@ -2187,13 +2199,13 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>385</v>
+        <v>346</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>385</v>
+        <v>346</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>386</v>
+        <v>347</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>35</v>
@@ -2229,13 +2241,13 @@
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>387</v>
+        <v>348</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>387</v>
+        <v>348</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>388</v>
+        <v>349</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>30</v>
@@ -2271,13 +2283,13 @@
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>389</v>
+        <v>350</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>389</v>
+        <v>350</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>390</v>
+        <v>351</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>35</v>
@@ -2313,13 +2325,13 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>391</v>
+        <v>352</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>391</v>
+        <v>352</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>392</v>
+        <v>353</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>30</v>
@@ -2355,13 +2367,13 @@
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>393</v>
+        <v>354</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>393</v>
+        <v>354</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>394</v>
+        <v>355</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>35</v>
@@ -2397,13 +2409,13 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>395</v>
+        <v>356</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>395</v>
+        <v>356</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>396</v>
+        <v>357</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>30</v>
@@ -2439,13 +2451,13 @@
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>397</v>
+        <v>358</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>397</v>
+        <v>358</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>398</v>
+        <v>359</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>35</v>
@@ -2481,13 +2493,13 @@
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>399</v>
+        <v>360</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>399</v>
+        <v>360</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>30</v>
@@ -2523,13 +2535,13 @@
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>401</v>
+        <v>362</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>401</v>
+        <v>362</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>402</v>
+        <v>363</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>35</v>
@@ -2565,13 +2577,13 @@
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>403</v>
+        <v>364</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>403</v>
+        <v>364</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>404</v>
+        <v>365</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>30</v>
@@ -2607,13 +2619,13 @@
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>405</v>
+        <v>366</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>405</v>
+        <v>366</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>406</v>
+        <v>367</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>35</v>
@@ -2649,13 +2661,13 @@
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>407</v>
+        <v>368</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>407</v>
+        <v>368</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>408</v>
+        <v>369</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>30</v>
@@ -2691,13 +2703,13 @@
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>409</v>
+        <v>370</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>409</v>
+        <v>370</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>410</v>
+        <v>371</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>35</v>
@@ -2733,13 +2745,13 @@
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="12" t="s">
-        <v>411</v>
+        <v>372</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>411</v>
+        <v>372</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>412</v>
+        <v>373</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>35</v>
@@ -2775,13 +2787,13 @@
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="12" t="s">
-        <v>413</v>
+        <v>374</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>413</v>
+        <v>374</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>414</v>
+        <v>375</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>35</v>
@@ -2817,13 +2829,13 @@
       </c>
       <c r="F20" s="12"/>
       <c r="G20" s="12" t="s">
-        <v>415</v>
+        <v>376</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>415</v>
+        <v>376</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>416</v>
+        <v>377</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>35</v>
@@ -2859,13 +2871,13 @@
       </c>
       <c r="F21" s="12"/>
       <c r="G21" s="12" t="s">
-        <v>417</v>
+        <v>378</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>417</v>
+        <v>378</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>418</v>
+        <v>379</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>35</v>
@@ -2926,8 +2938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0775DEA-3893-49AA-8C48-45DC29C761B9}">
   <dimension ref="A1:AF21"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2:T21"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3108,13 +3120,13 @@
         <v>54</v>
       </c>
       <c r="R2" s="14" t="s">
-        <v>339</v>
+        <v>380</v>
       </c>
       <c r="S2" s="14" t="s">
-        <v>339</v>
+        <v>380</v>
       </c>
       <c r="T2" s="22" t="s">
-        <v>340</v>
+        <v>381</v>
       </c>
       <c r="U2" s="15" t="s">
         <v>134</v>
@@ -3201,13 +3213,13 @@
         <v>54</v>
       </c>
       <c r="R3" s="14" t="s">
-        <v>341</v>
+        <v>382</v>
       </c>
       <c r="S3" s="14" t="s">
-        <v>341</v>
+        <v>382</v>
       </c>
       <c r="T3" s="22" t="s">
-        <v>342</v>
+        <v>383</v>
       </c>
       <c r="U3" s="15" t="s">
         <v>134</v>
@@ -3294,13 +3306,13 @@
         <v>54</v>
       </c>
       <c r="R4" s="14" t="s">
-        <v>343</v>
+        <v>384</v>
       </c>
       <c r="S4" s="14" t="s">
-        <v>343</v>
+        <v>384</v>
       </c>
       <c r="T4" s="22" t="s">
-        <v>344</v>
+        <v>385</v>
       </c>
       <c r="U4" s="15" t="s">
         <v>134</v>
@@ -3387,13 +3399,13 @@
         <v>54</v>
       </c>
       <c r="R5" s="14" t="s">
-        <v>345</v>
+        <v>386</v>
       </c>
       <c r="S5" s="14" t="s">
-        <v>345</v>
+        <v>386</v>
       </c>
       <c r="T5" s="22" t="s">
-        <v>346</v>
+        <v>387</v>
       </c>
       <c r="U5" s="15" t="s">
         <v>134</v>
@@ -3480,13 +3492,13 @@
         <v>54</v>
       </c>
       <c r="R6" s="14" t="s">
-        <v>347</v>
+        <v>388</v>
       </c>
       <c r="S6" s="14" t="s">
-        <v>347</v>
+        <v>388</v>
       </c>
       <c r="T6" s="22" t="s">
-        <v>348</v>
+        <v>389</v>
       </c>
       <c r="U6" s="15" t="s">
         <v>134</v>
@@ -3573,13 +3585,13 @@
         <v>54</v>
       </c>
       <c r="R7" s="14" t="s">
-        <v>349</v>
+        <v>390</v>
       </c>
       <c r="S7" s="14" t="s">
-        <v>349</v>
+        <v>390</v>
       </c>
       <c r="T7" s="22" t="s">
-        <v>350</v>
+        <v>391</v>
       </c>
       <c r="U7" s="15" t="s">
         <v>134</v>
@@ -3666,13 +3678,13 @@
         <v>54</v>
       </c>
       <c r="R8" s="14" t="s">
-        <v>351</v>
+        <v>392</v>
       </c>
       <c r="S8" s="14" t="s">
-        <v>351</v>
+        <v>392</v>
       </c>
       <c r="T8" s="22" t="s">
-        <v>352</v>
+        <v>393</v>
       </c>
       <c r="U8" s="15" t="s">
         <v>134</v>
@@ -3759,21 +3771,21 @@
         <v>54</v>
       </c>
       <c r="R9" s="14" t="s">
-        <v>353</v>
+        <v>394</v>
       </c>
       <c r="S9" s="14" t="s">
-        <v>353</v>
+        <v>394</v>
       </c>
       <c r="T9" s="22" t="s">
-        <v>354</v>
+        <v>395</v>
       </c>
       <c r="U9" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="V9" s="35" t="s">
+      <c r="V9" s="27" t="s">
         <v>286</v>
       </c>
-      <c r="W9" s="35" t="s">
+      <c r="W9" s="27" t="s">
         <v>305</v>
       </c>
       <c r="X9" s="14" t="s">
@@ -3852,13 +3864,13 @@
         <v>54</v>
       </c>
       <c r="R10" s="14" t="s">
-        <v>355</v>
+        <v>396</v>
       </c>
       <c r="S10" s="14" t="s">
-        <v>355</v>
+        <v>396</v>
       </c>
       <c r="T10" s="22" t="s">
-        <v>356</v>
+        <v>397</v>
       </c>
       <c r="U10" s="15" t="s">
         <v>134</v>
@@ -3945,21 +3957,21 @@
         <v>54</v>
       </c>
       <c r="R11" s="14" t="s">
-        <v>357</v>
+        <v>398</v>
       </c>
       <c r="S11" s="14" t="s">
-        <v>357</v>
+        <v>398</v>
       </c>
       <c r="T11" s="22" t="s">
-        <v>358</v>
+        <v>399</v>
       </c>
       <c r="U11" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="V11" s="35" t="s">
+      <c r="V11" s="27" t="s">
         <v>288</v>
       </c>
-      <c r="W11" s="35" t="s">
+      <c r="W11" s="27" t="s">
         <v>307</v>
       </c>
       <c r="X11" s="14" t="s">
@@ -4038,13 +4050,13 @@
         <v>54</v>
       </c>
       <c r="R12" s="14" t="s">
-        <v>359</v>
+        <v>400</v>
       </c>
       <c r="S12" s="14" t="s">
-        <v>359</v>
+        <v>400</v>
       </c>
       <c r="T12" s="22" t="s">
-        <v>360</v>
+        <v>401</v>
       </c>
       <c r="U12" s="15" t="s">
         <v>134</v>
@@ -4131,13 +4143,13 @@
         <v>54</v>
       </c>
       <c r="R13" s="14" t="s">
-        <v>361</v>
+        <v>402</v>
       </c>
       <c r="S13" s="14" t="s">
-        <v>361</v>
+        <v>402</v>
       </c>
       <c r="T13" s="22" t="s">
-        <v>362</v>
+        <v>403</v>
       </c>
       <c r="U13" s="15" t="s">
         <v>134</v>
@@ -4145,7 +4157,7 @@
       <c r="V13" s="26" t="s">
         <v>338</v>
       </c>
-      <c r="W13" s="35" t="s">
+      <c r="W13" s="27" t="s">
         <v>309</v>
       </c>
       <c r="X13" s="14" t="s">
@@ -4224,13 +4236,13 @@
         <v>54</v>
       </c>
       <c r="R14" s="14" t="s">
-        <v>363</v>
+        <v>404</v>
       </c>
       <c r="S14" s="14" t="s">
-        <v>363</v>
+        <v>404</v>
       </c>
       <c r="T14" s="22" t="s">
-        <v>364</v>
+        <v>405</v>
       </c>
       <c r="U14" s="15" t="s">
         <v>134</v>
@@ -4317,13 +4329,13 @@
         <v>54</v>
       </c>
       <c r="R15" s="14" t="s">
-        <v>365</v>
+        <v>406</v>
       </c>
       <c r="S15" s="14" t="s">
-        <v>365</v>
+        <v>406</v>
       </c>
       <c r="T15" s="22" t="s">
-        <v>366</v>
+        <v>407</v>
       </c>
       <c r="U15" s="15" t="s">
         <v>134</v>
@@ -4410,13 +4422,13 @@
         <v>54</v>
       </c>
       <c r="R16" s="14" t="s">
-        <v>367</v>
+        <v>408</v>
       </c>
       <c r="S16" s="14" t="s">
-        <v>367</v>
+        <v>408</v>
       </c>
       <c r="T16" s="22" t="s">
-        <v>368</v>
+        <v>409</v>
       </c>
       <c r="U16" s="15" t="s">
         <v>134</v>
@@ -4503,13 +4515,13 @@
         <v>54</v>
       </c>
       <c r="R17" s="14" t="s">
-        <v>369</v>
+        <v>410</v>
       </c>
       <c r="S17" s="14" t="s">
-        <v>369</v>
+        <v>410</v>
       </c>
       <c r="T17" s="22" t="s">
-        <v>370</v>
+        <v>411</v>
       </c>
       <c r="U17" s="15" t="s">
         <v>134</v>
@@ -4559,7 +4571,7 @@
         <v>85</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>278</v>
+        <v>339</v>
       </c>
       <c r="G18" s="14" t="s">
         <v>227</v>
@@ -4595,13 +4607,13 @@
         <v>54</v>
       </c>
       <c r="R18" s="14" t="s">
-        <v>371</v>
+        <v>412</v>
       </c>
       <c r="S18" s="14" t="s">
-        <v>371</v>
+        <v>412</v>
       </c>
       <c r="T18" s="22" t="s">
-        <v>372</v>
+        <v>413</v>
       </c>
       <c r="U18" s="15" t="s">
         <v>134</v>
@@ -4687,13 +4699,13 @@
         <v>54</v>
       </c>
       <c r="R19" s="14" t="s">
-        <v>373</v>
+        <v>414</v>
       </c>
       <c r="S19" s="14" t="s">
-        <v>373</v>
+        <v>414</v>
       </c>
       <c r="T19" s="22" t="s">
-        <v>374</v>
+        <v>415</v>
       </c>
       <c r="U19" s="15" t="s">
         <v>134</v>
@@ -4779,13 +4791,13 @@
         <v>54</v>
       </c>
       <c r="R20" s="14" t="s">
-        <v>375</v>
+        <v>416</v>
       </c>
       <c r="S20" s="14" t="s">
-        <v>375</v>
+        <v>416</v>
       </c>
       <c r="T20" s="22" t="s">
-        <v>376</v>
+        <v>417</v>
       </c>
       <c r="U20" s="15" t="s">
         <v>134</v>
@@ -4793,7 +4805,7 @@
       <c r="V20" s="14" t="s">
         <v>296</v>
       </c>
-      <c r="W20" s="14" t="s">
+      <c r="W20" s="36" t="s">
         <v>316</v>
       </c>
       <c r="X20" s="14" t="s">
@@ -4871,13 +4883,13 @@
         <v>54</v>
       </c>
       <c r="R21" s="19" t="s">
-        <v>377</v>
+        <v>418</v>
       </c>
       <c r="S21" s="19" t="s">
-        <v>377</v>
+        <v>418</v>
       </c>
       <c r="T21" s="25" t="s">
-        <v>378</v>
+        <v>419</v>
       </c>
       <c r="U21" s="15" t="s">
         <v>134</v>
@@ -4945,8 +4957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FABAB06A-EAA7-4BA7-8A4C-8C5EF7E0517A}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C21"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4959,30 +4971,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>275</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="30"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="str">
         <f>CONCATENATE($G2,$I$2)</f>
-        <v>EthanBaker5</v>
+        <v>EthanBaker6</v>
       </c>
       <c r="B2" s="1" t="str">
         <f>CONCATENATE($G2,$I$2)</f>
-        <v>EthanBaker5</v>
+        <v>EthanBaker6</v>
       </c>
       <c r="C2" s="2" t="str">
         <f>CONCATENATE($G2,$I$2,$H$2)</f>
-        <v>EthanBaker5@gmail.com</v>
+        <v>EthanBaker6@gmail.com</v>
       </c>
       <c r="G2" t="s">
         <v>135</v>
@@ -4991,21 +5003,21 @@
         <v>75</v>
       </c>
       <c r="I2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
         <f t="shared" ref="A3:B21" si="0">CONCATENATE($G3,$I$2)</f>
-        <v>DelanieCarman5</v>
+        <v>DelanieCarman6</v>
       </c>
       <c r="B3" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DelanieCarman5</v>
+        <v>DelanieCarman6</v>
       </c>
       <c r="C3" s="2" t="str">
         <f t="shared" ref="C3:C21" si="1">CONCATENATE($G3,$I$2,$H$2)</f>
-        <v>DelanieCarman5@gmail.com</v>
+        <v>DelanieCarman6@gmail.com</v>
       </c>
       <c r="G3" t="s">
         <v>136</v>
@@ -5014,15 +5026,15 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>BretAgnew5</v>
+        <v>BretAgnew6</v>
       </c>
       <c r="B4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>BretAgnew5</v>
+        <v>BretAgnew6</v>
       </c>
       <c r="C4" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>BretAgnew5@gmail.com</v>
+        <v>BretAgnew6@gmail.com</v>
       </c>
       <c r="G4" t="s">
         <v>137</v>
@@ -5031,15 +5043,15 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EdgardoTaylor5</v>
+        <v>EdgardoTaylor6</v>
       </c>
       <c r="B5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EdgardoTaylor5</v>
+        <v>EdgardoTaylor6</v>
       </c>
       <c r="C5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>EdgardoTaylor5@gmail.com</v>
+        <v>EdgardoTaylor6@gmail.com</v>
       </c>
       <c r="G5" t="s">
         <v>138</v>
@@ -5048,15 +5060,15 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TyrekReis5</v>
+        <v>TyrekReis6</v>
       </c>
       <c r="B6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TyrekReis5</v>
+        <v>TyrekReis6</v>
       </c>
       <c r="C6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>TyrekReis5@gmail.com</v>
+        <v>TyrekReis6@gmail.com</v>
       </c>
       <c r="G6" t="s">
         <v>139</v>
@@ -5065,15 +5077,15 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LeannaChow5</v>
+        <v>LeannaChow6</v>
       </c>
       <c r="B7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LeannaChow5</v>
+        <v>LeannaChow6</v>
       </c>
       <c r="C7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LeannaChow5@gmail.com</v>
+        <v>LeannaChow6@gmail.com</v>
       </c>
       <c r="G7" t="s">
         <v>140</v>
@@ -5082,15 +5094,15 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TuckerCarlson5</v>
+        <v>TuckerCarlson6</v>
       </c>
       <c r="B8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TuckerCarlson5</v>
+        <v>TuckerCarlson6</v>
       </c>
       <c r="C8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>TuckerCarlson5@gmail.com</v>
+        <v>TuckerCarlson6@gmail.com</v>
       </c>
       <c r="G8" t="s">
         <v>141</v>
@@ -5099,15 +5111,15 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AnnmarieConnor5</v>
+        <v>AnnmarieConnor6</v>
       </c>
       <c r="B9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AnnmarieConnor5</v>
+        <v>AnnmarieConnor6</v>
       </c>
       <c r="C9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>AnnmarieConnor5@gmail.com</v>
+        <v>AnnmarieConnor6@gmail.com</v>
       </c>
       <c r="G9" t="s">
         <v>142</v>
@@ -5116,15 +5128,15 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MoniqueWitte5</v>
+        <v>MoniqueWitte6</v>
       </c>
       <c r="B10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MoniqueWitte5</v>
+        <v>MoniqueWitte6</v>
       </c>
       <c r="C10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MoniqueWitte5@gmail.com</v>
+        <v>MoniqueWitte6@gmail.com</v>
       </c>
       <c r="G10" t="s">
         <v>143</v>
@@ -5133,15 +5145,15 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MikelWhitlock5</v>
+        <v>MikelWhitlock6</v>
       </c>
       <c r="B11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MikelWhitlock5</v>
+        <v>MikelWhitlock6</v>
       </c>
       <c r="C11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MikelWhitlock5@gmail.com</v>
+        <v>MikelWhitlock6@gmail.com</v>
       </c>
       <c r="G11" t="s">
         <v>144</v>
@@ -5150,15 +5162,15 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>VincentAmaya5</v>
+        <v>VincentAmaya6</v>
       </c>
       <c r="B12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>VincentAmaya5</v>
+        <v>VincentAmaya6</v>
       </c>
       <c r="C12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>VincentAmaya5@gmail.com</v>
+        <v>VincentAmaya6@gmail.com</v>
       </c>
       <c r="G12" t="s">
         <v>145</v>
@@ -5167,15 +5179,15 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>KeiraQuiroz5</v>
+        <v>KeiraQuiroz6</v>
       </c>
       <c r="B13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>KeiraQuiroz5</v>
+        <v>KeiraQuiroz6</v>
       </c>
       <c r="C13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>KeiraQuiroz5@gmail.com</v>
+        <v>KeiraQuiroz6@gmail.com</v>
       </c>
       <c r="G13" t="s">
         <v>146</v>
@@ -5184,15 +5196,15 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EllisCreech5</v>
+        <v>EllisCreech6</v>
       </c>
       <c r="B14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EllisCreech5</v>
+        <v>EllisCreech6</v>
       </c>
       <c r="C14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>EllisCreech5@gmail.com</v>
+        <v>EllisCreech6@gmail.com</v>
       </c>
       <c r="G14" t="s">
         <v>147</v>
@@ -5201,15 +5213,15 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DionteCreel5</v>
+        <v>DionteCreel6</v>
       </c>
       <c r="B15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DionteCreel5</v>
+        <v>DionteCreel6</v>
       </c>
       <c r="C15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DionteCreel5@gmail.com</v>
+        <v>DionteCreel6@gmail.com</v>
       </c>
       <c r="G15" t="s">
         <v>148</v>
@@ -5218,15 +5230,15 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NicholeFoust5</v>
+        <v>NicholeFoust6</v>
       </c>
       <c r="B16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NicholeFoust5</v>
+        <v>NicholeFoust6</v>
       </c>
       <c r="C16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>NicholeFoust5@gmail.com</v>
+        <v>NicholeFoust6@gmail.com</v>
       </c>
       <c r="G16" t="s">
         <v>149</v>
@@ -5235,15 +5247,15 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>ManuelConnell5</v>
+        <v>ManuelConnell6</v>
       </c>
       <c r="B17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>ManuelConnell5</v>
+        <v>ManuelConnell6</v>
       </c>
       <c r="C17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>ManuelConnell5@gmail.com</v>
+        <v>ManuelConnell6@gmail.com</v>
       </c>
       <c r="G17" t="s">
         <v>150</v>
@@ -5252,15 +5264,15 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LourdesElam5</v>
+        <v>LourdesElam6</v>
       </c>
       <c r="B18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LourdesElam5</v>
+        <v>LourdesElam6</v>
       </c>
       <c r="C18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LourdesElam5@gmail.com</v>
+        <v>LourdesElam6@gmail.com</v>
       </c>
       <c r="G18" t="s">
         <v>151</v>
@@ -5269,15 +5281,15 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LincolnFrederick5</v>
+        <v>LincolnFrederick6</v>
       </c>
       <c r="B19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LincolnFrederick5</v>
+        <v>LincolnFrederick6</v>
       </c>
       <c r="C19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LincolnFrederick5@gmail.com</v>
+        <v>LincolnFrederick6@gmail.com</v>
       </c>
       <c r="G19" t="s">
         <v>152</v>
@@ -5286,15 +5298,15 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AlisaCash5</v>
+        <v>AlisaCash6</v>
       </c>
       <c r="B20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AlisaCash5</v>
+        <v>AlisaCash6</v>
       </c>
       <c r="C20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>AlisaCash5@gmail.com</v>
+        <v>AlisaCash6@gmail.com</v>
       </c>
       <c r="G20" t="s">
         <v>153</v>
@@ -5303,45 +5315,45 @@
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LucilleGriffiths5</v>
+        <v>LucilleGriffiths6</v>
       </c>
       <c r="B21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LucilleGriffiths5</v>
+        <v>LucilleGriffiths6</v>
       </c>
       <c r="C21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LucilleGriffiths5@gmail.com</v>
+        <v>LucilleGriffiths6@gmail.com</v>
       </c>
       <c r="G21" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="23" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="32" t="s">
         <v>276</v>
       </c>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="34"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="35"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="str">
         <f>CONCATENATE($G23,$I$23)</f>
-        <v>DonnellJernigan10</v>
+        <v>DonnellJernigan11</v>
       </c>
       <c r="B23" s="1" t="str">
         <f>CONCATENATE($G23,$I$23)</f>
-        <v>DonnellJernigan10</v>
+        <v>DonnellJernigan11</v>
       </c>
       <c r="C23" s="2" t="str">
         <f>CONCATENATE($G23,$I$23,$H$23)</f>
-        <v>DonnellJernigan10@gmail.com</v>
+        <v>DonnellJernigan11@gmail.com</v>
       </c>
       <c r="G23" s="24" t="s">
         <v>155</v>
@@ -5350,21 +5362,21 @@
         <v>75</v>
       </c>
       <c r="I23">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="str">
         <f t="shared" ref="A24:B42" si="2">CONCATENATE($G24,$I$23)</f>
-        <v>MalikOtoole10</v>
+        <v>MalikOtoole11</v>
       </c>
       <c r="B24" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MalikOtoole10</v>
+        <v>MalikOtoole11</v>
       </c>
       <c r="C24" s="2" t="str">
         <f t="shared" ref="C24:C42" si="3">CONCATENATE($G24,$I$23,$H$23)</f>
-        <v>MalikOtoole10@gmail.com</v>
+        <v>MalikOtoole11@gmail.com</v>
       </c>
       <c r="G24" t="s">
         <v>156</v>
@@ -5373,15 +5385,15 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AlanCaudill10</v>
+        <v>AlanCaudill11</v>
       </c>
       <c r="B25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AlanCaudill10</v>
+        <v>AlanCaudill11</v>
       </c>
       <c r="C25" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AlanCaudill10@gmail.com</v>
+        <v>AlanCaudill11@gmail.com</v>
       </c>
       <c r="G25" t="s">
         <v>157</v>
@@ -5390,15 +5402,15 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AdanApplegate10</v>
+        <v>AdanApplegate11</v>
       </c>
       <c r="B26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AdanApplegate10</v>
+        <v>AdanApplegate11</v>
       </c>
       <c r="C26" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AdanApplegate10@gmail.com</v>
+        <v>AdanApplegate11@gmail.com</v>
       </c>
       <c r="G26" t="s">
         <v>158</v>
@@ -5407,15 +5419,15 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AiyanaWhitworth10</v>
+        <v>AiyanaWhitworth11</v>
       </c>
       <c r="B27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AiyanaWhitworth10</v>
+        <v>AiyanaWhitworth11</v>
       </c>
       <c r="C27" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AiyanaWhitworth10@gmail.com</v>
+        <v>AiyanaWhitworth11@gmail.com</v>
       </c>
       <c r="G27" t="s">
         <v>159</v>
@@ -5424,15 +5436,15 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MercedezBrien10</v>
+        <v>MercedezBrien11</v>
       </c>
       <c r="B28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MercedezBrien10</v>
+        <v>MercedezBrien11</v>
       </c>
       <c r="C28" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>MercedezBrien10@gmail.com</v>
+        <v>MercedezBrien11@gmail.com</v>
       </c>
       <c r="G28" t="s">
         <v>160</v>
@@ -5441,15 +5453,15 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DuaneHager10</v>
+        <v>DuaneHager11</v>
       </c>
       <c r="B29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DuaneHager10</v>
+        <v>DuaneHager11</v>
       </c>
       <c r="C29" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DuaneHager10@gmail.com</v>
+        <v>DuaneHager11@gmail.com</v>
       </c>
       <c r="G29" t="s">
         <v>161</v>
@@ -5458,15 +5470,15 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>LorenBell10</v>
+        <v>LorenBell11</v>
       </c>
       <c r="B30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>LorenBell10</v>
+        <v>LorenBell11</v>
       </c>
       <c r="C30" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>LorenBell10@gmail.com</v>
+        <v>LorenBell11@gmail.com</v>
       </c>
       <c r="G30" t="s">
         <v>162</v>
@@ -5475,15 +5487,15 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>GeraldHiller10</v>
+        <v>GeraldHiller11</v>
       </c>
       <c r="B31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>GeraldHiller10</v>
+        <v>GeraldHiller11</v>
       </c>
       <c r="C31" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>GeraldHiller10@gmail.com</v>
+        <v>GeraldHiller11@gmail.com</v>
       </c>
       <c r="G31" t="s">
         <v>163</v>
@@ -5492,15 +5504,15 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DeionBranch10</v>
+        <v>DeionBranch11</v>
       </c>
       <c r="B32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DeionBranch10</v>
+        <v>DeionBranch11</v>
       </c>
       <c r="C32" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DeionBranch10@gmail.com</v>
+        <v>DeionBranch11@gmail.com</v>
       </c>
       <c r="G32" t="s">
         <v>164</v>
@@ -5509,15 +5521,15 @@
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DakotaHalstead10</v>
+        <v>DakotaHalstead11</v>
       </c>
       <c r="B33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DakotaHalstead10</v>
+        <v>DakotaHalstead11</v>
       </c>
       <c r="C33" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DakotaHalstead10@gmail.com</v>
+        <v>DakotaHalstead11@gmail.com</v>
       </c>
       <c r="G33" t="s">
         <v>165</v>
@@ -5526,15 +5538,15 @@
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ElliottFurman10</v>
+        <v>ElliottFurman11</v>
       </c>
       <c r="B34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ElliottFurman10</v>
+        <v>ElliottFurman11</v>
       </c>
       <c r="C34" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>ElliottFurman10@gmail.com</v>
+        <v>ElliottFurman11@gmail.com</v>
       </c>
       <c r="G34" t="s">
         <v>166</v>
@@ -5543,15 +5555,15 @@
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MiltonCamp10</v>
+        <v>MiltonCamp11</v>
       </c>
       <c r="B35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MiltonCamp10</v>
+        <v>MiltonCamp11</v>
       </c>
       <c r="C35" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>MiltonCamp10@gmail.com</v>
+        <v>MiltonCamp11@gmail.com</v>
       </c>
       <c r="G35" t="s">
         <v>167</v>
@@ -5560,15 +5572,15 @@
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DawnChester10</v>
+        <v>DawnChester11</v>
       </c>
       <c r="B36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DawnChester10</v>
+        <v>DawnChester11</v>
       </c>
       <c r="C36" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DawnChester10@gmail.com</v>
+        <v>DawnChester11@gmail.com</v>
       </c>
       <c r="G36" t="s">
         <v>168</v>
@@ -5577,15 +5589,15 @@
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ZacheryPetrie10</v>
+        <v>ZacheryPetrie11</v>
       </c>
       <c r="B37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ZacheryPetrie10</v>
+        <v>ZacheryPetrie11</v>
       </c>
       <c r="C37" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>ZacheryPetrie10@gmail.com</v>
+        <v>ZacheryPetrie11@gmail.com</v>
       </c>
       <c r="G37" t="s">
         <v>169</v>
@@ -5594,15 +5606,15 @@
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>EstebanAngel10</v>
+        <v>EstebanAngel11</v>
       </c>
       <c r="B38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>EstebanAngel10</v>
+        <v>EstebanAngel11</v>
       </c>
       <c r="C38" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>EstebanAngel10@gmail.com</v>
+        <v>EstebanAngel11@gmail.com</v>
       </c>
       <c r="G38" t="s">
         <v>170</v>
@@ -5611,15 +5623,15 @@
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>JimmyBlankenship10</v>
+        <v>JimmyBlankenship11</v>
       </c>
       <c r="B39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>JimmyBlankenship10</v>
+        <v>JimmyBlankenship11</v>
       </c>
       <c r="C39" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>JimmyBlankenship10@gmail.com</v>
+        <v>JimmyBlankenship11@gmail.com</v>
       </c>
       <c r="G39" t="s">
         <v>171</v>
@@ -5628,15 +5640,15 @@
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AllysaGrice10</v>
+        <v>AllysaGrice11</v>
       </c>
       <c r="B40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AllysaGrice10</v>
+        <v>AllysaGrice11</v>
       </c>
       <c r="C40" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AllysaGrice10@gmail.com</v>
+        <v>AllysaGrice11@gmail.com</v>
       </c>
       <c r="G40" t="s">
         <v>172</v>
@@ -5645,15 +5657,15 @@
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AugustineYoo10</v>
+        <v>AugustineYoo11</v>
       </c>
       <c r="B41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AugustineYoo10</v>
+        <v>AugustineYoo11</v>
       </c>
       <c r="C41" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AugustineYoo10@gmail.com</v>
+        <v>AugustineYoo11@gmail.com</v>
       </c>
       <c r="G41" t="s">
         <v>173</v>
@@ -5662,15 +5674,15 @@
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BrandiSouthard10</v>
+        <v>BrandiSouthard11</v>
       </c>
       <c r="B42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BrandiSouthard10</v>
+        <v>BrandiSouthard11</v>
       </c>
       <c r="C42" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>BrandiSouthard10@gmail.com</v>
+        <v>BrandiSouthard11@gmail.com</v>
       </c>
       <c r="G42" t="s">
         <v>174</v>

</xml_diff>

<commit_message>
updated data and pom file v 124
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/Test_Data.xlsx
+++ b/src/main/resources/test_data/Test_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verkh\IdeaProjects\pom6\src\main\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF95AB2-36CF-49BD-814A-5555BAC494C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451CBEA1-6234-4C2A-A97C-1F3D2BC4CD6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="594" activeTab="1" xr2:uid="{56D596F5-221D-421D-9FC5-55182B639D44}"/>
+    <workbookView xWindow="0" yWindow="1500" windowWidth="23040" windowHeight="12180" tabRatio="594" activeTab="1" xr2:uid="{56D596F5-221D-421D-9FC5-55182B639D44}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="2" r:id="rId1"/>
@@ -1060,244 +1060,244 @@
     <t>3</t>
   </si>
   <si>
-    <t>EthanBaker10</t>
-  </si>
-  <si>
-    <t>EthanBaker10@gmail.com</t>
-  </si>
-  <si>
-    <t>DelanieCarman10</t>
-  </si>
-  <si>
-    <t>DelanieCarman10@gmail.com</t>
-  </si>
-  <si>
-    <t>BretAgnew10</t>
-  </si>
-  <si>
-    <t>BretAgnew10@gmail.com</t>
-  </si>
-  <si>
-    <t>EdgardoTaylor10</t>
-  </si>
-  <si>
-    <t>EdgardoTaylor10@gmail.com</t>
-  </si>
-  <si>
-    <t>TyrekReis10</t>
-  </si>
-  <si>
-    <t>TyrekReis10@gmail.com</t>
-  </si>
-  <si>
-    <t>LeannaChow10</t>
-  </si>
-  <si>
-    <t>LeannaChow10@gmail.com</t>
-  </si>
-  <si>
-    <t>TuckerCarlson10</t>
-  </si>
-  <si>
-    <t>TuckerCarlson10@gmail.com</t>
-  </si>
-  <si>
-    <t>AnnmarieConnor10</t>
-  </si>
-  <si>
-    <t>AnnmarieConnor10@gmail.com</t>
-  </si>
-  <si>
-    <t>MoniqueWitte10</t>
-  </si>
-  <si>
-    <t>MoniqueWitte10@gmail.com</t>
-  </si>
-  <si>
-    <t>MikelWhitlock10</t>
-  </si>
-  <si>
-    <t>MikelWhitlock10@gmail.com</t>
-  </si>
-  <si>
-    <t>VincentAmaya10</t>
-  </si>
-  <si>
-    <t>VincentAmaya10@gmail.com</t>
-  </si>
-  <si>
-    <t>KeiraQuiroz10</t>
-  </si>
-  <si>
-    <t>KeiraQuiroz10@gmail.com</t>
-  </si>
-  <si>
-    <t>EllisCreech10</t>
-  </si>
-  <si>
-    <t>EllisCreech10@gmail.com</t>
-  </si>
-  <si>
-    <t>DionteCreel10</t>
-  </si>
-  <si>
-    <t>DionteCreel10@gmail.com</t>
-  </si>
-  <si>
-    <t>NicholeFoust10</t>
-  </si>
-  <si>
-    <t>NicholeFoust10@gmail.com</t>
-  </si>
-  <si>
-    <t>ManuelConnell10</t>
-  </si>
-  <si>
-    <t>ManuelConnell10@gmail.com</t>
-  </si>
-  <si>
-    <t>LourdesElam10</t>
-  </si>
-  <si>
-    <t>LourdesElam10@gmail.com</t>
-  </si>
-  <si>
-    <t>LincolnFrederick10</t>
-  </si>
-  <si>
-    <t>LincolnFrederick10@gmail.com</t>
-  </si>
-  <si>
-    <t>AlisaCash10</t>
-  </si>
-  <si>
-    <t>AlisaCash10@gmail.com</t>
-  </si>
-  <si>
-    <t>LucilleGriffiths10</t>
-  </si>
-  <si>
-    <t>LucilleGriffiths10@gmail.com</t>
-  </si>
-  <si>
-    <t>DonnellJernigan15</t>
-  </si>
-  <si>
-    <t>DonnellJernigan15@gmail.com</t>
-  </si>
-  <si>
-    <t>MalikOtoole15</t>
-  </si>
-  <si>
-    <t>MalikOtoole15@gmail.com</t>
-  </si>
-  <si>
-    <t>AlanCaudill15</t>
-  </si>
-  <si>
-    <t>AlanCaudill15@gmail.com</t>
-  </si>
-  <si>
-    <t>AdanApplegate15</t>
-  </si>
-  <si>
-    <t>AdanApplegate15@gmail.com</t>
-  </si>
-  <si>
-    <t>AiyanaWhitworth15</t>
-  </si>
-  <si>
-    <t>AiyanaWhitworth15@gmail.com</t>
-  </si>
-  <si>
-    <t>MercedezBrien15</t>
-  </si>
-  <si>
-    <t>MercedezBrien15@gmail.com</t>
-  </si>
-  <si>
-    <t>DuaneHager15</t>
-  </si>
-  <si>
-    <t>DuaneHager15@gmail.com</t>
-  </si>
-  <si>
-    <t>LorenBell15</t>
-  </si>
-  <si>
-    <t>LorenBell15@gmail.com</t>
-  </si>
-  <si>
-    <t>GeraldHiller15</t>
-  </si>
-  <si>
-    <t>GeraldHiller15@gmail.com</t>
-  </si>
-  <si>
-    <t>DeionBranch15</t>
-  </si>
-  <si>
-    <t>DeionBranch15@gmail.com</t>
-  </si>
-  <si>
-    <t>DakotaHalstead15</t>
-  </si>
-  <si>
-    <t>DakotaHalstead15@gmail.com</t>
-  </si>
-  <si>
-    <t>ElliottFurman15</t>
-  </si>
-  <si>
-    <t>ElliottFurman15@gmail.com</t>
-  </si>
-  <si>
-    <t>MiltonCamp15</t>
-  </si>
-  <si>
-    <t>MiltonCamp15@gmail.com</t>
-  </si>
-  <si>
-    <t>DawnChester15</t>
-  </si>
-  <si>
-    <t>DawnChester15@gmail.com</t>
-  </si>
-  <si>
-    <t>ZacheryPetrie15</t>
-  </si>
-  <si>
-    <t>ZacheryPetrie15@gmail.com</t>
-  </si>
-  <si>
-    <t>EstebanAngel15</t>
-  </si>
-  <si>
-    <t>EstebanAngel15@gmail.com</t>
-  </si>
-  <si>
-    <t>JimmyBlankenship15</t>
-  </si>
-  <si>
-    <t>JimmyBlankenship15@gmail.com</t>
-  </si>
-  <si>
-    <t>AllysaGrice15</t>
-  </si>
-  <si>
-    <t>AllysaGrice15@gmail.com</t>
-  </si>
-  <si>
-    <t>AugustineYoo15</t>
-  </si>
-  <si>
-    <t>AugustineYoo15@gmail.com</t>
-  </si>
-  <si>
-    <t>BrandiSouthard15</t>
-  </si>
-  <si>
-    <t>BrandiSouthard15@gmail.com</t>
+    <t>EthanBaker11</t>
+  </si>
+  <si>
+    <t>EthanBaker11@gmail.com</t>
+  </si>
+  <si>
+    <t>DelanieCarman11</t>
+  </si>
+  <si>
+    <t>DelanieCarman11@gmail.com</t>
+  </si>
+  <si>
+    <t>BretAgnew11</t>
+  </si>
+  <si>
+    <t>BretAgnew11@gmail.com</t>
+  </si>
+  <si>
+    <t>EdgardoTaylor11</t>
+  </si>
+  <si>
+    <t>EdgardoTaylor11@gmail.com</t>
+  </si>
+  <si>
+    <t>TyrekReis11</t>
+  </si>
+  <si>
+    <t>TyrekReis11@gmail.com</t>
+  </si>
+  <si>
+    <t>LeannaChow11</t>
+  </si>
+  <si>
+    <t>LeannaChow11@gmail.com</t>
+  </si>
+  <si>
+    <t>TuckerCarlson11</t>
+  </si>
+  <si>
+    <t>TuckerCarlson11@gmail.com</t>
+  </si>
+  <si>
+    <t>AnnmarieConnor11</t>
+  </si>
+  <si>
+    <t>AnnmarieConnor11@gmail.com</t>
+  </si>
+  <si>
+    <t>MoniqueWitte11</t>
+  </si>
+  <si>
+    <t>MoniqueWitte11@gmail.com</t>
+  </si>
+  <si>
+    <t>MikelWhitlock11</t>
+  </si>
+  <si>
+    <t>MikelWhitlock11@gmail.com</t>
+  </si>
+  <si>
+    <t>VincentAmaya11</t>
+  </si>
+  <si>
+    <t>VincentAmaya11@gmail.com</t>
+  </si>
+  <si>
+    <t>KeiraQuiroz11</t>
+  </si>
+  <si>
+    <t>KeiraQuiroz11@gmail.com</t>
+  </si>
+  <si>
+    <t>EllisCreech11</t>
+  </si>
+  <si>
+    <t>EllisCreech11@gmail.com</t>
+  </si>
+  <si>
+    <t>DionteCreel11</t>
+  </si>
+  <si>
+    <t>DionteCreel11@gmail.com</t>
+  </si>
+  <si>
+    <t>NicholeFoust11</t>
+  </si>
+  <si>
+    <t>NicholeFoust11@gmail.com</t>
+  </si>
+  <si>
+    <t>ManuelConnell11</t>
+  </si>
+  <si>
+    <t>ManuelConnell11@gmail.com</t>
+  </si>
+  <si>
+    <t>LourdesElam11</t>
+  </si>
+  <si>
+    <t>LourdesElam11@gmail.com</t>
+  </si>
+  <si>
+    <t>LincolnFrederick11</t>
+  </si>
+  <si>
+    <t>LincolnFrederick11@gmail.com</t>
+  </si>
+  <si>
+    <t>AlisaCash11</t>
+  </si>
+  <si>
+    <t>AlisaCash11@gmail.com</t>
+  </si>
+  <si>
+    <t>LucilleGriffiths11</t>
+  </si>
+  <si>
+    <t>LucilleGriffiths11@gmail.com</t>
+  </si>
+  <si>
+    <t>DonnellJernigan16</t>
+  </si>
+  <si>
+    <t>DonnellJernigan16@gmail.com</t>
+  </si>
+  <si>
+    <t>MalikOtoole16</t>
+  </si>
+  <si>
+    <t>MalikOtoole16@gmail.com</t>
+  </si>
+  <si>
+    <t>AlanCaudill16</t>
+  </si>
+  <si>
+    <t>AlanCaudill16@gmail.com</t>
+  </si>
+  <si>
+    <t>AdanApplegate16</t>
+  </si>
+  <si>
+    <t>AdanApplegate16@gmail.com</t>
+  </si>
+  <si>
+    <t>AiyanaWhitworth16</t>
+  </si>
+  <si>
+    <t>AiyanaWhitworth16@gmail.com</t>
+  </si>
+  <si>
+    <t>MercedezBrien16</t>
+  </si>
+  <si>
+    <t>MercedezBrien16@gmail.com</t>
+  </si>
+  <si>
+    <t>DuaneHager16</t>
+  </si>
+  <si>
+    <t>DuaneHager16@gmail.com</t>
+  </si>
+  <si>
+    <t>LorenBell16</t>
+  </si>
+  <si>
+    <t>LorenBell16@gmail.com</t>
+  </si>
+  <si>
+    <t>GeraldHiller16</t>
+  </si>
+  <si>
+    <t>GeraldHiller16@gmail.com</t>
+  </si>
+  <si>
+    <t>DeionBranch16</t>
+  </si>
+  <si>
+    <t>DeionBranch16@gmail.com</t>
+  </si>
+  <si>
+    <t>DakotaHalstead16</t>
+  </si>
+  <si>
+    <t>DakotaHalstead16@gmail.com</t>
+  </si>
+  <si>
+    <t>ElliottFurman16</t>
+  </si>
+  <si>
+    <t>ElliottFurman16@gmail.com</t>
+  </si>
+  <si>
+    <t>MiltonCamp16</t>
+  </si>
+  <si>
+    <t>MiltonCamp16@gmail.com</t>
+  </si>
+  <si>
+    <t>DawnChester16</t>
+  </si>
+  <si>
+    <t>DawnChester16@gmail.com</t>
+  </si>
+  <si>
+    <t>ZacheryPetrie16</t>
+  </si>
+  <si>
+    <t>ZacheryPetrie16@gmail.com</t>
+  </si>
+  <si>
+    <t>EstebanAngel16</t>
+  </si>
+  <si>
+    <t>EstebanAngel16@gmail.com</t>
+  </si>
+  <si>
+    <t>JimmyBlankenship16</t>
+  </si>
+  <si>
+    <t>JimmyBlankenship16@gmail.com</t>
+  </si>
+  <si>
+    <t>AllysaGrice16</t>
+  </si>
+  <si>
+    <t>AllysaGrice16@gmail.com</t>
+  </si>
+  <si>
+    <t>AugustineYoo16</t>
+  </si>
+  <si>
+    <t>AugustineYoo16@gmail.com</t>
+  </si>
+  <si>
+    <t>BrandiSouthard16</t>
+  </si>
+  <si>
+    <t>BrandiSouthard16@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -4957,7 +4957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FABAB06A-EAA7-4BA7-8A4C-8C5EF7E0517A}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A23" sqref="A23:C42"/>
     </sheetView>
   </sheetViews>
@@ -4986,15 +4986,15 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="str">
         <f>CONCATENATE($G2,$I$2)</f>
-        <v>EthanBaker10</v>
+        <v>EthanBaker11</v>
       </c>
       <c r="B2" s="1" t="str">
         <f>CONCATENATE($G2,$I$2)</f>
-        <v>EthanBaker10</v>
+        <v>EthanBaker11</v>
       </c>
       <c r="C2" s="2" t="str">
         <f>CONCATENATE($G2,$I$2,$H$2)</f>
-        <v>EthanBaker10@gmail.com</v>
+        <v>EthanBaker11@gmail.com</v>
       </c>
       <c r="G2" t="s">
         <v>135</v>
@@ -5003,21 +5003,21 @@
         <v>75</v>
       </c>
       <c r="I2">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
         <f t="shared" ref="A3:B21" si="0">CONCATENATE($G3,$I$2)</f>
-        <v>DelanieCarman10</v>
+        <v>DelanieCarman11</v>
       </c>
       <c r="B3" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DelanieCarman10</v>
+        <v>DelanieCarman11</v>
       </c>
       <c r="C3" s="2" t="str">
         <f t="shared" ref="C3:C21" si="1">CONCATENATE($G3,$I$2,$H$2)</f>
-        <v>DelanieCarman10@gmail.com</v>
+        <v>DelanieCarman11@gmail.com</v>
       </c>
       <c r="G3" t="s">
         <v>136</v>
@@ -5026,15 +5026,15 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>BretAgnew10</v>
+        <v>BretAgnew11</v>
       </c>
       <c r="B4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>BretAgnew10</v>
+        <v>BretAgnew11</v>
       </c>
       <c r="C4" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>BretAgnew10@gmail.com</v>
+        <v>BretAgnew11@gmail.com</v>
       </c>
       <c r="G4" t="s">
         <v>137</v>
@@ -5043,15 +5043,15 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EdgardoTaylor10</v>
+        <v>EdgardoTaylor11</v>
       </c>
       <c r="B5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EdgardoTaylor10</v>
+        <v>EdgardoTaylor11</v>
       </c>
       <c r="C5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>EdgardoTaylor10@gmail.com</v>
+        <v>EdgardoTaylor11@gmail.com</v>
       </c>
       <c r="G5" t="s">
         <v>138</v>
@@ -5060,15 +5060,15 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TyrekReis10</v>
+        <v>TyrekReis11</v>
       </c>
       <c r="B6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TyrekReis10</v>
+        <v>TyrekReis11</v>
       </c>
       <c r="C6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>TyrekReis10@gmail.com</v>
+        <v>TyrekReis11@gmail.com</v>
       </c>
       <c r="G6" t="s">
         <v>139</v>
@@ -5077,15 +5077,15 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LeannaChow10</v>
+        <v>LeannaChow11</v>
       </c>
       <c r="B7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LeannaChow10</v>
+        <v>LeannaChow11</v>
       </c>
       <c r="C7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LeannaChow10@gmail.com</v>
+        <v>LeannaChow11@gmail.com</v>
       </c>
       <c r="G7" t="s">
         <v>140</v>
@@ -5094,15 +5094,15 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TuckerCarlson10</v>
+        <v>TuckerCarlson11</v>
       </c>
       <c r="B8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TuckerCarlson10</v>
+        <v>TuckerCarlson11</v>
       </c>
       <c r="C8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>TuckerCarlson10@gmail.com</v>
+        <v>TuckerCarlson11@gmail.com</v>
       </c>
       <c r="G8" t="s">
         <v>141</v>
@@ -5111,15 +5111,15 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AnnmarieConnor10</v>
+        <v>AnnmarieConnor11</v>
       </c>
       <c r="B9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AnnmarieConnor10</v>
+        <v>AnnmarieConnor11</v>
       </c>
       <c r="C9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>AnnmarieConnor10@gmail.com</v>
+        <v>AnnmarieConnor11@gmail.com</v>
       </c>
       <c r="G9" t="s">
         <v>142</v>
@@ -5128,15 +5128,15 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MoniqueWitte10</v>
+        <v>MoniqueWitte11</v>
       </c>
       <c r="B10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MoniqueWitte10</v>
+        <v>MoniqueWitte11</v>
       </c>
       <c r="C10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MoniqueWitte10@gmail.com</v>
+        <v>MoniqueWitte11@gmail.com</v>
       </c>
       <c r="G10" t="s">
         <v>143</v>
@@ -5145,15 +5145,15 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MikelWhitlock10</v>
+        <v>MikelWhitlock11</v>
       </c>
       <c r="B11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MikelWhitlock10</v>
+        <v>MikelWhitlock11</v>
       </c>
       <c r="C11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MikelWhitlock10@gmail.com</v>
+        <v>MikelWhitlock11@gmail.com</v>
       </c>
       <c r="G11" t="s">
         <v>144</v>
@@ -5162,15 +5162,15 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>VincentAmaya10</v>
+        <v>VincentAmaya11</v>
       </c>
       <c r="B12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>VincentAmaya10</v>
+        <v>VincentAmaya11</v>
       </c>
       <c r="C12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>VincentAmaya10@gmail.com</v>
+        <v>VincentAmaya11@gmail.com</v>
       </c>
       <c r="G12" t="s">
         <v>145</v>
@@ -5179,15 +5179,15 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>KeiraQuiroz10</v>
+        <v>KeiraQuiroz11</v>
       </c>
       <c r="B13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>KeiraQuiroz10</v>
+        <v>KeiraQuiroz11</v>
       </c>
       <c r="C13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>KeiraQuiroz10@gmail.com</v>
+        <v>KeiraQuiroz11@gmail.com</v>
       </c>
       <c r="G13" t="s">
         <v>146</v>
@@ -5196,15 +5196,15 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EllisCreech10</v>
+        <v>EllisCreech11</v>
       </c>
       <c r="B14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EllisCreech10</v>
+        <v>EllisCreech11</v>
       </c>
       <c r="C14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>EllisCreech10@gmail.com</v>
+        <v>EllisCreech11@gmail.com</v>
       </c>
       <c r="G14" t="s">
         <v>147</v>
@@ -5213,15 +5213,15 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DionteCreel10</v>
+        <v>DionteCreel11</v>
       </c>
       <c r="B15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DionteCreel10</v>
+        <v>DionteCreel11</v>
       </c>
       <c r="C15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DionteCreel10@gmail.com</v>
+        <v>DionteCreel11@gmail.com</v>
       </c>
       <c r="G15" t="s">
         <v>148</v>
@@ -5230,15 +5230,15 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NicholeFoust10</v>
+        <v>NicholeFoust11</v>
       </c>
       <c r="B16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NicholeFoust10</v>
+        <v>NicholeFoust11</v>
       </c>
       <c r="C16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>NicholeFoust10@gmail.com</v>
+        <v>NicholeFoust11@gmail.com</v>
       </c>
       <c r="G16" t="s">
         <v>149</v>
@@ -5247,15 +5247,15 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>ManuelConnell10</v>
+        <v>ManuelConnell11</v>
       </c>
       <c r="B17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>ManuelConnell10</v>
+        <v>ManuelConnell11</v>
       </c>
       <c r="C17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>ManuelConnell10@gmail.com</v>
+        <v>ManuelConnell11@gmail.com</v>
       </c>
       <c r="G17" t="s">
         <v>150</v>
@@ -5264,15 +5264,15 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LourdesElam10</v>
+        <v>LourdesElam11</v>
       </c>
       <c r="B18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LourdesElam10</v>
+        <v>LourdesElam11</v>
       </c>
       <c r="C18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LourdesElam10@gmail.com</v>
+        <v>LourdesElam11@gmail.com</v>
       </c>
       <c r="G18" t="s">
         <v>151</v>
@@ -5281,15 +5281,15 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LincolnFrederick10</v>
+        <v>LincolnFrederick11</v>
       </c>
       <c r="B19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LincolnFrederick10</v>
+        <v>LincolnFrederick11</v>
       </c>
       <c r="C19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LincolnFrederick10@gmail.com</v>
+        <v>LincolnFrederick11@gmail.com</v>
       </c>
       <c r="G19" t="s">
         <v>152</v>
@@ -5298,15 +5298,15 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AlisaCash10</v>
+        <v>AlisaCash11</v>
       </c>
       <c r="B20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AlisaCash10</v>
+        <v>AlisaCash11</v>
       </c>
       <c r="C20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>AlisaCash10@gmail.com</v>
+        <v>AlisaCash11@gmail.com</v>
       </c>
       <c r="G20" t="s">
         <v>153</v>
@@ -5315,15 +5315,15 @@
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LucilleGriffiths10</v>
+        <v>LucilleGriffiths11</v>
       </c>
       <c r="B21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LucilleGriffiths10</v>
+        <v>LucilleGriffiths11</v>
       </c>
       <c r="C21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LucilleGriffiths10@gmail.com</v>
+        <v>LucilleGriffiths11@gmail.com</v>
       </c>
       <c r="G21" t="s">
         <v>154</v>
@@ -5345,15 +5345,15 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="str">
         <f>CONCATENATE($G23,$I$23)</f>
-        <v>DonnellJernigan15</v>
+        <v>DonnellJernigan16</v>
       </c>
       <c r="B23" s="1" t="str">
         <f>CONCATENATE($G23,$I$23)</f>
-        <v>DonnellJernigan15</v>
+        <v>DonnellJernigan16</v>
       </c>
       <c r="C23" s="2" t="str">
         <f>CONCATENATE($G23,$I$23,$H$23)</f>
-        <v>DonnellJernigan15@gmail.com</v>
+        <v>DonnellJernigan16@gmail.com</v>
       </c>
       <c r="G23" s="24" t="s">
         <v>155</v>
@@ -5362,21 +5362,21 @@
         <v>75</v>
       </c>
       <c r="I23">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="str">
         <f t="shared" ref="A24:B42" si="2">CONCATENATE($G24,$I$23)</f>
-        <v>MalikOtoole15</v>
+        <v>MalikOtoole16</v>
       </c>
       <c r="B24" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MalikOtoole15</v>
+        <v>MalikOtoole16</v>
       </c>
       <c r="C24" s="2" t="str">
         <f t="shared" ref="C24:C42" si="3">CONCATENATE($G24,$I$23,$H$23)</f>
-        <v>MalikOtoole15@gmail.com</v>
+        <v>MalikOtoole16@gmail.com</v>
       </c>
       <c r="G24" t="s">
         <v>156</v>
@@ -5385,15 +5385,15 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AlanCaudill15</v>
+        <v>AlanCaudill16</v>
       </c>
       <c r="B25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AlanCaudill15</v>
+        <v>AlanCaudill16</v>
       </c>
       <c r="C25" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AlanCaudill15@gmail.com</v>
+        <v>AlanCaudill16@gmail.com</v>
       </c>
       <c r="G25" t="s">
         <v>157</v>
@@ -5402,15 +5402,15 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AdanApplegate15</v>
+        <v>AdanApplegate16</v>
       </c>
       <c r="B26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AdanApplegate15</v>
+        <v>AdanApplegate16</v>
       </c>
       <c r="C26" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AdanApplegate15@gmail.com</v>
+        <v>AdanApplegate16@gmail.com</v>
       </c>
       <c r="G26" t="s">
         <v>158</v>
@@ -5419,15 +5419,15 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AiyanaWhitworth15</v>
+        <v>AiyanaWhitworth16</v>
       </c>
       <c r="B27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AiyanaWhitworth15</v>
+        <v>AiyanaWhitworth16</v>
       </c>
       <c r="C27" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AiyanaWhitworth15@gmail.com</v>
+        <v>AiyanaWhitworth16@gmail.com</v>
       </c>
       <c r="G27" t="s">
         <v>159</v>
@@ -5436,15 +5436,15 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MercedezBrien15</v>
+        <v>MercedezBrien16</v>
       </c>
       <c r="B28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MercedezBrien15</v>
+        <v>MercedezBrien16</v>
       </c>
       <c r="C28" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>MercedezBrien15@gmail.com</v>
+        <v>MercedezBrien16@gmail.com</v>
       </c>
       <c r="G28" t="s">
         <v>160</v>
@@ -5453,15 +5453,15 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DuaneHager15</v>
+        <v>DuaneHager16</v>
       </c>
       <c r="B29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DuaneHager15</v>
+        <v>DuaneHager16</v>
       </c>
       <c r="C29" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DuaneHager15@gmail.com</v>
+        <v>DuaneHager16@gmail.com</v>
       </c>
       <c r="G29" t="s">
         <v>161</v>
@@ -5470,15 +5470,15 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>LorenBell15</v>
+        <v>LorenBell16</v>
       </c>
       <c r="B30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>LorenBell15</v>
+        <v>LorenBell16</v>
       </c>
       <c r="C30" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>LorenBell15@gmail.com</v>
+        <v>LorenBell16@gmail.com</v>
       </c>
       <c r="G30" t="s">
         <v>162</v>
@@ -5487,15 +5487,15 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>GeraldHiller15</v>
+        <v>GeraldHiller16</v>
       </c>
       <c r="B31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>GeraldHiller15</v>
+        <v>GeraldHiller16</v>
       </c>
       <c r="C31" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>GeraldHiller15@gmail.com</v>
+        <v>GeraldHiller16@gmail.com</v>
       </c>
       <c r="G31" t="s">
         <v>163</v>
@@ -5504,15 +5504,15 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DeionBranch15</v>
+        <v>DeionBranch16</v>
       </c>
       <c r="B32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DeionBranch15</v>
+        <v>DeionBranch16</v>
       </c>
       <c r="C32" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DeionBranch15@gmail.com</v>
+        <v>DeionBranch16@gmail.com</v>
       </c>
       <c r="G32" t="s">
         <v>164</v>
@@ -5521,15 +5521,15 @@
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DakotaHalstead15</v>
+        <v>DakotaHalstead16</v>
       </c>
       <c r="B33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DakotaHalstead15</v>
+        <v>DakotaHalstead16</v>
       </c>
       <c r="C33" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DakotaHalstead15@gmail.com</v>
+        <v>DakotaHalstead16@gmail.com</v>
       </c>
       <c r="G33" t="s">
         <v>165</v>
@@ -5538,15 +5538,15 @@
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ElliottFurman15</v>
+        <v>ElliottFurman16</v>
       </c>
       <c r="B34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ElliottFurman15</v>
+        <v>ElliottFurman16</v>
       </c>
       <c r="C34" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>ElliottFurman15@gmail.com</v>
+        <v>ElliottFurman16@gmail.com</v>
       </c>
       <c r="G34" t="s">
         <v>166</v>
@@ -5555,15 +5555,15 @@
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MiltonCamp15</v>
+        <v>MiltonCamp16</v>
       </c>
       <c r="B35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MiltonCamp15</v>
+        <v>MiltonCamp16</v>
       </c>
       <c r="C35" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>MiltonCamp15@gmail.com</v>
+        <v>MiltonCamp16@gmail.com</v>
       </c>
       <c r="G35" t="s">
         <v>167</v>
@@ -5572,15 +5572,15 @@
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DawnChester15</v>
+        <v>DawnChester16</v>
       </c>
       <c r="B36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DawnChester15</v>
+        <v>DawnChester16</v>
       </c>
       <c r="C36" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DawnChester15@gmail.com</v>
+        <v>DawnChester16@gmail.com</v>
       </c>
       <c r="G36" t="s">
         <v>168</v>
@@ -5589,15 +5589,15 @@
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ZacheryPetrie15</v>
+        <v>ZacheryPetrie16</v>
       </c>
       <c r="B37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ZacheryPetrie15</v>
+        <v>ZacheryPetrie16</v>
       </c>
       <c r="C37" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>ZacheryPetrie15@gmail.com</v>
+        <v>ZacheryPetrie16@gmail.com</v>
       </c>
       <c r="G37" t="s">
         <v>169</v>
@@ -5606,15 +5606,15 @@
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>EstebanAngel15</v>
+        <v>EstebanAngel16</v>
       </c>
       <c r="B38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>EstebanAngel15</v>
+        <v>EstebanAngel16</v>
       </c>
       <c r="C38" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>EstebanAngel15@gmail.com</v>
+        <v>EstebanAngel16@gmail.com</v>
       </c>
       <c r="G38" t="s">
         <v>170</v>
@@ -5623,15 +5623,15 @@
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>JimmyBlankenship15</v>
+        <v>JimmyBlankenship16</v>
       </c>
       <c r="B39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>JimmyBlankenship15</v>
+        <v>JimmyBlankenship16</v>
       </c>
       <c r="C39" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>JimmyBlankenship15@gmail.com</v>
+        <v>JimmyBlankenship16@gmail.com</v>
       </c>
       <c r="G39" t="s">
         <v>171</v>
@@ -5640,15 +5640,15 @@
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AllysaGrice15</v>
+        <v>AllysaGrice16</v>
       </c>
       <c r="B40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AllysaGrice15</v>
+        <v>AllysaGrice16</v>
       </c>
       <c r="C40" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AllysaGrice15@gmail.com</v>
+        <v>AllysaGrice16@gmail.com</v>
       </c>
       <c r="G40" t="s">
         <v>172</v>
@@ -5657,15 +5657,15 @@
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AugustineYoo15</v>
+        <v>AugustineYoo16</v>
       </c>
       <c r="B41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AugustineYoo15</v>
+        <v>AugustineYoo16</v>
       </c>
       <c r="C41" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AugustineYoo15@gmail.com</v>
+        <v>AugustineYoo16@gmail.com</v>
       </c>
       <c r="G41" t="s">
         <v>173</v>
@@ -5674,15 +5674,15 @@
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BrandiSouthard15</v>
+        <v>BrandiSouthard16</v>
       </c>
       <c r="B42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BrandiSouthard15</v>
+        <v>BrandiSouthard16</v>
       </c>
       <c r="C42" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>BrandiSouthard15@gmail.com</v>
+        <v>BrandiSouthard16@gmail.com</v>
       </c>
       <c r="G42" t="s">
         <v>174</v>

</xml_diff>

<commit_message>
updated data and extend reports pom file added
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/Test_Data.xlsx
+++ b/src/main/resources/test_data/Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verkh\IdeaProjects\pom6\src\main\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451CBEA1-6234-4C2A-A97C-1F3D2BC4CD6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECEC714-2F79-4ACE-948E-082340DCAF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1500" windowWidth="23040" windowHeight="12180" tabRatio="594" activeTab="1" xr2:uid="{56D596F5-221D-421D-9FC5-55182B639D44}"/>
   </bookViews>
@@ -1060,244 +1060,244 @@
     <t>3</t>
   </si>
   <si>
-    <t>EthanBaker11</t>
-  </si>
-  <si>
-    <t>EthanBaker11@gmail.com</t>
-  </si>
-  <si>
-    <t>DelanieCarman11</t>
-  </si>
-  <si>
-    <t>DelanieCarman11@gmail.com</t>
-  </si>
-  <si>
-    <t>BretAgnew11</t>
-  </si>
-  <si>
-    <t>BretAgnew11@gmail.com</t>
-  </si>
-  <si>
-    <t>EdgardoTaylor11</t>
-  </si>
-  <si>
-    <t>EdgardoTaylor11@gmail.com</t>
-  </si>
-  <si>
-    <t>TyrekReis11</t>
-  </si>
-  <si>
-    <t>TyrekReis11@gmail.com</t>
-  </si>
-  <si>
-    <t>LeannaChow11</t>
-  </si>
-  <si>
-    <t>LeannaChow11@gmail.com</t>
-  </si>
-  <si>
-    <t>TuckerCarlson11</t>
-  </si>
-  <si>
-    <t>TuckerCarlson11@gmail.com</t>
-  </si>
-  <si>
-    <t>AnnmarieConnor11</t>
-  </si>
-  <si>
-    <t>AnnmarieConnor11@gmail.com</t>
-  </si>
-  <si>
-    <t>MoniqueWitte11</t>
-  </si>
-  <si>
-    <t>MoniqueWitte11@gmail.com</t>
-  </si>
-  <si>
-    <t>MikelWhitlock11</t>
-  </si>
-  <si>
-    <t>MikelWhitlock11@gmail.com</t>
-  </si>
-  <si>
-    <t>VincentAmaya11</t>
-  </si>
-  <si>
-    <t>VincentAmaya11@gmail.com</t>
-  </si>
-  <si>
-    <t>KeiraQuiroz11</t>
-  </si>
-  <si>
-    <t>KeiraQuiroz11@gmail.com</t>
-  </si>
-  <si>
-    <t>EllisCreech11</t>
-  </si>
-  <si>
-    <t>EllisCreech11@gmail.com</t>
-  </si>
-  <si>
-    <t>DionteCreel11</t>
-  </si>
-  <si>
-    <t>DionteCreel11@gmail.com</t>
-  </si>
-  <si>
-    <t>NicholeFoust11</t>
-  </si>
-  <si>
-    <t>NicholeFoust11@gmail.com</t>
-  </si>
-  <si>
-    <t>ManuelConnell11</t>
-  </si>
-  <si>
-    <t>ManuelConnell11@gmail.com</t>
-  </si>
-  <si>
-    <t>LourdesElam11</t>
-  </si>
-  <si>
-    <t>LourdesElam11@gmail.com</t>
-  </si>
-  <si>
-    <t>LincolnFrederick11</t>
-  </si>
-  <si>
-    <t>LincolnFrederick11@gmail.com</t>
-  </si>
-  <si>
-    <t>AlisaCash11</t>
-  </si>
-  <si>
-    <t>AlisaCash11@gmail.com</t>
-  </si>
-  <si>
-    <t>LucilleGriffiths11</t>
-  </si>
-  <si>
-    <t>LucilleGriffiths11@gmail.com</t>
-  </si>
-  <si>
-    <t>DonnellJernigan16</t>
-  </si>
-  <si>
-    <t>DonnellJernigan16@gmail.com</t>
-  </si>
-  <si>
-    <t>MalikOtoole16</t>
-  </si>
-  <si>
-    <t>MalikOtoole16@gmail.com</t>
-  </si>
-  <si>
-    <t>AlanCaudill16</t>
-  </si>
-  <si>
-    <t>AlanCaudill16@gmail.com</t>
-  </si>
-  <si>
-    <t>AdanApplegate16</t>
-  </si>
-  <si>
-    <t>AdanApplegate16@gmail.com</t>
-  </si>
-  <si>
-    <t>AiyanaWhitworth16</t>
-  </si>
-  <si>
-    <t>AiyanaWhitworth16@gmail.com</t>
-  </si>
-  <si>
-    <t>MercedezBrien16</t>
-  </si>
-  <si>
-    <t>MercedezBrien16@gmail.com</t>
-  </si>
-  <si>
-    <t>DuaneHager16</t>
-  </si>
-  <si>
-    <t>DuaneHager16@gmail.com</t>
-  </si>
-  <si>
-    <t>LorenBell16</t>
-  </si>
-  <si>
-    <t>LorenBell16@gmail.com</t>
-  </si>
-  <si>
-    <t>GeraldHiller16</t>
-  </si>
-  <si>
-    <t>GeraldHiller16@gmail.com</t>
-  </si>
-  <si>
-    <t>DeionBranch16</t>
-  </si>
-  <si>
-    <t>DeionBranch16@gmail.com</t>
-  </si>
-  <si>
-    <t>DakotaHalstead16</t>
-  </si>
-  <si>
-    <t>DakotaHalstead16@gmail.com</t>
-  </si>
-  <si>
-    <t>ElliottFurman16</t>
-  </si>
-  <si>
-    <t>ElliottFurman16@gmail.com</t>
-  </si>
-  <si>
-    <t>MiltonCamp16</t>
-  </si>
-  <si>
-    <t>MiltonCamp16@gmail.com</t>
-  </si>
-  <si>
-    <t>DawnChester16</t>
-  </si>
-  <si>
-    <t>DawnChester16@gmail.com</t>
-  </si>
-  <si>
-    <t>ZacheryPetrie16</t>
-  </si>
-  <si>
-    <t>ZacheryPetrie16@gmail.com</t>
-  </si>
-  <si>
-    <t>EstebanAngel16</t>
-  </si>
-  <si>
-    <t>EstebanAngel16@gmail.com</t>
-  </si>
-  <si>
-    <t>JimmyBlankenship16</t>
-  </si>
-  <si>
-    <t>JimmyBlankenship16@gmail.com</t>
-  </si>
-  <si>
-    <t>AllysaGrice16</t>
-  </si>
-  <si>
-    <t>AllysaGrice16@gmail.com</t>
-  </si>
-  <si>
-    <t>AugustineYoo16</t>
-  </si>
-  <si>
-    <t>AugustineYoo16@gmail.com</t>
-  </si>
-  <si>
-    <t>BrandiSouthard16</t>
-  </si>
-  <si>
-    <t>BrandiSouthard16@gmail.com</t>
+    <t>EthanBaker12</t>
+  </si>
+  <si>
+    <t>EthanBaker12@gmail.com</t>
+  </si>
+  <si>
+    <t>DelanieCarman12</t>
+  </si>
+  <si>
+    <t>DelanieCarman12@gmail.com</t>
+  </si>
+  <si>
+    <t>BretAgnew12</t>
+  </si>
+  <si>
+    <t>BretAgnew12@gmail.com</t>
+  </si>
+  <si>
+    <t>EdgardoTaylor12</t>
+  </si>
+  <si>
+    <t>EdgardoTaylor12@gmail.com</t>
+  </si>
+  <si>
+    <t>TyrekReis12</t>
+  </si>
+  <si>
+    <t>TyrekReis12@gmail.com</t>
+  </si>
+  <si>
+    <t>LeannaChow12</t>
+  </si>
+  <si>
+    <t>LeannaChow12@gmail.com</t>
+  </si>
+  <si>
+    <t>TuckerCarlson12</t>
+  </si>
+  <si>
+    <t>TuckerCarlson12@gmail.com</t>
+  </si>
+  <si>
+    <t>AnnmarieConnor12</t>
+  </si>
+  <si>
+    <t>AnnmarieConnor12@gmail.com</t>
+  </si>
+  <si>
+    <t>MoniqueWitte12</t>
+  </si>
+  <si>
+    <t>MoniqueWitte12@gmail.com</t>
+  </si>
+  <si>
+    <t>MikelWhitlock12</t>
+  </si>
+  <si>
+    <t>MikelWhitlock12@gmail.com</t>
+  </si>
+  <si>
+    <t>VincentAmaya12</t>
+  </si>
+  <si>
+    <t>VincentAmaya12@gmail.com</t>
+  </si>
+  <si>
+    <t>KeiraQuiroz12</t>
+  </si>
+  <si>
+    <t>KeiraQuiroz12@gmail.com</t>
+  </si>
+  <si>
+    <t>EllisCreech12</t>
+  </si>
+  <si>
+    <t>EllisCreech12@gmail.com</t>
+  </si>
+  <si>
+    <t>DionteCreel12</t>
+  </si>
+  <si>
+    <t>DionteCreel12@gmail.com</t>
+  </si>
+  <si>
+    <t>NicholeFoust12</t>
+  </si>
+  <si>
+    <t>NicholeFoust12@gmail.com</t>
+  </si>
+  <si>
+    <t>ManuelConnell12</t>
+  </si>
+  <si>
+    <t>ManuelConnell12@gmail.com</t>
+  </si>
+  <si>
+    <t>LourdesElam12</t>
+  </si>
+  <si>
+    <t>LourdesElam12@gmail.com</t>
+  </si>
+  <si>
+    <t>LincolnFrederick12</t>
+  </si>
+  <si>
+    <t>LincolnFrederick12@gmail.com</t>
+  </si>
+  <si>
+    <t>AlisaCash12</t>
+  </si>
+  <si>
+    <t>AlisaCash12@gmail.com</t>
+  </si>
+  <si>
+    <t>LucilleGriffiths12</t>
+  </si>
+  <si>
+    <t>LucilleGriffiths12@gmail.com</t>
+  </si>
+  <si>
+    <t>DonnellJernigan17</t>
+  </si>
+  <si>
+    <t>DonnellJernigan17@gmail.com</t>
+  </si>
+  <si>
+    <t>MalikOtoole17</t>
+  </si>
+  <si>
+    <t>MalikOtoole17@gmail.com</t>
+  </si>
+  <si>
+    <t>AlanCaudill17</t>
+  </si>
+  <si>
+    <t>AlanCaudill17@gmail.com</t>
+  </si>
+  <si>
+    <t>AdanApplegate17</t>
+  </si>
+  <si>
+    <t>AdanApplegate17@gmail.com</t>
+  </si>
+  <si>
+    <t>AiyanaWhitworth17</t>
+  </si>
+  <si>
+    <t>AiyanaWhitworth17@gmail.com</t>
+  </si>
+  <si>
+    <t>MercedezBrien17</t>
+  </si>
+  <si>
+    <t>MercedezBrien17@gmail.com</t>
+  </si>
+  <si>
+    <t>DuaneHager17</t>
+  </si>
+  <si>
+    <t>DuaneHager17@gmail.com</t>
+  </si>
+  <si>
+    <t>LorenBell17</t>
+  </si>
+  <si>
+    <t>LorenBell17@gmail.com</t>
+  </si>
+  <si>
+    <t>GeraldHiller17</t>
+  </si>
+  <si>
+    <t>GeraldHiller17@gmail.com</t>
+  </si>
+  <si>
+    <t>DeionBranch17</t>
+  </si>
+  <si>
+    <t>DeionBranch17@gmail.com</t>
+  </si>
+  <si>
+    <t>DakotaHalstead17</t>
+  </si>
+  <si>
+    <t>DakotaHalstead17@gmail.com</t>
+  </si>
+  <si>
+    <t>ElliottFurman17</t>
+  </si>
+  <si>
+    <t>ElliottFurman17@gmail.com</t>
+  </si>
+  <si>
+    <t>MiltonCamp17</t>
+  </si>
+  <si>
+    <t>MiltonCamp17@gmail.com</t>
+  </si>
+  <si>
+    <t>DawnChester17</t>
+  </si>
+  <si>
+    <t>DawnChester17@gmail.com</t>
+  </si>
+  <si>
+    <t>ZacheryPetrie17</t>
+  </si>
+  <si>
+    <t>ZacheryPetrie17@gmail.com</t>
+  </si>
+  <si>
+    <t>EstebanAngel17</t>
+  </si>
+  <si>
+    <t>EstebanAngel17@gmail.com</t>
+  </si>
+  <si>
+    <t>JimmyBlankenship17</t>
+  </si>
+  <si>
+    <t>JimmyBlankenship17@gmail.com</t>
+  </si>
+  <si>
+    <t>AllysaGrice17</t>
+  </si>
+  <si>
+    <t>AllysaGrice17@gmail.com</t>
+  </si>
+  <si>
+    <t>AugustineYoo17</t>
+  </si>
+  <si>
+    <t>AugustineYoo17@gmail.com</t>
+  </si>
+  <si>
+    <t>BrandiSouthard17</t>
+  </si>
+  <si>
+    <t>BrandiSouthard17@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2939,7 +2939,7 @@
   <dimension ref="A1:AF21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2:T21"/>
+      <selection activeCell="R2" sqref="R2:T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4957,8 +4957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FABAB06A-EAA7-4BA7-8A4C-8C5EF7E0517A}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:C42"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4986,15 +4986,15 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="str">
         <f>CONCATENATE($G2,$I$2)</f>
-        <v>EthanBaker11</v>
+        <v>EthanBaker12</v>
       </c>
       <c r="B2" s="1" t="str">
         <f>CONCATENATE($G2,$I$2)</f>
-        <v>EthanBaker11</v>
+        <v>EthanBaker12</v>
       </c>
       <c r="C2" s="2" t="str">
         <f>CONCATENATE($G2,$I$2,$H$2)</f>
-        <v>EthanBaker11@gmail.com</v>
+        <v>EthanBaker12@gmail.com</v>
       </c>
       <c r="G2" t="s">
         <v>135</v>
@@ -5003,21 +5003,21 @@
         <v>75</v>
       </c>
       <c r="I2">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
         <f t="shared" ref="A3:B21" si="0">CONCATENATE($G3,$I$2)</f>
-        <v>DelanieCarman11</v>
+        <v>DelanieCarman12</v>
       </c>
       <c r="B3" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DelanieCarman11</v>
+        <v>DelanieCarman12</v>
       </c>
       <c r="C3" s="2" t="str">
         <f t="shared" ref="C3:C21" si="1">CONCATENATE($G3,$I$2,$H$2)</f>
-        <v>DelanieCarman11@gmail.com</v>
+        <v>DelanieCarman12@gmail.com</v>
       </c>
       <c r="G3" t="s">
         <v>136</v>
@@ -5026,15 +5026,15 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>BretAgnew11</v>
+        <v>BretAgnew12</v>
       </c>
       <c r="B4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>BretAgnew11</v>
+        <v>BretAgnew12</v>
       </c>
       <c r="C4" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>BretAgnew11@gmail.com</v>
+        <v>BretAgnew12@gmail.com</v>
       </c>
       <c r="G4" t="s">
         <v>137</v>
@@ -5043,15 +5043,15 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EdgardoTaylor11</v>
+        <v>EdgardoTaylor12</v>
       </c>
       <c r="B5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EdgardoTaylor11</v>
+        <v>EdgardoTaylor12</v>
       </c>
       <c r="C5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>EdgardoTaylor11@gmail.com</v>
+        <v>EdgardoTaylor12@gmail.com</v>
       </c>
       <c r="G5" t="s">
         <v>138</v>
@@ -5060,15 +5060,15 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TyrekReis11</v>
+        <v>TyrekReis12</v>
       </c>
       <c r="B6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TyrekReis11</v>
+        <v>TyrekReis12</v>
       </c>
       <c r="C6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>TyrekReis11@gmail.com</v>
+        <v>TyrekReis12@gmail.com</v>
       </c>
       <c r="G6" t="s">
         <v>139</v>
@@ -5077,15 +5077,15 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LeannaChow11</v>
+        <v>LeannaChow12</v>
       </c>
       <c r="B7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LeannaChow11</v>
+        <v>LeannaChow12</v>
       </c>
       <c r="C7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LeannaChow11@gmail.com</v>
+        <v>LeannaChow12@gmail.com</v>
       </c>
       <c r="G7" t="s">
         <v>140</v>
@@ -5094,15 +5094,15 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TuckerCarlson11</v>
+        <v>TuckerCarlson12</v>
       </c>
       <c r="B8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TuckerCarlson11</v>
+        <v>TuckerCarlson12</v>
       </c>
       <c r="C8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>TuckerCarlson11@gmail.com</v>
+        <v>TuckerCarlson12@gmail.com</v>
       </c>
       <c r="G8" t="s">
         <v>141</v>
@@ -5111,15 +5111,15 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AnnmarieConnor11</v>
+        <v>AnnmarieConnor12</v>
       </c>
       <c r="B9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AnnmarieConnor11</v>
+        <v>AnnmarieConnor12</v>
       </c>
       <c r="C9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>AnnmarieConnor11@gmail.com</v>
+        <v>AnnmarieConnor12@gmail.com</v>
       </c>
       <c r="G9" t="s">
         <v>142</v>
@@ -5128,15 +5128,15 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MoniqueWitte11</v>
+        <v>MoniqueWitte12</v>
       </c>
       <c r="B10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MoniqueWitte11</v>
+        <v>MoniqueWitte12</v>
       </c>
       <c r="C10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MoniqueWitte11@gmail.com</v>
+        <v>MoniqueWitte12@gmail.com</v>
       </c>
       <c r="G10" t="s">
         <v>143</v>
@@ -5145,15 +5145,15 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MikelWhitlock11</v>
+        <v>MikelWhitlock12</v>
       </c>
       <c r="B11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MikelWhitlock11</v>
+        <v>MikelWhitlock12</v>
       </c>
       <c r="C11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MikelWhitlock11@gmail.com</v>
+        <v>MikelWhitlock12@gmail.com</v>
       </c>
       <c r="G11" t="s">
         <v>144</v>
@@ -5162,15 +5162,15 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>VincentAmaya11</v>
+        <v>VincentAmaya12</v>
       </c>
       <c r="B12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>VincentAmaya11</v>
+        <v>VincentAmaya12</v>
       </c>
       <c r="C12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>VincentAmaya11@gmail.com</v>
+        <v>VincentAmaya12@gmail.com</v>
       </c>
       <c r="G12" t="s">
         <v>145</v>
@@ -5179,15 +5179,15 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>KeiraQuiroz11</v>
+        <v>KeiraQuiroz12</v>
       </c>
       <c r="B13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>KeiraQuiroz11</v>
+        <v>KeiraQuiroz12</v>
       </c>
       <c r="C13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>KeiraQuiroz11@gmail.com</v>
+        <v>KeiraQuiroz12@gmail.com</v>
       </c>
       <c r="G13" t="s">
         <v>146</v>
@@ -5196,15 +5196,15 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EllisCreech11</v>
+        <v>EllisCreech12</v>
       </c>
       <c r="B14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EllisCreech11</v>
+        <v>EllisCreech12</v>
       </c>
       <c r="C14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>EllisCreech11@gmail.com</v>
+        <v>EllisCreech12@gmail.com</v>
       </c>
       <c r="G14" t="s">
         <v>147</v>
@@ -5213,15 +5213,15 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DionteCreel11</v>
+        <v>DionteCreel12</v>
       </c>
       <c r="B15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DionteCreel11</v>
+        <v>DionteCreel12</v>
       </c>
       <c r="C15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DionteCreel11@gmail.com</v>
+        <v>DionteCreel12@gmail.com</v>
       </c>
       <c r="G15" t="s">
         <v>148</v>
@@ -5230,15 +5230,15 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NicholeFoust11</v>
+        <v>NicholeFoust12</v>
       </c>
       <c r="B16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NicholeFoust11</v>
+        <v>NicholeFoust12</v>
       </c>
       <c r="C16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>NicholeFoust11@gmail.com</v>
+        <v>NicholeFoust12@gmail.com</v>
       </c>
       <c r="G16" t="s">
         <v>149</v>
@@ -5247,15 +5247,15 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>ManuelConnell11</v>
+        <v>ManuelConnell12</v>
       </c>
       <c r="B17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>ManuelConnell11</v>
+        <v>ManuelConnell12</v>
       </c>
       <c r="C17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>ManuelConnell11@gmail.com</v>
+        <v>ManuelConnell12@gmail.com</v>
       </c>
       <c r="G17" t="s">
         <v>150</v>
@@ -5264,15 +5264,15 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LourdesElam11</v>
+        <v>LourdesElam12</v>
       </c>
       <c r="B18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LourdesElam11</v>
+        <v>LourdesElam12</v>
       </c>
       <c r="C18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LourdesElam11@gmail.com</v>
+        <v>LourdesElam12@gmail.com</v>
       </c>
       <c r="G18" t="s">
         <v>151</v>
@@ -5281,15 +5281,15 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LincolnFrederick11</v>
+        <v>LincolnFrederick12</v>
       </c>
       <c r="B19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LincolnFrederick11</v>
+        <v>LincolnFrederick12</v>
       </c>
       <c r="C19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LincolnFrederick11@gmail.com</v>
+        <v>LincolnFrederick12@gmail.com</v>
       </c>
       <c r="G19" t="s">
         <v>152</v>
@@ -5298,15 +5298,15 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AlisaCash11</v>
+        <v>AlisaCash12</v>
       </c>
       <c r="B20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AlisaCash11</v>
+        <v>AlisaCash12</v>
       </c>
       <c r="C20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>AlisaCash11@gmail.com</v>
+        <v>AlisaCash12@gmail.com</v>
       </c>
       <c r="G20" t="s">
         <v>153</v>
@@ -5315,15 +5315,15 @@
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LucilleGriffiths11</v>
+        <v>LucilleGriffiths12</v>
       </c>
       <c r="B21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LucilleGriffiths11</v>
+        <v>LucilleGriffiths12</v>
       </c>
       <c r="C21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LucilleGriffiths11@gmail.com</v>
+        <v>LucilleGriffiths12@gmail.com</v>
       </c>
       <c r="G21" t="s">
         <v>154</v>
@@ -5345,15 +5345,15 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="str">
         <f>CONCATENATE($G23,$I$23)</f>
-        <v>DonnellJernigan16</v>
+        <v>DonnellJernigan17</v>
       </c>
       <c r="B23" s="1" t="str">
         <f>CONCATENATE($G23,$I$23)</f>
-        <v>DonnellJernigan16</v>
+        <v>DonnellJernigan17</v>
       </c>
       <c r="C23" s="2" t="str">
         <f>CONCATENATE($G23,$I$23,$H$23)</f>
-        <v>DonnellJernigan16@gmail.com</v>
+        <v>DonnellJernigan17@gmail.com</v>
       </c>
       <c r="G23" s="24" t="s">
         <v>155</v>
@@ -5362,21 +5362,21 @@
         <v>75</v>
       </c>
       <c r="I23">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="str">
         <f t="shared" ref="A24:B42" si="2">CONCATENATE($G24,$I$23)</f>
-        <v>MalikOtoole16</v>
+        <v>MalikOtoole17</v>
       </c>
       <c r="B24" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MalikOtoole16</v>
+        <v>MalikOtoole17</v>
       </c>
       <c r="C24" s="2" t="str">
         <f t="shared" ref="C24:C42" si="3">CONCATENATE($G24,$I$23,$H$23)</f>
-        <v>MalikOtoole16@gmail.com</v>
+        <v>MalikOtoole17@gmail.com</v>
       </c>
       <c r="G24" t="s">
         <v>156</v>
@@ -5385,15 +5385,15 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AlanCaudill16</v>
+        <v>AlanCaudill17</v>
       </c>
       <c r="B25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AlanCaudill16</v>
+        <v>AlanCaudill17</v>
       </c>
       <c r="C25" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AlanCaudill16@gmail.com</v>
+        <v>AlanCaudill17@gmail.com</v>
       </c>
       <c r="G25" t="s">
         <v>157</v>
@@ -5402,15 +5402,15 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AdanApplegate16</v>
+        <v>AdanApplegate17</v>
       </c>
       <c r="B26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AdanApplegate16</v>
+        <v>AdanApplegate17</v>
       </c>
       <c r="C26" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AdanApplegate16@gmail.com</v>
+        <v>AdanApplegate17@gmail.com</v>
       </c>
       <c r="G26" t="s">
         <v>158</v>
@@ -5419,15 +5419,15 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AiyanaWhitworth16</v>
+        <v>AiyanaWhitworth17</v>
       </c>
       <c r="B27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AiyanaWhitworth16</v>
+        <v>AiyanaWhitworth17</v>
       </c>
       <c r="C27" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AiyanaWhitworth16@gmail.com</v>
+        <v>AiyanaWhitworth17@gmail.com</v>
       </c>
       <c r="G27" t="s">
         <v>159</v>
@@ -5436,15 +5436,15 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MercedezBrien16</v>
+        <v>MercedezBrien17</v>
       </c>
       <c r="B28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MercedezBrien16</v>
+        <v>MercedezBrien17</v>
       </c>
       <c r="C28" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>MercedezBrien16@gmail.com</v>
+        <v>MercedezBrien17@gmail.com</v>
       </c>
       <c r="G28" t="s">
         <v>160</v>
@@ -5453,15 +5453,15 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DuaneHager16</v>
+        <v>DuaneHager17</v>
       </c>
       <c r="B29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DuaneHager16</v>
+        <v>DuaneHager17</v>
       </c>
       <c r="C29" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DuaneHager16@gmail.com</v>
+        <v>DuaneHager17@gmail.com</v>
       </c>
       <c r="G29" t="s">
         <v>161</v>
@@ -5470,15 +5470,15 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>LorenBell16</v>
+        <v>LorenBell17</v>
       </c>
       <c r="B30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>LorenBell16</v>
+        <v>LorenBell17</v>
       </c>
       <c r="C30" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>LorenBell16@gmail.com</v>
+        <v>LorenBell17@gmail.com</v>
       </c>
       <c r="G30" t="s">
         <v>162</v>
@@ -5487,15 +5487,15 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>GeraldHiller16</v>
+        <v>GeraldHiller17</v>
       </c>
       <c r="B31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>GeraldHiller16</v>
+        <v>GeraldHiller17</v>
       </c>
       <c r="C31" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>GeraldHiller16@gmail.com</v>
+        <v>GeraldHiller17@gmail.com</v>
       </c>
       <c r="G31" t="s">
         <v>163</v>
@@ -5504,15 +5504,15 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DeionBranch16</v>
+        <v>DeionBranch17</v>
       </c>
       <c r="B32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DeionBranch16</v>
+        <v>DeionBranch17</v>
       </c>
       <c r="C32" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DeionBranch16@gmail.com</v>
+        <v>DeionBranch17@gmail.com</v>
       </c>
       <c r="G32" t="s">
         <v>164</v>
@@ -5521,15 +5521,15 @@
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DakotaHalstead16</v>
+        <v>DakotaHalstead17</v>
       </c>
       <c r="B33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DakotaHalstead16</v>
+        <v>DakotaHalstead17</v>
       </c>
       <c r="C33" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DakotaHalstead16@gmail.com</v>
+        <v>DakotaHalstead17@gmail.com</v>
       </c>
       <c r="G33" t="s">
         <v>165</v>
@@ -5538,15 +5538,15 @@
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ElliottFurman16</v>
+        <v>ElliottFurman17</v>
       </c>
       <c r="B34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ElliottFurman16</v>
+        <v>ElliottFurman17</v>
       </c>
       <c r="C34" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>ElliottFurman16@gmail.com</v>
+        <v>ElliottFurman17@gmail.com</v>
       </c>
       <c r="G34" t="s">
         <v>166</v>
@@ -5555,15 +5555,15 @@
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MiltonCamp16</v>
+        <v>MiltonCamp17</v>
       </c>
       <c r="B35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MiltonCamp16</v>
+        <v>MiltonCamp17</v>
       </c>
       <c r="C35" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>MiltonCamp16@gmail.com</v>
+        <v>MiltonCamp17@gmail.com</v>
       </c>
       <c r="G35" t="s">
         <v>167</v>
@@ -5572,15 +5572,15 @@
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DawnChester16</v>
+        <v>DawnChester17</v>
       </c>
       <c r="B36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DawnChester16</v>
+        <v>DawnChester17</v>
       </c>
       <c r="C36" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DawnChester16@gmail.com</v>
+        <v>DawnChester17@gmail.com</v>
       </c>
       <c r="G36" t="s">
         <v>168</v>
@@ -5589,15 +5589,15 @@
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ZacheryPetrie16</v>
+        <v>ZacheryPetrie17</v>
       </c>
       <c r="B37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ZacheryPetrie16</v>
+        <v>ZacheryPetrie17</v>
       </c>
       <c r="C37" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>ZacheryPetrie16@gmail.com</v>
+        <v>ZacheryPetrie17@gmail.com</v>
       </c>
       <c r="G37" t="s">
         <v>169</v>
@@ -5606,15 +5606,15 @@
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>EstebanAngel16</v>
+        <v>EstebanAngel17</v>
       </c>
       <c r="B38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>EstebanAngel16</v>
+        <v>EstebanAngel17</v>
       </c>
       <c r="C38" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>EstebanAngel16@gmail.com</v>
+        <v>EstebanAngel17@gmail.com</v>
       </c>
       <c r="G38" t="s">
         <v>170</v>
@@ -5623,15 +5623,15 @@
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>JimmyBlankenship16</v>
+        <v>JimmyBlankenship17</v>
       </c>
       <c r="B39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>JimmyBlankenship16</v>
+        <v>JimmyBlankenship17</v>
       </c>
       <c r="C39" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>JimmyBlankenship16@gmail.com</v>
+        <v>JimmyBlankenship17@gmail.com</v>
       </c>
       <c r="G39" t="s">
         <v>171</v>
@@ -5640,15 +5640,15 @@
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AllysaGrice16</v>
+        <v>AllysaGrice17</v>
       </c>
       <c r="B40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AllysaGrice16</v>
+        <v>AllysaGrice17</v>
       </c>
       <c r="C40" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AllysaGrice16@gmail.com</v>
+        <v>AllysaGrice17@gmail.com</v>
       </c>
       <c r="G40" t="s">
         <v>172</v>
@@ -5657,15 +5657,15 @@
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AugustineYoo16</v>
+        <v>AugustineYoo17</v>
       </c>
       <c r="B41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AugustineYoo16</v>
+        <v>AugustineYoo17</v>
       </c>
       <c r="C41" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AugustineYoo16@gmail.com</v>
+        <v>AugustineYoo17@gmail.com</v>
       </c>
       <c r="G41" t="s">
         <v>173</v>
@@ -5674,15 +5674,15 @@
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BrandiSouthard16</v>
+        <v>BrandiSouthard17</v>
       </c>
       <c r="B42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BrandiSouthard16</v>
+        <v>BrandiSouthard17</v>
       </c>
       <c r="C42" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>BrandiSouthard16@gmail.com</v>
+        <v>BrandiSouthard17@gmail.com</v>
       </c>
       <c r="G42" t="s">
         <v>174</v>

</xml_diff>

<commit_message>
updated data and return pom file
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/Test_Data.xlsx
+++ b/src/main/resources/test_data/Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verkh\IdeaProjects\pom6\src\main\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5769F9-98C2-4FEC-91CC-1EBF24359363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05883D7-BDAB-4B28-8817-DC8A47211DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1500" windowWidth="23040" windowHeight="12180" tabRatio="594" activeTab="1" xr2:uid="{56D596F5-221D-421D-9FC5-55182B639D44}"/>
   </bookViews>
@@ -1048,244 +1048,244 @@
     <t>3</t>
   </si>
   <si>
-    <t>EthanBaker13</t>
-  </si>
-  <si>
-    <t>EthanBaker13@gmail.com</t>
-  </si>
-  <si>
-    <t>DelanieCarman13</t>
-  </si>
-  <si>
-    <t>DelanieCarman13@gmail.com</t>
-  </si>
-  <si>
-    <t>BretAgnew13</t>
-  </si>
-  <si>
-    <t>BretAgnew13@gmail.com</t>
-  </si>
-  <si>
-    <t>EdgardoTaylor13</t>
-  </si>
-  <si>
-    <t>EdgardoTaylor13@gmail.com</t>
-  </si>
-  <si>
-    <t>TyrekReis13</t>
-  </si>
-  <si>
-    <t>TyrekReis13@gmail.com</t>
-  </si>
-  <si>
-    <t>LeannaChow13</t>
-  </si>
-  <si>
-    <t>LeannaChow13@gmail.com</t>
-  </si>
-  <si>
-    <t>TuckerCarlson13</t>
-  </si>
-  <si>
-    <t>TuckerCarlson13@gmail.com</t>
-  </si>
-  <si>
-    <t>AnnmarieConnor13</t>
-  </si>
-  <si>
-    <t>AnnmarieConnor13@gmail.com</t>
-  </si>
-  <si>
-    <t>MoniqueWitte13</t>
-  </si>
-  <si>
-    <t>MoniqueWitte13@gmail.com</t>
-  </si>
-  <si>
-    <t>MikelWhitlock13</t>
-  </si>
-  <si>
-    <t>MikelWhitlock13@gmail.com</t>
-  </si>
-  <si>
-    <t>VincentAmaya13</t>
-  </si>
-  <si>
-    <t>VincentAmaya13@gmail.com</t>
-  </si>
-  <si>
-    <t>KeiraQuiroz13</t>
-  </si>
-  <si>
-    <t>KeiraQuiroz13@gmail.com</t>
-  </si>
-  <si>
-    <t>EllisCreech13</t>
-  </si>
-  <si>
-    <t>EllisCreech13@gmail.com</t>
-  </si>
-  <si>
-    <t>DionteCreel13</t>
-  </si>
-  <si>
-    <t>DionteCreel13@gmail.com</t>
-  </si>
-  <si>
-    <t>NicholeFoust13</t>
-  </si>
-  <si>
-    <t>NicholeFoust13@gmail.com</t>
-  </si>
-  <si>
-    <t>ManuelConnell13</t>
-  </si>
-  <si>
-    <t>ManuelConnell13@gmail.com</t>
-  </si>
-  <si>
-    <t>LourdesElam13</t>
-  </si>
-  <si>
-    <t>LourdesElam13@gmail.com</t>
-  </si>
-  <si>
-    <t>LincolnFrederick13</t>
-  </si>
-  <si>
-    <t>LincolnFrederick13@gmail.com</t>
-  </si>
-  <si>
-    <t>AlisaCash13</t>
-  </si>
-  <si>
-    <t>AlisaCash13@gmail.com</t>
-  </si>
-  <si>
-    <t>LucilleGriffiths13</t>
-  </si>
-  <si>
-    <t>LucilleGriffiths13@gmail.com</t>
-  </si>
-  <si>
-    <t>DonnellJernigan18</t>
-  </si>
-  <si>
-    <t>DonnellJernigan18@gmail.com</t>
-  </si>
-  <si>
-    <t>MalikOtoole18</t>
-  </si>
-  <si>
-    <t>MalikOtoole18@gmail.com</t>
-  </si>
-  <si>
-    <t>AlanCaudill18</t>
-  </si>
-  <si>
-    <t>AlanCaudill18@gmail.com</t>
-  </si>
-  <si>
-    <t>AdanApplegate18</t>
-  </si>
-  <si>
-    <t>AdanApplegate18@gmail.com</t>
-  </si>
-  <si>
-    <t>AiyanaWhitworth18</t>
-  </si>
-  <si>
-    <t>AiyanaWhitworth18@gmail.com</t>
-  </si>
-  <si>
-    <t>MercedezBrien18</t>
-  </si>
-  <si>
-    <t>MercedezBrien18@gmail.com</t>
-  </si>
-  <si>
-    <t>DuaneHager18</t>
-  </si>
-  <si>
-    <t>DuaneHager18@gmail.com</t>
-  </si>
-  <si>
-    <t>LorenBell18</t>
-  </si>
-  <si>
-    <t>LorenBell18@gmail.com</t>
-  </si>
-  <si>
-    <t>GeraldHiller18</t>
-  </si>
-  <si>
-    <t>GeraldHiller18@gmail.com</t>
-  </si>
-  <si>
-    <t>DeionBranch18</t>
-  </si>
-  <si>
-    <t>DeionBranch18@gmail.com</t>
-  </si>
-  <si>
-    <t>DakotaHalstead18</t>
-  </si>
-  <si>
-    <t>DakotaHalstead18@gmail.com</t>
-  </si>
-  <si>
-    <t>ElliottFurman18</t>
-  </si>
-  <si>
-    <t>ElliottFurman18@gmail.com</t>
-  </si>
-  <si>
-    <t>MiltonCamp18</t>
-  </si>
-  <si>
-    <t>MiltonCamp18@gmail.com</t>
-  </si>
-  <si>
-    <t>DawnChester18</t>
-  </si>
-  <si>
-    <t>DawnChester18@gmail.com</t>
-  </si>
-  <si>
-    <t>ZacheryPetrie18</t>
-  </si>
-  <si>
-    <t>ZacheryPetrie18@gmail.com</t>
-  </si>
-  <si>
-    <t>EstebanAngel18</t>
-  </si>
-  <si>
-    <t>EstebanAngel18@gmail.com</t>
-  </si>
-  <si>
-    <t>JimmyBlankenship18</t>
-  </si>
-  <si>
-    <t>JimmyBlankenship18@gmail.com</t>
-  </si>
-  <si>
-    <t>AllysaGrice18</t>
-  </si>
-  <si>
-    <t>AllysaGrice18@gmail.com</t>
-  </si>
-  <si>
-    <t>AugustineYoo18</t>
-  </si>
-  <si>
-    <t>AugustineYoo18@gmail.com</t>
-  </si>
-  <si>
-    <t>BrandiSouthard18</t>
-  </si>
-  <si>
-    <t>BrandiSouthard18@gmail.com</t>
+    <t>EthanBaker14</t>
+  </si>
+  <si>
+    <t>EthanBaker14@gmail.com</t>
+  </si>
+  <si>
+    <t>DelanieCarman14</t>
+  </si>
+  <si>
+    <t>DelanieCarman14@gmail.com</t>
+  </si>
+  <si>
+    <t>BretAgnew14</t>
+  </si>
+  <si>
+    <t>BretAgnew14@gmail.com</t>
+  </si>
+  <si>
+    <t>EdgardoTaylor14</t>
+  </si>
+  <si>
+    <t>EdgardoTaylor14@gmail.com</t>
+  </si>
+  <si>
+    <t>TyrekReis14</t>
+  </si>
+  <si>
+    <t>TyrekReis14@gmail.com</t>
+  </si>
+  <si>
+    <t>LeannaChow14</t>
+  </si>
+  <si>
+    <t>LeannaChow14@gmail.com</t>
+  </si>
+  <si>
+    <t>TuckerCarlson14</t>
+  </si>
+  <si>
+    <t>TuckerCarlson14@gmail.com</t>
+  </si>
+  <si>
+    <t>AnnmarieConnor14</t>
+  </si>
+  <si>
+    <t>AnnmarieConnor14@gmail.com</t>
+  </si>
+  <si>
+    <t>MoniqueWitte14</t>
+  </si>
+  <si>
+    <t>MoniqueWitte14@gmail.com</t>
+  </si>
+  <si>
+    <t>MikelWhitlock14</t>
+  </si>
+  <si>
+    <t>MikelWhitlock14@gmail.com</t>
+  </si>
+  <si>
+    <t>VincentAmaya14</t>
+  </si>
+  <si>
+    <t>VincentAmaya14@gmail.com</t>
+  </si>
+  <si>
+    <t>KeiraQuiroz14</t>
+  </si>
+  <si>
+    <t>KeiraQuiroz14@gmail.com</t>
+  </si>
+  <si>
+    <t>EllisCreech14</t>
+  </si>
+  <si>
+    <t>EllisCreech14@gmail.com</t>
+  </si>
+  <si>
+    <t>DionteCreel14</t>
+  </si>
+  <si>
+    <t>DionteCreel14@gmail.com</t>
+  </si>
+  <si>
+    <t>NicholeFoust14</t>
+  </si>
+  <si>
+    <t>NicholeFoust14@gmail.com</t>
+  </si>
+  <si>
+    <t>ManuelConnell14</t>
+  </si>
+  <si>
+    <t>ManuelConnell14@gmail.com</t>
+  </si>
+  <si>
+    <t>LourdesElam14</t>
+  </si>
+  <si>
+    <t>LourdesElam14@gmail.com</t>
+  </si>
+  <si>
+    <t>LincolnFrederick14</t>
+  </si>
+  <si>
+    <t>LincolnFrederick14@gmail.com</t>
+  </si>
+  <si>
+    <t>AlisaCash14</t>
+  </si>
+  <si>
+    <t>AlisaCash14@gmail.com</t>
+  </si>
+  <si>
+    <t>LucilleGriffiths14</t>
+  </si>
+  <si>
+    <t>LucilleGriffiths14@gmail.com</t>
+  </si>
+  <si>
+    <t>DonnellJernigan19</t>
+  </si>
+  <si>
+    <t>DonnellJernigan19@gmail.com</t>
+  </si>
+  <si>
+    <t>MalikOtoole19</t>
+  </si>
+  <si>
+    <t>MalikOtoole19@gmail.com</t>
+  </si>
+  <si>
+    <t>AlanCaudill19</t>
+  </si>
+  <si>
+    <t>AlanCaudill19@gmail.com</t>
+  </si>
+  <si>
+    <t>AdanApplegate19</t>
+  </si>
+  <si>
+    <t>AdanApplegate19@gmail.com</t>
+  </si>
+  <si>
+    <t>AiyanaWhitworth19</t>
+  </si>
+  <si>
+    <t>AiyanaWhitworth19@gmail.com</t>
+  </si>
+  <si>
+    <t>MercedezBrien19</t>
+  </si>
+  <si>
+    <t>MercedezBrien19@gmail.com</t>
+  </si>
+  <si>
+    <t>DuaneHager19</t>
+  </si>
+  <si>
+    <t>DuaneHager19@gmail.com</t>
+  </si>
+  <si>
+    <t>LorenBell19</t>
+  </si>
+  <si>
+    <t>LorenBell19@gmail.com</t>
+  </si>
+  <si>
+    <t>GeraldHiller19</t>
+  </si>
+  <si>
+    <t>GeraldHiller19@gmail.com</t>
+  </si>
+  <si>
+    <t>DeionBranch19</t>
+  </si>
+  <si>
+    <t>DeionBranch19@gmail.com</t>
+  </si>
+  <si>
+    <t>DakotaHalstead19</t>
+  </si>
+  <si>
+    <t>DakotaHalstead19@gmail.com</t>
+  </si>
+  <si>
+    <t>ElliottFurman19</t>
+  </si>
+  <si>
+    <t>ElliottFurman19@gmail.com</t>
+  </si>
+  <si>
+    <t>MiltonCamp19</t>
+  </si>
+  <si>
+    <t>MiltonCamp19@gmail.com</t>
+  </si>
+  <si>
+    <t>DawnChester19</t>
+  </si>
+  <si>
+    <t>DawnChester19@gmail.com</t>
+  </si>
+  <si>
+    <t>ZacheryPetrie19</t>
+  </si>
+  <si>
+    <t>ZacheryPetrie19@gmail.com</t>
+  </si>
+  <si>
+    <t>EstebanAngel19</t>
+  </si>
+  <si>
+    <t>EstebanAngel19@gmail.com</t>
+  </si>
+  <si>
+    <t>JimmyBlankenship19</t>
+  </si>
+  <si>
+    <t>JimmyBlankenship19@gmail.com</t>
+  </si>
+  <si>
+    <t>AllysaGrice19</t>
+  </si>
+  <si>
+    <t>AllysaGrice19@gmail.com</t>
+  </si>
+  <si>
+    <t>AugustineYoo19</t>
+  </si>
+  <si>
+    <t>AugustineYoo19@gmail.com</t>
+  </si>
+  <si>
+    <t>BrandiSouthard19</t>
+  </si>
+  <si>
+    <t>BrandiSouthard19@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -4948,15 +4948,15 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="str">
         <f>CONCATENATE($G2,$I$2)</f>
-        <v>EthanBaker13</v>
+        <v>EthanBaker14</v>
       </c>
       <c r="B2" s="1" t="str">
         <f>CONCATENATE($G2,$I$2)</f>
-        <v>EthanBaker13</v>
+        <v>EthanBaker14</v>
       </c>
       <c r="C2" s="2" t="str">
         <f>CONCATENATE($G2,$I$2,$H$2)</f>
-        <v>EthanBaker13@gmail.com</v>
+        <v>EthanBaker14@gmail.com</v>
       </c>
       <c r="G2" t="s">
         <v>131</v>
@@ -4965,21 +4965,21 @@
         <v>71</v>
       </c>
       <c r="I2">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
         <f t="shared" ref="A3:B21" si="0">CONCATENATE($G3,$I$2)</f>
-        <v>DelanieCarman13</v>
+        <v>DelanieCarman14</v>
       </c>
       <c r="B3" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DelanieCarman13</v>
+        <v>DelanieCarman14</v>
       </c>
       <c r="C3" s="2" t="str">
         <f t="shared" ref="C3:C21" si="1">CONCATENATE($G3,$I$2,$H$2)</f>
-        <v>DelanieCarman13@gmail.com</v>
+        <v>DelanieCarman14@gmail.com</v>
       </c>
       <c r="G3" t="s">
         <v>132</v>
@@ -4988,15 +4988,15 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>BretAgnew13</v>
+        <v>BretAgnew14</v>
       </c>
       <c r="B4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>BretAgnew13</v>
+        <v>BretAgnew14</v>
       </c>
       <c r="C4" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>BretAgnew13@gmail.com</v>
+        <v>BretAgnew14@gmail.com</v>
       </c>
       <c r="G4" t="s">
         <v>133</v>
@@ -5005,15 +5005,15 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EdgardoTaylor13</v>
+        <v>EdgardoTaylor14</v>
       </c>
       <c r="B5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EdgardoTaylor13</v>
+        <v>EdgardoTaylor14</v>
       </c>
       <c r="C5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>EdgardoTaylor13@gmail.com</v>
+        <v>EdgardoTaylor14@gmail.com</v>
       </c>
       <c r="G5" t="s">
         <v>134</v>
@@ -5022,15 +5022,15 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TyrekReis13</v>
+        <v>TyrekReis14</v>
       </c>
       <c r="B6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TyrekReis13</v>
+        <v>TyrekReis14</v>
       </c>
       <c r="C6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>TyrekReis13@gmail.com</v>
+        <v>TyrekReis14@gmail.com</v>
       </c>
       <c r="G6" t="s">
         <v>135</v>
@@ -5039,15 +5039,15 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LeannaChow13</v>
+        <v>LeannaChow14</v>
       </c>
       <c r="B7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LeannaChow13</v>
+        <v>LeannaChow14</v>
       </c>
       <c r="C7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LeannaChow13@gmail.com</v>
+        <v>LeannaChow14@gmail.com</v>
       </c>
       <c r="G7" t="s">
         <v>136</v>
@@ -5056,15 +5056,15 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TuckerCarlson13</v>
+        <v>TuckerCarlson14</v>
       </c>
       <c r="B8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TuckerCarlson13</v>
+        <v>TuckerCarlson14</v>
       </c>
       <c r="C8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>TuckerCarlson13@gmail.com</v>
+        <v>TuckerCarlson14@gmail.com</v>
       </c>
       <c r="G8" t="s">
         <v>137</v>
@@ -5073,15 +5073,15 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AnnmarieConnor13</v>
+        <v>AnnmarieConnor14</v>
       </c>
       <c r="B9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AnnmarieConnor13</v>
+        <v>AnnmarieConnor14</v>
       </c>
       <c r="C9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>AnnmarieConnor13@gmail.com</v>
+        <v>AnnmarieConnor14@gmail.com</v>
       </c>
       <c r="G9" t="s">
         <v>138</v>
@@ -5090,15 +5090,15 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MoniqueWitte13</v>
+        <v>MoniqueWitte14</v>
       </c>
       <c r="B10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MoniqueWitte13</v>
+        <v>MoniqueWitte14</v>
       </c>
       <c r="C10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MoniqueWitte13@gmail.com</v>
+        <v>MoniqueWitte14@gmail.com</v>
       </c>
       <c r="G10" t="s">
         <v>139</v>
@@ -5107,15 +5107,15 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MikelWhitlock13</v>
+        <v>MikelWhitlock14</v>
       </c>
       <c r="B11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MikelWhitlock13</v>
+        <v>MikelWhitlock14</v>
       </c>
       <c r="C11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MikelWhitlock13@gmail.com</v>
+        <v>MikelWhitlock14@gmail.com</v>
       </c>
       <c r="G11" t="s">
         <v>140</v>
@@ -5124,15 +5124,15 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>VincentAmaya13</v>
+        <v>VincentAmaya14</v>
       </c>
       <c r="B12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>VincentAmaya13</v>
+        <v>VincentAmaya14</v>
       </c>
       <c r="C12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>VincentAmaya13@gmail.com</v>
+        <v>VincentAmaya14@gmail.com</v>
       </c>
       <c r="G12" t="s">
         <v>141</v>
@@ -5141,15 +5141,15 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>KeiraQuiroz13</v>
+        <v>KeiraQuiroz14</v>
       </c>
       <c r="B13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>KeiraQuiroz13</v>
+        <v>KeiraQuiroz14</v>
       </c>
       <c r="C13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>KeiraQuiroz13@gmail.com</v>
+        <v>KeiraQuiroz14@gmail.com</v>
       </c>
       <c r="G13" t="s">
         <v>142</v>
@@ -5158,15 +5158,15 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EllisCreech13</v>
+        <v>EllisCreech14</v>
       </c>
       <c r="B14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EllisCreech13</v>
+        <v>EllisCreech14</v>
       </c>
       <c r="C14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>EllisCreech13@gmail.com</v>
+        <v>EllisCreech14@gmail.com</v>
       </c>
       <c r="G14" t="s">
         <v>143</v>
@@ -5175,15 +5175,15 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DionteCreel13</v>
+        <v>DionteCreel14</v>
       </c>
       <c r="B15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DionteCreel13</v>
+        <v>DionteCreel14</v>
       </c>
       <c r="C15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DionteCreel13@gmail.com</v>
+        <v>DionteCreel14@gmail.com</v>
       </c>
       <c r="G15" t="s">
         <v>144</v>
@@ -5192,15 +5192,15 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NicholeFoust13</v>
+        <v>NicholeFoust14</v>
       </c>
       <c r="B16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NicholeFoust13</v>
+        <v>NicholeFoust14</v>
       </c>
       <c r="C16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>NicholeFoust13@gmail.com</v>
+        <v>NicholeFoust14@gmail.com</v>
       </c>
       <c r="G16" t="s">
         <v>145</v>
@@ -5209,15 +5209,15 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>ManuelConnell13</v>
+        <v>ManuelConnell14</v>
       </c>
       <c r="B17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>ManuelConnell13</v>
+        <v>ManuelConnell14</v>
       </c>
       <c r="C17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>ManuelConnell13@gmail.com</v>
+        <v>ManuelConnell14@gmail.com</v>
       </c>
       <c r="G17" t="s">
         <v>146</v>
@@ -5226,15 +5226,15 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LourdesElam13</v>
+        <v>LourdesElam14</v>
       </c>
       <c r="B18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LourdesElam13</v>
+        <v>LourdesElam14</v>
       </c>
       <c r="C18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LourdesElam13@gmail.com</v>
+        <v>LourdesElam14@gmail.com</v>
       </c>
       <c r="G18" t="s">
         <v>147</v>
@@ -5243,15 +5243,15 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LincolnFrederick13</v>
+        <v>LincolnFrederick14</v>
       </c>
       <c r="B19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LincolnFrederick13</v>
+        <v>LincolnFrederick14</v>
       </c>
       <c r="C19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LincolnFrederick13@gmail.com</v>
+        <v>LincolnFrederick14@gmail.com</v>
       </c>
       <c r="G19" t="s">
         <v>148</v>
@@ -5260,15 +5260,15 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AlisaCash13</v>
+        <v>AlisaCash14</v>
       </c>
       <c r="B20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AlisaCash13</v>
+        <v>AlisaCash14</v>
       </c>
       <c r="C20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>AlisaCash13@gmail.com</v>
+        <v>AlisaCash14@gmail.com</v>
       </c>
       <c r="G20" t="s">
         <v>149</v>
@@ -5277,15 +5277,15 @@
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LucilleGriffiths13</v>
+        <v>LucilleGriffiths14</v>
       </c>
       <c r="B21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LucilleGriffiths13</v>
+        <v>LucilleGriffiths14</v>
       </c>
       <c r="C21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LucilleGriffiths13@gmail.com</v>
+        <v>LucilleGriffiths14@gmail.com</v>
       </c>
       <c r="G21" t="s">
         <v>150</v>
@@ -5307,15 +5307,15 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="str">
         <f>CONCATENATE($G23,$I$23)</f>
-        <v>DonnellJernigan18</v>
+        <v>DonnellJernigan19</v>
       </c>
       <c r="B23" s="1" t="str">
         <f>CONCATENATE($G23,$I$23)</f>
-        <v>DonnellJernigan18</v>
+        <v>DonnellJernigan19</v>
       </c>
       <c r="C23" s="2" t="str">
         <f>CONCATENATE($G23,$I$23,$H$23)</f>
-        <v>DonnellJernigan18@gmail.com</v>
+        <v>DonnellJernigan19@gmail.com</v>
       </c>
       <c r="G23" s="24" t="s">
         <v>151</v>
@@ -5324,21 +5324,21 @@
         <v>71</v>
       </c>
       <c r="I23">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="str">
         <f t="shared" ref="A24:B42" si="2">CONCATENATE($G24,$I$23)</f>
-        <v>MalikOtoole18</v>
+        <v>MalikOtoole19</v>
       </c>
       <c r="B24" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MalikOtoole18</v>
+        <v>MalikOtoole19</v>
       </c>
       <c r="C24" s="2" t="str">
         <f t="shared" ref="C24:C42" si="3">CONCATENATE($G24,$I$23,$H$23)</f>
-        <v>MalikOtoole18@gmail.com</v>
+        <v>MalikOtoole19@gmail.com</v>
       </c>
       <c r="G24" t="s">
         <v>152</v>
@@ -5347,15 +5347,15 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AlanCaudill18</v>
+        <v>AlanCaudill19</v>
       </c>
       <c r="B25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AlanCaudill18</v>
+        <v>AlanCaudill19</v>
       </c>
       <c r="C25" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AlanCaudill18@gmail.com</v>
+        <v>AlanCaudill19@gmail.com</v>
       </c>
       <c r="G25" t="s">
         <v>153</v>
@@ -5364,15 +5364,15 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AdanApplegate18</v>
+        <v>AdanApplegate19</v>
       </c>
       <c r="B26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AdanApplegate18</v>
+        <v>AdanApplegate19</v>
       </c>
       <c r="C26" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AdanApplegate18@gmail.com</v>
+        <v>AdanApplegate19@gmail.com</v>
       </c>
       <c r="G26" t="s">
         <v>154</v>
@@ -5381,15 +5381,15 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AiyanaWhitworth18</v>
+        <v>AiyanaWhitworth19</v>
       </c>
       <c r="B27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AiyanaWhitworth18</v>
+        <v>AiyanaWhitworth19</v>
       </c>
       <c r="C27" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AiyanaWhitworth18@gmail.com</v>
+        <v>AiyanaWhitworth19@gmail.com</v>
       </c>
       <c r="G27" t="s">
         <v>155</v>
@@ -5398,15 +5398,15 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MercedezBrien18</v>
+        <v>MercedezBrien19</v>
       </c>
       <c r="B28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MercedezBrien18</v>
+        <v>MercedezBrien19</v>
       </c>
       <c r="C28" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>MercedezBrien18@gmail.com</v>
+        <v>MercedezBrien19@gmail.com</v>
       </c>
       <c r="G28" t="s">
         <v>156</v>
@@ -5415,15 +5415,15 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DuaneHager18</v>
+        <v>DuaneHager19</v>
       </c>
       <c r="B29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DuaneHager18</v>
+        <v>DuaneHager19</v>
       </c>
       <c r="C29" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DuaneHager18@gmail.com</v>
+        <v>DuaneHager19@gmail.com</v>
       </c>
       <c r="G29" t="s">
         <v>157</v>
@@ -5432,15 +5432,15 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>LorenBell18</v>
+        <v>LorenBell19</v>
       </c>
       <c r="B30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>LorenBell18</v>
+        <v>LorenBell19</v>
       </c>
       <c r="C30" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>LorenBell18@gmail.com</v>
+        <v>LorenBell19@gmail.com</v>
       </c>
       <c r="G30" t="s">
         <v>158</v>
@@ -5449,15 +5449,15 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>GeraldHiller18</v>
+        <v>GeraldHiller19</v>
       </c>
       <c r="B31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>GeraldHiller18</v>
+        <v>GeraldHiller19</v>
       </c>
       <c r="C31" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>GeraldHiller18@gmail.com</v>
+        <v>GeraldHiller19@gmail.com</v>
       </c>
       <c r="G31" t="s">
         <v>159</v>
@@ -5466,15 +5466,15 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DeionBranch18</v>
+        <v>DeionBranch19</v>
       </c>
       <c r="B32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DeionBranch18</v>
+        <v>DeionBranch19</v>
       </c>
       <c r="C32" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DeionBranch18@gmail.com</v>
+        <v>DeionBranch19@gmail.com</v>
       </c>
       <c r="G32" t="s">
         <v>160</v>
@@ -5483,15 +5483,15 @@
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DakotaHalstead18</v>
+        <v>DakotaHalstead19</v>
       </c>
       <c r="B33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DakotaHalstead18</v>
+        <v>DakotaHalstead19</v>
       </c>
       <c r="C33" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DakotaHalstead18@gmail.com</v>
+        <v>DakotaHalstead19@gmail.com</v>
       </c>
       <c r="G33" t="s">
         <v>161</v>
@@ -5500,15 +5500,15 @@
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ElliottFurman18</v>
+        <v>ElliottFurman19</v>
       </c>
       <c r="B34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ElliottFurman18</v>
+        <v>ElliottFurman19</v>
       </c>
       <c r="C34" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>ElliottFurman18@gmail.com</v>
+        <v>ElliottFurman19@gmail.com</v>
       </c>
       <c r="G34" t="s">
         <v>162</v>
@@ -5517,15 +5517,15 @@
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MiltonCamp18</v>
+        <v>MiltonCamp19</v>
       </c>
       <c r="B35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MiltonCamp18</v>
+        <v>MiltonCamp19</v>
       </c>
       <c r="C35" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>MiltonCamp18@gmail.com</v>
+        <v>MiltonCamp19@gmail.com</v>
       </c>
       <c r="G35" t="s">
         <v>163</v>
@@ -5534,15 +5534,15 @@
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DawnChester18</v>
+        <v>DawnChester19</v>
       </c>
       <c r="B36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DawnChester18</v>
+        <v>DawnChester19</v>
       </c>
       <c r="C36" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DawnChester18@gmail.com</v>
+        <v>DawnChester19@gmail.com</v>
       </c>
       <c r="G36" t="s">
         <v>164</v>
@@ -5551,15 +5551,15 @@
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ZacheryPetrie18</v>
+        <v>ZacheryPetrie19</v>
       </c>
       <c r="B37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ZacheryPetrie18</v>
+        <v>ZacheryPetrie19</v>
       </c>
       <c r="C37" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>ZacheryPetrie18@gmail.com</v>
+        <v>ZacheryPetrie19@gmail.com</v>
       </c>
       <c r="G37" t="s">
         <v>165</v>
@@ -5568,15 +5568,15 @@
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>EstebanAngel18</v>
+        <v>EstebanAngel19</v>
       </c>
       <c r="B38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>EstebanAngel18</v>
+        <v>EstebanAngel19</v>
       </c>
       <c r="C38" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>EstebanAngel18@gmail.com</v>
+        <v>EstebanAngel19@gmail.com</v>
       </c>
       <c r="G38" t="s">
         <v>166</v>
@@ -5585,15 +5585,15 @@
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>JimmyBlankenship18</v>
+        <v>JimmyBlankenship19</v>
       </c>
       <c r="B39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>JimmyBlankenship18</v>
+        <v>JimmyBlankenship19</v>
       </c>
       <c r="C39" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>JimmyBlankenship18@gmail.com</v>
+        <v>JimmyBlankenship19@gmail.com</v>
       </c>
       <c r="G39" t="s">
         <v>167</v>
@@ -5602,15 +5602,15 @@
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AllysaGrice18</v>
+        <v>AllysaGrice19</v>
       </c>
       <c r="B40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AllysaGrice18</v>
+        <v>AllysaGrice19</v>
       </c>
       <c r="C40" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AllysaGrice18@gmail.com</v>
+        <v>AllysaGrice19@gmail.com</v>
       </c>
       <c r="G40" t="s">
         <v>168</v>
@@ -5619,15 +5619,15 @@
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AugustineYoo18</v>
+        <v>AugustineYoo19</v>
       </c>
       <c r="B41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AugustineYoo18</v>
+        <v>AugustineYoo19</v>
       </c>
       <c r="C41" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AugustineYoo18@gmail.com</v>
+        <v>AugustineYoo19@gmail.com</v>
       </c>
       <c r="G41" t="s">
         <v>169</v>
@@ -5636,15 +5636,15 @@
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BrandiSouthard18</v>
+        <v>BrandiSouthard19</v>
       </c>
       <c r="B42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BrandiSouthard18</v>
+        <v>BrandiSouthard19</v>
       </c>
       <c r="C42" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>BrandiSouthard18@gmail.com</v>
+        <v>BrandiSouthard19@gmail.com</v>
       </c>
       <c r="G42" t="s">
         <v>170</v>

</xml_diff>

<commit_message>
updated data and pom file
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/Test_Data.xlsx
+++ b/src/main/resources/test_data/Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verkh\IdeaProjects\pom6\src\main\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05883D7-BDAB-4B28-8817-DC8A47211DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677FFA95-6AF8-4996-905A-2E11BAEC6516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1500" windowWidth="23040" windowHeight="12180" tabRatio="594" activeTab="1" xr2:uid="{56D596F5-221D-421D-9FC5-55182B639D44}"/>
   </bookViews>
@@ -1048,244 +1048,244 @@
     <t>3</t>
   </si>
   <si>
-    <t>EthanBaker14</t>
-  </si>
-  <si>
-    <t>EthanBaker14@gmail.com</t>
-  </si>
-  <si>
-    <t>DelanieCarman14</t>
-  </si>
-  <si>
-    <t>DelanieCarman14@gmail.com</t>
-  </si>
-  <si>
-    <t>BretAgnew14</t>
-  </si>
-  <si>
-    <t>BretAgnew14@gmail.com</t>
-  </si>
-  <si>
-    <t>EdgardoTaylor14</t>
-  </si>
-  <si>
-    <t>EdgardoTaylor14@gmail.com</t>
-  </si>
-  <si>
-    <t>TyrekReis14</t>
-  </si>
-  <si>
-    <t>TyrekReis14@gmail.com</t>
-  </si>
-  <si>
-    <t>LeannaChow14</t>
-  </si>
-  <si>
-    <t>LeannaChow14@gmail.com</t>
-  </si>
-  <si>
-    <t>TuckerCarlson14</t>
-  </si>
-  <si>
-    <t>TuckerCarlson14@gmail.com</t>
-  </si>
-  <si>
-    <t>AnnmarieConnor14</t>
-  </si>
-  <si>
-    <t>AnnmarieConnor14@gmail.com</t>
-  </si>
-  <si>
-    <t>MoniqueWitte14</t>
-  </si>
-  <si>
-    <t>MoniqueWitte14@gmail.com</t>
-  </si>
-  <si>
-    <t>MikelWhitlock14</t>
-  </si>
-  <si>
-    <t>MikelWhitlock14@gmail.com</t>
-  </si>
-  <si>
-    <t>VincentAmaya14</t>
-  </si>
-  <si>
-    <t>VincentAmaya14@gmail.com</t>
-  </si>
-  <si>
-    <t>KeiraQuiroz14</t>
-  </si>
-  <si>
-    <t>KeiraQuiroz14@gmail.com</t>
-  </si>
-  <si>
-    <t>EllisCreech14</t>
-  </si>
-  <si>
-    <t>EllisCreech14@gmail.com</t>
-  </si>
-  <si>
-    <t>DionteCreel14</t>
-  </si>
-  <si>
-    <t>DionteCreel14@gmail.com</t>
-  </si>
-  <si>
-    <t>NicholeFoust14</t>
-  </si>
-  <si>
-    <t>NicholeFoust14@gmail.com</t>
-  </si>
-  <si>
-    <t>ManuelConnell14</t>
-  </si>
-  <si>
-    <t>ManuelConnell14@gmail.com</t>
-  </si>
-  <si>
-    <t>LourdesElam14</t>
-  </si>
-  <si>
-    <t>LourdesElam14@gmail.com</t>
-  </si>
-  <si>
-    <t>LincolnFrederick14</t>
-  </si>
-  <si>
-    <t>LincolnFrederick14@gmail.com</t>
-  </si>
-  <si>
-    <t>AlisaCash14</t>
-  </si>
-  <si>
-    <t>AlisaCash14@gmail.com</t>
-  </si>
-  <si>
-    <t>LucilleGriffiths14</t>
-  </si>
-  <si>
-    <t>LucilleGriffiths14@gmail.com</t>
-  </si>
-  <si>
-    <t>DonnellJernigan19</t>
-  </si>
-  <si>
-    <t>DonnellJernigan19@gmail.com</t>
-  </si>
-  <si>
-    <t>MalikOtoole19</t>
-  </si>
-  <si>
-    <t>MalikOtoole19@gmail.com</t>
-  </si>
-  <si>
-    <t>AlanCaudill19</t>
-  </si>
-  <si>
-    <t>AlanCaudill19@gmail.com</t>
-  </si>
-  <si>
-    <t>AdanApplegate19</t>
-  </si>
-  <si>
-    <t>AdanApplegate19@gmail.com</t>
-  </si>
-  <si>
-    <t>AiyanaWhitworth19</t>
-  </si>
-  <si>
-    <t>AiyanaWhitworth19@gmail.com</t>
-  </si>
-  <si>
-    <t>MercedezBrien19</t>
-  </si>
-  <si>
-    <t>MercedezBrien19@gmail.com</t>
-  </si>
-  <si>
-    <t>DuaneHager19</t>
-  </si>
-  <si>
-    <t>DuaneHager19@gmail.com</t>
-  </si>
-  <si>
-    <t>LorenBell19</t>
-  </si>
-  <si>
-    <t>LorenBell19@gmail.com</t>
-  </si>
-  <si>
-    <t>GeraldHiller19</t>
-  </si>
-  <si>
-    <t>GeraldHiller19@gmail.com</t>
-  </si>
-  <si>
-    <t>DeionBranch19</t>
-  </si>
-  <si>
-    <t>DeionBranch19@gmail.com</t>
-  </si>
-  <si>
-    <t>DakotaHalstead19</t>
-  </si>
-  <si>
-    <t>DakotaHalstead19@gmail.com</t>
-  </si>
-  <si>
-    <t>ElliottFurman19</t>
-  </si>
-  <si>
-    <t>ElliottFurman19@gmail.com</t>
-  </si>
-  <si>
-    <t>MiltonCamp19</t>
-  </si>
-  <si>
-    <t>MiltonCamp19@gmail.com</t>
-  </si>
-  <si>
-    <t>DawnChester19</t>
-  </si>
-  <si>
-    <t>DawnChester19@gmail.com</t>
-  </si>
-  <si>
-    <t>ZacheryPetrie19</t>
-  </si>
-  <si>
-    <t>ZacheryPetrie19@gmail.com</t>
-  </si>
-  <si>
-    <t>EstebanAngel19</t>
-  </si>
-  <si>
-    <t>EstebanAngel19@gmail.com</t>
-  </si>
-  <si>
-    <t>JimmyBlankenship19</t>
-  </si>
-  <si>
-    <t>JimmyBlankenship19@gmail.com</t>
-  </si>
-  <si>
-    <t>AllysaGrice19</t>
-  </si>
-  <si>
-    <t>AllysaGrice19@gmail.com</t>
-  </si>
-  <si>
-    <t>AugustineYoo19</t>
-  </si>
-  <si>
-    <t>AugustineYoo19@gmail.com</t>
-  </si>
-  <si>
-    <t>BrandiSouthard19</t>
-  </si>
-  <si>
-    <t>BrandiSouthard19@gmail.com</t>
+    <t>EthanBaker15</t>
+  </si>
+  <si>
+    <t>EthanBaker15@gmail.com</t>
+  </si>
+  <si>
+    <t>DelanieCarman15</t>
+  </si>
+  <si>
+    <t>DelanieCarman15@gmail.com</t>
+  </si>
+  <si>
+    <t>BretAgnew15</t>
+  </si>
+  <si>
+    <t>BretAgnew15@gmail.com</t>
+  </si>
+  <si>
+    <t>EdgardoTaylor15</t>
+  </si>
+  <si>
+    <t>EdgardoTaylor15@gmail.com</t>
+  </si>
+  <si>
+    <t>TyrekReis15</t>
+  </si>
+  <si>
+    <t>TyrekReis15@gmail.com</t>
+  </si>
+  <si>
+    <t>LeannaChow15</t>
+  </si>
+  <si>
+    <t>LeannaChow15@gmail.com</t>
+  </si>
+  <si>
+    <t>TuckerCarlson15</t>
+  </si>
+  <si>
+    <t>TuckerCarlson15@gmail.com</t>
+  </si>
+  <si>
+    <t>AnnmarieConnor15</t>
+  </si>
+  <si>
+    <t>AnnmarieConnor15@gmail.com</t>
+  </si>
+  <si>
+    <t>MoniqueWitte15</t>
+  </si>
+  <si>
+    <t>MoniqueWitte15@gmail.com</t>
+  </si>
+  <si>
+    <t>MikelWhitlock15</t>
+  </si>
+  <si>
+    <t>MikelWhitlock15@gmail.com</t>
+  </si>
+  <si>
+    <t>VincentAmaya15</t>
+  </si>
+  <si>
+    <t>VincentAmaya15@gmail.com</t>
+  </si>
+  <si>
+    <t>KeiraQuiroz15</t>
+  </si>
+  <si>
+    <t>KeiraQuiroz15@gmail.com</t>
+  </si>
+  <si>
+    <t>EllisCreech15</t>
+  </si>
+  <si>
+    <t>EllisCreech15@gmail.com</t>
+  </si>
+  <si>
+    <t>DionteCreel15</t>
+  </si>
+  <si>
+    <t>DionteCreel15@gmail.com</t>
+  </si>
+  <si>
+    <t>NicholeFoust15</t>
+  </si>
+  <si>
+    <t>NicholeFoust15@gmail.com</t>
+  </si>
+  <si>
+    <t>ManuelConnell15</t>
+  </si>
+  <si>
+    <t>ManuelConnell15@gmail.com</t>
+  </si>
+  <si>
+    <t>LourdesElam15</t>
+  </si>
+  <si>
+    <t>LourdesElam15@gmail.com</t>
+  </si>
+  <si>
+    <t>LincolnFrederick15</t>
+  </si>
+  <si>
+    <t>LincolnFrederick15@gmail.com</t>
+  </si>
+  <si>
+    <t>AlisaCash15</t>
+  </si>
+  <si>
+    <t>AlisaCash15@gmail.com</t>
+  </si>
+  <si>
+    <t>LucilleGriffiths15</t>
+  </si>
+  <si>
+    <t>LucilleGriffiths15@gmail.com</t>
+  </si>
+  <si>
+    <t>DonnellJernigan20</t>
+  </si>
+  <si>
+    <t>DonnellJernigan20@gmail.com</t>
+  </si>
+  <si>
+    <t>MalikOtoole20</t>
+  </si>
+  <si>
+    <t>MalikOtoole20@gmail.com</t>
+  </si>
+  <si>
+    <t>AlanCaudill20</t>
+  </si>
+  <si>
+    <t>AlanCaudill20@gmail.com</t>
+  </si>
+  <si>
+    <t>AdanApplegate20</t>
+  </si>
+  <si>
+    <t>AdanApplegate20@gmail.com</t>
+  </si>
+  <si>
+    <t>AiyanaWhitworth20</t>
+  </si>
+  <si>
+    <t>AiyanaWhitworth20@gmail.com</t>
+  </si>
+  <si>
+    <t>MercedezBrien20</t>
+  </si>
+  <si>
+    <t>MercedezBrien20@gmail.com</t>
+  </si>
+  <si>
+    <t>DuaneHager20</t>
+  </si>
+  <si>
+    <t>DuaneHager20@gmail.com</t>
+  </si>
+  <si>
+    <t>LorenBell20</t>
+  </si>
+  <si>
+    <t>LorenBell20@gmail.com</t>
+  </si>
+  <si>
+    <t>GeraldHiller20</t>
+  </si>
+  <si>
+    <t>GeraldHiller20@gmail.com</t>
+  </si>
+  <si>
+    <t>DeionBranch20</t>
+  </si>
+  <si>
+    <t>DeionBranch20@gmail.com</t>
+  </si>
+  <si>
+    <t>DakotaHalstead20</t>
+  </si>
+  <si>
+    <t>DakotaHalstead20@gmail.com</t>
+  </si>
+  <si>
+    <t>ElliottFurman20</t>
+  </si>
+  <si>
+    <t>ElliottFurman20@gmail.com</t>
+  </si>
+  <si>
+    <t>MiltonCamp20</t>
+  </si>
+  <si>
+    <t>MiltonCamp20@gmail.com</t>
+  </si>
+  <si>
+    <t>DawnChester20</t>
+  </si>
+  <si>
+    <t>DawnChester20@gmail.com</t>
+  </si>
+  <si>
+    <t>ZacheryPetrie20</t>
+  </si>
+  <si>
+    <t>ZacheryPetrie20@gmail.com</t>
+  </si>
+  <si>
+    <t>EstebanAngel20</t>
+  </si>
+  <si>
+    <t>EstebanAngel20@gmail.com</t>
+  </si>
+  <si>
+    <t>JimmyBlankenship20</t>
+  </si>
+  <si>
+    <t>JimmyBlankenship20@gmail.com</t>
+  </si>
+  <si>
+    <t>AllysaGrice20</t>
+  </si>
+  <si>
+    <t>AllysaGrice20@gmail.com</t>
+  </si>
+  <si>
+    <t>AugustineYoo20</t>
+  </si>
+  <si>
+    <t>AugustineYoo20@gmail.com</t>
+  </si>
+  <si>
+    <t>BrandiSouthard20</t>
+  </si>
+  <si>
+    <t>BrandiSouthard20@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -4948,15 +4948,15 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="str">
         <f>CONCATENATE($G2,$I$2)</f>
-        <v>EthanBaker14</v>
+        <v>EthanBaker15</v>
       </c>
       <c r="B2" s="1" t="str">
         <f>CONCATENATE($G2,$I$2)</f>
-        <v>EthanBaker14</v>
+        <v>EthanBaker15</v>
       </c>
       <c r="C2" s="2" t="str">
         <f>CONCATENATE($G2,$I$2,$H$2)</f>
-        <v>EthanBaker14@gmail.com</v>
+        <v>EthanBaker15@gmail.com</v>
       </c>
       <c r="G2" t="s">
         <v>131</v>
@@ -4965,21 +4965,21 @@
         <v>71</v>
       </c>
       <c r="I2">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
         <f t="shared" ref="A3:B21" si="0">CONCATENATE($G3,$I$2)</f>
-        <v>DelanieCarman14</v>
+        <v>DelanieCarman15</v>
       </c>
       <c r="B3" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DelanieCarman14</v>
+        <v>DelanieCarman15</v>
       </c>
       <c r="C3" s="2" t="str">
         <f t="shared" ref="C3:C21" si="1">CONCATENATE($G3,$I$2,$H$2)</f>
-        <v>DelanieCarman14@gmail.com</v>
+        <v>DelanieCarman15@gmail.com</v>
       </c>
       <c r="G3" t="s">
         <v>132</v>
@@ -4988,15 +4988,15 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>BretAgnew14</v>
+        <v>BretAgnew15</v>
       </c>
       <c r="B4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>BretAgnew14</v>
+        <v>BretAgnew15</v>
       </c>
       <c r="C4" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>BretAgnew14@gmail.com</v>
+        <v>BretAgnew15@gmail.com</v>
       </c>
       <c r="G4" t="s">
         <v>133</v>
@@ -5005,15 +5005,15 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EdgardoTaylor14</v>
+        <v>EdgardoTaylor15</v>
       </c>
       <c r="B5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EdgardoTaylor14</v>
+        <v>EdgardoTaylor15</v>
       </c>
       <c r="C5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>EdgardoTaylor14@gmail.com</v>
+        <v>EdgardoTaylor15@gmail.com</v>
       </c>
       <c r="G5" t="s">
         <v>134</v>
@@ -5022,15 +5022,15 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TyrekReis14</v>
+        <v>TyrekReis15</v>
       </c>
       <c r="B6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TyrekReis14</v>
+        <v>TyrekReis15</v>
       </c>
       <c r="C6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>TyrekReis14@gmail.com</v>
+        <v>TyrekReis15@gmail.com</v>
       </c>
       <c r="G6" t="s">
         <v>135</v>
@@ -5039,15 +5039,15 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LeannaChow14</v>
+        <v>LeannaChow15</v>
       </c>
       <c r="B7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LeannaChow14</v>
+        <v>LeannaChow15</v>
       </c>
       <c r="C7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LeannaChow14@gmail.com</v>
+        <v>LeannaChow15@gmail.com</v>
       </c>
       <c r="G7" t="s">
         <v>136</v>
@@ -5056,15 +5056,15 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TuckerCarlson14</v>
+        <v>TuckerCarlson15</v>
       </c>
       <c r="B8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TuckerCarlson14</v>
+        <v>TuckerCarlson15</v>
       </c>
       <c r="C8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>TuckerCarlson14@gmail.com</v>
+        <v>TuckerCarlson15@gmail.com</v>
       </c>
       <c r="G8" t="s">
         <v>137</v>
@@ -5073,15 +5073,15 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AnnmarieConnor14</v>
+        <v>AnnmarieConnor15</v>
       </c>
       <c r="B9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AnnmarieConnor14</v>
+        <v>AnnmarieConnor15</v>
       </c>
       <c r="C9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>AnnmarieConnor14@gmail.com</v>
+        <v>AnnmarieConnor15@gmail.com</v>
       </c>
       <c r="G9" t="s">
         <v>138</v>
@@ -5090,15 +5090,15 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MoniqueWitte14</v>
+        <v>MoniqueWitte15</v>
       </c>
       <c r="B10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MoniqueWitte14</v>
+        <v>MoniqueWitte15</v>
       </c>
       <c r="C10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MoniqueWitte14@gmail.com</v>
+        <v>MoniqueWitte15@gmail.com</v>
       </c>
       <c r="G10" t="s">
         <v>139</v>
@@ -5107,15 +5107,15 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MikelWhitlock14</v>
+        <v>MikelWhitlock15</v>
       </c>
       <c r="B11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MikelWhitlock14</v>
+        <v>MikelWhitlock15</v>
       </c>
       <c r="C11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MikelWhitlock14@gmail.com</v>
+        <v>MikelWhitlock15@gmail.com</v>
       </c>
       <c r="G11" t="s">
         <v>140</v>
@@ -5124,15 +5124,15 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>VincentAmaya14</v>
+        <v>VincentAmaya15</v>
       </c>
       <c r="B12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>VincentAmaya14</v>
+        <v>VincentAmaya15</v>
       </c>
       <c r="C12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>VincentAmaya14@gmail.com</v>
+        <v>VincentAmaya15@gmail.com</v>
       </c>
       <c r="G12" t="s">
         <v>141</v>
@@ -5141,15 +5141,15 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>KeiraQuiroz14</v>
+        <v>KeiraQuiroz15</v>
       </c>
       <c r="B13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>KeiraQuiroz14</v>
+        <v>KeiraQuiroz15</v>
       </c>
       <c r="C13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>KeiraQuiroz14@gmail.com</v>
+        <v>KeiraQuiroz15@gmail.com</v>
       </c>
       <c r="G13" t="s">
         <v>142</v>
@@ -5158,15 +5158,15 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EllisCreech14</v>
+        <v>EllisCreech15</v>
       </c>
       <c r="B14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EllisCreech14</v>
+        <v>EllisCreech15</v>
       </c>
       <c r="C14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>EllisCreech14@gmail.com</v>
+        <v>EllisCreech15@gmail.com</v>
       </c>
       <c r="G14" t="s">
         <v>143</v>
@@ -5175,15 +5175,15 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DionteCreel14</v>
+        <v>DionteCreel15</v>
       </c>
       <c r="B15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DionteCreel14</v>
+        <v>DionteCreel15</v>
       </c>
       <c r="C15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DionteCreel14@gmail.com</v>
+        <v>DionteCreel15@gmail.com</v>
       </c>
       <c r="G15" t="s">
         <v>144</v>
@@ -5192,15 +5192,15 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NicholeFoust14</v>
+        <v>NicholeFoust15</v>
       </c>
       <c r="B16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NicholeFoust14</v>
+        <v>NicholeFoust15</v>
       </c>
       <c r="C16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>NicholeFoust14@gmail.com</v>
+        <v>NicholeFoust15@gmail.com</v>
       </c>
       <c r="G16" t="s">
         <v>145</v>
@@ -5209,15 +5209,15 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>ManuelConnell14</v>
+        <v>ManuelConnell15</v>
       </c>
       <c r="B17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>ManuelConnell14</v>
+        <v>ManuelConnell15</v>
       </c>
       <c r="C17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>ManuelConnell14@gmail.com</v>
+        <v>ManuelConnell15@gmail.com</v>
       </c>
       <c r="G17" t="s">
         <v>146</v>
@@ -5226,15 +5226,15 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LourdesElam14</v>
+        <v>LourdesElam15</v>
       </c>
       <c r="B18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LourdesElam14</v>
+        <v>LourdesElam15</v>
       </c>
       <c r="C18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LourdesElam14@gmail.com</v>
+        <v>LourdesElam15@gmail.com</v>
       </c>
       <c r="G18" t="s">
         <v>147</v>
@@ -5243,15 +5243,15 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LincolnFrederick14</v>
+        <v>LincolnFrederick15</v>
       </c>
       <c r="B19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LincolnFrederick14</v>
+        <v>LincolnFrederick15</v>
       </c>
       <c r="C19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LincolnFrederick14@gmail.com</v>
+        <v>LincolnFrederick15@gmail.com</v>
       </c>
       <c r="G19" t="s">
         <v>148</v>
@@ -5260,15 +5260,15 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AlisaCash14</v>
+        <v>AlisaCash15</v>
       </c>
       <c r="B20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AlisaCash14</v>
+        <v>AlisaCash15</v>
       </c>
       <c r="C20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>AlisaCash14@gmail.com</v>
+        <v>AlisaCash15@gmail.com</v>
       </c>
       <c r="G20" t="s">
         <v>149</v>
@@ -5277,15 +5277,15 @@
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LucilleGriffiths14</v>
+        <v>LucilleGriffiths15</v>
       </c>
       <c r="B21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LucilleGriffiths14</v>
+        <v>LucilleGriffiths15</v>
       </c>
       <c r="C21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LucilleGriffiths14@gmail.com</v>
+        <v>LucilleGriffiths15@gmail.com</v>
       </c>
       <c r="G21" t="s">
         <v>150</v>
@@ -5307,15 +5307,15 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="str">
         <f>CONCATENATE($G23,$I$23)</f>
-        <v>DonnellJernigan19</v>
+        <v>DonnellJernigan20</v>
       </c>
       <c r="B23" s="1" t="str">
         <f>CONCATENATE($G23,$I$23)</f>
-        <v>DonnellJernigan19</v>
+        <v>DonnellJernigan20</v>
       </c>
       <c r="C23" s="2" t="str">
         <f>CONCATENATE($G23,$I$23,$H$23)</f>
-        <v>DonnellJernigan19@gmail.com</v>
+        <v>DonnellJernigan20@gmail.com</v>
       </c>
       <c r="G23" s="24" t="s">
         <v>151</v>
@@ -5324,21 +5324,21 @@
         <v>71</v>
       </c>
       <c r="I23">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="str">
         <f t="shared" ref="A24:B42" si="2">CONCATENATE($G24,$I$23)</f>
-        <v>MalikOtoole19</v>
+        <v>MalikOtoole20</v>
       </c>
       <c r="B24" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MalikOtoole19</v>
+        <v>MalikOtoole20</v>
       </c>
       <c r="C24" s="2" t="str">
         <f t="shared" ref="C24:C42" si="3">CONCATENATE($G24,$I$23,$H$23)</f>
-        <v>MalikOtoole19@gmail.com</v>
+        <v>MalikOtoole20@gmail.com</v>
       </c>
       <c r="G24" t="s">
         <v>152</v>
@@ -5347,15 +5347,15 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AlanCaudill19</v>
+        <v>AlanCaudill20</v>
       </c>
       <c r="B25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AlanCaudill19</v>
+        <v>AlanCaudill20</v>
       </c>
       <c r="C25" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AlanCaudill19@gmail.com</v>
+        <v>AlanCaudill20@gmail.com</v>
       </c>
       <c r="G25" t="s">
         <v>153</v>
@@ -5364,15 +5364,15 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AdanApplegate19</v>
+        <v>AdanApplegate20</v>
       </c>
       <c r="B26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AdanApplegate19</v>
+        <v>AdanApplegate20</v>
       </c>
       <c r="C26" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AdanApplegate19@gmail.com</v>
+        <v>AdanApplegate20@gmail.com</v>
       </c>
       <c r="G26" t="s">
         <v>154</v>
@@ -5381,15 +5381,15 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AiyanaWhitworth19</v>
+        <v>AiyanaWhitworth20</v>
       </c>
       <c r="B27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AiyanaWhitworth19</v>
+        <v>AiyanaWhitworth20</v>
       </c>
       <c r="C27" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AiyanaWhitworth19@gmail.com</v>
+        <v>AiyanaWhitworth20@gmail.com</v>
       </c>
       <c r="G27" t="s">
         <v>155</v>
@@ -5398,15 +5398,15 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MercedezBrien19</v>
+        <v>MercedezBrien20</v>
       </c>
       <c r="B28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MercedezBrien19</v>
+        <v>MercedezBrien20</v>
       </c>
       <c r="C28" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>MercedezBrien19@gmail.com</v>
+        <v>MercedezBrien20@gmail.com</v>
       </c>
       <c r="G28" t="s">
         <v>156</v>
@@ -5415,15 +5415,15 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DuaneHager19</v>
+        <v>DuaneHager20</v>
       </c>
       <c r="B29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DuaneHager19</v>
+        <v>DuaneHager20</v>
       </c>
       <c r="C29" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DuaneHager19@gmail.com</v>
+        <v>DuaneHager20@gmail.com</v>
       </c>
       <c r="G29" t="s">
         <v>157</v>
@@ -5432,15 +5432,15 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>LorenBell19</v>
+        <v>LorenBell20</v>
       </c>
       <c r="B30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>LorenBell19</v>
+        <v>LorenBell20</v>
       </c>
       <c r="C30" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>LorenBell19@gmail.com</v>
+        <v>LorenBell20@gmail.com</v>
       </c>
       <c r="G30" t="s">
         <v>158</v>
@@ -5449,15 +5449,15 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>GeraldHiller19</v>
+        <v>GeraldHiller20</v>
       </c>
       <c r="B31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>GeraldHiller19</v>
+        <v>GeraldHiller20</v>
       </c>
       <c r="C31" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>GeraldHiller19@gmail.com</v>
+        <v>GeraldHiller20@gmail.com</v>
       </c>
       <c r="G31" t="s">
         <v>159</v>
@@ -5466,15 +5466,15 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DeionBranch19</v>
+        <v>DeionBranch20</v>
       </c>
       <c r="B32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DeionBranch19</v>
+        <v>DeionBranch20</v>
       </c>
       <c r="C32" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DeionBranch19@gmail.com</v>
+        <v>DeionBranch20@gmail.com</v>
       </c>
       <c r="G32" t="s">
         <v>160</v>
@@ -5483,15 +5483,15 @@
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DakotaHalstead19</v>
+        <v>DakotaHalstead20</v>
       </c>
       <c r="B33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DakotaHalstead19</v>
+        <v>DakotaHalstead20</v>
       </c>
       <c r="C33" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DakotaHalstead19@gmail.com</v>
+        <v>DakotaHalstead20@gmail.com</v>
       </c>
       <c r="G33" t="s">
         <v>161</v>
@@ -5500,15 +5500,15 @@
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ElliottFurman19</v>
+        <v>ElliottFurman20</v>
       </c>
       <c r="B34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ElliottFurman19</v>
+        <v>ElliottFurman20</v>
       </c>
       <c r="C34" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>ElliottFurman19@gmail.com</v>
+        <v>ElliottFurman20@gmail.com</v>
       </c>
       <c r="G34" t="s">
         <v>162</v>
@@ -5517,15 +5517,15 @@
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MiltonCamp19</v>
+        <v>MiltonCamp20</v>
       </c>
       <c r="B35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MiltonCamp19</v>
+        <v>MiltonCamp20</v>
       </c>
       <c r="C35" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>MiltonCamp19@gmail.com</v>
+        <v>MiltonCamp20@gmail.com</v>
       </c>
       <c r="G35" t="s">
         <v>163</v>
@@ -5534,15 +5534,15 @@
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DawnChester19</v>
+        <v>DawnChester20</v>
       </c>
       <c r="B36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DawnChester19</v>
+        <v>DawnChester20</v>
       </c>
       <c r="C36" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DawnChester19@gmail.com</v>
+        <v>DawnChester20@gmail.com</v>
       </c>
       <c r="G36" t="s">
         <v>164</v>
@@ -5551,15 +5551,15 @@
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ZacheryPetrie19</v>
+        <v>ZacheryPetrie20</v>
       </c>
       <c r="B37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ZacheryPetrie19</v>
+        <v>ZacheryPetrie20</v>
       </c>
       <c r="C37" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>ZacheryPetrie19@gmail.com</v>
+        <v>ZacheryPetrie20@gmail.com</v>
       </c>
       <c r="G37" t="s">
         <v>165</v>
@@ -5568,15 +5568,15 @@
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>EstebanAngel19</v>
+        <v>EstebanAngel20</v>
       </c>
       <c r="B38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>EstebanAngel19</v>
+        <v>EstebanAngel20</v>
       </c>
       <c r="C38" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>EstebanAngel19@gmail.com</v>
+        <v>EstebanAngel20@gmail.com</v>
       </c>
       <c r="G38" t="s">
         <v>166</v>
@@ -5585,15 +5585,15 @@
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>JimmyBlankenship19</v>
+        <v>JimmyBlankenship20</v>
       </c>
       <c r="B39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>JimmyBlankenship19</v>
+        <v>JimmyBlankenship20</v>
       </c>
       <c r="C39" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>JimmyBlankenship19@gmail.com</v>
+        <v>JimmyBlankenship20@gmail.com</v>
       </c>
       <c r="G39" t="s">
         <v>167</v>
@@ -5602,15 +5602,15 @@
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AllysaGrice19</v>
+        <v>AllysaGrice20</v>
       </c>
       <c r="B40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AllysaGrice19</v>
+        <v>AllysaGrice20</v>
       </c>
       <c r="C40" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AllysaGrice19@gmail.com</v>
+        <v>AllysaGrice20@gmail.com</v>
       </c>
       <c r="G40" t="s">
         <v>168</v>
@@ -5619,15 +5619,15 @@
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AugustineYoo19</v>
+        <v>AugustineYoo20</v>
       </c>
       <c r="B41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AugustineYoo19</v>
+        <v>AugustineYoo20</v>
       </c>
       <c r="C41" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AugustineYoo19@gmail.com</v>
+        <v>AugustineYoo20@gmail.com</v>
       </c>
       <c r="G41" t="s">
         <v>169</v>
@@ -5636,15 +5636,15 @@
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BrandiSouthard19</v>
+        <v>BrandiSouthard20</v>
       </c>
       <c r="B42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BrandiSouthard19</v>
+        <v>BrandiSouthard20</v>
       </c>
       <c r="C42" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>BrandiSouthard19@gmail.com</v>
+        <v>BrandiSouthard20@gmail.com</v>
       </c>
       <c r="G42" t="s">
         <v>170</v>

</xml_diff>

<commit_message>
updated maven-surefire-plugin pom file
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/Test_Data.xlsx
+++ b/src/main/resources/test_data/Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verkh\IdeaProjects\pom6\src\main\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677FFA95-6AF8-4996-905A-2E11BAEC6516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5D64B9-B437-443A-AE31-3130F9217AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1500" windowWidth="23040" windowHeight="12180" tabRatio="594" activeTab="1" xr2:uid="{56D596F5-221D-421D-9FC5-55182B639D44}"/>
   </bookViews>
@@ -1048,244 +1048,244 @@
     <t>3</t>
   </si>
   <si>
-    <t>EthanBaker15</t>
-  </si>
-  <si>
-    <t>EthanBaker15@gmail.com</t>
-  </si>
-  <si>
-    <t>DelanieCarman15</t>
-  </si>
-  <si>
-    <t>DelanieCarman15@gmail.com</t>
-  </si>
-  <si>
-    <t>BretAgnew15</t>
-  </si>
-  <si>
-    <t>BretAgnew15@gmail.com</t>
-  </si>
-  <si>
-    <t>EdgardoTaylor15</t>
-  </si>
-  <si>
-    <t>EdgardoTaylor15@gmail.com</t>
-  </si>
-  <si>
-    <t>TyrekReis15</t>
-  </si>
-  <si>
-    <t>TyrekReis15@gmail.com</t>
-  </si>
-  <si>
-    <t>LeannaChow15</t>
-  </si>
-  <si>
-    <t>LeannaChow15@gmail.com</t>
-  </si>
-  <si>
-    <t>TuckerCarlson15</t>
-  </si>
-  <si>
-    <t>TuckerCarlson15@gmail.com</t>
-  </si>
-  <si>
-    <t>AnnmarieConnor15</t>
-  </si>
-  <si>
-    <t>AnnmarieConnor15@gmail.com</t>
-  </si>
-  <si>
-    <t>MoniqueWitte15</t>
-  </si>
-  <si>
-    <t>MoniqueWitte15@gmail.com</t>
-  </si>
-  <si>
-    <t>MikelWhitlock15</t>
-  </si>
-  <si>
-    <t>MikelWhitlock15@gmail.com</t>
-  </si>
-  <si>
-    <t>VincentAmaya15</t>
-  </si>
-  <si>
-    <t>VincentAmaya15@gmail.com</t>
-  </si>
-  <si>
-    <t>KeiraQuiroz15</t>
-  </si>
-  <si>
-    <t>KeiraQuiroz15@gmail.com</t>
-  </si>
-  <si>
-    <t>EllisCreech15</t>
-  </si>
-  <si>
-    <t>EllisCreech15@gmail.com</t>
-  </si>
-  <si>
-    <t>DionteCreel15</t>
-  </si>
-  <si>
-    <t>DionteCreel15@gmail.com</t>
-  </si>
-  <si>
-    <t>NicholeFoust15</t>
-  </si>
-  <si>
-    <t>NicholeFoust15@gmail.com</t>
-  </si>
-  <si>
-    <t>ManuelConnell15</t>
-  </si>
-  <si>
-    <t>ManuelConnell15@gmail.com</t>
-  </si>
-  <si>
-    <t>LourdesElam15</t>
-  </si>
-  <si>
-    <t>LourdesElam15@gmail.com</t>
-  </si>
-  <si>
-    <t>LincolnFrederick15</t>
-  </si>
-  <si>
-    <t>LincolnFrederick15@gmail.com</t>
-  </si>
-  <si>
-    <t>AlisaCash15</t>
-  </si>
-  <si>
-    <t>AlisaCash15@gmail.com</t>
-  </si>
-  <si>
-    <t>LucilleGriffiths15</t>
-  </si>
-  <si>
-    <t>LucilleGriffiths15@gmail.com</t>
-  </si>
-  <si>
-    <t>DonnellJernigan20</t>
-  </si>
-  <si>
-    <t>DonnellJernigan20@gmail.com</t>
-  </si>
-  <si>
-    <t>MalikOtoole20</t>
-  </si>
-  <si>
-    <t>MalikOtoole20@gmail.com</t>
-  </si>
-  <si>
-    <t>AlanCaudill20</t>
-  </si>
-  <si>
-    <t>AlanCaudill20@gmail.com</t>
-  </si>
-  <si>
-    <t>AdanApplegate20</t>
-  </si>
-  <si>
-    <t>AdanApplegate20@gmail.com</t>
-  </si>
-  <si>
-    <t>AiyanaWhitworth20</t>
-  </si>
-  <si>
-    <t>AiyanaWhitworth20@gmail.com</t>
-  </si>
-  <si>
-    <t>MercedezBrien20</t>
-  </si>
-  <si>
-    <t>MercedezBrien20@gmail.com</t>
-  </si>
-  <si>
-    <t>DuaneHager20</t>
-  </si>
-  <si>
-    <t>DuaneHager20@gmail.com</t>
-  </si>
-  <si>
-    <t>LorenBell20</t>
-  </si>
-  <si>
-    <t>LorenBell20@gmail.com</t>
-  </si>
-  <si>
-    <t>GeraldHiller20</t>
-  </si>
-  <si>
-    <t>GeraldHiller20@gmail.com</t>
-  </si>
-  <si>
-    <t>DeionBranch20</t>
-  </si>
-  <si>
-    <t>DeionBranch20@gmail.com</t>
-  </si>
-  <si>
-    <t>DakotaHalstead20</t>
-  </si>
-  <si>
-    <t>DakotaHalstead20@gmail.com</t>
-  </si>
-  <si>
-    <t>ElliottFurman20</t>
-  </si>
-  <si>
-    <t>ElliottFurman20@gmail.com</t>
-  </si>
-  <si>
-    <t>MiltonCamp20</t>
-  </si>
-  <si>
-    <t>MiltonCamp20@gmail.com</t>
-  </si>
-  <si>
-    <t>DawnChester20</t>
-  </si>
-  <si>
-    <t>DawnChester20@gmail.com</t>
-  </si>
-  <si>
-    <t>ZacheryPetrie20</t>
-  </si>
-  <si>
-    <t>ZacheryPetrie20@gmail.com</t>
-  </si>
-  <si>
-    <t>EstebanAngel20</t>
-  </si>
-  <si>
-    <t>EstebanAngel20@gmail.com</t>
-  </si>
-  <si>
-    <t>JimmyBlankenship20</t>
-  </si>
-  <si>
-    <t>JimmyBlankenship20@gmail.com</t>
-  </si>
-  <si>
-    <t>AllysaGrice20</t>
-  </si>
-  <si>
-    <t>AllysaGrice20@gmail.com</t>
-  </si>
-  <si>
-    <t>AugustineYoo20</t>
-  </si>
-  <si>
-    <t>AugustineYoo20@gmail.com</t>
-  </si>
-  <si>
-    <t>BrandiSouthard20</t>
-  </si>
-  <si>
-    <t>BrandiSouthard20@gmail.com</t>
+    <t>EthanBaker16</t>
+  </si>
+  <si>
+    <t>EthanBaker16@gmail.com</t>
+  </si>
+  <si>
+    <t>DelanieCarman16</t>
+  </si>
+  <si>
+    <t>DelanieCarman16@gmail.com</t>
+  </si>
+  <si>
+    <t>BretAgnew16</t>
+  </si>
+  <si>
+    <t>BretAgnew16@gmail.com</t>
+  </si>
+  <si>
+    <t>EdgardoTaylor16</t>
+  </si>
+  <si>
+    <t>EdgardoTaylor16@gmail.com</t>
+  </si>
+  <si>
+    <t>TyrekReis16</t>
+  </si>
+  <si>
+    <t>TyrekReis16@gmail.com</t>
+  </si>
+  <si>
+    <t>LeannaChow16</t>
+  </si>
+  <si>
+    <t>LeannaChow16@gmail.com</t>
+  </si>
+  <si>
+    <t>TuckerCarlson16</t>
+  </si>
+  <si>
+    <t>TuckerCarlson16@gmail.com</t>
+  </si>
+  <si>
+    <t>AnnmarieConnor16</t>
+  </si>
+  <si>
+    <t>AnnmarieConnor16@gmail.com</t>
+  </si>
+  <si>
+    <t>MoniqueWitte16</t>
+  </si>
+  <si>
+    <t>MoniqueWitte16@gmail.com</t>
+  </si>
+  <si>
+    <t>MikelWhitlock16</t>
+  </si>
+  <si>
+    <t>MikelWhitlock16@gmail.com</t>
+  </si>
+  <si>
+    <t>VincentAmaya16</t>
+  </si>
+  <si>
+    <t>VincentAmaya16@gmail.com</t>
+  </si>
+  <si>
+    <t>KeiraQuiroz16</t>
+  </si>
+  <si>
+    <t>KeiraQuiroz16@gmail.com</t>
+  </si>
+  <si>
+    <t>EllisCreech16</t>
+  </si>
+  <si>
+    <t>EllisCreech16@gmail.com</t>
+  </si>
+  <si>
+    <t>DionteCreel16</t>
+  </si>
+  <si>
+    <t>DionteCreel16@gmail.com</t>
+  </si>
+  <si>
+    <t>NicholeFoust16</t>
+  </si>
+  <si>
+    <t>NicholeFoust16@gmail.com</t>
+  </si>
+  <si>
+    <t>ManuelConnell16</t>
+  </si>
+  <si>
+    <t>ManuelConnell16@gmail.com</t>
+  </si>
+  <si>
+    <t>LourdesElam16</t>
+  </si>
+  <si>
+    <t>LourdesElam16@gmail.com</t>
+  </si>
+  <si>
+    <t>LincolnFrederick16</t>
+  </si>
+  <si>
+    <t>LincolnFrederick16@gmail.com</t>
+  </si>
+  <si>
+    <t>AlisaCash16</t>
+  </si>
+  <si>
+    <t>AlisaCash16@gmail.com</t>
+  </si>
+  <si>
+    <t>LucilleGriffiths16</t>
+  </si>
+  <si>
+    <t>LucilleGriffiths16@gmail.com</t>
+  </si>
+  <si>
+    <t>DonnellJernigan21</t>
+  </si>
+  <si>
+    <t>DonnellJernigan21@gmail.com</t>
+  </si>
+  <si>
+    <t>MalikOtoole21</t>
+  </si>
+  <si>
+    <t>MalikOtoole21@gmail.com</t>
+  </si>
+  <si>
+    <t>AlanCaudill21</t>
+  </si>
+  <si>
+    <t>AlanCaudill21@gmail.com</t>
+  </si>
+  <si>
+    <t>AdanApplegate21</t>
+  </si>
+  <si>
+    <t>AdanApplegate21@gmail.com</t>
+  </si>
+  <si>
+    <t>AiyanaWhitworth21</t>
+  </si>
+  <si>
+    <t>AiyanaWhitworth21@gmail.com</t>
+  </si>
+  <si>
+    <t>MercedezBrien21</t>
+  </si>
+  <si>
+    <t>MercedezBrien21@gmail.com</t>
+  </si>
+  <si>
+    <t>DuaneHager21</t>
+  </si>
+  <si>
+    <t>DuaneHager21@gmail.com</t>
+  </si>
+  <si>
+    <t>LorenBell21</t>
+  </si>
+  <si>
+    <t>LorenBell21@gmail.com</t>
+  </si>
+  <si>
+    <t>GeraldHiller21</t>
+  </si>
+  <si>
+    <t>GeraldHiller21@gmail.com</t>
+  </si>
+  <si>
+    <t>DeionBranch21</t>
+  </si>
+  <si>
+    <t>DeionBranch21@gmail.com</t>
+  </si>
+  <si>
+    <t>DakotaHalstead21</t>
+  </si>
+  <si>
+    <t>DakotaHalstead21@gmail.com</t>
+  </si>
+  <si>
+    <t>ElliottFurman21</t>
+  </si>
+  <si>
+    <t>ElliottFurman21@gmail.com</t>
+  </si>
+  <si>
+    <t>MiltonCamp21</t>
+  </si>
+  <si>
+    <t>MiltonCamp21@gmail.com</t>
+  </si>
+  <si>
+    <t>DawnChester21</t>
+  </si>
+  <si>
+    <t>DawnChester21@gmail.com</t>
+  </si>
+  <si>
+    <t>ZacheryPetrie21</t>
+  </si>
+  <si>
+    <t>ZacheryPetrie21@gmail.com</t>
+  </si>
+  <si>
+    <t>EstebanAngel21</t>
+  </si>
+  <si>
+    <t>EstebanAngel21@gmail.com</t>
+  </si>
+  <si>
+    <t>JimmyBlankenship21</t>
+  </si>
+  <si>
+    <t>JimmyBlankenship21@gmail.com</t>
+  </si>
+  <si>
+    <t>AllysaGrice21</t>
+  </si>
+  <si>
+    <t>AllysaGrice21@gmail.com</t>
+  </si>
+  <si>
+    <t>AugustineYoo21</t>
+  </si>
+  <si>
+    <t>AugustineYoo21@gmail.com</t>
+  </si>
+  <si>
+    <t>BrandiSouthard21</t>
+  </si>
+  <si>
+    <t>BrandiSouthard21@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -4919,7 +4919,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FABAB06A-EAA7-4BA7-8A4C-8C5EF7E0517A}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="A23" sqref="A23:C42"/>
     </sheetView>
   </sheetViews>
@@ -4948,15 +4948,15 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="str">
         <f>CONCATENATE($G2,$I$2)</f>
-        <v>EthanBaker15</v>
+        <v>EthanBaker16</v>
       </c>
       <c r="B2" s="1" t="str">
         <f>CONCATENATE($G2,$I$2)</f>
-        <v>EthanBaker15</v>
+        <v>EthanBaker16</v>
       </c>
       <c r="C2" s="2" t="str">
         <f>CONCATENATE($G2,$I$2,$H$2)</f>
-        <v>EthanBaker15@gmail.com</v>
+        <v>EthanBaker16@gmail.com</v>
       </c>
       <c r="G2" t="s">
         <v>131</v>
@@ -4965,21 +4965,21 @@
         <v>71</v>
       </c>
       <c r="I2">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
         <f t="shared" ref="A3:B21" si="0">CONCATENATE($G3,$I$2)</f>
-        <v>DelanieCarman15</v>
+        <v>DelanieCarman16</v>
       </c>
       <c r="B3" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DelanieCarman15</v>
+        <v>DelanieCarman16</v>
       </c>
       <c r="C3" s="2" t="str">
         <f t="shared" ref="C3:C21" si="1">CONCATENATE($G3,$I$2,$H$2)</f>
-        <v>DelanieCarman15@gmail.com</v>
+        <v>DelanieCarman16@gmail.com</v>
       </c>
       <c r="G3" t="s">
         <v>132</v>
@@ -4988,15 +4988,15 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>BretAgnew15</v>
+        <v>BretAgnew16</v>
       </c>
       <c r="B4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>BretAgnew15</v>
+        <v>BretAgnew16</v>
       </c>
       <c r="C4" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>BretAgnew15@gmail.com</v>
+        <v>BretAgnew16@gmail.com</v>
       </c>
       <c r="G4" t="s">
         <v>133</v>
@@ -5005,15 +5005,15 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EdgardoTaylor15</v>
+        <v>EdgardoTaylor16</v>
       </c>
       <c r="B5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EdgardoTaylor15</v>
+        <v>EdgardoTaylor16</v>
       </c>
       <c r="C5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>EdgardoTaylor15@gmail.com</v>
+        <v>EdgardoTaylor16@gmail.com</v>
       </c>
       <c r="G5" t="s">
         <v>134</v>
@@ -5022,15 +5022,15 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TyrekReis15</v>
+        <v>TyrekReis16</v>
       </c>
       <c r="B6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TyrekReis15</v>
+        <v>TyrekReis16</v>
       </c>
       <c r="C6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>TyrekReis15@gmail.com</v>
+        <v>TyrekReis16@gmail.com</v>
       </c>
       <c r="G6" t="s">
         <v>135</v>
@@ -5039,15 +5039,15 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LeannaChow15</v>
+        <v>LeannaChow16</v>
       </c>
       <c r="B7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LeannaChow15</v>
+        <v>LeannaChow16</v>
       </c>
       <c r="C7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LeannaChow15@gmail.com</v>
+        <v>LeannaChow16@gmail.com</v>
       </c>
       <c r="G7" t="s">
         <v>136</v>
@@ -5056,15 +5056,15 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TuckerCarlson15</v>
+        <v>TuckerCarlson16</v>
       </c>
       <c r="B8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TuckerCarlson15</v>
+        <v>TuckerCarlson16</v>
       </c>
       <c r="C8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>TuckerCarlson15@gmail.com</v>
+        <v>TuckerCarlson16@gmail.com</v>
       </c>
       <c r="G8" t="s">
         <v>137</v>
@@ -5073,15 +5073,15 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AnnmarieConnor15</v>
+        <v>AnnmarieConnor16</v>
       </c>
       <c r="B9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AnnmarieConnor15</v>
+        <v>AnnmarieConnor16</v>
       </c>
       <c r="C9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>AnnmarieConnor15@gmail.com</v>
+        <v>AnnmarieConnor16@gmail.com</v>
       </c>
       <c r="G9" t="s">
         <v>138</v>
@@ -5090,15 +5090,15 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MoniqueWitte15</v>
+        <v>MoniqueWitte16</v>
       </c>
       <c r="B10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MoniqueWitte15</v>
+        <v>MoniqueWitte16</v>
       </c>
       <c r="C10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MoniqueWitte15@gmail.com</v>
+        <v>MoniqueWitte16@gmail.com</v>
       </c>
       <c r="G10" t="s">
         <v>139</v>
@@ -5107,15 +5107,15 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MikelWhitlock15</v>
+        <v>MikelWhitlock16</v>
       </c>
       <c r="B11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MikelWhitlock15</v>
+        <v>MikelWhitlock16</v>
       </c>
       <c r="C11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MikelWhitlock15@gmail.com</v>
+        <v>MikelWhitlock16@gmail.com</v>
       </c>
       <c r="G11" t="s">
         <v>140</v>
@@ -5124,15 +5124,15 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>VincentAmaya15</v>
+        <v>VincentAmaya16</v>
       </c>
       <c r="B12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>VincentAmaya15</v>
+        <v>VincentAmaya16</v>
       </c>
       <c r="C12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>VincentAmaya15@gmail.com</v>
+        <v>VincentAmaya16@gmail.com</v>
       </c>
       <c r="G12" t="s">
         <v>141</v>
@@ -5141,15 +5141,15 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>KeiraQuiroz15</v>
+        <v>KeiraQuiroz16</v>
       </c>
       <c r="B13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>KeiraQuiroz15</v>
+        <v>KeiraQuiroz16</v>
       </c>
       <c r="C13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>KeiraQuiroz15@gmail.com</v>
+        <v>KeiraQuiroz16@gmail.com</v>
       </c>
       <c r="G13" t="s">
         <v>142</v>
@@ -5158,15 +5158,15 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EllisCreech15</v>
+        <v>EllisCreech16</v>
       </c>
       <c r="B14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EllisCreech15</v>
+        <v>EllisCreech16</v>
       </c>
       <c r="C14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>EllisCreech15@gmail.com</v>
+        <v>EllisCreech16@gmail.com</v>
       </c>
       <c r="G14" t="s">
         <v>143</v>
@@ -5175,15 +5175,15 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DionteCreel15</v>
+        <v>DionteCreel16</v>
       </c>
       <c r="B15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DionteCreel15</v>
+        <v>DionteCreel16</v>
       </c>
       <c r="C15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DionteCreel15@gmail.com</v>
+        <v>DionteCreel16@gmail.com</v>
       </c>
       <c r="G15" t="s">
         <v>144</v>
@@ -5192,15 +5192,15 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NicholeFoust15</v>
+        <v>NicholeFoust16</v>
       </c>
       <c r="B16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NicholeFoust15</v>
+        <v>NicholeFoust16</v>
       </c>
       <c r="C16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>NicholeFoust15@gmail.com</v>
+        <v>NicholeFoust16@gmail.com</v>
       </c>
       <c r="G16" t="s">
         <v>145</v>
@@ -5209,15 +5209,15 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>ManuelConnell15</v>
+        <v>ManuelConnell16</v>
       </c>
       <c r="B17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>ManuelConnell15</v>
+        <v>ManuelConnell16</v>
       </c>
       <c r="C17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>ManuelConnell15@gmail.com</v>
+        <v>ManuelConnell16@gmail.com</v>
       </c>
       <c r="G17" t="s">
         <v>146</v>
@@ -5226,15 +5226,15 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LourdesElam15</v>
+        <v>LourdesElam16</v>
       </c>
       <c r="B18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LourdesElam15</v>
+        <v>LourdesElam16</v>
       </c>
       <c r="C18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LourdesElam15@gmail.com</v>
+        <v>LourdesElam16@gmail.com</v>
       </c>
       <c r="G18" t="s">
         <v>147</v>
@@ -5243,15 +5243,15 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LincolnFrederick15</v>
+        <v>LincolnFrederick16</v>
       </c>
       <c r="B19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LincolnFrederick15</v>
+        <v>LincolnFrederick16</v>
       </c>
       <c r="C19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LincolnFrederick15@gmail.com</v>
+        <v>LincolnFrederick16@gmail.com</v>
       </c>
       <c r="G19" t="s">
         <v>148</v>
@@ -5260,15 +5260,15 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AlisaCash15</v>
+        <v>AlisaCash16</v>
       </c>
       <c r="B20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AlisaCash15</v>
+        <v>AlisaCash16</v>
       </c>
       <c r="C20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>AlisaCash15@gmail.com</v>
+        <v>AlisaCash16@gmail.com</v>
       </c>
       <c r="G20" t="s">
         <v>149</v>
@@ -5277,15 +5277,15 @@
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LucilleGriffiths15</v>
+        <v>LucilleGriffiths16</v>
       </c>
       <c r="B21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LucilleGriffiths15</v>
+        <v>LucilleGriffiths16</v>
       </c>
       <c r="C21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LucilleGriffiths15@gmail.com</v>
+        <v>LucilleGriffiths16@gmail.com</v>
       </c>
       <c r="G21" t="s">
         <v>150</v>
@@ -5307,15 +5307,15 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="str">
         <f>CONCATENATE($G23,$I$23)</f>
-        <v>DonnellJernigan20</v>
+        <v>DonnellJernigan21</v>
       </c>
       <c r="B23" s="1" t="str">
         <f>CONCATENATE($G23,$I$23)</f>
-        <v>DonnellJernigan20</v>
+        <v>DonnellJernigan21</v>
       </c>
       <c r="C23" s="2" t="str">
         <f>CONCATENATE($G23,$I$23,$H$23)</f>
-        <v>DonnellJernigan20@gmail.com</v>
+        <v>DonnellJernigan21@gmail.com</v>
       </c>
       <c r="G23" s="24" t="s">
         <v>151</v>
@@ -5324,21 +5324,21 @@
         <v>71</v>
       </c>
       <c r="I23">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="str">
         <f t="shared" ref="A24:B42" si="2">CONCATENATE($G24,$I$23)</f>
-        <v>MalikOtoole20</v>
+        <v>MalikOtoole21</v>
       </c>
       <c r="B24" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MalikOtoole20</v>
+        <v>MalikOtoole21</v>
       </c>
       <c r="C24" s="2" t="str">
         <f t="shared" ref="C24:C42" si="3">CONCATENATE($G24,$I$23,$H$23)</f>
-        <v>MalikOtoole20@gmail.com</v>
+        <v>MalikOtoole21@gmail.com</v>
       </c>
       <c r="G24" t="s">
         <v>152</v>
@@ -5347,15 +5347,15 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AlanCaudill20</v>
+        <v>AlanCaudill21</v>
       </c>
       <c r="B25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AlanCaudill20</v>
+        <v>AlanCaudill21</v>
       </c>
       <c r="C25" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AlanCaudill20@gmail.com</v>
+        <v>AlanCaudill21@gmail.com</v>
       </c>
       <c r="G25" t="s">
         <v>153</v>
@@ -5364,15 +5364,15 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AdanApplegate20</v>
+        <v>AdanApplegate21</v>
       </c>
       <c r="B26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AdanApplegate20</v>
+        <v>AdanApplegate21</v>
       </c>
       <c r="C26" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AdanApplegate20@gmail.com</v>
+        <v>AdanApplegate21@gmail.com</v>
       </c>
       <c r="G26" t="s">
         <v>154</v>
@@ -5381,15 +5381,15 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AiyanaWhitworth20</v>
+        <v>AiyanaWhitworth21</v>
       </c>
       <c r="B27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AiyanaWhitworth20</v>
+        <v>AiyanaWhitworth21</v>
       </c>
       <c r="C27" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AiyanaWhitworth20@gmail.com</v>
+        <v>AiyanaWhitworth21@gmail.com</v>
       </c>
       <c r="G27" t="s">
         <v>155</v>
@@ -5398,15 +5398,15 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MercedezBrien20</v>
+        <v>MercedezBrien21</v>
       </c>
       <c r="B28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MercedezBrien20</v>
+        <v>MercedezBrien21</v>
       </c>
       <c r="C28" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>MercedezBrien20@gmail.com</v>
+        <v>MercedezBrien21@gmail.com</v>
       </c>
       <c r="G28" t="s">
         <v>156</v>
@@ -5415,15 +5415,15 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DuaneHager20</v>
+        <v>DuaneHager21</v>
       </c>
       <c r="B29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DuaneHager20</v>
+        <v>DuaneHager21</v>
       </c>
       <c r="C29" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DuaneHager20@gmail.com</v>
+        <v>DuaneHager21@gmail.com</v>
       </c>
       <c r="G29" t="s">
         <v>157</v>
@@ -5432,15 +5432,15 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>LorenBell20</v>
+        <v>LorenBell21</v>
       </c>
       <c r="B30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>LorenBell20</v>
+        <v>LorenBell21</v>
       </c>
       <c r="C30" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>LorenBell20@gmail.com</v>
+        <v>LorenBell21@gmail.com</v>
       </c>
       <c r="G30" t="s">
         <v>158</v>
@@ -5449,15 +5449,15 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>GeraldHiller20</v>
+        <v>GeraldHiller21</v>
       </c>
       <c r="B31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>GeraldHiller20</v>
+        <v>GeraldHiller21</v>
       </c>
       <c r="C31" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>GeraldHiller20@gmail.com</v>
+        <v>GeraldHiller21@gmail.com</v>
       </c>
       <c r="G31" t="s">
         <v>159</v>
@@ -5466,15 +5466,15 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DeionBranch20</v>
+        <v>DeionBranch21</v>
       </c>
       <c r="B32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DeionBranch20</v>
+        <v>DeionBranch21</v>
       </c>
       <c r="C32" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DeionBranch20@gmail.com</v>
+        <v>DeionBranch21@gmail.com</v>
       </c>
       <c r="G32" t="s">
         <v>160</v>
@@ -5483,15 +5483,15 @@
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DakotaHalstead20</v>
+        <v>DakotaHalstead21</v>
       </c>
       <c r="B33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DakotaHalstead20</v>
+        <v>DakotaHalstead21</v>
       </c>
       <c r="C33" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DakotaHalstead20@gmail.com</v>
+        <v>DakotaHalstead21@gmail.com</v>
       </c>
       <c r="G33" t="s">
         <v>161</v>
@@ -5500,15 +5500,15 @@
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ElliottFurman20</v>
+        <v>ElliottFurman21</v>
       </c>
       <c r="B34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ElliottFurman20</v>
+        <v>ElliottFurman21</v>
       </c>
       <c r="C34" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>ElliottFurman20@gmail.com</v>
+        <v>ElliottFurman21@gmail.com</v>
       </c>
       <c r="G34" t="s">
         <v>162</v>
@@ -5517,15 +5517,15 @@
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MiltonCamp20</v>
+        <v>MiltonCamp21</v>
       </c>
       <c r="B35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MiltonCamp20</v>
+        <v>MiltonCamp21</v>
       </c>
       <c r="C35" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>MiltonCamp20@gmail.com</v>
+        <v>MiltonCamp21@gmail.com</v>
       </c>
       <c r="G35" t="s">
         <v>163</v>
@@ -5534,15 +5534,15 @@
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DawnChester20</v>
+        <v>DawnChester21</v>
       </c>
       <c r="B36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DawnChester20</v>
+        <v>DawnChester21</v>
       </c>
       <c r="C36" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DawnChester20@gmail.com</v>
+        <v>DawnChester21@gmail.com</v>
       </c>
       <c r="G36" t="s">
         <v>164</v>
@@ -5551,15 +5551,15 @@
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ZacheryPetrie20</v>
+        <v>ZacheryPetrie21</v>
       </c>
       <c r="B37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ZacheryPetrie20</v>
+        <v>ZacheryPetrie21</v>
       </c>
       <c r="C37" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>ZacheryPetrie20@gmail.com</v>
+        <v>ZacheryPetrie21@gmail.com</v>
       </c>
       <c r="G37" t="s">
         <v>165</v>
@@ -5568,15 +5568,15 @@
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>EstebanAngel20</v>
+        <v>EstebanAngel21</v>
       </c>
       <c r="B38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>EstebanAngel20</v>
+        <v>EstebanAngel21</v>
       </c>
       <c r="C38" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>EstebanAngel20@gmail.com</v>
+        <v>EstebanAngel21@gmail.com</v>
       </c>
       <c r="G38" t="s">
         <v>166</v>
@@ -5585,15 +5585,15 @@
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>JimmyBlankenship20</v>
+        <v>JimmyBlankenship21</v>
       </c>
       <c r="B39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>JimmyBlankenship20</v>
+        <v>JimmyBlankenship21</v>
       </c>
       <c r="C39" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>JimmyBlankenship20@gmail.com</v>
+        <v>JimmyBlankenship21@gmail.com</v>
       </c>
       <c r="G39" t="s">
         <v>167</v>
@@ -5602,15 +5602,15 @@
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AllysaGrice20</v>
+        <v>AllysaGrice21</v>
       </c>
       <c r="B40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AllysaGrice20</v>
+        <v>AllysaGrice21</v>
       </c>
       <c r="C40" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AllysaGrice20@gmail.com</v>
+        <v>AllysaGrice21@gmail.com</v>
       </c>
       <c r="G40" t="s">
         <v>168</v>
@@ -5619,15 +5619,15 @@
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AugustineYoo20</v>
+        <v>AugustineYoo21</v>
       </c>
       <c r="B41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AugustineYoo20</v>
+        <v>AugustineYoo21</v>
       </c>
       <c r="C41" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AugustineYoo20@gmail.com</v>
+        <v>AugustineYoo21@gmail.com</v>
       </c>
       <c r="G41" t="s">
         <v>169</v>
@@ -5636,15 +5636,15 @@
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BrandiSouthard20</v>
+        <v>BrandiSouthard21</v>
       </c>
       <c r="B42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BrandiSouthard20</v>
+        <v>BrandiSouthard21</v>
       </c>
       <c r="C42" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>BrandiSouthard20@gmail.com</v>
+        <v>BrandiSouthard21@gmail.com</v>
       </c>
       <c r="G42" t="s">
         <v>170</v>

</xml_diff>

<commit_message>
updated config, pom, data files
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/Test_Data.xlsx
+++ b/src/main/resources/test_data/Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verkh\IdeaProjects\pom6\src\main\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1851B68-B078-491E-AE11-AB54450305AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF61E4FE-12BF-4065-94D2-51EDE96F0B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1500" windowWidth="23040" windowHeight="12180" tabRatio="594" activeTab="1" xr2:uid="{56D596F5-221D-421D-9FC5-55182B639D44}"/>
   </bookViews>
@@ -1048,244 +1048,244 @@
     <t>3</t>
   </si>
   <si>
-    <t>EthanBaker17</t>
-  </si>
-  <si>
-    <t>EthanBaker17@gmail.com</t>
-  </si>
-  <si>
-    <t>DelanieCarman17</t>
-  </si>
-  <si>
-    <t>DelanieCarman17@gmail.com</t>
-  </si>
-  <si>
-    <t>BretAgnew17</t>
-  </si>
-  <si>
-    <t>BretAgnew17@gmail.com</t>
-  </si>
-  <si>
-    <t>EdgardoTaylor17</t>
-  </si>
-  <si>
-    <t>EdgardoTaylor17@gmail.com</t>
-  </si>
-  <si>
-    <t>TyrekReis17</t>
-  </si>
-  <si>
-    <t>TyrekReis17@gmail.com</t>
-  </si>
-  <si>
-    <t>LeannaChow17</t>
-  </si>
-  <si>
-    <t>LeannaChow17@gmail.com</t>
-  </si>
-  <si>
-    <t>TuckerCarlson17</t>
-  </si>
-  <si>
-    <t>TuckerCarlson17@gmail.com</t>
-  </si>
-  <si>
-    <t>AnnmarieConnor17</t>
-  </si>
-  <si>
-    <t>AnnmarieConnor17@gmail.com</t>
-  </si>
-  <si>
-    <t>MoniqueWitte17</t>
-  </si>
-  <si>
-    <t>MoniqueWitte17@gmail.com</t>
-  </si>
-  <si>
-    <t>MikelWhitlock17</t>
-  </si>
-  <si>
-    <t>MikelWhitlock17@gmail.com</t>
-  </si>
-  <si>
-    <t>VincentAmaya17</t>
-  </si>
-  <si>
-    <t>VincentAmaya17@gmail.com</t>
-  </si>
-  <si>
-    <t>KeiraQuiroz17</t>
-  </si>
-  <si>
-    <t>KeiraQuiroz17@gmail.com</t>
-  </si>
-  <si>
-    <t>EllisCreech17</t>
-  </si>
-  <si>
-    <t>EllisCreech17@gmail.com</t>
-  </si>
-  <si>
-    <t>DionteCreel17</t>
-  </si>
-  <si>
-    <t>DionteCreel17@gmail.com</t>
-  </si>
-  <si>
-    <t>NicholeFoust17</t>
-  </si>
-  <si>
-    <t>NicholeFoust17@gmail.com</t>
-  </si>
-  <si>
-    <t>ManuelConnell17</t>
-  </si>
-  <si>
-    <t>ManuelConnell17@gmail.com</t>
-  </si>
-  <si>
-    <t>LourdesElam17</t>
-  </si>
-  <si>
-    <t>LourdesElam17@gmail.com</t>
-  </si>
-  <si>
-    <t>LincolnFrederick17</t>
-  </si>
-  <si>
-    <t>LincolnFrederick17@gmail.com</t>
-  </si>
-  <si>
-    <t>AlisaCash17</t>
-  </si>
-  <si>
-    <t>AlisaCash17@gmail.com</t>
-  </si>
-  <si>
-    <t>LucilleGriffiths17</t>
-  </si>
-  <si>
-    <t>LucilleGriffiths17@gmail.com</t>
-  </si>
-  <si>
-    <t>DonnellJernigan22</t>
-  </si>
-  <si>
-    <t>DonnellJernigan22@gmail.com</t>
-  </si>
-  <si>
-    <t>MalikOtoole22</t>
-  </si>
-  <si>
-    <t>MalikOtoole22@gmail.com</t>
-  </si>
-  <si>
-    <t>AlanCaudill22</t>
-  </si>
-  <si>
-    <t>AlanCaudill22@gmail.com</t>
-  </si>
-  <si>
-    <t>AdanApplegate22</t>
-  </si>
-  <si>
-    <t>AdanApplegate22@gmail.com</t>
-  </si>
-  <si>
-    <t>AiyanaWhitworth22</t>
-  </si>
-  <si>
-    <t>AiyanaWhitworth22@gmail.com</t>
-  </si>
-  <si>
-    <t>MercedezBrien22</t>
-  </si>
-  <si>
-    <t>MercedezBrien22@gmail.com</t>
-  </si>
-  <si>
-    <t>DuaneHager22</t>
-  </si>
-  <si>
-    <t>DuaneHager22@gmail.com</t>
-  </si>
-  <si>
-    <t>LorenBell22</t>
-  </si>
-  <si>
-    <t>LorenBell22@gmail.com</t>
-  </si>
-  <si>
-    <t>GeraldHiller22</t>
-  </si>
-  <si>
-    <t>GeraldHiller22@gmail.com</t>
-  </si>
-  <si>
-    <t>DeionBranch22</t>
-  </si>
-  <si>
-    <t>DeionBranch22@gmail.com</t>
-  </si>
-  <si>
-    <t>DakotaHalstead22</t>
-  </si>
-  <si>
-    <t>DakotaHalstead22@gmail.com</t>
-  </si>
-  <si>
-    <t>ElliottFurman22</t>
-  </si>
-  <si>
-    <t>ElliottFurman22@gmail.com</t>
-  </si>
-  <si>
-    <t>MiltonCamp22</t>
-  </si>
-  <si>
-    <t>MiltonCamp22@gmail.com</t>
-  </si>
-  <si>
-    <t>DawnChester22</t>
-  </si>
-  <si>
-    <t>DawnChester22@gmail.com</t>
-  </si>
-  <si>
-    <t>ZacheryPetrie22</t>
-  </si>
-  <si>
-    <t>ZacheryPetrie22@gmail.com</t>
-  </si>
-  <si>
-    <t>EstebanAngel22</t>
-  </si>
-  <si>
-    <t>EstebanAngel22@gmail.com</t>
-  </si>
-  <si>
-    <t>JimmyBlankenship22</t>
-  </si>
-  <si>
-    <t>JimmyBlankenship22@gmail.com</t>
-  </si>
-  <si>
-    <t>AllysaGrice22</t>
-  </si>
-  <si>
-    <t>AllysaGrice22@gmail.com</t>
-  </si>
-  <si>
-    <t>AugustineYoo22</t>
-  </si>
-  <si>
-    <t>AugustineYoo22@gmail.com</t>
-  </si>
-  <si>
-    <t>BrandiSouthard22</t>
-  </si>
-  <si>
-    <t>BrandiSouthard22@gmail.com</t>
+    <t>EthanBaker18</t>
+  </si>
+  <si>
+    <t>EthanBaker18@gmail.com</t>
+  </si>
+  <si>
+    <t>DelanieCarman18</t>
+  </si>
+  <si>
+    <t>DelanieCarman18@gmail.com</t>
+  </si>
+  <si>
+    <t>BretAgnew18</t>
+  </si>
+  <si>
+    <t>BretAgnew18@gmail.com</t>
+  </si>
+  <si>
+    <t>EdgardoTaylor18</t>
+  </si>
+  <si>
+    <t>EdgardoTaylor18@gmail.com</t>
+  </si>
+  <si>
+    <t>TyrekReis18</t>
+  </si>
+  <si>
+    <t>TyrekReis18@gmail.com</t>
+  </si>
+  <si>
+    <t>LeannaChow18</t>
+  </si>
+  <si>
+    <t>LeannaChow18@gmail.com</t>
+  </si>
+  <si>
+    <t>TuckerCarlson18</t>
+  </si>
+  <si>
+    <t>TuckerCarlson18@gmail.com</t>
+  </si>
+  <si>
+    <t>AnnmarieConnor18</t>
+  </si>
+  <si>
+    <t>AnnmarieConnor18@gmail.com</t>
+  </si>
+  <si>
+    <t>MoniqueWitte18</t>
+  </si>
+  <si>
+    <t>MoniqueWitte18@gmail.com</t>
+  </si>
+  <si>
+    <t>MikelWhitlock18</t>
+  </si>
+  <si>
+    <t>MikelWhitlock18@gmail.com</t>
+  </si>
+  <si>
+    <t>VincentAmaya18</t>
+  </si>
+  <si>
+    <t>VincentAmaya18@gmail.com</t>
+  </si>
+  <si>
+    <t>KeiraQuiroz18</t>
+  </si>
+  <si>
+    <t>KeiraQuiroz18@gmail.com</t>
+  </si>
+  <si>
+    <t>EllisCreech18</t>
+  </si>
+  <si>
+    <t>EllisCreech18@gmail.com</t>
+  </si>
+  <si>
+    <t>DionteCreel18</t>
+  </si>
+  <si>
+    <t>DionteCreel18@gmail.com</t>
+  </si>
+  <si>
+    <t>NicholeFoust18</t>
+  </si>
+  <si>
+    <t>NicholeFoust18@gmail.com</t>
+  </si>
+  <si>
+    <t>ManuelConnell18</t>
+  </si>
+  <si>
+    <t>ManuelConnell18@gmail.com</t>
+  </si>
+  <si>
+    <t>LourdesElam18</t>
+  </si>
+  <si>
+    <t>LourdesElam18@gmail.com</t>
+  </si>
+  <si>
+    <t>LincolnFrederick18</t>
+  </si>
+  <si>
+    <t>LincolnFrederick18@gmail.com</t>
+  </si>
+  <si>
+    <t>AlisaCash18</t>
+  </si>
+  <si>
+    <t>AlisaCash18@gmail.com</t>
+  </si>
+  <si>
+    <t>LucilleGriffiths18</t>
+  </si>
+  <si>
+    <t>LucilleGriffiths18@gmail.com</t>
+  </si>
+  <si>
+    <t>DonnellJernigan23</t>
+  </si>
+  <si>
+    <t>DonnellJernigan23@gmail.com</t>
+  </si>
+  <si>
+    <t>MalikOtoole23</t>
+  </si>
+  <si>
+    <t>MalikOtoole23@gmail.com</t>
+  </si>
+  <si>
+    <t>AlanCaudill23</t>
+  </si>
+  <si>
+    <t>AlanCaudill23@gmail.com</t>
+  </si>
+  <si>
+    <t>AdanApplegate23</t>
+  </si>
+  <si>
+    <t>AdanApplegate23@gmail.com</t>
+  </si>
+  <si>
+    <t>AiyanaWhitworth23</t>
+  </si>
+  <si>
+    <t>AiyanaWhitworth23@gmail.com</t>
+  </si>
+  <si>
+    <t>MercedezBrien23</t>
+  </si>
+  <si>
+    <t>MercedezBrien23@gmail.com</t>
+  </si>
+  <si>
+    <t>DuaneHager23</t>
+  </si>
+  <si>
+    <t>DuaneHager23@gmail.com</t>
+  </si>
+  <si>
+    <t>LorenBell23</t>
+  </si>
+  <si>
+    <t>LorenBell23@gmail.com</t>
+  </si>
+  <si>
+    <t>GeraldHiller23</t>
+  </si>
+  <si>
+    <t>GeraldHiller23@gmail.com</t>
+  </si>
+  <si>
+    <t>DeionBranch23</t>
+  </si>
+  <si>
+    <t>DeionBranch23@gmail.com</t>
+  </si>
+  <si>
+    <t>DakotaHalstead23</t>
+  </si>
+  <si>
+    <t>DakotaHalstead23@gmail.com</t>
+  </si>
+  <si>
+    <t>ElliottFurman23</t>
+  </si>
+  <si>
+    <t>ElliottFurman23@gmail.com</t>
+  </si>
+  <si>
+    <t>MiltonCamp23</t>
+  </si>
+  <si>
+    <t>MiltonCamp23@gmail.com</t>
+  </si>
+  <si>
+    <t>DawnChester23</t>
+  </si>
+  <si>
+    <t>DawnChester23@gmail.com</t>
+  </si>
+  <si>
+    <t>ZacheryPetrie23</t>
+  </si>
+  <si>
+    <t>ZacheryPetrie23@gmail.com</t>
+  </si>
+  <si>
+    <t>EstebanAngel23</t>
+  </si>
+  <si>
+    <t>EstebanAngel23@gmail.com</t>
+  </si>
+  <si>
+    <t>JimmyBlankenship23</t>
+  </si>
+  <si>
+    <t>JimmyBlankenship23@gmail.com</t>
+  </si>
+  <si>
+    <t>AllysaGrice23</t>
+  </si>
+  <si>
+    <t>AllysaGrice23@gmail.com</t>
+  </si>
+  <si>
+    <t>AugustineYoo23</t>
+  </si>
+  <si>
+    <t>AugustineYoo23@gmail.com</t>
+  </si>
+  <si>
+    <t>BrandiSouthard23</t>
+  </si>
+  <si>
+    <t>BrandiSouthard23@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -4919,7 +4919,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FABAB06A-EAA7-4BA7-8A4C-8C5EF7E0517A}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="A23" sqref="A23:C42"/>
     </sheetView>
   </sheetViews>
@@ -4948,15 +4948,15 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="str">
         <f>CONCATENATE($G2,$I$2)</f>
-        <v>EthanBaker17</v>
+        <v>EthanBaker18</v>
       </c>
       <c r="B2" s="1" t="str">
         <f>CONCATENATE($G2,$I$2)</f>
-        <v>EthanBaker17</v>
+        <v>EthanBaker18</v>
       </c>
       <c r="C2" s="2" t="str">
         <f>CONCATENATE($G2,$I$2,$H$2)</f>
-        <v>EthanBaker17@gmail.com</v>
+        <v>EthanBaker18@gmail.com</v>
       </c>
       <c r="G2" t="s">
         <v>131</v>
@@ -4965,21 +4965,21 @@
         <v>71</v>
       </c>
       <c r="I2">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
         <f t="shared" ref="A3:B21" si="0">CONCATENATE($G3,$I$2)</f>
-        <v>DelanieCarman17</v>
+        <v>DelanieCarman18</v>
       </c>
       <c r="B3" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DelanieCarman17</v>
+        <v>DelanieCarman18</v>
       </c>
       <c r="C3" s="2" t="str">
         <f t="shared" ref="C3:C21" si="1">CONCATENATE($G3,$I$2,$H$2)</f>
-        <v>DelanieCarman17@gmail.com</v>
+        <v>DelanieCarman18@gmail.com</v>
       </c>
       <c r="G3" t="s">
         <v>132</v>
@@ -4988,15 +4988,15 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>BretAgnew17</v>
+        <v>BretAgnew18</v>
       </c>
       <c r="B4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>BretAgnew17</v>
+        <v>BretAgnew18</v>
       </c>
       <c r="C4" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>BretAgnew17@gmail.com</v>
+        <v>BretAgnew18@gmail.com</v>
       </c>
       <c r="G4" t="s">
         <v>133</v>
@@ -5005,15 +5005,15 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EdgardoTaylor17</v>
+        <v>EdgardoTaylor18</v>
       </c>
       <c r="B5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EdgardoTaylor17</v>
+        <v>EdgardoTaylor18</v>
       </c>
       <c r="C5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>EdgardoTaylor17@gmail.com</v>
+        <v>EdgardoTaylor18@gmail.com</v>
       </c>
       <c r="G5" t="s">
         <v>134</v>
@@ -5022,15 +5022,15 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TyrekReis17</v>
+        <v>TyrekReis18</v>
       </c>
       <c r="B6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TyrekReis17</v>
+        <v>TyrekReis18</v>
       </c>
       <c r="C6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>TyrekReis17@gmail.com</v>
+        <v>TyrekReis18@gmail.com</v>
       </c>
       <c r="G6" t="s">
         <v>135</v>
@@ -5039,15 +5039,15 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LeannaChow17</v>
+        <v>LeannaChow18</v>
       </c>
       <c r="B7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LeannaChow17</v>
+        <v>LeannaChow18</v>
       </c>
       <c r="C7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LeannaChow17@gmail.com</v>
+        <v>LeannaChow18@gmail.com</v>
       </c>
       <c r="G7" t="s">
         <v>136</v>
@@ -5056,15 +5056,15 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TuckerCarlson17</v>
+        <v>TuckerCarlson18</v>
       </c>
       <c r="B8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TuckerCarlson17</v>
+        <v>TuckerCarlson18</v>
       </c>
       <c r="C8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>TuckerCarlson17@gmail.com</v>
+        <v>TuckerCarlson18@gmail.com</v>
       </c>
       <c r="G8" t="s">
         <v>137</v>
@@ -5073,15 +5073,15 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AnnmarieConnor17</v>
+        <v>AnnmarieConnor18</v>
       </c>
       <c r="B9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AnnmarieConnor17</v>
+        <v>AnnmarieConnor18</v>
       </c>
       <c r="C9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>AnnmarieConnor17@gmail.com</v>
+        <v>AnnmarieConnor18@gmail.com</v>
       </c>
       <c r="G9" t="s">
         <v>138</v>
@@ -5090,15 +5090,15 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MoniqueWitte17</v>
+        <v>MoniqueWitte18</v>
       </c>
       <c r="B10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MoniqueWitte17</v>
+        <v>MoniqueWitte18</v>
       </c>
       <c r="C10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MoniqueWitte17@gmail.com</v>
+        <v>MoniqueWitte18@gmail.com</v>
       </c>
       <c r="G10" t="s">
         <v>139</v>
@@ -5107,15 +5107,15 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MikelWhitlock17</v>
+        <v>MikelWhitlock18</v>
       </c>
       <c r="B11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MikelWhitlock17</v>
+        <v>MikelWhitlock18</v>
       </c>
       <c r="C11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MikelWhitlock17@gmail.com</v>
+        <v>MikelWhitlock18@gmail.com</v>
       </c>
       <c r="G11" t="s">
         <v>140</v>
@@ -5124,15 +5124,15 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>VincentAmaya17</v>
+        <v>VincentAmaya18</v>
       </c>
       <c r="B12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>VincentAmaya17</v>
+        <v>VincentAmaya18</v>
       </c>
       <c r="C12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>VincentAmaya17@gmail.com</v>
+        <v>VincentAmaya18@gmail.com</v>
       </c>
       <c r="G12" t="s">
         <v>141</v>
@@ -5141,15 +5141,15 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>KeiraQuiroz17</v>
+        <v>KeiraQuiroz18</v>
       </c>
       <c r="B13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>KeiraQuiroz17</v>
+        <v>KeiraQuiroz18</v>
       </c>
       <c r="C13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>KeiraQuiroz17@gmail.com</v>
+        <v>KeiraQuiroz18@gmail.com</v>
       </c>
       <c r="G13" t="s">
         <v>142</v>
@@ -5158,15 +5158,15 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EllisCreech17</v>
+        <v>EllisCreech18</v>
       </c>
       <c r="B14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EllisCreech17</v>
+        <v>EllisCreech18</v>
       </c>
       <c r="C14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>EllisCreech17@gmail.com</v>
+        <v>EllisCreech18@gmail.com</v>
       </c>
       <c r="G14" t="s">
         <v>143</v>
@@ -5175,15 +5175,15 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DionteCreel17</v>
+        <v>DionteCreel18</v>
       </c>
       <c r="B15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DionteCreel17</v>
+        <v>DionteCreel18</v>
       </c>
       <c r="C15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DionteCreel17@gmail.com</v>
+        <v>DionteCreel18@gmail.com</v>
       </c>
       <c r="G15" t="s">
         <v>144</v>
@@ -5192,15 +5192,15 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NicholeFoust17</v>
+        <v>NicholeFoust18</v>
       </c>
       <c r="B16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NicholeFoust17</v>
+        <v>NicholeFoust18</v>
       </c>
       <c r="C16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>NicholeFoust17@gmail.com</v>
+        <v>NicholeFoust18@gmail.com</v>
       </c>
       <c r="G16" t="s">
         <v>145</v>
@@ -5209,15 +5209,15 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>ManuelConnell17</v>
+        <v>ManuelConnell18</v>
       </c>
       <c r="B17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>ManuelConnell17</v>
+        <v>ManuelConnell18</v>
       </c>
       <c r="C17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>ManuelConnell17@gmail.com</v>
+        <v>ManuelConnell18@gmail.com</v>
       </c>
       <c r="G17" t="s">
         <v>146</v>
@@ -5226,15 +5226,15 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LourdesElam17</v>
+        <v>LourdesElam18</v>
       </c>
       <c r="B18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LourdesElam17</v>
+        <v>LourdesElam18</v>
       </c>
       <c r="C18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LourdesElam17@gmail.com</v>
+        <v>LourdesElam18@gmail.com</v>
       </c>
       <c r="G18" t="s">
         <v>147</v>
@@ -5243,15 +5243,15 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LincolnFrederick17</v>
+        <v>LincolnFrederick18</v>
       </c>
       <c r="B19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LincolnFrederick17</v>
+        <v>LincolnFrederick18</v>
       </c>
       <c r="C19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LincolnFrederick17@gmail.com</v>
+        <v>LincolnFrederick18@gmail.com</v>
       </c>
       <c r="G19" t="s">
         <v>148</v>
@@ -5260,15 +5260,15 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AlisaCash17</v>
+        <v>AlisaCash18</v>
       </c>
       <c r="B20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AlisaCash17</v>
+        <v>AlisaCash18</v>
       </c>
       <c r="C20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>AlisaCash17@gmail.com</v>
+        <v>AlisaCash18@gmail.com</v>
       </c>
       <c r="G20" t="s">
         <v>149</v>
@@ -5277,15 +5277,15 @@
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LucilleGriffiths17</v>
+        <v>LucilleGriffiths18</v>
       </c>
       <c r="B21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LucilleGriffiths17</v>
+        <v>LucilleGriffiths18</v>
       </c>
       <c r="C21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LucilleGriffiths17@gmail.com</v>
+        <v>LucilleGriffiths18@gmail.com</v>
       </c>
       <c r="G21" t="s">
         <v>150</v>
@@ -5307,15 +5307,15 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="str">
         <f>CONCATENATE($G23,$I$23)</f>
-        <v>DonnellJernigan22</v>
+        <v>DonnellJernigan23</v>
       </c>
       <c r="B23" s="1" t="str">
         <f>CONCATENATE($G23,$I$23)</f>
-        <v>DonnellJernigan22</v>
+        <v>DonnellJernigan23</v>
       </c>
       <c r="C23" s="2" t="str">
         <f>CONCATENATE($G23,$I$23,$H$23)</f>
-        <v>DonnellJernigan22@gmail.com</v>
+        <v>DonnellJernigan23@gmail.com</v>
       </c>
       <c r="G23" s="24" t="s">
         <v>151</v>
@@ -5324,21 +5324,21 @@
         <v>71</v>
       </c>
       <c r="I23">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="str">
         <f t="shared" ref="A24:B42" si="2">CONCATENATE($G24,$I$23)</f>
-        <v>MalikOtoole22</v>
+        <v>MalikOtoole23</v>
       </c>
       <c r="B24" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MalikOtoole22</v>
+        <v>MalikOtoole23</v>
       </c>
       <c r="C24" s="2" t="str">
         <f t="shared" ref="C24:C42" si="3">CONCATENATE($G24,$I$23,$H$23)</f>
-        <v>MalikOtoole22@gmail.com</v>
+        <v>MalikOtoole23@gmail.com</v>
       </c>
       <c r="G24" t="s">
         <v>152</v>
@@ -5347,15 +5347,15 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AlanCaudill22</v>
+        <v>AlanCaudill23</v>
       </c>
       <c r="B25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AlanCaudill22</v>
+        <v>AlanCaudill23</v>
       </c>
       <c r="C25" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AlanCaudill22@gmail.com</v>
+        <v>AlanCaudill23@gmail.com</v>
       </c>
       <c r="G25" t="s">
         <v>153</v>
@@ -5364,15 +5364,15 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AdanApplegate22</v>
+        <v>AdanApplegate23</v>
       </c>
       <c r="B26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AdanApplegate22</v>
+        <v>AdanApplegate23</v>
       </c>
       <c r="C26" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AdanApplegate22@gmail.com</v>
+        <v>AdanApplegate23@gmail.com</v>
       </c>
       <c r="G26" t="s">
         <v>154</v>
@@ -5381,15 +5381,15 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AiyanaWhitworth22</v>
+        <v>AiyanaWhitworth23</v>
       </c>
       <c r="B27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AiyanaWhitworth22</v>
+        <v>AiyanaWhitworth23</v>
       </c>
       <c r="C27" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AiyanaWhitworth22@gmail.com</v>
+        <v>AiyanaWhitworth23@gmail.com</v>
       </c>
       <c r="G27" t="s">
         <v>155</v>
@@ -5398,15 +5398,15 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MercedezBrien22</v>
+        <v>MercedezBrien23</v>
       </c>
       <c r="B28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MercedezBrien22</v>
+        <v>MercedezBrien23</v>
       </c>
       <c r="C28" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>MercedezBrien22@gmail.com</v>
+        <v>MercedezBrien23@gmail.com</v>
       </c>
       <c r="G28" t="s">
         <v>156</v>
@@ -5415,15 +5415,15 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DuaneHager22</v>
+        <v>DuaneHager23</v>
       </c>
       <c r="B29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DuaneHager22</v>
+        <v>DuaneHager23</v>
       </c>
       <c r="C29" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DuaneHager22@gmail.com</v>
+        <v>DuaneHager23@gmail.com</v>
       </c>
       <c r="G29" t="s">
         <v>157</v>
@@ -5432,15 +5432,15 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>LorenBell22</v>
+        <v>LorenBell23</v>
       </c>
       <c r="B30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>LorenBell22</v>
+        <v>LorenBell23</v>
       </c>
       <c r="C30" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>LorenBell22@gmail.com</v>
+        <v>LorenBell23@gmail.com</v>
       </c>
       <c r="G30" t="s">
         <v>158</v>
@@ -5449,15 +5449,15 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>GeraldHiller22</v>
+        <v>GeraldHiller23</v>
       </c>
       <c r="B31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>GeraldHiller22</v>
+        <v>GeraldHiller23</v>
       </c>
       <c r="C31" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>GeraldHiller22@gmail.com</v>
+        <v>GeraldHiller23@gmail.com</v>
       </c>
       <c r="G31" t="s">
         <v>159</v>
@@ -5466,15 +5466,15 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DeionBranch22</v>
+        <v>DeionBranch23</v>
       </c>
       <c r="B32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DeionBranch22</v>
+        <v>DeionBranch23</v>
       </c>
       <c r="C32" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DeionBranch22@gmail.com</v>
+        <v>DeionBranch23@gmail.com</v>
       </c>
       <c r="G32" t="s">
         <v>160</v>
@@ -5483,15 +5483,15 @@
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DakotaHalstead22</v>
+        <v>DakotaHalstead23</v>
       </c>
       <c r="B33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DakotaHalstead22</v>
+        <v>DakotaHalstead23</v>
       </c>
       <c r="C33" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DakotaHalstead22@gmail.com</v>
+        <v>DakotaHalstead23@gmail.com</v>
       </c>
       <c r="G33" t="s">
         <v>161</v>
@@ -5500,15 +5500,15 @@
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ElliottFurman22</v>
+        <v>ElliottFurman23</v>
       </c>
       <c r="B34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ElliottFurman22</v>
+        <v>ElliottFurman23</v>
       </c>
       <c r="C34" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>ElliottFurman22@gmail.com</v>
+        <v>ElliottFurman23@gmail.com</v>
       </c>
       <c r="G34" t="s">
         <v>162</v>
@@ -5517,15 +5517,15 @@
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MiltonCamp22</v>
+        <v>MiltonCamp23</v>
       </c>
       <c r="B35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MiltonCamp22</v>
+        <v>MiltonCamp23</v>
       </c>
       <c r="C35" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>MiltonCamp22@gmail.com</v>
+        <v>MiltonCamp23@gmail.com</v>
       </c>
       <c r="G35" t="s">
         <v>163</v>
@@ -5534,15 +5534,15 @@
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DawnChester22</v>
+        <v>DawnChester23</v>
       </c>
       <c r="B36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DawnChester22</v>
+        <v>DawnChester23</v>
       </c>
       <c r="C36" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DawnChester22@gmail.com</v>
+        <v>DawnChester23@gmail.com</v>
       </c>
       <c r="G36" t="s">
         <v>164</v>
@@ -5551,15 +5551,15 @@
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ZacheryPetrie22</v>
+        <v>ZacheryPetrie23</v>
       </c>
       <c r="B37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ZacheryPetrie22</v>
+        <v>ZacheryPetrie23</v>
       </c>
       <c r="C37" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>ZacheryPetrie22@gmail.com</v>
+        <v>ZacheryPetrie23@gmail.com</v>
       </c>
       <c r="G37" t="s">
         <v>165</v>
@@ -5568,15 +5568,15 @@
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>EstebanAngel22</v>
+        <v>EstebanAngel23</v>
       </c>
       <c r="B38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>EstebanAngel22</v>
+        <v>EstebanAngel23</v>
       </c>
       <c r="C38" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>EstebanAngel22@gmail.com</v>
+        <v>EstebanAngel23@gmail.com</v>
       </c>
       <c r="G38" t="s">
         <v>166</v>
@@ -5585,15 +5585,15 @@
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>JimmyBlankenship22</v>
+        <v>JimmyBlankenship23</v>
       </c>
       <c r="B39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>JimmyBlankenship22</v>
+        <v>JimmyBlankenship23</v>
       </c>
       <c r="C39" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>JimmyBlankenship22@gmail.com</v>
+        <v>JimmyBlankenship23@gmail.com</v>
       </c>
       <c r="G39" t="s">
         <v>167</v>
@@ -5602,15 +5602,15 @@
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AllysaGrice22</v>
+        <v>AllysaGrice23</v>
       </c>
       <c r="B40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AllysaGrice22</v>
+        <v>AllysaGrice23</v>
       </c>
       <c r="C40" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AllysaGrice22@gmail.com</v>
+        <v>AllysaGrice23@gmail.com</v>
       </c>
       <c r="G40" t="s">
         <v>168</v>
@@ -5619,15 +5619,15 @@
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AugustineYoo22</v>
+        <v>AugustineYoo23</v>
       </c>
       <c r="B41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AugustineYoo22</v>
+        <v>AugustineYoo23</v>
       </c>
       <c r="C41" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AugustineYoo22@gmail.com</v>
+        <v>AugustineYoo23@gmail.com</v>
       </c>
       <c r="G41" t="s">
         <v>169</v>
@@ -5636,15 +5636,15 @@
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BrandiSouthard22</v>
+        <v>BrandiSouthard23</v>
       </c>
       <c r="B42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BrandiSouthard22</v>
+        <v>BrandiSouthard23</v>
       </c>
       <c r="C42" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>BrandiSouthard22@gmail.com</v>
+        <v>BrandiSouthard23@gmail.com</v>
       </c>
       <c r="G42" t="s">
         <v>170</v>

</xml_diff>

<commit_message>
updated pom, data files
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/Test_Data.xlsx
+++ b/src/main/resources/test_data/Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verkh\IdeaProjects\pom6\src\main\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF61E4FE-12BF-4065-94D2-51EDE96F0B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A80F477-0EA7-49F4-931B-86047B4496B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1500" windowWidth="23040" windowHeight="12180" tabRatio="594" activeTab="1" xr2:uid="{56D596F5-221D-421D-9FC5-55182B639D44}"/>
   </bookViews>
@@ -1048,244 +1048,244 @@
     <t>3</t>
   </si>
   <si>
-    <t>EthanBaker18</t>
-  </si>
-  <si>
-    <t>EthanBaker18@gmail.com</t>
-  </si>
-  <si>
-    <t>DelanieCarman18</t>
-  </si>
-  <si>
-    <t>DelanieCarman18@gmail.com</t>
-  </si>
-  <si>
-    <t>BretAgnew18</t>
-  </si>
-  <si>
-    <t>BretAgnew18@gmail.com</t>
-  </si>
-  <si>
-    <t>EdgardoTaylor18</t>
-  </si>
-  <si>
-    <t>EdgardoTaylor18@gmail.com</t>
-  </si>
-  <si>
-    <t>TyrekReis18</t>
-  </si>
-  <si>
-    <t>TyrekReis18@gmail.com</t>
-  </si>
-  <si>
-    <t>LeannaChow18</t>
-  </si>
-  <si>
-    <t>LeannaChow18@gmail.com</t>
-  </si>
-  <si>
-    <t>TuckerCarlson18</t>
-  </si>
-  <si>
-    <t>TuckerCarlson18@gmail.com</t>
-  </si>
-  <si>
-    <t>AnnmarieConnor18</t>
-  </si>
-  <si>
-    <t>AnnmarieConnor18@gmail.com</t>
-  </si>
-  <si>
-    <t>MoniqueWitte18</t>
-  </si>
-  <si>
-    <t>MoniqueWitte18@gmail.com</t>
-  </si>
-  <si>
-    <t>MikelWhitlock18</t>
-  </si>
-  <si>
-    <t>MikelWhitlock18@gmail.com</t>
-  </si>
-  <si>
-    <t>VincentAmaya18</t>
-  </si>
-  <si>
-    <t>VincentAmaya18@gmail.com</t>
-  </si>
-  <si>
-    <t>KeiraQuiroz18</t>
-  </si>
-  <si>
-    <t>KeiraQuiroz18@gmail.com</t>
-  </si>
-  <si>
-    <t>EllisCreech18</t>
-  </si>
-  <si>
-    <t>EllisCreech18@gmail.com</t>
-  </si>
-  <si>
-    <t>DionteCreel18</t>
-  </si>
-  <si>
-    <t>DionteCreel18@gmail.com</t>
-  </si>
-  <si>
-    <t>NicholeFoust18</t>
-  </si>
-  <si>
-    <t>NicholeFoust18@gmail.com</t>
-  </si>
-  <si>
-    <t>ManuelConnell18</t>
-  </si>
-  <si>
-    <t>ManuelConnell18@gmail.com</t>
-  </si>
-  <si>
-    <t>LourdesElam18</t>
-  </si>
-  <si>
-    <t>LourdesElam18@gmail.com</t>
-  </si>
-  <si>
-    <t>LincolnFrederick18</t>
-  </si>
-  <si>
-    <t>LincolnFrederick18@gmail.com</t>
-  </si>
-  <si>
-    <t>AlisaCash18</t>
-  </si>
-  <si>
-    <t>AlisaCash18@gmail.com</t>
-  </si>
-  <si>
-    <t>LucilleGriffiths18</t>
-  </si>
-  <si>
-    <t>LucilleGriffiths18@gmail.com</t>
-  </si>
-  <si>
-    <t>DonnellJernigan23</t>
-  </si>
-  <si>
-    <t>DonnellJernigan23@gmail.com</t>
-  </si>
-  <si>
-    <t>MalikOtoole23</t>
-  </si>
-  <si>
-    <t>MalikOtoole23@gmail.com</t>
-  </si>
-  <si>
-    <t>AlanCaudill23</t>
-  </si>
-  <si>
-    <t>AlanCaudill23@gmail.com</t>
-  </si>
-  <si>
-    <t>AdanApplegate23</t>
-  </si>
-  <si>
-    <t>AdanApplegate23@gmail.com</t>
-  </si>
-  <si>
-    <t>AiyanaWhitworth23</t>
-  </si>
-  <si>
-    <t>AiyanaWhitworth23@gmail.com</t>
-  </si>
-  <si>
-    <t>MercedezBrien23</t>
-  </si>
-  <si>
-    <t>MercedezBrien23@gmail.com</t>
-  </si>
-  <si>
-    <t>DuaneHager23</t>
-  </si>
-  <si>
-    <t>DuaneHager23@gmail.com</t>
-  </si>
-  <si>
-    <t>LorenBell23</t>
-  </si>
-  <si>
-    <t>LorenBell23@gmail.com</t>
-  </si>
-  <si>
-    <t>GeraldHiller23</t>
-  </si>
-  <si>
-    <t>GeraldHiller23@gmail.com</t>
-  </si>
-  <si>
-    <t>DeionBranch23</t>
-  </si>
-  <si>
-    <t>DeionBranch23@gmail.com</t>
-  </si>
-  <si>
-    <t>DakotaHalstead23</t>
-  </si>
-  <si>
-    <t>DakotaHalstead23@gmail.com</t>
-  </si>
-  <si>
-    <t>ElliottFurman23</t>
-  </si>
-  <si>
-    <t>ElliottFurman23@gmail.com</t>
-  </si>
-  <si>
-    <t>MiltonCamp23</t>
-  </si>
-  <si>
-    <t>MiltonCamp23@gmail.com</t>
-  </si>
-  <si>
-    <t>DawnChester23</t>
-  </si>
-  <si>
-    <t>DawnChester23@gmail.com</t>
-  </si>
-  <si>
-    <t>ZacheryPetrie23</t>
-  </si>
-  <si>
-    <t>ZacheryPetrie23@gmail.com</t>
-  </si>
-  <si>
-    <t>EstebanAngel23</t>
-  </si>
-  <si>
-    <t>EstebanAngel23@gmail.com</t>
-  </si>
-  <si>
-    <t>JimmyBlankenship23</t>
-  </si>
-  <si>
-    <t>JimmyBlankenship23@gmail.com</t>
-  </si>
-  <si>
-    <t>AllysaGrice23</t>
-  </si>
-  <si>
-    <t>AllysaGrice23@gmail.com</t>
-  </si>
-  <si>
-    <t>AugustineYoo23</t>
-  </si>
-  <si>
-    <t>AugustineYoo23@gmail.com</t>
-  </si>
-  <si>
-    <t>BrandiSouthard23</t>
-  </si>
-  <si>
-    <t>BrandiSouthard23@gmail.com</t>
+    <t>EthanBaker19</t>
+  </si>
+  <si>
+    <t>EthanBaker19@gmail.com</t>
+  </si>
+  <si>
+    <t>DelanieCarman19</t>
+  </si>
+  <si>
+    <t>DelanieCarman19@gmail.com</t>
+  </si>
+  <si>
+    <t>BretAgnew19</t>
+  </si>
+  <si>
+    <t>BretAgnew19@gmail.com</t>
+  </si>
+  <si>
+    <t>EdgardoTaylor19</t>
+  </si>
+  <si>
+    <t>EdgardoTaylor19@gmail.com</t>
+  </si>
+  <si>
+    <t>TyrekReis19</t>
+  </si>
+  <si>
+    <t>TyrekReis19@gmail.com</t>
+  </si>
+  <si>
+    <t>LeannaChow19</t>
+  </si>
+  <si>
+    <t>LeannaChow19@gmail.com</t>
+  </si>
+  <si>
+    <t>TuckerCarlson19</t>
+  </si>
+  <si>
+    <t>TuckerCarlson19@gmail.com</t>
+  </si>
+  <si>
+    <t>AnnmarieConnor19</t>
+  </si>
+  <si>
+    <t>AnnmarieConnor19@gmail.com</t>
+  </si>
+  <si>
+    <t>MoniqueWitte19</t>
+  </si>
+  <si>
+    <t>MoniqueWitte19@gmail.com</t>
+  </si>
+  <si>
+    <t>MikelWhitlock19</t>
+  </si>
+  <si>
+    <t>MikelWhitlock19@gmail.com</t>
+  </si>
+  <si>
+    <t>VincentAmaya19</t>
+  </si>
+  <si>
+    <t>VincentAmaya19@gmail.com</t>
+  </si>
+  <si>
+    <t>KeiraQuiroz19</t>
+  </si>
+  <si>
+    <t>KeiraQuiroz19@gmail.com</t>
+  </si>
+  <si>
+    <t>EllisCreech19</t>
+  </si>
+  <si>
+    <t>EllisCreech19@gmail.com</t>
+  </si>
+  <si>
+    <t>DionteCreel19</t>
+  </si>
+  <si>
+    <t>DionteCreel19@gmail.com</t>
+  </si>
+  <si>
+    <t>NicholeFoust19</t>
+  </si>
+  <si>
+    <t>NicholeFoust19@gmail.com</t>
+  </si>
+  <si>
+    <t>ManuelConnell19</t>
+  </si>
+  <si>
+    <t>ManuelConnell19@gmail.com</t>
+  </si>
+  <si>
+    <t>LourdesElam19</t>
+  </si>
+  <si>
+    <t>LourdesElam19@gmail.com</t>
+  </si>
+  <si>
+    <t>LincolnFrederick19</t>
+  </si>
+  <si>
+    <t>LincolnFrederick19@gmail.com</t>
+  </si>
+  <si>
+    <t>AlisaCash19</t>
+  </si>
+  <si>
+    <t>AlisaCash19@gmail.com</t>
+  </si>
+  <si>
+    <t>LucilleGriffiths19</t>
+  </si>
+  <si>
+    <t>LucilleGriffiths19@gmail.com</t>
+  </si>
+  <si>
+    <t>DonnellJernigan24</t>
+  </si>
+  <si>
+    <t>DonnellJernigan24@gmail.com</t>
+  </si>
+  <si>
+    <t>MalikOtoole24</t>
+  </si>
+  <si>
+    <t>MalikOtoole24@gmail.com</t>
+  </si>
+  <si>
+    <t>AlanCaudill24</t>
+  </si>
+  <si>
+    <t>AlanCaudill24@gmail.com</t>
+  </si>
+  <si>
+    <t>AdanApplegate24</t>
+  </si>
+  <si>
+    <t>AdanApplegate24@gmail.com</t>
+  </si>
+  <si>
+    <t>AiyanaWhitworth24</t>
+  </si>
+  <si>
+    <t>AiyanaWhitworth24@gmail.com</t>
+  </si>
+  <si>
+    <t>MercedezBrien24</t>
+  </si>
+  <si>
+    <t>MercedezBrien24@gmail.com</t>
+  </si>
+  <si>
+    <t>DuaneHager24</t>
+  </si>
+  <si>
+    <t>DuaneHager24@gmail.com</t>
+  </si>
+  <si>
+    <t>LorenBell24</t>
+  </si>
+  <si>
+    <t>LorenBell24@gmail.com</t>
+  </si>
+  <si>
+    <t>GeraldHiller24</t>
+  </si>
+  <si>
+    <t>GeraldHiller24@gmail.com</t>
+  </si>
+  <si>
+    <t>DeionBranch24</t>
+  </si>
+  <si>
+    <t>DeionBranch24@gmail.com</t>
+  </si>
+  <si>
+    <t>DakotaHalstead24</t>
+  </si>
+  <si>
+    <t>DakotaHalstead24@gmail.com</t>
+  </si>
+  <si>
+    <t>ElliottFurman24</t>
+  </si>
+  <si>
+    <t>ElliottFurman24@gmail.com</t>
+  </si>
+  <si>
+    <t>MiltonCamp24</t>
+  </si>
+  <si>
+    <t>MiltonCamp24@gmail.com</t>
+  </si>
+  <si>
+    <t>DawnChester24</t>
+  </si>
+  <si>
+    <t>DawnChester24@gmail.com</t>
+  </si>
+  <si>
+    <t>ZacheryPetrie24</t>
+  </si>
+  <si>
+    <t>ZacheryPetrie24@gmail.com</t>
+  </si>
+  <si>
+    <t>EstebanAngel24</t>
+  </si>
+  <si>
+    <t>EstebanAngel24@gmail.com</t>
+  </si>
+  <si>
+    <t>JimmyBlankenship24</t>
+  </si>
+  <si>
+    <t>JimmyBlankenship24@gmail.com</t>
+  </si>
+  <si>
+    <t>AllysaGrice24</t>
+  </si>
+  <si>
+    <t>AllysaGrice24@gmail.com</t>
+  </si>
+  <si>
+    <t>AugustineYoo24</t>
+  </si>
+  <si>
+    <t>AugustineYoo24@gmail.com</t>
+  </si>
+  <si>
+    <t>BrandiSouthard24</t>
+  </si>
+  <si>
+    <t>BrandiSouthard24@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -4919,7 +4919,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FABAB06A-EAA7-4BA7-8A4C-8C5EF7E0517A}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="A23" sqref="A23:C42"/>
     </sheetView>
   </sheetViews>
@@ -4948,15 +4948,15 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="str">
         <f>CONCATENATE($G2,$I$2)</f>
-        <v>EthanBaker18</v>
+        <v>EthanBaker19</v>
       </c>
       <c r="B2" s="1" t="str">
         <f>CONCATENATE($G2,$I$2)</f>
-        <v>EthanBaker18</v>
+        <v>EthanBaker19</v>
       </c>
       <c r="C2" s="2" t="str">
         <f>CONCATENATE($G2,$I$2,$H$2)</f>
-        <v>EthanBaker18@gmail.com</v>
+        <v>EthanBaker19@gmail.com</v>
       </c>
       <c r="G2" t="s">
         <v>131</v>
@@ -4965,21 +4965,21 @@
         <v>71</v>
       </c>
       <c r="I2">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
         <f t="shared" ref="A3:B21" si="0">CONCATENATE($G3,$I$2)</f>
-        <v>DelanieCarman18</v>
+        <v>DelanieCarman19</v>
       </c>
       <c r="B3" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DelanieCarman18</v>
+        <v>DelanieCarman19</v>
       </c>
       <c r="C3" s="2" t="str">
         <f t="shared" ref="C3:C21" si="1">CONCATENATE($G3,$I$2,$H$2)</f>
-        <v>DelanieCarman18@gmail.com</v>
+        <v>DelanieCarman19@gmail.com</v>
       </c>
       <c r="G3" t="s">
         <v>132</v>
@@ -4988,15 +4988,15 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>BretAgnew18</v>
+        <v>BretAgnew19</v>
       </c>
       <c r="B4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>BretAgnew18</v>
+        <v>BretAgnew19</v>
       </c>
       <c r="C4" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>BretAgnew18@gmail.com</v>
+        <v>BretAgnew19@gmail.com</v>
       </c>
       <c r="G4" t="s">
         <v>133</v>
@@ -5005,15 +5005,15 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EdgardoTaylor18</v>
+        <v>EdgardoTaylor19</v>
       </c>
       <c r="B5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EdgardoTaylor18</v>
+        <v>EdgardoTaylor19</v>
       </c>
       <c r="C5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>EdgardoTaylor18@gmail.com</v>
+        <v>EdgardoTaylor19@gmail.com</v>
       </c>
       <c r="G5" t="s">
         <v>134</v>
@@ -5022,15 +5022,15 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TyrekReis18</v>
+        <v>TyrekReis19</v>
       </c>
       <c r="B6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TyrekReis18</v>
+        <v>TyrekReis19</v>
       </c>
       <c r="C6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>TyrekReis18@gmail.com</v>
+        <v>TyrekReis19@gmail.com</v>
       </c>
       <c r="G6" t="s">
         <v>135</v>
@@ -5039,15 +5039,15 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LeannaChow18</v>
+        <v>LeannaChow19</v>
       </c>
       <c r="B7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LeannaChow18</v>
+        <v>LeannaChow19</v>
       </c>
       <c r="C7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LeannaChow18@gmail.com</v>
+        <v>LeannaChow19@gmail.com</v>
       </c>
       <c r="G7" t="s">
         <v>136</v>
@@ -5056,15 +5056,15 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TuckerCarlson18</v>
+        <v>TuckerCarlson19</v>
       </c>
       <c r="B8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TuckerCarlson18</v>
+        <v>TuckerCarlson19</v>
       </c>
       <c r="C8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>TuckerCarlson18@gmail.com</v>
+        <v>TuckerCarlson19@gmail.com</v>
       </c>
       <c r="G8" t="s">
         <v>137</v>
@@ -5073,15 +5073,15 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AnnmarieConnor18</v>
+        <v>AnnmarieConnor19</v>
       </c>
       <c r="B9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AnnmarieConnor18</v>
+        <v>AnnmarieConnor19</v>
       </c>
       <c r="C9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>AnnmarieConnor18@gmail.com</v>
+        <v>AnnmarieConnor19@gmail.com</v>
       </c>
       <c r="G9" t="s">
         <v>138</v>
@@ -5090,15 +5090,15 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MoniqueWitte18</v>
+        <v>MoniqueWitte19</v>
       </c>
       <c r="B10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MoniqueWitte18</v>
+        <v>MoniqueWitte19</v>
       </c>
       <c r="C10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MoniqueWitte18@gmail.com</v>
+        <v>MoniqueWitte19@gmail.com</v>
       </c>
       <c r="G10" t="s">
         <v>139</v>
@@ -5107,15 +5107,15 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MikelWhitlock18</v>
+        <v>MikelWhitlock19</v>
       </c>
       <c r="B11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MikelWhitlock18</v>
+        <v>MikelWhitlock19</v>
       </c>
       <c r="C11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MikelWhitlock18@gmail.com</v>
+        <v>MikelWhitlock19@gmail.com</v>
       </c>
       <c r="G11" t="s">
         <v>140</v>
@@ -5124,15 +5124,15 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>VincentAmaya18</v>
+        <v>VincentAmaya19</v>
       </c>
       <c r="B12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>VincentAmaya18</v>
+        <v>VincentAmaya19</v>
       </c>
       <c r="C12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>VincentAmaya18@gmail.com</v>
+        <v>VincentAmaya19@gmail.com</v>
       </c>
       <c r="G12" t="s">
         <v>141</v>
@@ -5141,15 +5141,15 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>KeiraQuiroz18</v>
+        <v>KeiraQuiroz19</v>
       </c>
       <c r="B13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>KeiraQuiroz18</v>
+        <v>KeiraQuiroz19</v>
       </c>
       <c r="C13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>KeiraQuiroz18@gmail.com</v>
+        <v>KeiraQuiroz19@gmail.com</v>
       </c>
       <c r="G13" t="s">
         <v>142</v>
@@ -5158,15 +5158,15 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EllisCreech18</v>
+        <v>EllisCreech19</v>
       </c>
       <c r="B14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EllisCreech18</v>
+        <v>EllisCreech19</v>
       </c>
       <c r="C14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>EllisCreech18@gmail.com</v>
+        <v>EllisCreech19@gmail.com</v>
       </c>
       <c r="G14" t="s">
         <v>143</v>
@@ -5175,15 +5175,15 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DionteCreel18</v>
+        <v>DionteCreel19</v>
       </c>
       <c r="B15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DionteCreel18</v>
+        <v>DionteCreel19</v>
       </c>
       <c r="C15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DionteCreel18@gmail.com</v>
+        <v>DionteCreel19@gmail.com</v>
       </c>
       <c r="G15" t="s">
         <v>144</v>
@@ -5192,15 +5192,15 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NicholeFoust18</v>
+        <v>NicholeFoust19</v>
       </c>
       <c r="B16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NicholeFoust18</v>
+        <v>NicholeFoust19</v>
       </c>
       <c r="C16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>NicholeFoust18@gmail.com</v>
+        <v>NicholeFoust19@gmail.com</v>
       </c>
       <c r="G16" t="s">
         <v>145</v>
@@ -5209,15 +5209,15 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>ManuelConnell18</v>
+        <v>ManuelConnell19</v>
       </c>
       <c r="B17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>ManuelConnell18</v>
+        <v>ManuelConnell19</v>
       </c>
       <c r="C17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>ManuelConnell18@gmail.com</v>
+        <v>ManuelConnell19@gmail.com</v>
       </c>
       <c r="G17" t="s">
         <v>146</v>
@@ -5226,15 +5226,15 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LourdesElam18</v>
+        <v>LourdesElam19</v>
       </c>
       <c r="B18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LourdesElam18</v>
+        <v>LourdesElam19</v>
       </c>
       <c r="C18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LourdesElam18@gmail.com</v>
+        <v>LourdesElam19@gmail.com</v>
       </c>
       <c r="G18" t="s">
         <v>147</v>
@@ -5243,15 +5243,15 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LincolnFrederick18</v>
+        <v>LincolnFrederick19</v>
       </c>
       <c r="B19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LincolnFrederick18</v>
+        <v>LincolnFrederick19</v>
       </c>
       <c r="C19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LincolnFrederick18@gmail.com</v>
+        <v>LincolnFrederick19@gmail.com</v>
       </c>
       <c r="G19" t="s">
         <v>148</v>
@@ -5260,15 +5260,15 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AlisaCash18</v>
+        <v>AlisaCash19</v>
       </c>
       <c r="B20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AlisaCash18</v>
+        <v>AlisaCash19</v>
       </c>
       <c r="C20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>AlisaCash18@gmail.com</v>
+        <v>AlisaCash19@gmail.com</v>
       </c>
       <c r="G20" t="s">
         <v>149</v>
@@ -5277,15 +5277,15 @@
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LucilleGriffiths18</v>
+        <v>LucilleGriffiths19</v>
       </c>
       <c r="B21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LucilleGriffiths18</v>
+        <v>LucilleGriffiths19</v>
       </c>
       <c r="C21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LucilleGriffiths18@gmail.com</v>
+        <v>LucilleGriffiths19@gmail.com</v>
       </c>
       <c r="G21" t="s">
         <v>150</v>
@@ -5307,15 +5307,15 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="str">
         <f>CONCATENATE($G23,$I$23)</f>
-        <v>DonnellJernigan23</v>
+        <v>DonnellJernigan24</v>
       </c>
       <c r="B23" s="1" t="str">
         <f>CONCATENATE($G23,$I$23)</f>
-        <v>DonnellJernigan23</v>
+        <v>DonnellJernigan24</v>
       </c>
       <c r="C23" s="2" t="str">
         <f>CONCATENATE($G23,$I$23,$H$23)</f>
-        <v>DonnellJernigan23@gmail.com</v>
+        <v>DonnellJernigan24@gmail.com</v>
       </c>
       <c r="G23" s="24" t="s">
         <v>151</v>
@@ -5324,21 +5324,21 @@
         <v>71</v>
       </c>
       <c r="I23">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="str">
         <f t="shared" ref="A24:B42" si="2">CONCATENATE($G24,$I$23)</f>
-        <v>MalikOtoole23</v>
+        <v>MalikOtoole24</v>
       </c>
       <c r="B24" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MalikOtoole23</v>
+        <v>MalikOtoole24</v>
       </c>
       <c r="C24" s="2" t="str">
         <f t="shared" ref="C24:C42" si="3">CONCATENATE($G24,$I$23,$H$23)</f>
-        <v>MalikOtoole23@gmail.com</v>
+        <v>MalikOtoole24@gmail.com</v>
       </c>
       <c r="G24" t="s">
         <v>152</v>
@@ -5347,15 +5347,15 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AlanCaudill23</v>
+        <v>AlanCaudill24</v>
       </c>
       <c r="B25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AlanCaudill23</v>
+        <v>AlanCaudill24</v>
       </c>
       <c r="C25" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AlanCaudill23@gmail.com</v>
+        <v>AlanCaudill24@gmail.com</v>
       </c>
       <c r="G25" t="s">
         <v>153</v>
@@ -5364,15 +5364,15 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AdanApplegate23</v>
+        <v>AdanApplegate24</v>
       </c>
       <c r="B26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AdanApplegate23</v>
+        <v>AdanApplegate24</v>
       </c>
       <c r="C26" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AdanApplegate23@gmail.com</v>
+        <v>AdanApplegate24@gmail.com</v>
       </c>
       <c r="G26" t="s">
         <v>154</v>
@@ -5381,15 +5381,15 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AiyanaWhitworth23</v>
+        <v>AiyanaWhitworth24</v>
       </c>
       <c r="B27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AiyanaWhitworth23</v>
+        <v>AiyanaWhitworth24</v>
       </c>
       <c r="C27" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AiyanaWhitworth23@gmail.com</v>
+        <v>AiyanaWhitworth24@gmail.com</v>
       </c>
       <c r="G27" t="s">
         <v>155</v>
@@ -5398,15 +5398,15 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MercedezBrien23</v>
+        <v>MercedezBrien24</v>
       </c>
       <c r="B28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MercedezBrien23</v>
+        <v>MercedezBrien24</v>
       </c>
       <c r="C28" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>MercedezBrien23@gmail.com</v>
+        <v>MercedezBrien24@gmail.com</v>
       </c>
       <c r="G28" t="s">
         <v>156</v>
@@ -5415,15 +5415,15 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DuaneHager23</v>
+        <v>DuaneHager24</v>
       </c>
       <c r="B29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DuaneHager23</v>
+        <v>DuaneHager24</v>
       </c>
       <c r="C29" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DuaneHager23@gmail.com</v>
+        <v>DuaneHager24@gmail.com</v>
       </c>
       <c r="G29" t="s">
         <v>157</v>
@@ -5432,15 +5432,15 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>LorenBell23</v>
+        <v>LorenBell24</v>
       </c>
       <c r="B30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>LorenBell23</v>
+        <v>LorenBell24</v>
       </c>
       <c r="C30" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>LorenBell23@gmail.com</v>
+        <v>LorenBell24@gmail.com</v>
       </c>
       <c r="G30" t="s">
         <v>158</v>
@@ -5449,15 +5449,15 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>GeraldHiller23</v>
+        <v>GeraldHiller24</v>
       </c>
       <c r="B31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>GeraldHiller23</v>
+        <v>GeraldHiller24</v>
       </c>
       <c r="C31" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>GeraldHiller23@gmail.com</v>
+        <v>GeraldHiller24@gmail.com</v>
       </c>
       <c r="G31" t="s">
         <v>159</v>
@@ -5466,15 +5466,15 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DeionBranch23</v>
+        <v>DeionBranch24</v>
       </c>
       <c r="B32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DeionBranch23</v>
+        <v>DeionBranch24</v>
       </c>
       <c r="C32" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DeionBranch23@gmail.com</v>
+        <v>DeionBranch24@gmail.com</v>
       </c>
       <c r="G32" t="s">
         <v>160</v>
@@ -5483,15 +5483,15 @@
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DakotaHalstead23</v>
+        <v>DakotaHalstead24</v>
       </c>
       <c r="B33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DakotaHalstead23</v>
+        <v>DakotaHalstead24</v>
       </c>
       <c r="C33" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DakotaHalstead23@gmail.com</v>
+        <v>DakotaHalstead24@gmail.com</v>
       </c>
       <c r="G33" t="s">
         <v>161</v>
@@ -5500,15 +5500,15 @@
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ElliottFurman23</v>
+        <v>ElliottFurman24</v>
       </c>
       <c r="B34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ElliottFurman23</v>
+        <v>ElliottFurman24</v>
       </c>
       <c r="C34" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>ElliottFurman23@gmail.com</v>
+        <v>ElliottFurman24@gmail.com</v>
       </c>
       <c r="G34" t="s">
         <v>162</v>
@@ -5517,15 +5517,15 @@
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MiltonCamp23</v>
+        <v>MiltonCamp24</v>
       </c>
       <c r="B35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MiltonCamp23</v>
+        <v>MiltonCamp24</v>
       </c>
       <c r="C35" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>MiltonCamp23@gmail.com</v>
+        <v>MiltonCamp24@gmail.com</v>
       </c>
       <c r="G35" t="s">
         <v>163</v>
@@ -5534,15 +5534,15 @@
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DawnChester23</v>
+        <v>DawnChester24</v>
       </c>
       <c r="B36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DawnChester23</v>
+        <v>DawnChester24</v>
       </c>
       <c r="C36" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DawnChester23@gmail.com</v>
+        <v>DawnChester24@gmail.com</v>
       </c>
       <c r="G36" t="s">
         <v>164</v>
@@ -5551,15 +5551,15 @@
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ZacheryPetrie23</v>
+        <v>ZacheryPetrie24</v>
       </c>
       <c r="B37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ZacheryPetrie23</v>
+        <v>ZacheryPetrie24</v>
       </c>
       <c r="C37" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>ZacheryPetrie23@gmail.com</v>
+        <v>ZacheryPetrie24@gmail.com</v>
       </c>
       <c r="G37" t="s">
         <v>165</v>
@@ -5568,15 +5568,15 @@
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>EstebanAngel23</v>
+        <v>EstebanAngel24</v>
       </c>
       <c r="B38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>EstebanAngel23</v>
+        <v>EstebanAngel24</v>
       </c>
       <c r="C38" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>EstebanAngel23@gmail.com</v>
+        <v>EstebanAngel24@gmail.com</v>
       </c>
       <c r="G38" t="s">
         <v>166</v>
@@ -5585,15 +5585,15 @@
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>JimmyBlankenship23</v>
+        <v>JimmyBlankenship24</v>
       </c>
       <c r="B39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>JimmyBlankenship23</v>
+        <v>JimmyBlankenship24</v>
       </c>
       <c r="C39" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>JimmyBlankenship23@gmail.com</v>
+        <v>JimmyBlankenship24@gmail.com</v>
       </c>
       <c r="G39" t="s">
         <v>167</v>
@@ -5602,15 +5602,15 @@
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AllysaGrice23</v>
+        <v>AllysaGrice24</v>
       </c>
       <c r="B40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AllysaGrice23</v>
+        <v>AllysaGrice24</v>
       </c>
       <c r="C40" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AllysaGrice23@gmail.com</v>
+        <v>AllysaGrice24@gmail.com</v>
       </c>
       <c r="G40" t="s">
         <v>168</v>
@@ -5619,15 +5619,15 @@
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AugustineYoo23</v>
+        <v>AugustineYoo24</v>
       </c>
       <c r="B41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AugustineYoo23</v>
+        <v>AugustineYoo24</v>
       </c>
       <c r="C41" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AugustineYoo23@gmail.com</v>
+        <v>AugustineYoo24@gmail.com</v>
       </c>
       <c r="G41" t="s">
         <v>169</v>
@@ -5636,15 +5636,15 @@
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BrandiSouthard23</v>
+        <v>BrandiSouthard24</v>
       </c>
       <c r="B42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BrandiSouthard23</v>
+        <v>BrandiSouthard24</v>
       </c>
       <c r="C42" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>BrandiSouthard23@gmail.com</v>
+        <v>BrandiSouthard24@gmail.com</v>
       </c>
       <c r="G42" t="s">
         <v>170</v>

</xml_diff>

<commit_message>
updated BaseTest, data files
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/Test_Data.xlsx
+++ b/src/main/resources/test_data/Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verkh\IdeaProjects\pom6\src\main\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A80F477-0EA7-49F4-931B-86047B4496B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E293759-037B-4F68-B0B2-242F498378EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1500" windowWidth="23040" windowHeight="12180" tabRatio="594" activeTab="1" xr2:uid="{56D596F5-221D-421D-9FC5-55182B639D44}"/>
   </bookViews>
@@ -1048,244 +1048,244 @@
     <t>3</t>
   </si>
   <si>
-    <t>EthanBaker19</t>
-  </si>
-  <si>
-    <t>EthanBaker19@gmail.com</t>
-  </si>
-  <si>
-    <t>DelanieCarman19</t>
-  </si>
-  <si>
-    <t>DelanieCarman19@gmail.com</t>
-  </si>
-  <si>
-    <t>BretAgnew19</t>
-  </si>
-  <si>
-    <t>BretAgnew19@gmail.com</t>
-  </si>
-  <si>
-    <t>EdgardoTaylor19</t>
-  </si>
-  <si>
-    <t>EdgardoTaylor19@gmail.com</t>
-  </si>
-  <si>
-    <t>TyrekReis19</t>
-  </si>
-  <si>
-    <t>TyrekReis19@gmail.com</t>
-  </si>
-  <si>
-    <t>LeannaChow19</t>
-  </si>
-  <si>
-    <t>LeannaChow19@gmail.com</t>
-  </si>
-  <si>
-    <t>TuckerCarlson19</t>
-  </si>
-  <si>
-    <t>TuckerCarlson19@gmail.com</t>
-  </si>
-  <si>
-    <t>AnnmarieConnor19</t>
-  </si>
-  <si>
-    <t>AnnmarieConnor19@gmail.com</t>
-  </si>
-  <si>
-    <t>MoniqueWitte19</t>
-  </si>
-  <si>
-    <t>MoniqueWitte19@gmail.com</t>
-  </si>
-  <si>
-    <t>MikelWhitlock19</t>
-  </si>
-  <si>
-    <t>MikelWhitlock19@gmail.com</t>
-  </si>
-  <si>
-    <t>VincentAmaya19</t>
-  </si>
-  <si>
-    <t>VincentAmaya19@gmail.com</t>
-  </si>
-  <si>
-    <t>KeiraQuiroz19</t>
-  </si>
-  <si>
-    <t>KeiraQuiroz19@gmail.com</t>
-  </si>
-  <si>
-    <t>EllisCreech19</t>
-  </si>
-  <si>
-    <t>EllisCreech19@gmail.com</t>
-  </si>
-  <si>
-    <t>DionteCreel19</t>
-  </si>
-  <si>
-    <t>DionteCreel19@gmail.com</t>
-  </si>
-  <si>
-    <t>NicholeFoust19</t>
-  </si>
-  <si>
-    <t>NicholeFoust19@gmail.com</t>
-  </si>
-  <si>
-    <t>ManuelConnell19</t>
-  </si>
-  <si>
-    <t>ManuelConnell19@gmail.com</t>
-  </si>
-  <si>
-    <t>LourdesElam19</t>
-  </si>
-  <si>
-    <t>LourdesElam19@gmail.com</t>
-  </si>
-  <si>
-    <t>LincolnFrederick19</t>
-  </si>
-  <si>
-    <t>LincolnFrederick19@gmail.com</t>
-  </si>
-  <si>
-    <t>AlisaCash19</t>
-  </si>
-  <si>
-    <t>AlisaCash19@gmail.com</t>
-  </si>
-  <si>
-    <t>LucilleGriffiths19</t>
-  </si>
-  <si>
-    <t>LucilleGriffiths19@gmail.com</t>
-  </si>
-  <si>
-    <t>DonnellJernigan24</t>
-  </si>
-  <si>
-    <t>DonnellJernigan24@gmail.com</t>
-  </si>
-  <si>
-    <t>MalikOtoole24</t>
-  </si>
-  <si>
-    <t>MalikOtoole24@gmail.com</t>
-  </si>
-  <si>
-    <t>AlanCaudill24</t>
-  </si>
-  <si>
-    <t>AlanCaudill24@gmail.com</t>
-  </si>
-  <si>
-    <t>AdanApplegate24</t>
-  </si>
-  <si>
-    <t>AdanApplegate24@gmail.com</t>
-  </si>
-  <si>
-    <t>AiyanaWhitworth24</t>
-  </si>
-  <si>
-    <t>AiyanaWhitworth24@gmail.com</t>
-  </si>
-  <si>
-    <t>MercedezBrien24</t>
-  </si>
-  <si>
-    <t>MercedezBrien24@gmail.com</t>
-  </si>
-  <si>
-    <t>DuaneHager24</t>
-  </si>
-  <si>
-    <t>DuaneHager24@gmail.com</t>
-  </si>
-  <si>
-    <t>LorenBell24</t>
-  </si>
-  <si>
-    <t>LorenBell24@gmail.com</t>
-  </si>
-  <si>
-    <t>GeraldHiller24</t>
-  </si>
-  <si>
-    <t>GeraldHiller24@gmail.com</t>
-  </si>
-  <si>
-    <t>DeionBranch24</t>
-  </si>
-  <si>
-    <t>DeionBranch24@gmail.com</t>
-  </si>
-  <si>
-    <t>DakotaHalstead24</t>
-  </si>
-  <si>
-    <t>DakotaHalstead24@gmail.com</t>
-  </si>
-  <si>
-    <t>ElliottFurman24</t>
-  </si>
-  <si>
-    <t>ElliottFurman24@gmail.com</t>
-  </si>
-  <si>
-    <t>MiltonCamp24</t>
-  </si>
-  <si>
-    <t>MiltonCamp24@gmail.com</t>
-  </si>
-  <si>
-    <t>DawnChester24</t>
-  </si>
-  <si>
-    <t>DawnChester24@gmail.com</t>
-  </si>
-  <si>
-    <t>ZacheryPetrie24</t>
-  </si>
-  <si>
-    <t>ZacheryPetrie24@gmail.com</t>
-  </si>
-  <si>
-    <t>EstebanAngel24</t>
-  </si>
-  <si>
-    <t>EstebanAngel24@gmail.com</t>
-  </si>
-  <si>
-    <t>JimmyBlankenship24</t>
-  </si>
-  <si>
-    <t>JimmyBlankenship24@gmail.com</t>
-  </si>
-  <si>
-    <t>AllysaGrice24</t>
-  </si>
-  <si>
-    <t>AllysaGrice24@gmail.com</t>
-  </si>
-  <si>
-    <t>AugustineYoo24</t>
-  </si>
-  <si>
-    <t>AugustineYoo24@gmail.com</t>
-  </si>
-  <si>
-    <t>BrandiSouthard24</t>
-  </si>
-  <si>
-    <t>BrandiSouthard24@gmail.com</t>
+    <t>EthanBaker20</t>
+  </si>
+  <si>
+    <t>EthanBaker20@gmail.com</t>
+  </si>
+  <si>
+    <t>DelanieCarman20</t>
+  </si>
+  <si>
+    <t>DelanieCarman20@gmail.com</t>
+  </si>
+  <si>
+    <t>BretAgnew20</t>
+  </si>
+  <si>
+    <t>BretAgnew20@gmail.com</t>
+  </si>
+  <si>
+    <t>EdgardoTaylor20</t>
+  </si>
+  <si>
+    <t>EdgardoTaylor20@gmail.com</t>
+  </si>
+  <si>
+    <t>TyrekReis20</t>
+  </si>
+  <si>
+    <t>TyrekReis20@gmail.com</t>
+  </si>
+  <si>
+    <t>LeannaChow20</t>
+  </si>
+  <si>
+    <t>LeannaChow20@gmail.com</t>
+  </si>
+  <si>
+    <t>TuckerCarlson20</t>
+  </si>
+  <si>
+    <t>TuckerCarlson20@gmail.com</t>
+  </si>
+  <si>
+    <t>AnnmarieConnor20</t>
+  </si>
+  <si>
+    <t>AnnmarieConnor20@gmail.com</t>
+  </si>
+  <si>
+    <t>MoniqueWitte20</t>
+  </si>
+  <si>
+    <t>MoniqueWitte20@gmail.com</t>
+  </si>
+  <si>
+    <t>MikelWhitlock20</t>
+  </si>
+  <si>
+    <t>MikelWhitlock20@gmail.com</t>
+  </si>
+  <si>
+    <t>VincentAmaya20</t>
+  </si>
+  <si>
+    <t>VincentAmaya20@gmail.com</t>
+  </si>
+  <si>
+    <t>KeiraQuiroz20</t>
+  </si>
+  <si>
+    <t>KeiraQuiroz20@gmail.com</t>
+  </si>
+  <si>
+    <t>EllisCreech20</t>
+  </si>
+  <si>
+    <t>EllisCreech20@gmail.com</t>
+  </si>
+  <si>
+    <t>DionteCreel20</t>
+  </si>
+  <si>
+    <t>DionteCreel20@gmail.com</t>
+  </si>
+  <si>
+    <t>NicholeFoust20</t>
+  </si>
+  <si>
+    <t>NicholeFoust20@gmail.com</t>
+  </si>
+  <si>
+    <t>ManuelConnell20</t>
+  </si>
+  <si>
+    <t>ManuelConnell20@gmail.com</t>
+  </si>
+  <si>
+    <t>LourdesElam20</t>
+  </si>
+  <si>
+    <t>LourdesElam20@gmail.com</t>
+  </si>
+  <si>
+    <t>LincolnFrederick20</t>
+  </si>
+  <si>
+    <t>LincolnFrederick20@gmail.com</t>
+  </si>
+  <si>
+    <t>AlisaCash20</t>
+  </si>
+  <si>
+    <t>AlisaCash20@gmail.com</t>
+  </si>
+  <si>
+    <t>LucilleGriffiths20</t>
+  </si>
+  <si>
+    <t>LucilleGriffiths20@gmail.com</t>
+  </si>
+  <si>
+    <t>DonnellJernigan25</t>
+  </si>
+  <si>
+    <t>DonnellJernigan25@gmail.com</t>
+  </si>
+  <si>
+    <t>MalikOtoole25</t>
+  </si>
+  <si>
+    <t>MalikOtoole25@gmail.com</t>
+  </si>
+  <si>
+    <t>AlanCaudill25</t>
+  </si>
+  <si>
+    <t>AlanCaudill25@gmail.com</t>
+  </si>
+  <si>
+    <t>AdanApplegate25</t>
+  </si>
+  <si>
+    <t>AdanApplegate25@gmail.com</t>
+  </si>
+  <si>
+    <t>AiyanaWhitworth25</t>
+  </si>
+  <si>
+    <t>AiyanaWhitworth25@gmail.com</t>
+  </si>
+  <si>
+    <t>MercedezBrien25</t>
+  </si>
+  <si>
+    <t>MercedezBrien25@gmail.com</t>
+  </si>
+  <si>
+    <t>DuaneHager25</t>
+  </si>
+  <si>
+    <t>DuaneHager25@gmail.com</t>
+  </si>
+  <si>
+    <t>LorenBell25</t>
+  </si>
+  <si>
+    <t>LorenBell25@gmail.com</t>
+  </si>
+  <si>
+    <t>GeraldHiller25</t>
+  </si>
+  <si>
+    <t>GeraldHiller25@gmail.com</t>
+  </si>
+  <si>
+    <t>DeionBranch25</t>
+  </si>
+  <si>
+    <t>DeionBranch25@gmail.com</t>
+  </si>
+  <si>
+    <t>DakotaHalstead25</t>
+  </si>
+  <si>
+    <t>DakotaHalstead25@gmail.com</t>
+  </si>
+  <si>
+    <t>ElliottFurman25</t>
+  </si>
+  <si>
+    <t>ElliottFurman25@gmail.com</t>
+  </si>
+  <si>
+    <t>MiltonCamp25</t>
+  </si>
+  <si>
+    <t>MiltonCamp25@gmail.com</t>
+  </si>
+  <si>
+    <t>DawnChester25</t>
+  </si>
+  <si>
+    <t>DawnChester25@gmail.com</t>
+  </si>
+  <si>
+    <t>ZacheryPetrie25</t>
+  </si>
+  <si>
+    <t>ZacheryPetrie25@gmail.com</t>
+  </si>
+  <si>
+    <t>EstebanAngel25</t>
+  </si>
+  <si>
+    <t>EstebanAngel25@gmail.com</t>
+  </si>
+  <si>
+    <t>JimmyBlankenship25</t>
+  </si>
+  <si>
+    <t>JimmyBlankenship25@gmail.com</t>
+  </si>
+  <si>
+    <t>AllysaGrice25</t>
+  </si>
+  <si>
+    <t>AllysaGrice25@gmail.com</t>
+  </si>
+  <si>
+    <t>AugustineYoo25</t>
+  </si>
+  <si>
+    <t>AugustineYoo25@gmail.com</t>
+  </si>
+  <si>
+    <t>BrandiSouthard25</t>
+  </si>
+  <si>
+    <t>BrandiSouthard25@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2900,8 +2900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0775DEA-3893-49AA-8C48-45DC29C761B9}">
   <dimension ref="A1:AF21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2:T21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4948,15 +4948,15 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="str">
         <f>CONCATENATE($G2,$I$2)</f>
-        <v>EthanBaker19</v>
+        <v>EthanBaker20</v>
       </c>
       <c r="B2" s="1" t="str">
         <f>CONCATENATE($G2,$I$2)</f>
-        <v>EthanBaker19</v>
+        <v>EthanBaker20</v>
       </c>
       <c r="C2" s="2" t="str">
         <f>CONCATENATE($G2,$I$2,$H$2)</f>
-        <v>EthanBaker19@gmail.com</v>
+        <v>EthanBaker20@gmail.com</v>
       </c>
       <c r="G2" t="s">
         <v>131</v>
@@ -4965,21 +4965,21 @@
         <v>71</v>
       </c>
       <c r="I2">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
         <f t="shared" ref="A3:B21" si="0">CONCATENATE($G3,$I$2)</f>
-        <v>DelanieCarman19</v>
+        <v>DelanieCarman20</v>
       </c>
       <c r="B3" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DelanieCarman19</v>
+        <v>DelanieCarman20</v>
       </c>
       <c r="C3" s="2" t="str">
         <f t="shared" ref="C3:C21" si="1">CONCATENATE($G3,$I$2,$H$2)</f>
-        <v>DelanieCarman19@gmail.com</v>
+        <v>DelanieCarman20@gmail.com</v>
       </c>
       <c r="G3" t="s">
         <v>132</v>
@@ -4988,15 +4988,15 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>BretAgnew19</v>
+        <v>BretAgnew20</v>
       </c>
       <c r="B4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>BretAgnew19</v>
+        <v>BretAgnew20</v>
       </c>
       <c r="C4" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>BretAgnew19@gmail.com</v>
+        <v>BretAgnew20@gmail.com</v>
       </c>
       <c r="G4" t="s">
         <v>133</v>
@@ -5005,15 +5005,15 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EdgardoTaylor19</v>
+        <v>EdgardoTaylor20</v>
       </c>
       <c r="B5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EdgardoTaylor19</v>
+        <v>EdgardoTaylor20</v>
       </c>
       <c r="C5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>EdgardoTaylor19@gmail.com</v>
+        <v>EdgardoTaylor20@gmail.com</v>
       </c>
       <c r="G5" t="s">
         <v>134</v>
@@ -5022,15 +5022,15 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TyrekReis19</v>
+        <v>TyrekReis20</v>
       </c>
       <c r="B6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TyrekReis19</v>
+        <v>TyrekReis20</v>
       </c>
       <c r="C6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>TyrekReis19@gmail.com</v>
+        <v>TyrekReis20@gmail.com</v>
       </c>
       <c r="G6" t="s">
         <v>135</v>
@@ -5039,15 +5039,15 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LeannaChow19</v>
+        <v>LeannaChow20</v>
       </c>
       <c r="B7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LeannaChow19</v>
+        <v>LeannaChow20</v>
       </c>
       <c r="C7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LeannaChow19@gmail.com</v>
+        <v>LeannaChow20@gmail.com</v>
       </c>
       <c r="G7" t="s">
         <v>136</v>
@@ -5056,15 +5056,15 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TuckerCarlson19</v>
+        <v>TuckerCarlson20</v>
       </c>
       <c r="B8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TuckerCarlson19</v>
+        <v>TuckerCarlson20</v>
       </c>
       <c r="C8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>TuckerCarlson19@gmail.com</v>
+        <v>TuckerCarlson20@gmail.com</v>
       </c>
       <c r="G8" t="s">
         <v>137</v>
@@ -5073,15 +5073,15 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AnnmarieConnor19</v>
+        <v>AnnmarieConnor20</v>
       </c>
       <c r="B9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AnnmarieConnor19</v>
+        <v>AnnmarieConnor20</v>
       </c>
       <c r="C9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>AnnmarieConnor19@gmail.com</v>
+        <v>AnnmarieConnor20@gmail.com</v>
       </c>
       <c r="G9" t="s">
         <v>138</v>
@@ -5090,15 +5090,15 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MoniqueWitte19</v>
+        <v>MoniqueWitte20</v>
       </c>
       <c r="B10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MoniqueWitte19</v>
+        <v>MoniqueWitte20</v>
       </c>
       <c r="C10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MoniqueWitte19@gmail.com</v>
+        <v>MoniqueWitte20@gmail.com</v>
       </c>
       <c r="G10" t="s">
         <v>139</v>
@@ -5107,15 +5107,15 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MikelWhitlock19</v>
+        <v>MikelWhitlock20</v>
       </c>
       <c r="B11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MikelWhitlock19</v>
+        <v>MikelWhitlock20</v>
       </c>
       <c r="C11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MikelWhitlock19@gmail.com</v>
+        <v>MikelWhitlock20@gmail.com</v>
       </c>
       <c r="G11" t="s">
         <v>140</v>
@@ -5124,15 +5124,15 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>VincentAmaya19</v>
+        <v>VincentAmaya20</v>
       </c>
       <c r="B12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>VincentAmaya19</v>
+        <v>VincentAmaya20</v>
       </c>
       <c r="C12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>VincentAmaya19@gmail.com</v>
+        <v>VincentAmaya20@gmail.com</v>
       </c>
       <c r="G12" t="s">
         <v>141</v>
@@ -5141,15 +5141,15 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>KeiraQuiroz19</v>
+        <v>KeiraQuiroz20</v>
       </c>
       <c r="B13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>KeiraQuiroz19</v>
+        <v>KeiraQuiroz20</v>
       </c>
       <c r="C13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>KeiraQuiroz19@gmail.com</v>
+        <v>KeiraQuiroz20@gmail.com</v>
       </c>
       <c r="G13" t="s">
         <v>142</v>
@@ -5158,15 +5158,15 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EllisCreech19</v>
+        <v>EllisCreech20</v>
       </c>
       <c r="B14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EllisCreech19</v>
+        <v>EllisCreech20</v>
       </c>
       <c r="C14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>EllisCreech19@gmail.com</v>
+        <v>EllisCreech20@gmail.com</v>
       </c>
       <c r="G14" t="s">
         <v>143</v>
@@ -5175,15 +5175,15 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DionteCreel19</v>
+        <v>DionteCreel20</v>
       </c>
       <c r="B15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DionteCreel19</v>
+        <v>DionteCreel20</v>
       </c>
       <c r="C15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DionteCreel19@gmail.com</v>
+        <v>DionteCreel20@gmail.com</v>
       </c>
       <c r="G15" t="s">
         <v>144</v>
@@ -5192,15 +5192,15 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NicholeFoust19</v>
+        <v>NicholeFoust20</v>
       </c>
       <c r="B16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NicholeFoust19</v>
+        <v>NicholeFoust20</v>
       </c>
       <c r="C16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>NicholeFoust19@gmail.com</v>
+        <v>NicholeFoust20@gmail.com</v>
       </c>
       <c r="G16" t="s">
         <v>145</v>
@@ -5209,15 +5209,15 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>ManuelConnell19</v>
+        <v>ManuelConnell20</v>
       </c>
       <c r="B17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>ManuelConnell19</v>
+        <v>ManuelConnell20</v>
       </c>
       <c r="C17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>ManuelConnell19@gmail.com</v>
+        <v>ManuelConnell20@gmail.com</v>
       </c>
       <c r="G17" t="s">
         <v>146</v>
@@ -5226,15 +5226,15 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LourdesElam19</v>
+        <v>LourdesElam20</v>
       </c>
       <c r="B18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LourdesElam19</v>
+        <v>LourdesElam20</v>
       </c>
       <c r="C18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LourdesElam19@gmail.com</v>
+        <v>LourdesElam20@gmail.com</v>
       </c>
       <c r="G18" t="s">
         <v>147</v>
@@ -5243,15 +5243,15 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LincolnFrederick19</v>
+        <v>LincolnFrederick20</v>
       </c>
       <c r="B19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LincolnFrederick19</v>
+        <v>LincolnFrederick20</v>
       </c>
       <c r="C19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LincolnFrederick19@gmail.com</v>
+        <v>LincolnFrederick20@gmail.com</v>
       </c>
       <c r="G19" t="s">
         <v>148</v>
@@ -5260,15 +5260,15 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AlisaCash19</v>
+        <v>AlisaCash20</v>
       </c>
       <c r="B20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AlisaCash19</v>
+        <v>AlisaCash20</v>
       </c>
       <c r="C20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>AlisaCash19@gmail.com</v>
+        <v>AlisaCash20@gmail.com</v>
       </c>
       <c r="G20" t="s">
         <v>149</v>
@@ -5277,15 +5277,15 @@
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LucilleGriffiths19</v>
+        <v>LucilleGriffiths20</v>
       </c>
       <c r="B21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LucilleGriffiths19</v>
+        <v>LucilleGriffiths20</v>
       </c>
       <c r="C21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LucilleGriffiths19@gmail.com</v>
+        <v>LucilleGriffiths20@gmail.com</v>
       </c>
       <c r="G21" t="s">
         <v>150</v>
@@ -5307,15 +5307,15 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="str">
         <f>CONCATENATE($G23,$I$23)</f>
-        <v>DonnellJernigan24</v>
+        <v>DonnellJernigan25</v>
       </c>
       <c r="B23" s="1" t="str">
         <f>CONCATENATE($G23,$I$23)</f>
-        <v>DonnellJernigan24</v>
+        <v>DonnellJernigan25</v>
       </c>
       <c r="C23" s="2" t="str">
         <f>CONCATENATE($G23,$I$23,$H$23)</f>
-        <v>DonnellJernigan24@gmail.com</v>
+        <v>DonnellJernigan25@gmail.com</v>
       </c>
       <c r="G23" s="24" t="s">
         <v>151</v>
@@ -5324,21 +5324,21 @@
         <v>71</v>
       </c>
       <c r="I23">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="str">
         <f t="shared" ref="A24:B42" si="2">CONCATENATE($G24,$I$23)</f>
-        <v>MalikOtoole24</v>
+        <v>MalikOtoole25</v>
       </c>
       <c r="B24" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MalikOtoole24</v>
+        <v>MalikOtoole25</v>
       </c>
       <c r="C24" s="2" t="str">
         <f t="shared" ref="C24:C42" si="3">CONCATENATE($G24,$I$23,$H$23)</f>
-        <v>MalikOtoole24@gmail.com</v>
+        <v>MalikOtoole25@gmail.com</v>
       </c>
       <c r="G24" t="s">
         <v>152</v>
@@ -5347,15 +5347,15 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AlanCaudill24</v>
+        <v>AlanCaudill25</v>
       </c>
       <c r="B25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AlanCaudill24</v>
+        <v>AlanCaudill25</v>
       </c>
       <c r="C25" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AlanCaudill24@gmail.com</v>
+        <v>AlanCaudill25@gmail.com</v>
       </c>
       <c r="G25" t="s">
         <v>153</v>
@@ -5364,15 +5364,15 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AdanApplegate24</v>
+        <v>AdanApplegate25</v>
       </c>
       <c r="B26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AdanApplegate24</v>
+        <v>AdanApplegate25</v>
       </c>
       <c r="C26" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AdanApplegate24@gmail.com</v>
+        <v>AdanApplegate25@gmail.com</v>
       </c>
       <c r="G26" t="s">
         <v>154</v>
@@ -5381,15 +5381,15 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AiyanaWhitworth24</v>
+        <v>AiyanaWhitworth25</v>
       </c>
       <c r="B27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AiyanaWhitworth24</v>
+        <v>AiyanaWhitworth25</v>
       </c>
       <c r="C27" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AiyanaWhitworth24@gmail.com</v>
+        <v>AiyanaWhitworth25@gmail.com</v>
       </c>
       <c r="G27" t="s">
         <v>155</v>
@@ -5398,15 +5398,15 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MercedezBrien24</v>
+        <v>MercedezBrien25</v>
       </c>
       <c r="B28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MercedezBrien24</v>
+        <v>MercedezBrien25</v>
       </c>
       <c r="C28" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>MercedezBrien24@gmail.com</v>
+        <v>MercedezBrien25@gmail.com</v>
       </c>
       <c r="G28" t="s">
         <v>156</v>
@@ -5415,15 +5415,15 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DuaneHager24</v>
+        <v>DuaneHager25</v>
       </c>
       <c r="B29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DuaneHager24</v>
+        <v>DuaneHager25</v>
       </c>
       <c r="C29" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DuaneHager24@gmail.com</v>
+        <v>DuaneHager25@gmail.com</v>
       </c>
       <c r="G29" t="s">
         <v>157</v>
@@ -5432,15 +5432,15 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>LorenBell24</v>
+        <v>LorenBell25</v>
       </c>
       <c r="B30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>LorenBell24</v>
+        <v>LorenBell25</v>
       </c>
       <c r="C30" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>LorenBell24@gmail.com</v>
+        <v>LorenBell25@gmail.com</v>
       </c>
       <c r="G30" t="s">
         <v>158</v>
@@ -5449,15 +5449,15 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>GeraldHiller24</v>
+        <v>GeraldHiller25</v>
       </c>
       <c r="B31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>GeraldHiller24</v>
+        <v>GeraldHiller25</v>
       </c>
       <c r="C31" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>GeraldHiller24@gmail.com</v>
+        <v>GeraldHiller25@gmail.com</v>
       </c>
       <c r="G31" t="s">
         <v>159</v>
@@ -5466,15 +5466,15 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DeionBranch24</v>
+        <v>DeionBranch25</v>
       </c>
       <c r="B32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DeionBranch24</v>
+        <v>DeionBranch25</v>
       </c>
       <c r="C32" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DeionBranch24@gmail.com</v>
+        <v>DeionBranch25@gmail.com</v>
       </c>
       <c r="G32" t="s">
         <v>160</v>
@@ -5483,15 +5483,15 @@
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DakotaHalstead24</v>
+        <v>DakotaHalstead25</v>
       </c>
       <c r="B33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DakotaHalstead24</v>
+        <v>DakotaHalstead25</v>
       </c>
       <c r="C33" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DakotaHalstead24@gmail.com</v>
+        <v>DakotaHalstead25@gmail.com</v>
       </c>
       <c r="G33" t="s">
         <v>161</v>
@@ -5500,15 +5500,15 @@
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ElliottFurman24</v>
+        <v>ElliottFurman25</v>
       </c>
       <c r="B34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ElliottFurman24</v>
+        <v>ElliottFurman25</v>
       </c>
       <c r="C34" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>ElliottFurman24@gmail.com</v>
+        <v>ElliottFurman25@gmail.com</v>
       </c>
       <c r="G34" t="s">
         <v>162</v>
@@ -5517,15 +5517,15 @@
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MiltonCamp24</v>
+        <v>MiltonCamp25</v>
       </c>
       <c r="B35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MiltonCamp24</v>
+        <v>MiltonCamp25</v>
       </c>
       <c r="C35" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>MiltonCamp24@gmail.com</v>
+        <v>MiltonCamp25@gmail.com</v>
       </c>
       <c r="G35" t="s">
         <v>163</v>
@@ -5534,15 +5534,15 @@
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DawnChester24</v>
+        <v>DawnChester25</v>
       </c>
       <c r="B36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DawnChester24</v>
+        <v>DawnChester25</v>
       </c>
       <c r="C36" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DawnChester24@gmail.com</v>
+        <v>DawnChester25@gmail.com</v>
       </c>
       <c r="G36" t="s">
         <v>164</v>
@@ -5551,15 +5551,15 @@
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ZacheryPetrie24</v>
+        <v>ZacheryPetrie25</v>
       </c>
       <c r="B37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ZacheryPetrie24</v>
+        <v>ZacheryPetrie25</v>
       </c>
       <c r="C37" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>ZacheryPetrie24@gmail.com</v>
+        <v>ZacheryPetrie25@gmail.com</v>
       </c>
       <c r="G37" t="s">
         <v>165</v>
@@ -5568,15 +5568,15 @@
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>EstebanAngel24</v>
+        <v>EstebanAngel25</v>
       </c>
       <c r="B38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>EstebanAngel24</v>
+        <v>EstebanAngel25</v>
       </c>
       <c r="C38" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>EstebanAngel24@gmail.com</v>
+        <v>EstebanAngel25@gmail.com</v>
       </c>
       <c r="G38" t="s">
         <v>166</v>
@@ -5585,15 +5585,15 @@
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>JimmyBlankenship24</v>
+        <v>JimmyBlankenship25</v>
       </c>
       <c r="B39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>JimmyBlankenship24</v>
+        <v>JimmyBlankenship25</v>
       </c>
       <c r="C39" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>JimmyBlankenship24@gmail.com</v>
+        <v>JimmyBlankenship25@gmail.com</v>
       </c>
       <c r="G39" t="s">
         <v>167</v>
@@ -5602,15 +5602,15 @@
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AllysaGrice24</v>
+        <v>AllysaGrice25</v>
       </c>
       <c r="B40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AllysaGrice24</v>
+        <v>AllysaGrice25</v>
       </c>
       <c r="C40" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AllysaGrice24@gmail.com</v>
+        <v>AllysaGrice25@gmail.com</v>
       </c>
       <c r="G40" t="s">
         <v>168</v>
@@ -5619,15 +5619,15 @@
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AugustineYoo24</v>
+        <v>AugustineYoo25</v>
       </c>
       <c r="B41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AugustineYoo24</v>
+        <v>AugustineYoo25</v>
       </c>
       <c r="C41" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AugustineYoo24@gmail.com</v>
+        <v>AugustineYoo25@gmail.com</v>
       </c>
       <c r="G41" t="s">
         <v>169</v>
@@ -5636,15 +5636,15 @@
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BrandiSouthard24</v>
+        <v>BrandiSouthard25</v>
       </c>
       <c r="B42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BrandiSouthard24</v>
+        <v>BrandiSouthard25</v>
       </c>
       <c r="C42" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>BrandiSouthard24@gmail.com</v>
+        <v>BrandiSouthard25@gmail.com</v>
       </c>
       <c r="G42" t="s">
         <v>170</v>

</xml_diff>

<commit_message>
updated config, data files
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/Test_Data.xlsx
+++ b/src/main/resources/test_data/Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verkh\IdeaProjects\pom6\src\main\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E293759-037B-4F68-B0B2-242F498378EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67989455-9B55-463D-8A69-AAF35FD48462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1500" windowWidth="23040" windowHeight="12180" tabRatio="594" activeTab="1" xr2:uid="{56D596F5-221D-421D-9FC5-55182B639D44}"/>
   </bookViews>
@@ -1048,244 +1048,244 @@
     <t>3</t>
   </si>
   <si>
-    <t>EthanBaker20</t>
-  </si>
-  <si>
-    <t>EthanBaker20@gmail.com</t>
-  </si>
-  <si>
-    <t>DelanieCarman20</t>
-  </si>
-  <si>
-    <t>DelanieCarman20@gmail.com</t>
-  </si>
-  <si>
-    <t>BretAgnew20</t>
-  </si>
-  <si>
-    <t>BretAgnew20@gmail.com</t>
-  </si>
-  <si>
-    <t>EdgardoTaylor20</t>
-  </si>
-  <si>
-    <t>EdgardoTaylor20@gmail.com</t>
-  </si>
-  <si>
-    <t>TyrekReis20</t>
-  </si>
-  <si>
-    <t>TyrekReis20@gmail.com</t>
-  </si>
-  <si>
-    <t>LeannaChow20</t>
-  </si>
-  <si>
-    <t>LeannaChow20@gmail.com</t>
-  </si>
-  <si>
-    <t>TuckerCarlson20</t>
-  </si>
-  <si>
-    <t>TuckerCarlson20@gmail.com</t>
-  </si>
-  <si>
-    <t>AnnmarieConnor20</t>
-  </si>
-  <si>
-    <t>AnnmarieConnor20@gmail.com</t>
-  </si>
-  <si>
-    <t>MoniqueWitte20</t>
-  </si>
-  <si>
-    <t>MoniqueWitte20@gmail.com</t>
-  </si>
-  <si>
-    <t>MikelWhitlock20</t>
-  </si>
-  <si>
-    <t>MikelWhitlock20@gmail.com</t>
-  </si>
-  <si>
-    <t>VincentAmaya20</t>
-  </si>
-  <si>
-    <t>VincentAmaya20@gmail.com</t>
-  </si>
-  <si>
-    <t>KeiraQuiroz20</t>
-  </si>
-  <si>
-    <t>KeiraQuiroz20@gmail.com</t>
-  </si>
-  <si>
-    <t>EllisCreech20</t>
-  </si>
-  <si>
-    <t>EllisCreech20@gmail.com</t>
-  </si>
-  <si>
-    <t>DionteCreel20</t>
-  </si>
-  <si>
-    <t>DionteCreel20@gmail.com</t>
-  </si>
-  <si>
-    <t>NicholeFoust20</t>
-  </si>
-  <si>
-    <t>NicholeFoust20@gmail.com</t>
-  </si>
-  <si>
-    <t>ManuelConnell20</t>
-  </si>
-  <si>
-    <t>ManuelConnell20@gmail.com</t>
-  </si>
-  <si>
-    <t>LourdesElam20</t>
-  </si>
-  <si>
-    <t>LourdesElam20@gmail.com</t>
-  </si>
-  <si>
-    <t>LincolnFrederick20</t>
-  </si>
-  <si>
-    <t>LincolnFrederick20@gmail.com</t>
-  </si>
-  <si>
-    <t>AlisaCash20</t>
-  </si>
-  <si>
-    <t>AlisaCash20@gmail.com</t>
-  </si>
-  <si>
-    <t>LucilleGriffiths20</t>
-  </si>
-  <si>
-    <t>LucilleGriffiths20@gmail.com</t>
-  </si>
-  <si>
-    <t>DonnellJernigan25</t>
-  </si>
-  <si>
-    <t>DonnellJernigan25@gmail.com</t>
-  </si>
-  <si>
-    <t>MalikOtoole25</t>
-  </si>
-  <si>
-    <t>MalikOtoole25@gmail.com</t>
-  </si>
-  <si>
-    <t>AlanCaudill25</t>
-  </si>
-  <si>
-    <t>AlanCaudill25@gmail.com</t>
-  </si>
-  <si>
-    <t>AdanApplegate25</t>
-  </si>
-  <si>
-    <t>AdanApplegate25@gmail.com</t>
-  </si>
-  <si>
-    <t>AiyanaWhitworth25</t>
-  </si>
-  <si>
-    <t>AiyanaWhitworth25@gmail.com</t>
-  </si>
-  <si>
-    <t>MercedezBrien25</t>
-  </si>
-  <si>
-    <t>MercedezBrien25@gmail.com</t>
-  </si>
-  <si>
-    <t>DuaneHager25</t>
-  </si>
-  <si>
-    <t>DuaneHager25@gmail.com</t>
-  </si>
-  <si>
-    <t>LorenBell25</t>
-  </si>
-  <si>
-    <t>LorenBell25@gmail.com</t>
-  </si>
-  <si>
-    <t>GeraldHiller25</t>
-  </si>
-  <si>
-    <t>GeraldHiller25@gmail.com</t>
-  </si>
-  <si>
-    <t>DeionBranch25</t>
-  </si>
-  <si>
-    <t>DeionBranch25@gmail.com</t>
-  </si>
-  <si>
-    <t>DakotaHalstead25</t>
-  </si>
-  <si>
-    <t>DakotaHalstead25@gmail.com</t>
-  </si>
-  <si>
-    <t>ElliottFurman25</t>
-  </si>
-  <si>
-    <t>ElliottFurman25@gmail.com</t>
-  </si>
-  <si>
-    <t>MiltonCamp25</t>
-  </si>
-  <si>
-    <t>MiltonCamp25@gmail.com</t>
-  </si>
-  <si>
-    <t>DawnChester25</t>
-  </si>
-  <si>
-    <t>DawnChester25@gmail.com</t>
-  </si>
-  <si>
-    <t>ZacheryPetrie25</t>
-  </si>
-  <si>
-    <t>ZacheryPetrie25@gmail.com</t>
-  </si>
-  <si>
-    <t>EstebanAngel25</t>
-  </si>
-  <si>
-    <t>EstebanAngel25@gmail.com</t>
-  </si>
-  <si>
-    <t>JimmyBlankenship25</t>
-  </si>
-  <si>
-    <t>JimmyBlankenship25@gmail.com</t>
-  </si>
-  <si>
-    <t>AllysaGrice25</t>
-  </si>
-  <si>
-    <t>AllysaGrice25@gmail.com</t>
-  </si>
-  <si>
-    <t>AugustineYoo25</t>
-  </si>
-  <si>
-    <t>AugustineYoo25@gmail.com</t>
-  </si>
-  <si>
-    <t>BrandiSouthard25</t>
-  </si>
-  <si>
-    <t>BrandiSouthard25@gmail.com</t>
+    <t>EthanBaker21</t>
+  </si>
+  <si>
+    <t>EthanBaker21@gmail.com</t>
+  </si>
+  <si>
+    <t>DelanieCarman21</t>
+  </si>
+  <si>
+    <t>DelanieCarman21@gmail.com</t>
+  </si>
+  <si>
+    <t>BretAgnew21</t>
+  </si>
+  <si>
+    <t>BretAgnew21@gmail.com</t>
+  </si>
+  <si>
+    <t>EdgardoTaylor21</t>
+  </si>
+  <si>
+    <t>EdgardoTaylor21@gmail.com</t>
+  </si>
+  <si>
+    <t>TyrekReis21</t>
+  </si>
+  <si>
+    <t>TyrekReis21@gmail.com</t>
+  </si>
+  <si>
+    <t>LeannaChow21</t>
+  </si>
+  <si>
+    <t>LeannaChow21@gmail.com</t>
+  </si>
+  <si>
+    <t>TuckerCarlson21</t>
+  </si>
+  <si>
+    <t>TuckerCarlson21@gmail.com</t>
+  </si>
+  <si>
+    <t>AnnmarieConnor21</t>
+  </si>
+  <si>
+    <t>AnnmarieConnor21@gmail.com</t>
+  </si>
+  <si>
+    <t>MoniqueWitte21</t>
+  </si>
+  <si>
+    <t>MoniqueWitte21@gmail.com</t>
+  </si>
+  <si>
+    <t>MikelWhitlock21</t>
+  </si>
+  <si>
+    <t>MikelWhitlock21@gmail.com</t>
+  </si>
+  <si>
+    <t>VincentAmaya21</t>
+  </si>
+  <si>
+    <t>VincentAmaya21@gmail.com</t>
+  </si>
+  <si>
+    <t>KeiraQuiroz21</t>
+  </si>
+  <si>
+    <t>KeiraQuiroz21@gmail.com</t>
+  </si>
+  <si>
+    <t>EllisCreech21</t>
+  </si>
+  <si>
+    <t>EllisCreech21@gmail.com</t>
+  </si>
+  <si>
+    <t>DionteCreel21</t>
+  </si>
+  <si>
+    <t>DionteCreel21@gmail.com</t>
+  </si>
+  <si>
+    <t>NicholeFoust21</t>
+  </si>
+  <si>
+    <t>NicholeFoust21@gmail.com</t>
+  </si>
+  <si>
+    <t>ManuelConnell21</t>
+  </si>
+  <si>
+    <t>ManuelConnell21@gmail.com</t>
+  </si>
+  <si>
+    <t>LourdesElam21</t>
+  </si>
+  <si>
+    <t>LourdesElam21@gmail.com</t>
+  </si>
+  <si>
+    <t>LincolnFrederick21</t>
+  </si>
+  <si>
+    <t>LincolnFrederick21@gmail.com</t>
+  </si>
+  <si>
+    <t>AlisaCash21</t>
+  </si>
+  <si>
+    <t>AlisaCash21@gmail.com</t>
+  </si>
+  <si>
+    <t>LucilleGriffiths21</t>
+  </si>
+  <si>
+    <t>LucilleGriffiths21@gmail.com</t>
+  </si>
+  <si>
+    <t>DonnellJernigan26</t>
+  </si>
+  <si>
+    <t>DonnellJernigan26@gmail.com</t>
+  </si>
+  <si>
+    <t>MalikOtoole26</t>
+  </si>
+  <si>
+    <t>MalikOtoole26@gmail.com</t>
+  </si>
+  <si>
+    <t>AlanCaudill26</t>
+  </si>
+  <si>
+    <t>AlanCaudill26@gmail.com</t>
+  </si>
+  <si>
+    <t>AdanApplegate26</t>
+  </si>
+  <si>
+    <t>AdanApplegate26@gmail.com</t>
+  </si>
+  <si>
+    <t>AiyanaWhitworth26</t>
+  </si>
+  <si>
+    <t>AiyanaWhitworth26@gmail.com</t>
+  </si>
+  <si>
+    <t>MercedezBrien26</t>
+  </si>
+  <si>
+    <t>MercedezBrien26@gmail.com</t>
+  </si>
+  <si>
+    <t>DuaneHager26</t>
+  </si>
+  <si>
+    <t>DuaneHager26@gmail.com</t>
+  </si>
+  <si>
+    <t>LorenBell26</t>
+  </si>
+  <si>
+    <t>LorenBell26@gmail.com</t>
+  </si>
+  <si>
+    <t>GeraldHiller26</t>
+  </si>
+  <si>
+    <t>GeraldHiller26@gmail.com</t>
+  </si>
+  <si>
+    <t>DeionBranch26</t>
+  </si>
+  <si>
+    <t>DeionBranch26@gmail.com</t>
+  </si>
+  <si>
+    <t>DakotaHalstead26</t>
+  </si>
+  <si>
+    <t>DakotaHalstead26@gmail.com</t>
+  </si>
+  <si>
+    <t>ElliottFurman26</t>
+  </si>
+  <si>
+    <t>ElliottFurman26@gmail.com</t>
+  </si>
+  <si>
+    <t>MiltonCamp26</t>
+  </si>
+  <si>
+    <t>MiltonCamp26@gmail.com</t>
+  </si>
+  <si>
+    <t>DawnChester26</t>
+  </si>
+  <si>
+    <t>DawnChester26@gmail.com</t>
+  </si>
+  <si>
+    <t>ZacheryPetrie26</t>
+  </si>
+  <si>
+    <t>ZacheryPetrie26@gmail.com</t>
+  </si>
+  <si>
+    <t>EstebanAngel26</t>
+  </si>
+  <si>
+    <t>EstebanAngel26@gmail.com</t>
+  </si>
+  <si>
+    <t>JimmyBlankenship26</t>
+  </si>
+  <si>
+    <t>JimmyBlankenship26@gmail.com</t>
+  </si>
+  <si>
+    <t>AllysaGrice26</t>
+  </si>
+  <si>
+    <t>AllysaGrice26@gmail.com</t>
+  </si>
+  <si>
+    <t>AugustineYoo26</t>
+  </si>
+  <si>
+    <t>AugustineYoo26@gmail.com</t>
+  </si>
+  <si>
+    <t>BrandiSouthard26</t>
+  </si>
+  <si>
+    <t>BrandiSouthard26@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2886,11 +2886,11 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" display="AutomationTestPalatine28@gmail.com" xr:uid="{FAA270D8-B32D-4263-B50A-619A8BA3431D}"/>
-    <hyperlink ref="I3:I17" r:id="rId2" display="AutomationTestPalatine28@gmail.com" xr:uid="{ADD3FDEB-C73A-4417-9838-6AD8DC4B2A00}"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{0B9699C5-0EC0-4F4F-B4E4-7C65C295DC75}"/>
+    <hyperlink ref="J3:J21" r:id="rId2" display="TestChicago112@gmail.com" xr:uid="{6EC234DC-2002-4F99-A743-60A20D68921C}"/>
     <hyperlink ref="I12" r:id="rId3" display="VincentAmaya1@gmail.com" xr:uid="{6D467585-22DC-4BE4-A44E-4F64ABA50F76}"/>
-    <hyperlink ref="J2" r:id="rId4" xr:uid="{0B9699C5-0EC0-4F4F-B4E4-7C65C295DC75}"/>
-    <hyperlink ref="J3:J21" r:id="rId5" display="TestChicago112@gmail.com" xr:uid="{6EC234DC-2002-4F99-A743-60A20D68921C}"/>
+    <hyperlink ref="I3:I17" r:id="rId4" display="AutomationTestPalatine28@gmail.com" xr:uid="{ADD3FDEB-C73A-4417-9838-6AD8DC4B2A00}"/>
+    <hyperlink ref="I2" r:id="rId5" display="AutomationTestPalatine28@gmail.com" xr:uid="{FAA270D8-B32D-4263-B50A-619A8BA3431D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2900,8 +2900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0775DEA-3893-49AA-8C48-45DC29C761B9}">
   <dimension ref="A1:AF21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2:T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4919,7 +4919,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FABAB06A-EAA7-4BA7-8A4C-8C5EF7E0517A}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A23" sqref="A23:C42"/>
     </sheetView>
   </sheetViews>
@@ -4948,15 +4948,15 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="str">
         <f>CONCATENATE($G2,$I$2)</f>
-        <v>EthanBaker20</v>
+        <v>EthanBaker21</v>
       </c>
       <c r="B2" s="1" t="str">
         <f>CONCATENATE($G2,$I$2)</f>
-        <v>EthanBaker20</v>
+        <v>EthanBaker21</v>
       </c>
       <c r="C2" s="2" t="str">
         <f>CONCATENATE($G2,$I$2,$H$2)</f>
-        <v>EthanBaker20@gmail.com</v>
+        <v>EthanBaker21@gmail.com</v>
       </c>
       <c r="G2" t="s">
         <v>131</v>
@@ -4965,21 +4965,21 @@
         <v>71</v>
       </c>
       <c r="I2">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
         <f t="shared" ref="A3:B21" si="0">CONCATENATE($G3,$I$2)</f>
-        <v>DelanieCarman20</v>
+        <v>DelanieCarman21</v>
       </c>
       <c r="B3" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DelanieCarman20</v>
+        <v>DelanieCarman21</v>
       </c>
       <c r="C3" s="2" t="str">
         <f t="shared" ref="C3:C21" si="1">CONCATENATE($G3,$I$2,$H$2)</f>
-        <v>DelanieCarman20@gmail.com</v>
+        <v>DelanieCarman21@gmail.com</v>
       </c>
       <c r="G3" t="s">
         <v>132</v>
@@ -4988,15 +4988,15 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>BretAgnew20</v>
+        <v>BretAgnew21</v>
       </c>
       <c r="B4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>BretAgnew20</v>
+        <v>BretAgnew21</v>
       </c>
       <c r="C4" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>BretAgnew20@gmail.com</v>
+        <v>BretAgnew21@gmail.com</v>
       </c>
       <c r="G4" t="s">
         <v>133</v>
@@ -5005,15 +5005,15 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EdgardoTaylor20</v>
+        <v>EdgardoTaylor21</v>
       </c>
       <c r="B5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EdgardoTaylor20</v>
+        <v>EdgardoTaylor21</v>
       </c>
       <c r="C5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>EdgardoTaylor20@gmail.com</v>
+        <v>EdgardoTaylor21@gmail.com</v>
       </c>
       <c r="G5" t="s">
         <v>134</v>
@@ -5022,15 +5022,15 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TyrekReis20</v>
+        <v>TyrekReis21</v>
       </c>
       <c r="B6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TyrekReis20</v>
+        <v>TyrekReis21</v>
       </c>
       <c r="C6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>TyrekReis20@gmail.com</v>
+        <v>TyrekReis21@gmail.com</v>
       </c>
       <c r="G6" t="s">
         <v>135</v>
@@ -5039,15 +5039,15 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LeannaChow20</v>
+        <v>LeannaChow21</v>
       </c>
       <c r="B7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LeannaChow20</v>
+        <v>LeannaChow21</v>
       </c>
       <c r="C7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LeannaChow20@gmail.com</v>
+        <v>LeannaChow21@gmail.com</v>
       </c>
       <c r="G7" t="s">
         <v>136</v>
@@ -5056,15 +5056,15 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TuckerCarlson20</v>
+        <v>TuckerCarlson21</v>
       </c>
       <c r="B8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TuckerCarlson20</v>
+        <v>TuckerCarlson21</v>
       </c>
       <c r="C8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>TuckerCarlson20@gmail.com</v>
+        <v>TuckerCarlson21@gmail.com</v>
       </c>
       <c r="G8" t="s">
         <v>137</v>
@@ -5073,15 +5073,15 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AnnmarieConnor20</v>
+        <v>AnnmarieConnor21</v>
       </c>
       <c r="B9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AnnmarieConnor20</v>
+        <v>AnnmarieConnor21</v>
       </c>
       <c r="C9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>AnnmarieConnor20@gmail.com</v>
+        <v>AnnmarieConnor21@gmail.com</v>
       </c>
       <c r="G9" t="s">
         <v>138</v>
@@ -5090,15 +5090,15 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MoniqueWitte20</v>
+        <v>MoniqueWitte21</v>
       </c>
       <c r="B10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MoniqueWitte20</v>
+        <v>MoniqueWitte21</v>
       </c>
       <c r="C10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MoniqueWitte20@gmail.com</v>
+        <v>MoniqueWitte21@gmail.com</v>
       </c>
       <c r="G10" t="s">
         <v>139</v>
@@ -5107,15 +5107,15 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MikelWhitlock20</v>
+        <v>MikelWhitlock21</v>
       </c>
       <c r="B11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MikelWhitlock20</v>
+        <v>MikelWhitlock21</v>
       </c>
       <c r="C11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MikelWhitlock20@gmail.com</v>
+        <v>MikelWhitlock21@gmail.com</v>
       </c>
       <c r="G11" t="s">
         <v>140</v>
@@ -5124,15 +5124,15 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>VincentAmaya20</v>
+        <v>VincentAmaya21</v>
       </c>
       <c r="B12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>VincentAmaya20</v>
+        <v>VincentAmaya21</v>
       </c>
       <c r="C12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>VincentAmaya20@gmail.com</v>
+        <v>VincentAmaya21@gmail.com</v>
       </c>
       <c r="G12" t="s">
         <v>141</v>
@@ -5141,15 +5141,15 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>KeiraQuiroz20</v>
+        <v>KeiraQuiroz21</v>
       </c>
       <c r="B13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>KeiraQuiroz20</v>
+        <v>KeiraQuiroz21</v>
       </c>
       <c r="C13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>KeiraQuiroz20@gmail.com</v>
+        <v>KeiraQuiroz21@gmail.com</v>
       </c>
       <c r="G13" t="s">
         <v>142</v>
@@ -5158,15 +5158,15 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EllisCreech20</v>
+        <v>EllisCreech21</v>
       </c>
       <c r="B14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EllisCreech20</v>
+        <v>EllisCreech21</v>
       </c>
       <c r="C14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>EllisCreech20@gmail.com</v>
+        <v>EllisCreech21@gmail.com</v>
       </c>
       <c r="G14" t="s">
         <v>143</v>
@@ -5175,15 +5175,15 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DionteCreel20</v>
+        <v>DionteCreel21</v>
       </c>
       <c r="B15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DionteCreel20</v>
+        <v>DionteCreel21</v>
       </c>
       <c r="C15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DionteCreel20@gmail.com</v>
+        <v>DionteCreel21@gmail.com</v>
       </c>
       <c r="G15" t="s">
         <v>144</v>
@@ -5192,15 +5192,15 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NicholeFoust20</v>
+        <v>NicholeFoust21</v>
       </c>
       <c r="B16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NicholeFoust20</v>
+        <v>NicholeFoust21</v>
       </c>
       <c r="C16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>NicholeFoust20@gmail.com</v>
+        <v>NicholeFoust21@gmail.com</v>
       </c>
       <c r="G16" t="s">
         <v>145</v>
@@ -5209,15 +5209,15 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>ManuelConnell20</v>
+        <v>ManuelConnell21</v>
       </c>
       <c r="B17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>ManuelConnell20</v>
+        <v>ManuelConnell21</v>
       </c>
       <c r="C17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>ManuelConnell20@gmail.com</v>
+        <v>ManuelConnell21@gmail.com</v>
       </c>
       <c r="G17" t="s">
         <v>146</v>
@@ -5226,15 +5226,15 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LourdesElam20</v>
+        <v>LourdesElam21</v>
       </c>
       <c r="B18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LourdesElam20</v>
+        <v>LourdesElam21</v>
       </c>
       <c r="C18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LourdesElam20@gmail.com</v>
+        <v>LourdesElam21@gmail.com</v>
       </c>
       <c r="G18" t="s">
         <v>147</v>
@@ -5243,15 +5243,15 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LincolnFrederick20</v>
+        <v>LincolnFrederick21</v>
       </c>
       <c r="B19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LincolnFrederick20</v>
+        <v>LincolnFrederick21</v>
       </c>
       <c r="C19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LincolnFrederick20@gmail.com</v>
+        <v>LincolnFrederick21@gmail.com</v>
       </c>
       <c r="G19" t="s">
         <v>148</v>
@@ -5260,15 +5260,15 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AlisaCash20</v>
+        <v>AlisaCash21</v>
       </c>
       <c r="B20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AlisaCash20</v>
+        <v>AlisaCash21</v>
       </c>
       <c r="C20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>AlisaCash20@gmail.com</v>
+        <v>AlisaCash21@gmail.com</v>
       </c>
       <c r="G20" t="s">
         <v>149</v>
@@ -5277,15 +5277,15 @@
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LucilleGriffiths20</v>
+        <v>LucilleGriffiths21</v>
       </c>
       <c r="B21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LucilleGriffiths20</v>
+        <v>LucilleGriffiths21</v>
       </c>
       <c r="C21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LucilleGriffiths20@gmail.com</v>
+        <v>LucilleGriffiths21@gmail.com</v>
       </c>
       <c r="G21" t="s">
         <v>150</v>
@@ -5307,15 +5307,15 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="str">
         <f>CONCATENATE($G23,$I$23)</f>
-        <v>DonnellJernigan25</v>
+        <v>DonnellJernigan26</v>
       </c>
       <c r="B23" s="1" t="str">
         <f>CONCATENATE($G23,$I$23)</f>
-        <v>DonnellJernigan25</v>
+        <v>DonnellJernigan26</v>
       </c>
       <c r="C23" s="2" t="str">
         <f>CONCATENATE($G23,$I$23,$H$23)</f>
-        <v>DonnellJernigan25@gmail.com</v>
+        <v>DonnellJernigan26@gmail.com</v>
       </c>
       <c r="G23" s="24" t="s">
         <v>151</v>
@@ -5324,21 +5324,21 @@
         <v>71</v>
       </c>
       <c r="I23">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="str">
         <f t="shared" ref="A24:B42" si="2">CONCATENATE($G24,$I$23)</f>
-        <v>MalikOtoole25</v>
+        <v>MalikOtoole26</v>
       </c>
       <c r="B24" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MalikOtoole25</v>
+        <v>MalikOtoole26</v>
       </c>
       <c r="C24" s="2" t="str">
         <f t="shared" ref="C24:C42" si="3">CONCATENATE($G24,$I$23,$H$23)</f>
-        <v>MalikOtoole25@gmail.com</v>
+        <v>MalikOtoole26@gmail.com</v>
       </c>
       <c r="G24" t="s">
         <v>152</v>
@@ -5347,15 +5347,15 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AlanCaudill25</v>
+        <v>AlanCaudill26</v>
       </c>
       <c r="B25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AlanCaudill25</v>
+        <v>AlanCaudill26</v>
       </c>
       <c r="C25" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AlanCaudill25@gmail.com</v>
+        <v>AlanCaudill26@gmail.com</v>
       </c>
       <c r="G25" t="s">
         <v>153</v>
@@ -5364,15 +5364,15 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AdanApplegate25</v>
+        <v>AdanApplegate26</v>
       </c>
       <c r="B26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AdanApplegate25</v>
+        <v>AdanApplegate26</v>
       </c>
       <c r="C26" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AdanApplegate25@gmail.com</v>
+        <v>AdanApplegate26@gmail.com</v>
       </c>
       <c r="G26" t="s">
         <v>154</v>
@@ -5381,15 +5381,15 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AiyanaWhitworth25</v>
+        <v>AiyanaWhitworth26</v>
       </c>
       <c r="B27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AiyanaWhitworth25</v>
+        <v>AiyanaWhitworth26</v>
       </c>
       <c r="C27" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AiyanaWhitworth25@gmail.com</v>
+        <v>AiyanaWhitworth26@gmail.com</v>
       </c>
       <c r="G27" t="s">
         <v>155</v>
@@ -5398,15 +5398,15 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MercedezBrien25</v>
+        <v>MercedezBrien26</v>
       </c>
       <c r="B28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MercedezBrien25</v>
+        <v>MercedezBrien26</v>
       </c>
       <c r="C28" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>MercedezBrien25@gmail.com</v>
+        <v>MercedezBrien26@gmail.com</v>
       </c>
       <c r="G28" t="s">
         <v>156</v>
@@ -5415,15 +5415,15 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DuaneHager25</v>
+        <v>DuaneHager26</v>
       </c>
       <c r="B29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DuaneHager25</v>
+        <v>DuaneHager26</v>
       </c>
       <c r="C29" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DuaneHager25@gmail.com</v>
+        <v>DuaneHager26@gmail.com</v>
       </c>
       <c r="G29" t="s">
         <v>157</v>
@@ -5432,15 +5432,15 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>LorenBell25</v>
+        <v>LorenBell26</v>
       </c>
       <c r="B30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>LorenBell25</v>
+        <v>LorenBell26</v>
       </c>
       <c r="C30" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>LorenBell25@gmail.com</v>
+        <v>LorenBell26@gmail.com</v>
       </c>
       <c r="G30" t="s">
         <v>158</v>
@@ -5449,15 +5449,15 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>GeraldHiller25</v>
+        <v>GeraldHiller26</v>
       </c>
       <c r="B31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>GeraldHiller25</v>
+        <v>GeraldHiller26</v>
       </c>
       <c r="C31" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>GeraldHiller25@gmail.com</v>
+        <v>GeraldHiller26@gmail.com</v>
       </c>
       <c r="G31" t="s">
         <v>159</v>
@@ -5466,15 +5466,15 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DeionBranch25</v>
+        <v>DeionBranch26</v>
       </c>
       <c r="B32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DeionBranch25</v>
+        <v>DeionBranch26</v>
       </c>
       <c r="C32" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DeionBranch25@gmail.com</v>
+        <v>DeionBranch26@gmail.com</v>
       </c>
       <c r="G32" t="s">
         <v>160</v>
@@ -5483,15 +5483,15 @@
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DakotaHalstead25</v>
+        <v>DakotaHalstead26</v>
       </c>
       <c r="B33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DakotaHalstead25</v>
+        <v>DakotaHalstead26</v>
       </c>
       <c r="C33" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DakotaHalstead25@gmail.com</v>
+        <v>DakotaHalstead26@gmail.com</v>
       </c>
       <c r="G33" t="s">
         <v>161</v>
@@ -5500,15 +5500,15 @@
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ElliottFurman25</v>
+        <v>ElliottFurman26</v>
       </c>
       <c r="B34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ElliottFurman25</v>
+        <v>ElliottFurman26</v>
       </c>
       <c r="C34" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>ElliottFurman25@gmail.com</v>
+        <v>ElliottFurman26@gmail.com</v>
       </c>
       <c r="G34" t="s">
         <v>162</v>
@@ -5517,15 +5517,15 @@
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MiltonCamp25</v>
+        <v>MiltonCamp26</v>
       </c>
       <c r="B35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>MiltonCamp25</v>
+        <v>MiltonCamp26</v>
       </c>
       <c r="C35" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>MiltonCamp25@gmail.com</v>
+        <v>MiltonCamp26@gmail.com</v>
       </c>
       <c r="G35" t="s">
         <v>163</v>
@@ -5534,15 +5534,15 @@
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DawnChester25</v>
+        <v>DawnChester26</v>
       </c>
       <c r="B36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>DawnChester25</v>
+        <v>DawnChester26</v>
       </c>
       <c r="C36" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>DawnChester25@gmail.com</v>
+        <v>DawnChester26@gmail.com</v>
       </c>
       <c r="G36" t="s">
         <v>164</v>
@@ -5551,15 +5551,15 @@
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ZacheryPetrie25</v>
+        <v>ZacheryPetrie26</v>
       </c>
       <c r="B37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>ZacheryPetrie25</v>
+        <v>ZacheryPetrie26</v>
       </c>
       <c r="C37" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>ZacheryPetrie25@gmail.com</v>
+        <v>ZacheryPetrie26@gmail.com</v>
       </c>
       <c r="G37" t="s">
         <v>165</v>
@@ -5568,15 +5568,15 @@
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>EstebanAngel25</v>
+        <v>EstebanAngel26</v>
       </c>
       <c r="B38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>EstebanAngel25</v>
+        <v>EstebanAngel26</v>
       </c>
       <c r="C38" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>EstebanAngel25@gmail.com</v>
+        <v>EstebanAngel26@gmail.com</v>
       </c>
       <c r="G38" t="s">
         <v>166</v>
@@ -5585,15 +5585,15 @@
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>JimmyBlankenship25</v>
+        <v>JimmyBlankenship26</v>
       </c>
       <c r="B39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>JimmyBlankenship25</v>
+        <v>JimmyBlankenship26</v>
       </c>
       <c r="C39" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>JimmyBlankenship25@gmail.com</v>
+        <v>JimmyBlankenship26@gmail.com</v>
       </c>
       <c r="G39" t="s">
         <v>167</v>
@@ -5602,15 +5602,15 @@
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AllysaGrice25</v>
+        <v>AllysaGrice26</v>
       </c>
       <c r="B40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AllysaGrice25</v>
+        <v>AllysaGrice26</v>
       </c>
       <c r="C40" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AllysaGrice25@gmail.com</v>
+        <v>AllysaGrice26@gmail.com</v>
       </c>
       <c r="G40" t="s">
         <v>168</v>
@@ -5619,15 +5619,15 @@
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AugustineYoo25</v>
+        <v>AugustineYoo26</v>
       </c>
       <c r="B41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>AugustineYoo25</v>
+        <v>AugustineYoo26</v>
       </c>
       <c r="C41" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>AugustineYoo25@gmail.com</v>
+        <v>AugustineYoo26@gmail.com</v>
       </c>
       <c r="G41" t="s">
         <v>169</v>
@@ -5636,15 +5636,15 @@
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BrandiSouthard25</v>
+        <v>BrandiSouthard26</v>
       </c>
       <c r="B42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>BrandiSouthard25</v>
+        <v>BrandiSouthard26</v>
       </c>
       <c r="C42" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>BrandiSouthard25@gmail.com</v>
+        <v>BrandiSouthard26@gmail.com</v>
       </c>
       <c r="G42" t="s">
         <v>170</v>

</xml_diff>

<commit_message>
updated config, POM files
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data/Test_Data.xlsx
+++ b/src/main/resources/test_data/Test_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verkh\IdeaProjects\pom6\src\main\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D672741F-A8C5-4F13-A15C-4257C3F0AC18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B3A7D2-F881-40F1-A93B-F101B3C3BCAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1500" windowWidth="23040" windowHeight="12180" tabRatio="594" activeTab="1" xr2:uid="{56D596F5-221D-421D-9FC5-55182B639D44}"/>
+    <workbookView xWindow="0" yWindow="1500" windowWidth="23040" windowHeight="12180" tabRatio="594" xr2:uid="{56D596F5-221D-421D-9FC5-55182B639D44}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="2" r:id="rId1"/>
@@ -1048,126 +1048,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>EthanBaker23</t>
-  </si>
-  <si>
-    <t>EthanBaker23@gmail.com</t>
-  </si>
-  <si>
-    <t>DelanieCarman23</t>
-  </si>
-  <si>
-    <t>DelanieCarman23@gmail.com</t>
-  </si>
-  <si>
-    <t>BretAgnew23</t>
-  </si>
-  <si>
-    <t>BretAgnew23@gmail.com</t>
-  </si>
-  <si>
-    <t>EdgardoTaylor23</t>
-  </si>
-  <si>
-    <t>EdgardoTaylor23@gmail.com</t>
-  </si>
-  <si>
-    <t>TyrekReis23</t>
-  </si>
-  <si>
-    <t>TyrekReis23@gmail.com</t>
-  </si>
-  <si>
-    <t>LeannaChow23</t>
-  </si>
-  <si>
-    <t>LeannaChow23@gmail.com</t>
-  </si>
-  <si>
-    <t>TuckerCarlson23</t>
-  </si>
-  <si>
-    <t>TuckerCarlson23@gmail.com</t>
-  </si>
-  <si>
-    <t>AnnmarieConnor23</t>
-  </si>
-  <si>
-    <t>AnnmarieConnor23@gmail.com</t>
-  </si>
-  <si>
-    <t>MoniqueWitte23</t>
-  </si>
-  <si>
-    <t>MoniqueWitte23@gmail.com</t>
-  </si>
-  <si>
-    <t>MikelWhitlock23</t>
-  </si>
-  <si>
-    <t>MikelWhitlock23@gmail.com</t>
-  </si>
-  <si>
-    <t>VincentAmaya23</t>
-  </si>
-  <si>
-    <t>VincentAmaya23@gmail.com</t>
-  </si>
-  <si>
-    <t>KeiraQuiroz23</t>
-  </si>
-  <si>
-    <t>KeiraQuiroz23@gmail.com</t>
-  </si>
-  <si>
-    <t>EllisCreech23</t>
-  </si>
-  <si>
-    <t>EllisCreech23@gmail.com</t>
-  </si>
-  <si>
-    <t>DionteCreel23</t>
-  </si>
-  <si>
-    <t>DionteCreel23@gmail.com</t>
-  </si>
-  <si>
-    <t>NicholeFoust23</t>
-  </si>
-  <si>
-    <t>NicholeFoust23@gmail.com</t>
-  </si>
-  <si>
-    <t>ManuelConnell23</t>
-  </si>
-  <si>
-    <t>ManuelConnell23@gmail.com</t>
-  </si>
-  <si>
-    <t>LourdesElam23</t>
-  </si>
-  <si>
-    <t>LourdesElam23@gmail.com</t>
-  </si>
-  <si>
-    <t>LincolnFrederick23</t>
-  </si>
-  <si>
-    <t>LincolnFrederick23@gmail.com</t>
-  </si>
-  <si>
-    <t>AlisaCash23</t>
-  </si>
-  <si>
-    <t>AlisaCash23@gmail.com</t>
-  </si>
-  <si>
-    <t>LucilleGriffiths23</t>
-  </si>
-  <si>
-    <t>LucilleGriffiths23@gmail.com</t>
-  </si>
-  <si>
     <t>DonnellJernigan28</t>
   </si>
   <si>
@@ -1286,6 +1166,126 @@
   </si>
   <si>
     <t>BrandiSouthard28@gmail.com</t>
+  </si>
+  <si>
+    <t>EthanBaker24</t>
+  </si>
+  <si>
+    <t>EthanBaker24@gmail.com</t>
+  </si>
+  <si>
+    <t>DelanieCarman24</t>
+  </si>
+  <si>
+    <t>DelanieCarman24@gmail.com</t>
+  </si>
+  <si>
+    <t>BretAgnew24</t>
+  </si>
+  <si>
+    <t>BretAgnew24@gmail.com</t>
+  </si>
+  <si>
+    <t>EdgardoTaylor24</t>
+  </si>
+  <si>
+    <t>EdgardoTaylor24@gmail.com</t>
+  </si>
+  <si>
+    <t>TyrekReis24</t>
+  </si>
+  <si>
+    <t>TyrekReis24@gmail.com</t>
+  </si>
+  <si>
+    <t>LeannaChow24</t>
+  </si>
+  <si>
+    <t>LeannaChow24@gmail.com</t>
+  </si>
+  <si>
+    <t>TuckerCarlson24</t>
+  </si>
+  <si>
+    <t>TuckerCarlson24@gmail.com</t>
+  </si>
+  <si>
+    <t>AnnmarieConnor24</t>
+  </si>
+  <si>
+    <t>AnnmarieConnor24@gmail.com</t>
+  </si>
+  <si>
+    <t>MoniqueWitte24</t>
+  </si>
+  <si>
+    <t>MoniqueWitte24@gmail.com</t>
+  </si>
+  <si>
+    <t>MikelWhitlock24</t>
+  </si>
+  <si>
+    <t>MikelWhitlock24@gmail.com</t>
+  </si>
+  <si>
+    <t>VincentAmaya24</t>
+  </si>
+  <si>
+    <t>VincentAmaya24@gmail.com</t>
+  </si>
+  <si>
+    <t>KeiraQuiroz24</t>
+  </si>
+  <si>
+    <t>KeiraQuiroz24@gmail.com</t>
+  </si>
+  <si>
+    <t>EllisCreech24</t>
+  </si>
+  <si>
+    <t>EllisCreech24@gmail.com</t>
+  </si>
+  <si>
+    <t>DionteCreel24</t>
+  </si>
+  <si>
+    <t>DionteCreel24@gmail.com</t>
+  </si>
+  <si>
+    <t>NicholeFoust24</t>
+  </si>
+  <si>
+    <t>NicholeFoust24@gmail.com</t>
+  </si>
+  <si>
+    <t>ManuelConnell24</t>
+  </si>
+  <si>
+    <t>ManuelConnell24@gmail.com</t>
+  </si>
+  <si>
+    <t>LourdesElam24</t>
+  </si>
+  <si>
+    <t>LourdesElam24@gmail.com</t>
+  </si>
+  <si>
+    <t>LincolnFrederick24</t>
+  </si>
+  <si>
+    <t>LincolnFrederick24@gmail.com</t>
+  </si>
+  <si>
+    <t>AlisaCash24</t>
+  </si>
+  <si>
+    <t>AlisaCash24@gmail.com</t>
+  </si>
+  <si>
+    <t>LucilleGriffiths24</t>
+  </si>
+  <si>
+    <t>LucilleGriffiths24@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1976,7 +1976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{955D89E2-A883-499B-AA82-70224D6F8F96}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2:I21"/>
     </sheetView>
   </sheetViews>
@@ -2060,13 +2060,13 @@
         <v>51</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>336</v>
+        <v>376</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>336</v>
+        <v>376</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>337</v>
+        <v>377</v>
       </c>
       <c r="J2" s="21" t="s">
         <v>50</v>
@@ -2103,13 +2103,13 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>338</v>
+        <v>378</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>338</v>
+        <v>378</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>339</v>
+        <v>379</v>
       </c>
       <c r="J3" s="21" t="s">
         <v>50</v>
@@ -2145,13 +2145,13 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>340</v>
+        <v>380</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>340</v>
+        <v>380</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>341</v>
+        <v>381</v>
       </c>
       <c r="J4" s="21" t="s">
         <v>50</v>
@@ -2187,13 +2187,13 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>342</v>
+        <v>382</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>342</v>
+        <v>382</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>343</v>
+        <v>383</v>
       </c>
       <c r="J5" s="21" t="s">
         <v>50</v>
@@ -2229,13 +2229,13 @@
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>344</v>
+        <v>384</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>344</v>
+        <v>384</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>345</v>
+        <v>385</v>
       </c>
       <c r="J6" s="21" t="s">
         <v>50</v>
@@ -2271,13 +2271,13 @@
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>346</v>
+        <v>386</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>346</v>
+        <v>386</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>347</v>
+        <v>387</v>
       </c>
       <c r="J7" s="21" t="s">
         <v>50</v>
@@ -2313,13 +2313,13 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>348</v>
+        <v>388</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>348</v>
+        <v>388</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>349</v>
+        <v>389</v>
       </c>
       <c r="J8" s="21" t="s">
         <v>50</v>
@@ -2355,13 +2355,13 @@
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>350</v>
+        <v>390</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>350</v>
+        <v>390</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>351</v>
+        <v>391</v>
       </c>
       <c r="J9" s="21" t="s">
         <v>50</v>
@@ -2397,13 +2397,13 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>352</v>
+        <v>392</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>352</v>
+        <v>392</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>353</v>
+        <v>393</v>
       </c>
       <c r="J10" s="21" t="s">
         <v>50</v>
@@ -2439,13 +2439,13 @@
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>354</v>
+        <v>394</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>354</v>
+        <v>394</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>355</v>
+        <v>395</v>
       </c>
       <c r="J11" s="21" t="s">
         <v>50</v>
@@ -2481,13 +2481,13 @@
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>356</v>
+        <v>396</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>356</v>
+        <v>396</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>357</v>
+        <v>397</v>
       </c>
       <c r="J12" s="21" t="s">
         <v>50</v>
@@ -2523,13 +2523,13 @@
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>358</v>
+        <v>398</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>358</v>
+        <v>398</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>359</v>
+        <v>399</v>
       </c>
       <c r="J13" s="21" t="s">
         <v>50</v>
@@ -2565,13 +2565,13 @@
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>360</v>
+        <v>400</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>360</v>
+        <v>400</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>361</v>
+        <v>401</v>
       </c>
       <c r="J14" s="21" t="s">
         <v>50</v>
@@ -2607,13 +2607,13 @@
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>362</v>
+        <v>402</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>362</v>
+        <v>402</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>363</v>
+        <v>403</v>
       </c>
       <c r="J15" s="21" t="s">
         <v>50</v>
@@ -2649,13 +2649,13 @@
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>364</v>
+        <v>404</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>364</v>
+        <v>404</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>365</v>
+        <v>405</v>
       </c>
       <c r="J16" s="21" t="s">
         <v>50</v>
@@ -2691,13 +2691,13 @@
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>366</v>
+        <v>406</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>366</v>
+        <v>406</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>367</v>
+        <v>407</v>
       </c>
       <c r="J17" s="21" t="s">
         <v>50</v>
@@ -2733,13 +2733,13 @@
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="12" t="s">
-        <v>368</v>
+        <v>408</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>368</v>
+        <v>408</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>369</v>
+        <v>409</v>
       </c>
       <c r="J18" s="21" t="s">
         <v>50</v>
@@ -2775,13 +2775,13 @@
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="12" t="s">
-        <v>370</v>
+        <v>410</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>370</v>
+        <v>410</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>371</v>
+        <v>411</v>
       </c>
       <c r="J19" s="21" t="s">
         <v>50</v>
@@ -2817,13 +2817,13 @@
       </c>
       <c r="F20" s="12"/>
       <c r="G20" s="12" t="s">
-        <v>372</v>
+        <v>412</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>372</v>
+        <v>412</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>373</v>
+        <v>413</v>
       </c>
       <c r="J20" s="21" t="s">
         <v>50</v>
@@ -2859,13 +2859,13 @@
       </c>
       <c r="F21" s="12"/>
       <c r="G21" s="12" t="s">
-        <v>374</v>
+        <v>414</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>374</v>
+        <v>414</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>375</v>
+        <v>415</v>
       </c>
       <c r="J21" s="21" t="s">
         <v>50</v>
@@ -2900,7 +2900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0775DEA-3893-49AA-8C48-45DC29C761B9}">
   <dimension ref="A1:AF21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="R2" sqref="R2:T21"/>
     </sheetView>
   </sheetViews>
@@ -3082,13 +3082,13 @@
         <v>50</v>
       </c>
       <c r="R2" s="14" t="s">
-        <v>376</v>
+        <v>336</v>
       </c>
       <c r="S2" s="14" t="s">
-        <v>376</v>
+        <v>336</v>
       </c>
       <c r="T2" s="22" t="s">
-        <v>377</v>
+        <v>337</v>
       </c>
       <c r="U2" s="15" t="s">
         <v>130</v>
@@ -3175,13 +3175,13 @@
         <v>50</v>
       </c>
       <c r="R3" s="14" t="s">
-        <v>378</v>
+        <v>338</v>
       </c>
       <c r="S3" s="14" t="s">
-        <v>378</v>
+        <v>338</v>
       </c>
       <c r="T3" s="22" t="s">
-        <v>379</v>
+        <v>339</v>
       </c>
       <c r="U3" s="15" t="s">
         <v>130</v>
@@ -3268,13 +3268,13 @@
         <v>50</v>
       </c>
       <c r="R4" s="14" t="s">
-        <v>380</v>
+        <v>340</v>
       </c>
       <c r="S4" s="14" t="s">
-        <v>380</v>
+        <v>340</v>
       </c>
       <c r="T4" s="22" t="s">
-        <v>381</v>
+        <v>341</v>
       </c>
       <c r="U4" s="15" t="s">
         <v>130</v>
@@ -3361,13 +3361,13 @@
         <v>50</v>
       </c>
       <c r="R5" s="14" t="s">
-        <v>382</v>
+        <v>342</v>
       </c>
       <c r="S5" s="14" t="s">
-        <v>382</v>
+        <v>342</v>
       </c>
       <c r="T5" s="22" t="s">
-        <v>383</v>
+        <v>343</v>
       </c>
       <c r="U5" s="15" t="s">
         <v>130</v>
@@ -3454,13 +3454,13 @@
         <v>50</v>
       </c>
       <c r="R6" s="14" t="s">
-        <v>384</v>
+        <v>344</v>
       </c>
       <c r="S6" s="14" t="s">
-        <v>384</v>
+        <v>344</v>
       </c>
       <c r="T6" s="22" t="s">
-        <v>385</v>
+        <v>345</v>
       </c>
       <c r="U6" s="15" t="s">
         <v>130</v>
@@ -3547,13 +3547,13 @@
         <v>50</v>
       </c>
       <c r="R7" s="14" t="s">
-        <v>386</v>
+        <v>346</v>
       </c>
       <c r="S7" s="14" t="s">
-        <v>386</v>
+        <v>346</v>
       </c>
       <c r="T7" s="22" t="s">
-        <v>387</v>
+        <v>347</v>
       </c>
       <c r="U7" s="15" t="s">
         <v>130</v>
@@ -3640,13 +3640,13 @@
         <v>50</v>
       </c>
       <c r="R8" s="14" t="s">
-        <v>388</v>
+        <v>348</v>
       </c>
       <c r="S8" s="14" t="s">
-        <v>388</v>
+        <v>348</v>
       </c>
       <c r="T8" s="22" t="s">
-        <v>389</v>
+        <v>349</v>
       </c>
       <c r="U8" s="15" t="s">
         <v>130</v>
@@ -3733,13 +3733,13 @@
         <v>50</v>
       </c>
       <c r="R9" s="14" t="s">
-        <v>390</v>
+        <v>350</v>
       </c>
       <c r="S9" s="14" t="s">
-        <v>390</v>
+        <v>350</v>
       </c>
       <c r="T9" s="22" t="s">
-        <v>391</v>
+        <v>351</v>
       </c>
       <c r="U9" s="15" t="s">
         <v>130</v>
@@ -3826,13 +3826,13 @@
         <v>50</v>
       </c>
       <c r="R10" s="14" t="s">
-        <v>392</v>
+        <v>352</v>
       </c>
       <c r="S10" s="14" t="s">
-        <v>392</v>
+        <v>352</v>
       </c>
       <c r="T10" s="22" t="s">
-        <v>393</v>
+        <v>353</v>
       </c>
       <c r="U10" s="15" t="s">
         <v>130</v>
@@ -3919,13 +3919,13 @@
         <v>50</v>
       </c>
       <c r="R11" s="14" t="s">
-        <v>394</v>
+        <v>354</v>
       </c>
       <c r="S11" s="14" t="s">
-        <v>394</v>
+        <v>354</v>
       </c>
       <c r="T11" s="22" t="s">
-        <v>395</v>
+        <v>355</v>
       </c>
       <c r="U11" s="15" t="s">
         <v>130</v>
@@ -4012,13 +4012,13 @@
         <v>50</v>
       </c>
       <c r="R12" s="14" t="s">
-        <v>396</v>
+        <v>356</v>
       </c>
       <c r="S12" s="14" t="s">
-        <v>396</v>
+        <v>356</v>
       </c>
       <c r="T12" s="22" t="s">
-        <v>397</v>
+        <v>357</v>
       </c>
       <c r="U12" s="15" t="s">
         <v>130</v>
@@ -4105,13 +4105,13 @@
         <v>50</v>
       </c>
       <c r="R13" s="14" t="s">
-        <v>398</v>
+        <v>358</v>
       </c>
       <c r="S13" s="14" t="s">
-        <v>398</v>
+        <v>358</v>
       </c>
       <c r="T13" s="22" t="s">
-        <v>399</v>
+        <v>359</v>
       </c>
       <c r="U13" s="15" t="s">
         <v>130</v>
@@ -4198,13 +4198,13 @@
         <v>50</v>
       </c>
       <c r="R14" s="14" t="s">
-        <v>400</v>
+        <v>360</v>
       </c>
       <c r="S14" s="14" t="s">
-        <v>400</v>
+        <v>360</v>
       </c>
       <c r="T14" s="22" t="s">
-        <v>401</v>
+        <v>361</v>
       </c>
       <c r="U14" s="15" t="s">
         <v>130</v>
@@ -4291,13 +4291,13 @@
         <v>50</v>
       </c>
       <c r="R15" s="14" t="s">
-        <v>402</v>
+        <v>362</v>
       </c>
       <c r="S15" s="14" t="s">
-        <v>402</v>
+        <v>362</v>
       </c>
       <c r="T15" s="22" t="s">
-        <v>403</v>
+        <v>363</v>
       </c>
       <c r="U15" s="15" t="s">
         <v>130</v>
@@ -4384,13 +4384,13 @@
         <v>50</v>
       </c>
       <c r="R16" s="14" t="s">
-        <v>404</v>
+        <v>364</v>
       </c>
       <c r="S16" s="14" t="s">
-        <v>404</v>
+        <v>364</v>
       </c>
       <c r="T16" s="22" t="s">
-        <v>405</v>
+        <v>365</v>
       </c>
       <c r="U16" s="15" t="s">
         <v>130</v>
@@ -4477,13 +4477,13 @@
         <v>50</v>
       </c>
       <c r="R17" s="14" t="s">
-        <v>406</v>
+        <v>366</v>
       </c>
       <c r="S17" s="14" t="s">
-        <v>406</v>
+        <v>366</v>
       </c>
       <c r="T17" s="22" t="s">
-        <v>407</v>
+        <v>367</v>
       </c>
       <c r="U17" s="15" t="s">
         <v>130</v>
@@ -4569,13 +4569,13 @@
         <v>50</v>
       </c>
       <c r="R18" s="14" t="s">
-        <v>408</v>
+        <v>368</v>
       </c>
       <c r="S18" s="14" t="s">
-        <v>408</v>
+        <v>368</v>
       </c>
       <c r="T18" s="22" t="s">
-        <v>409</v>
+        <v>369</v>
       </c>
       <c r="U18" s="15" t="s">
         <v>130</v>
@@ -4661,13 +4661,13 @@
         <v>50</v>
       </c>
       <c r="R19" s="14" t="s">
-        <v>410</v>
+        <v>370</v>
       </c>
       <c r="S19" s="14" t="s">
-        <v>410</v>
+        <v>370</v>
       </c>
       <c r="T19" s="22" t="s">
-        <v>411</v>
+        <v>371</v>
       </c>
       <c r="U19" s="15" t="s">
         <v>130</v>
@@ -4753,13 +4753,13 @@
         <v>50</v>
       </c>
       <c r="R20" s="14" t="s">
-        <v>412</v>
+        <v>372</v>
       </c>
       <c r="S20" s="14" t="s">
-        <v>412</v>
+        <v>372</v>
       </c>
       <c r="T20" s="22" t="s">
-        <v>413</v>
+        <v>373</v>
       </c>
       <c r="U20" s="15" t="s">
         <v>130</v>
@@ -4845,13 +4845,13 @@
         <v>50</v>
       </c>
       <c r="R21" s="19" t="s">
-        <v>414</v>
+        <v>374</v>
       </c>
       <c r="S21" s="19" t="s">
-        <v>414</v>
+        <v>374</v>
       </c>
       <c r="T21" s="25" t="s">
-        <v>415</v>
+        <v>375</v>
       </c>
       <c r="U21" s="15" t="s">
         <v>130</v>
@@ -4919,8 +4919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FABAB06A-EAA7-4BA7-8A4C-8C5EF7E0517A}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:C42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4948,15 +4948,15 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="str">
         <f>CONCATENATE($G2,$I$2)</f>
-        <v>EthanBaker23</v>
+        <v>EthanBaker24</v>
       </c>
       <c r="B2" s="1" t="str">
         <f>CONCATENATE($G2,$I$2)</f>
-        <v>EthanBaker23</v>
+        <v>EthanBaker24</v>
       </c>
       <c r="C2" s="2" t="str">
         <f>CONCATENATE($G2,$I$2,$H$2)</f>
-        <v>EthanBaker23@gmail.com</v>
+        <v>EthanBaker24@gmail.com</v>
       </c>
       <c r="G2" t="s">
         <v>131</v>
@@ -4965,21 +4965,21 @@
         <v>71</v>
       </c>
       <c r="I2">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
         <f t="shared" ref="A3:B21" si="0">CONCATENATE($G3,$I$2)</f>
-        <v>DelanieCarman23</v>
+        <v>DelanieCarman24</v>
       </c>
       <c r="B3" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DelanieCarman23</v>
+        <v>DelanieCarman24</v>
       </c>
       <c r="C3" s="2" t="str">
         <f t="shared" ref="C3:C21" si="1">CONCATENATE($G3,$I$2,$H$2)</f>
-        <v>DelanieCarman23@gmail.com</v>
+        <v>DelanieCarman24@gmail.com</v>
       </c>
       <c r="G3" t="s">
         <v>132</v>
@@ -4988,15 +4988,15 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>BretAgnew23</v>
+        <v>BretAgnew24</v>
       </c>
       <c r="B4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>BretAgnew23</v>
+        <v>BretAgnew24</v>
       </c>
       <c r="C4" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>BretAgnew23@gmail.com</v>
+        <v>BretAgnew24@gmail.com</v>
       </c>
       <c r="G4" t="s">
         <v>133</v>
@@ -5005,15 +5005,15 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EdgardoTaylor23</v>
+        <v>EdgardoTaylor24</v>
       </c>
       <c r="B5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EdgardoTaylor23</v>
+        <v>EdgardoTaylor24</v>
       </c>
       <c r="C5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>EdgardoTaylor23@gmail.com</v>
+        <v>EdgardoTaylor24@gmail.com</v>
       </c>
       <c r="G5" t="s">
         <v>134</v>
@@ -5022,15 +5022,15 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TyrekReis23</v>
+        <v>TyrekReis24</v>
       </c>
       <c r="B6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TyrekReis23</v>
+        <v>TyrekReis24</v>
       </c>
       <c r="C6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>TyrekReis23@gmail.com</v>
+        <v>TyrekReis24@gmail.com</v>
       </c>
       <c r="G6" t="s">
         <v>135</v>
@@ -5039,15 +5039,15 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LeannaChow23</v>
+        <v>LeannaChow24</v>
       </c>
       <c r="B7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LeannaChow23</v>
+        <v>LeannaChow24</v>
       </c>
       <c r="C7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LeannaChow23@gmail.com</v>
+        <v>LeannaChow24@gmail.com</v>
       </c>
       <c r="G7" t="s">
         <v>136</v>
@@ -5056,15 +5056,15 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TuckerCarlson23</v>
+        <v>TuckerCarlson24</v>
       </c>
       <c r="B8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>TuckerCarlson23</v>
+        <v>TuckerCarlson24</v>
       </c>
       <c r="C8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>TuckerCarlson23@gmail.com</v>
+        <v>TuckerCarlson24@gmail.com</v>
       </c>
       <c r="G8" t="s">
         <v>137</v>
@@ -5073,15 +5073,15 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AnnmarieConnor23</v>
+        <v>AnnmarieConnor24</v>
       </c>
       <c r="B9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AnnmarieConnor23</v>
+        <v>AnnmarieConnor24</v>
       </c>
       <c r="C9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>AnnmarieConnor23@gmail.com</v>
+        <v>AnnmarieConnor24@gmail.com</v>
       </c>
       <c r="G9" t="s">
         <v>138</v>
@@ -5090,15 +5090,15 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MoniqueWitte23</v>
+        <v>MoniqueWitte24</v>
       </c>
       <c r="B10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MoniqueWitte23</v>
+        <v>MoniqueWitte24</v>
       </c>
       <c r="C10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MoniqueWitte23@gmail.com</v>
+        <v>MoniqueWitte24@gmail.com</v>
       </c>
       <c r="G10" t="s">
         <v>139</v>
@@ -5107,15 +5107,15 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MikelWhitlock23</v>
+        <v>MikelWhitlock24</v>
       </c>
       <c r="B11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>MikelWhitlock23</v>
+        <v>MikelWhitlock24</v>
       </c>
       <c r="C11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MikelWhitlock23@gmail.com</v>
+        <v>MikelWhitlock24@gmail.com</v>
       </c>
       <c r="G11" t="s">
         <v>140</v>
@@ -5124,15 +5124,15 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>VincentAmaya23</v>
+        <v>VincentAmaya24</v>
       </c>
       <c r="B12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>VincentAmaya23</v>
+        <v>VincentAmaya24</v>
       </c>
       <c r="C12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>VincentAmaya23@gmail.com</v>
+        <v>VincentAmaya24@gmail.com</v>
       </c>
       <c r="G12" t="s">
         <v>141</v>
@@ -5141,15 +5141,15 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>KeiraQuiroz23</v>
+        <v>KeiraQuiroz24</v>
       </c>
       <c r="B13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>KeiraQuiroz23</v>
+        <v>KeiraQuiroz24</v>
       </c>
       <c r="C13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>KeiraQuiroz23@gmail.com</v>
+        <v>KeiraQuiroz24@gmail.com</v>
       </c>
       <c r="G13" t="s">
         <v>142</v>
@@ -5158,15 +5158,15 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EllisCreech23</v>
+        <v>EllisCreech24</v>
       </c>
       <c r="B14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>EllisCreech23</v>
+        <v>EllisCreech24</v>
       </c>
       <c r="C14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>EllisCreech23@gmail.com</v>
+        <v>EllisCreech24@gmail.com</v>
       </c>
       <c r="G14" t="s">
         <v>143</v>
@@ -5175,15 +5175,15 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DionteCreel23</v>
+        <v>DionteCreel24</v>
       </c>
       <c r="B15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>DionteCreel23</v>
+        <v>DionteCreel24</v>
       </c>
       <c r="C15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DionteCreel23@gmail.com</v>
+        <v>DionteCreel24@gmail.com</v>
       </c>
       <c r="G15" t="s">
         <v>144</v>
@@ -5192,15 +5192,15 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NicholeFoust23</v>
+        <v>NicholeFoust24</v>
       </c>
       <c r="B16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NicholeFoust23</v>
+        <v>NicholeFoust24</v>
       </c>
       <c r="C16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>NicholeFoust23@gmail.com</v>
+        <v>NicholeFoust24@gmail.com</v>
       </c>
       <c r="G16" t="s">
         <v>145</v>
@@ -5209,15 +5209,15 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>ManuelConnell23</v>
+        <v>ManuelConnell24</v>
       </c>
       <c r="B17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>ManuelConnell23</v>
+        <v>ManuelConnell24</v>
       </c>
       <c r="C17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>ManuelConnell23@gmail.com</v>
+        <v>ManuelConnell24@gmail.com</v>
       </c>
       <c r="G17" t="s">
         <v>146</v>
@@ -5226,15 +5226,15 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LourdesElam23</v>
+        <v>LourdesElam24</v>
       </c>
       <c r="B18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LourdesElam23</v>
+        <v>LourdesElam24</v>
       </c>
       <c r="C18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LourdesElam23@gmail.com</v>
+        <v>LourdesElam24@gmail.com</v>
       </c>
       <c r="G18" t="s">
         <v>147</v>
@@ -5243,15 +5243,15 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LincolnFrederick23</v>
+        <v>LincolnFrederick24</v>
       </c>
       <c r="B19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LincolnFrederick23</v>
+        <v>LincolnFrederick24</v>
       </c>
       <c r="C19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LincolnFrederick23@gmail.com</v>
+        <v>LincolnFrederick24@gmail.com</v>
       </c>
       <c r="G19" t="s">
         <v>148</v>
@@ -5260,15 +5260,15 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AlisaCash23</v>
+        <v>AlisaCash24</v>
       </c>
       <c r="B20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>AlisaCash23</v>
+        <v>AlisaCash24</v>
       </c>
       <c r="C20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>AlisaCash23@gmail.com</v>
+        <v>AlisaCash24@gmail.com</v>
       </c>
       <c r="G20" t="s">
         <v>149</v>
@@ -5277,15 +5277,15 @@
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LucilleGriffiths23</v>
+        <v>LucilleGriffiths24</v>
       </c>
       <c r="B21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>LucilleGriffiths23</v>
+        <v>LucilleGriffiths24</v>
       </c>
       <c r="C21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LucilleGriffiths23@gmail.com</v>
+        <v>LucilleGriffiths24@gmail.com</v>
       </c>
       <c r="G21" t="s">
         <v>150</v>

</xml_diff>